<commit_message>
📊 Horarios actualizados Línea 141 - 810
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-23.xlsx
+++ b/data/horarios-141-2026-01-23.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 00:07:17</t>
+          <t>Última actualización: 01:10:33</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 2</t>
+          <t>Total filas: 3</t>
         </is>
       </c>
     </row>
@@ -478,7 +478,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>00:07:17</t>
+          <t>01:10:32</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>65</v>
+        <v>2</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -503,7 +503,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>00:07:17</t>
+          <t>01:10:32</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -517,9 +517,34 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>111</v>
+        <v>48</v>
       </c>
       <c r="E7" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>01:10:32</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>02:58</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>108</v>
+      </c>
+      <c r="E8" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -536,7 +561,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -554,14 +579,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 00:07:17</t>
+          <t>Última actualización: 01:10:33</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 1</t>
+          <t>Total filas: 2</t>
         </is>
       </c>
     </row>
@@ -595,7 +620,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>00:07:17</t>
+          <t>01:10:32</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -609,9 +634,34 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>65</v>
+        <v>2</v>
       </c>
       <c r="E6" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>01:10:32</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>02:58</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>108</v>
+      </c>
+      <c r="E7" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -646,7 +696,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 00:07:17</t>
+          <t>Última actualización: 01:10:33</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 811
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-23.xlsx
+++ b/data/horarios-141-2026-01-23.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 01:10:33</t>
+          <t>Última actualización: 01:55:51</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 3</t>
+          <t>Total filas: 5</t>
         </is>
       </c>
     </row>
@@ -503,7 +503,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>01:10:32</t>
+          <t>01:55:51</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -517,7 +517,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>48</v>
+        <v>3</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -545,6 +545,56 @@
         <v>108</v>
       </c>
       <c r="E8" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>01:55:51</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>03:12</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>77</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>01:55:51</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>03:48</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>113</v>
+      </c>
+      <c r="E10" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -561,7 +611,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -579,14 +629,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 01:10:33</t>
+          <t>Última actualización: 01:55:51</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 2</t>
+          <t>Total filas: 3</t>
         </is>
       </c>
     </row>
@@ -662,6 +712,31 @@
         <v>108</v>
       </c>
       <c r="E7" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>01:55:51</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>03:12</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>77</v>
+      </c>
+      <c r="E8" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -696,7 +771,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 01:10:33</t>
+          <t>Última actualización: 01:55:51</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 812
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-23.xlsx
+++ b/data/horarios-141-2026-01-23.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 01:55:51</t>
+          <t>Última actualización: 02:21:47</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 5</t>
+          <t>Total filas: 7</t>
         </is>
       </c>
     </row>
@@ -528,7 +528,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>01:10:32</t>
+          <t>02:21:47</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -542,7 +542,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>108</v>
+        <v>37</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -595,6 +595,56 @@
         <v>113</v>
       </c>
       <c r="E10" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>02:21:47</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>03:56</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>95</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>02:21:47</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>04:01</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>100</v>
+      </c>
+      <c r="E12" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -629,7 +679,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 01:55:51</t>
+          <t>Última actualización: 02:21:47</t>
         </is>
       </c>
     </row>
@@ -695,7 +745,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>01:10:32</t>
+          <t>02:21:47</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -709,7 +759,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>108</v>
+        <v>37</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -771,7 +821,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 01:55:51</t>
+          <t>Última actualización: 02:21:47</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 813
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-23.xlsx
+++ b/data/horarios-141-2026-01-23.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 02:21:47</t>
+          <t>Última actualización: 02:48:52</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 7</t>
+          <t>Total filas: 9</t>
         </is>
       </c>
     </row>
@@ -528,12 +528,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>02:21:47</t>
+          <t>02:48:52</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>02:58</t>
+          <t>02:57</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -542,7 +542,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -553,12 +553,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>01:55:51</t>
+          <t>02:21:47</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>03:12</t>
+          <t>02:58</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -567,7 +567,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>77</v>
+        <v>37</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -583,16 +583,16 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>03:48</t>
+          <t>03:12</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>113</v>
+        <v>77</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -603,12 +603,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>02:21:47</t>
+          <t>02:48:52</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>03:56</t>
+          <t>03:48</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -617,7 +617,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>95</v>
+        <v>60</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -633,18 +633,68 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
+          <t>03:56</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>95</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>02:48:52</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
           <t>04:01</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="C13" t="inlineStr">
         <is>
           <t>81_EL PELIGRO</t>
         </is>
       </c>
-      <c r="D12" t="n">
-        <v>100</v>
-      </c>
-      <c r="E12" t="inlineStr">
+      <c r="D13" t="n">
+        <v>73</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>02:48:52</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>04:45</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>117</v>
+      </c>
+      <c r="E14" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -661,7 +711,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -679,14 +729,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 02:21:47</t>
+          <t>Última actualización: 02:48:52</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 3</t>
+          <t>Total filas: 5</t>
         </is>
       </c>
     </row>
@@ -745,12 +795,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>02:21:47</t>
+          <t>02:48:52</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>02:58</t>
+          <t>02:57</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -759,7 +809,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -770,23 +820,73 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>02:21:47</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>02:58</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>37</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
           <t>01:55:51</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B9" t="inlineStr">
         <is>
           <t>03:12</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>215_ALUAR</t>
         </is>
       </c>
-      <c r="D8" t="n">
+      <c r="D9" t="n">
         <v>77</v>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>02:48:52</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>04:45</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>117</v>
+      </c>
+      <c r="E10" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -821,7 +921,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 02:21:47</t>
+          <t>Última actualización: 02:48:52</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 814
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-23.xlsx
+++ b/data/horarios-141-2026-01-23.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 02:48:52</t>
+          <t>Última actualización: 02:58:51</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 9</t>
+          <t>Total filas: 10</t>
         </is>
       </c>
     </row>
@@ -553,7 +553,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>02:21:47</t>
+          <t>02:58:51</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -567,7 +567,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -603,7 +603,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>02:48:52</t>
+          <t>02:58:51</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -617,7 +617,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -653,7 +653,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>02:48:52</t>
+          <t>02:58:51</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -667,7 +667,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -678,7 +678,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>02:48:52</t>
+          <t>02:58:51</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -692,9 +692,34 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="E14" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>02:58:51</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>04:53</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>115</v>
+      </c>
+      <c r="E15" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -729,7 +754,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 02:48:52</t>
+          <t>Última actualización: 02:58:51</t>
         </is>
       </c>
     </row>
@@ -820,7 +845,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>02:21:47</t>
+          <t>02:58:51</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -834,7 +859,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -870,7 +895,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>02:48:52</t>
+          <t>02:58:51</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -884,7 +909,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -921,7 +946,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 02:48:52</t>
+          <t>Última actualización: 02:58:51</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 815
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-23.xlsx
+++ b/data/horarios-141-2026-01-23.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 02:58:51</t>
+          <t>Última actualización: 03:35:49</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 10</t>
+          <t>Total filas: 15</t>
         </is>
       </c>
     </row>
@@ -603,12 +603,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>02:58:51</t>
+          <t>03:35:49</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>03:48</t>
+          <t>03:38</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -617,7 +617,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -628,12 +628,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>02:21:47</t>
+          <t>02:58:51</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>03:56</t>
+          <t>03:48</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>95</v>
+        <v>50</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -653,21 +653,21 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>02:58:51</t>
+          <t>02:21:47</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>04:01</t>
+          <t>03:56</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>63</v>
+        <v>95</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -678,21 +678,21 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>02:58:51</t>
+          <t>03:35:49</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>04:45</t>
+          <t>04:01</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>107</v>
+        <v>26</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -703,23 +703,148 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>02:58:51</t>
+          <t>03:35:49</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
+          <t>04:45</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>70</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>03:35:49</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
           <t>04:53</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="C16" t="inlineStr">
         <is>
           <t>11_ETCHEVERRY</t>
         </is>
       </c>
-      <c r="D15" t="n">
-        <v>115</v>
-      </c>
-      <c r="E15" t="inlineStr">
+      <c r="D16" t="n">
+        <v>78</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>03:35:49</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>05:16</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>101</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>03:35:49</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>05:22</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>107</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>03:35:49</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>05:28</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>113</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>03:35:49</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>05:34</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>119</v>
+      </c>
+      <c r="E20" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -736,7 +861,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -754,14 +879,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 02:58:51</t>
+          <t>Última actualización: 03:35:49</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 5</t>
+          <t>Total filas: 6</t>
         </is>
       </c>
     </row>
@@ -895,7 +1020,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>02:58:51</t>
+          <t>03:35:49</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -909,9 +1034,34 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>107</v>
+        <v>70</v>
       </c>
       <c r="E10" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>03:35:49</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>05:34</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>119</v>
+      </c>
+      <c r="E11" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -946,7 +1096,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 02:58:51</t>
+          <t>Última actualización: 03:35:49</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 816
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-23.xlsx
+++ b/data/horarios-141-2026-01-23.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 03:35:49</t>
+          <t>Última actualización: 04:01:13</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 15</t>
+          <t>Total filas: 19</t>
         </is>
       </c>
     </row>
@@ -678,7 +678,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>03:35:49</t>
+          <t>04:01:13</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -692,7 +692,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -728,21 +728,21 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>03:35:49</t>
+          <t>04:01:13</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>04:53</t>
+          <t>04:46</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>78</v>
+        <v>45</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -753,21 +753,21 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>03:35:49</t>
+          <t>04:01:13</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>05:16</t>
+          <t>04:53</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>101</v>
+        <v>52</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -778,21 +778,21 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>03:35:49</t>
+          <t>04:01:13</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>05:22</t>
+          <t>05:16</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>107</v>
+        <v>75</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -803,21 +803,21 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>03:35:49</t>
+          <t>04:01:13</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>05:28</t>
+          <t>05:22</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>113</v>
+        <v>81</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -833,18 +833,118 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
+          <t>05:28</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>113</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>03:35:49</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
           <t>05:34</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="C21" t="inlineStr">
         <is>
           <t>215B_EL PATO</t>
         </is>
       </c>
-      <c r="D20" t="n">
+      <c r="D21" t="n">
         <v>119</v>
       </c>
-      <c r="E20" t="inlineStr">
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>04:01:13</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>05:35</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>94</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>04:01:13</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>05:37</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>96</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>04:01:13</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>05:46</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>105</v>
+      </c>
+      <c r="E24" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -861,7 +961,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -879,14 +979,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 03:35:49</t>
+          <t>Última actualización: 04:01:13</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 6</t>
+          <t>Total filas: 8</t>
         </is>
       </c>
     </row>
@@ -1045,23 +1145,73 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>04:01:13</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>04:46</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>45</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
           <t>03:35:49</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B12" t="inlineStr">
         <is>
           <t>05:34</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C12" t="inlineStr">
         <is>
           <t>215B_EL PATO</t>
         </is>
       </c>
-      <c r="D11" t="n">
+      <c r="D12" t="n">
         <v>119</v>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>04:01:13</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>05:35</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>94</v>
+      </c>
+      <c r="E13" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1078,7 +1228,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1096,14 +1246,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 03:35:49</t>
+          <t>Última actualización: 04:01:13</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 1</t>
+          <t>Total filas: 2</t>
         </is>
       </c>
     </row>
@@ -1154,6 +1304,31 @@
         <v>1</v>
       </c>
       <c r="E6" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>04:01:13</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>05:44</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>103</v>
+      </c>
+      <c r="E7" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 817
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-23.xlsx
+++ b/data/horarios-141-2026-01-23.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:01:13</t>
+          <t>Última actualización: 04:35:25</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 19</t>
+          <t>Total filas: 27</t>
         </is>
       </c>
     </row>
@@ -728,7 +728,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>04:01:13</t>
+          <t>04:35:25</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -742,7 +742,7 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>45</v>
+        <v>11</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -753,7 +753,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>04:01:13</t>
+          <t>04:35:25</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -767,7 +767,7 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>52</v>
+        <v>18</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -778,21 +778,21 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>04:01:13</t>
+          <t>04:35:25</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>05:16</t>
+          <t>05:15</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>75</v>
+        <v>40</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -803,21 +803,21 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>04:01:13</t>
+          <t>04:35:25</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>05:22</t>
+          <t>05:16</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>81</v>
+        <v>41</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -828,21 +828,21 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>03:35:49</t>
+          <t>04:35:25</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>05:28</t>
+          <t>05:22</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>113</v>
+        <v>47</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -858,16 +858,16 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>05:34</t>
+          <t>05:28</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -878,12 +878,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>04:01:13</t>
+          <t>04:35:25</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>05:35</t>
+          <t>05:34</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -892,7 +892,7 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>94</v>
+        <v>59</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -908,16 +908,16 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>05:37</t>
+          <t>05:35</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -933,18 +933,218 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
+          <t>05:37</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>96</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>04:35:25</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
           <t>05:46</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
+      <c r="C25" t="inlineStr">
         <is>
           <t>15_ABASTO</t>
         </is>
       </c>
-      <c r="D24" t="n">
-        <v>105</v>
-      </c>
-      <c r="E24" t="inlineStr">
+      <c r="D25" t="n">
+        <v>71</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>04:35:25</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>06:04</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>89</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>04:35:25</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>06:11</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>96</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>04:35:25</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>06:14</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>225_HARAS DEL SUR</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>99</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>04:35:25</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>06:21</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>106</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>04:35:25</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>06:27</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>112</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>04:35:25</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>06:29</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>86_EST CHICA-ESC AGRARIA</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>114</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>04:35:25</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>06:31</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>116</v>
+      </c>
+      <c r="E32" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -961,7 +1161,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -979,14 +1179,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:01:13</t>
+          <t>Última actualización: 04:35:25</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 8</t>
+          <t>Total filas: 9</t>
         </is>
       </c>
     </row>
@@ -1145,7 +1345,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>04:01:13</t>
+          <t>04:35:25</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1159,7 +1359,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>45</v>
+        <v>11</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -1170,7 +1370,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>03:35:49</t>
+          <t>04:35:25</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1184,7 +1384,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>119</v>
+        <v>59</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -1212,6 +1412,31 @@
         <v>94</v>
       </c>
       <c r="E13" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>04:35:25</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>06:11</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>96</v>
+      </c>
+      <c r="E14" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1228,7 +1453,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1246,14 +1471,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:01:13</t>
+          <t>Última actualización: 04:35:25</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 2</t>
+          <t>Total filas: 4</t>
         </is>
       </c>
     </row>
@@ -1312,7 +1537,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>04:01:13</t>
+          <t>04:35:25</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -1326,11 +1551,61 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>103</v>
+        <v>69</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
           <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>04:35:25</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>06:09</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>94</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>04:35:25</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>06:33</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>118</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 818
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-23.xlsx
+++ b/data/horarios-141-2026-01-23.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:35:25</t>
+          <t>Última actualización: 04:48:57</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 27</t>
+          <t>Total filas: 34</t>
         </is>
       </c>
     </row>
@@ -753,7 +753,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>04:35:25</t>
+          <t>04:48:57</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -767,7 +767,7 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -778,12 +778,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>04:35:25</t>
+          <t>04:48:57</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>05:15</t>
+          <t>05:14</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -792,7 +792,7 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -808,16 +808,16 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>05:16</t>
+          <t>05:15</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -828,21 +828,21 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>04:35:25</t>
+          <t>04:48:57</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>05:22</t>
+          <t>05:16</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -853,21 +853,21 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>03:35:49</t>
+          <t>04:48:57</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>05:28</t>
+          <t>05:21</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>113</v>
+        <v>33</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -883,16 +883,16 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>05:34</t>
+          <t>05:22</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -903,21 +903,21 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>04:01:13</t>
+          <t>03:35:49</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>05:35</t>
+          <t>05:28</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>94</v>
+        <v>113</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -928,21 +928,21 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>04:01:13</t>
+          <t>04:48:57</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>05:37</t>
+          <t>05:34</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>96</v>
+        <v>46</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -953,21 +953,21 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>04:35:25</t>
+          <t>04:01:13</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>05:46</t>
+          <t>05:35</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>71</v>
+        <v>94</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -978,21 +978,21 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>04:35:25</t>
+          <t>04:01:13</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>06:04</t>
+          <t>05:37</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -1003,21 +1003,21 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>04:35:25</t>
+          <t>04:48:57</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>06:11</t>
+          <t>05:46</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>96</v>
+        <v>58</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -1028,21 +1028,21 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>04:35:25</t>
+          <t>04:48:57</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>06:14</t>
+          <t>06:04</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>225_HARAS DEL SUR</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>99</v>
+        <v>76</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1053,21 +1053,21 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>04:35:25</t>
+          <t>04:48:57</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>06:21</t>
+          <t>06:11</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1078,21 +1078,21 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>04:35:25</t>
+          <t>04:48:57</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>06:27</t>
+          <t>06:13</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_HARAS DEL SUR</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>112</v>
+        <v>85</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1108,16 +1108,16 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>06:29</t>
+          <t>06:14</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>86_EST CHICA-ESC AGRARIA</t>
+          <t>225_HARAS DEL SUR</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1128,23 +1128,198 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
+          <t>04:48:57</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>06:20</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>92</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
           <t>04:35:25</t>
         </is>
       </c>
-      <c r="B32" t="inlineStr">
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>06:21</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>106</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>04:48:57</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>06:26</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>98</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>04:35:25</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>06:27</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>112</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>04:48:57</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>06:29</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>86_EST CHICA-ESC AGRARIA</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>101</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>04:48:57</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
         <is>
           <t>06:31</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr">
+      <c r="C37" t="inlineStr">
         <is>
           <t>16_SANTA ANA</t>
         </is>
       </c>
-      <c r="D32" t="n">
-        <v>116</v>
-      </c>
-      <c r="E32" t="inlineStr">
+      <c r="D37" t="n">
+        <v>103</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>04:48:57</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>06:43</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>225_C ROCA-H SUR</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>115</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>04:48:57</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>06:46</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>118</v>
+      </c>
+      <c r="E39" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1161,7 +1336,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1179,14 +1354,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:35:25</t>
+          <t>Última actualización: 04:48:57</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 9</t>
+          <t>Total filas: 10</t>
         </is>
       </c>
     </row>
@@ -1370,7 +1545,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>04:35:25</t>
+          <t>04:48:57</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1384,7 +1559,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -1420,7 +1595,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>04:35:25</t>
+          <t>04:48:57</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1434,9 +1609,34 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E14" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>04:48:57</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>06:46</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>118</v>
+      </c>
+      <c r="E15" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1453,7 +1653,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1471,14 +1671,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:35:25</t>
+          <t>Última actualización: 04:48:57</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 4</t>
+          <t>Total filas: 7</t>
         </is>
       </c>
     </row>
@@ -1537,12 +1737,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>04:35:25</t>
+          <t>04:48:57</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>05:44</t>
+          <t>05:43</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1551,7 +1751,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -1567,7 +1767,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>06:09</t>
+          <t>05:44</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -1576,7 +1776,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>94</v>
+        <v>69</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -1587,23 +1787,98 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>04:48:57</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>06:08</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>80</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
           <t>04:35:25</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>06:09</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>94</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>04:48:57</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>06:32</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>104</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>04:35:25</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
         <is>
           <t>06:33</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C12" t="inlineStr">
         <is>
           <t>215C_LA PLATA</t>
         </is>
       </c>
-      <c r="D9" t="n">
+      <c r="D12" t="n">
         <v>118</v>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="E12" t="inlineStr">
         <is>
           <t>L6203</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 819
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-23.xlsx
+++ b/data/horarios-141-2026-01-23.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:48:57</t>
+          <t>Última actualización: 04:56:11</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 34</t>
+          <t>Total filas: 38</t>
         </is>
       </c>
     </row>
@@ -828,7 +828,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>04:48:57</t>
+          <t>04:56:11</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -842,7 +842,7 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -878,7 +878,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>04:35:25</t>
+          <t>04:56:11</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -892,7 +892,7 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -953,7 +953,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>04:01:13</t>
+          <t>04:56:11</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -967,7 +967,7 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>94</v>
+        <v>39</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -1003,7 +1003,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>04:48:57</t>
+          <t>04:56:11</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1017,7 +1017,7 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -1028,21 +1028,21 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>04:48:57</t>
+          <t>04:56:11</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>06:04</t>
+          <t>05:54</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1053,21 +1053,21 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>04:48:57</t>
+          <t>04:56:11</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>06:11</t>
+          <t>06:04</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1078,21 +1078,21 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>04:48:57</t>
+          <t>04:56:11</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>06:13</t>
+          <t>06:11</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>225_HARAS DEL SUR</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1103,12 +1103,12 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>04:35:25</t>
+          <t>04:48:57</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>06:14</t>
+          <t>06:13</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1117,7 +1117,7 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1128,21 +1128,21 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>04:48:57</t>
+          <t>04:56:11</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>06:20</t>
+          <t>06:14</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>225_HARAS DEL SUR</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -1153,12 +1153,12 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>04:35:25</t>
+          <t>04:48:57</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>06:21</t>
+          <t>06:20</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1167,7 +1167,7 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1178,21 +1178,21 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>04:48:57</t>
+          <t>04:56:11</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>06:26</t>
+          <t>06:21</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1203,12 +1203,12 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>04:35:25</t>
+          <t>04:48:57</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>06:27</t>
+          <t>06:26</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1217,7 +1217,7 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1228,21 +1228,21 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>04:48:57</t>
+          <t>04:56:11</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>06:29</t>
+          <t>06:27</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>86_EST CHICA-ESC AGRARIA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1258,16 +1258,16 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>06:31</t>
+          <t>06:29</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>86_EST CHICA-ESC AGRARIA</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -1278,21 +1278,21 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>04:48:57</t>
+          <t>04:56:11</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>06:43</t>
+          <t>06:30</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>86_EST CHICA-ESC AGRARIA</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>115</v>
+        <v>94</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -1303,23 +1303,123 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
+          <t>04:56:11</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>06:31</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>95</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
           <t>04:48:57</t>
         </is>
       </c>
-      <c r="B39" t="inlineStr">
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>06:43</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>225_C ROCA-H SUR</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>115</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>04:56:11</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>06:44</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>225_C ROCA-H SUR</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>108</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>04:48:57</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
         <is>
           <t>06:46</t>
         </is>
       </c>
-      <c r="C39" t="inlineStr">
+      <c r="C42" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D39" t="n">
+      <c r="D42" t="n">
         <v>118</v>
       </c>
-      <c r="E39" t="inlineStr">
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>04:56:11</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>06:47</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>111</v>
+      </c>
+      <c r="E43" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1336,7 +1436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1354,14 +1454,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:48:57</t>
+          <t>Última actualización: 04:56:11</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 10</t>
+          <t>Total filas: 11</t>
         </is>
       </c>
     </row>
@@ -1570,7 +1670,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>04:01:13</t>
+          <t>04:56:11</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1584,7 +1684,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>94</v>
+        <v>39</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -1595,7 +1695,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>04:48:57</t>
+          <t>04:56:11</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1609,7 +1709,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -1637,6 +1737,31 @@
         <v>118</v>
       </c>
       <c r="E15" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>04:56:11</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>06:47</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>111</v>
+      </c>
+      <c r="E16" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1671,7 +1796,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:48:57</t>
+          <t>Última actualización: 04:56:11</t>
         </is>
       </c>
     </row>
@@ -1762,7 +1887,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>04:35:25</t>
+          <t>04:56:11</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -1776,7 +1901,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -1812,7 +1937,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>04:35:25</t>
+          <t>04:56:11</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1826,7 +1951,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -1862,7 +1987,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>04:35:25</t>
+          <t>04:56:11</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1876,7 +2001,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 820
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-23.xlsx
+++ b/data/horarios-141-2026-01-23.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:56:11</t>
+          <t>Última actualización: 05:21:16</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 38</t>
+          <t>Total filas: 44</t>
         </is>
       </c>
     </row>
@@ -903,21 +903,21 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>03:35:49</t>
+          <t>05:21:16</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>05:28</t>
+          <t>05:26</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>113</v>
+        <v>5</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -928,21 +928,21 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>04:48:57</t>
+          <t>03:35:49</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>05:34</t>
+          <t>05:28</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>46</v>
+        <v>113</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -953,12 +953,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>04:56:11</t>
+          <t>04:48:57</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>05:35</t>
+          <t>05:34</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -967,7 +967,7 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -978,21 +978,21 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>04:01:13</t>
+          <t>05:21:16</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>05:37</t>
+          <t>05:35</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>96</v>
+        <v>14</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -1003,21 +1003,21 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>04:56:11</t>
+          <t>04:01:13</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>05:46</t>
+          <t>05:37</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>50</v>
+        <v>96</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -1028,21 +1028,21 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>04:56:11</t>
+          <t>05:21:16</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>05:54</t>
+          <t>05:46</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>58</v>
+        <v>25</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1053,21 +1053,21 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>04:56:11</t>
+          <t>05:21:16</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>06:04</t>
+          <t>05:54</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>68</v>
+        <v>33</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1078,21 +1078,21 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>04:56:11</t>
+          <t>05:21:16</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>06:11</t>
+          <t>06:04</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>75</v>
+        <v>43</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1103,21 +1103,21 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>04:48:57</t>
+          <t>05:21:16</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>06:13</t>
+          <t>06:11</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>225_HARAS DEL SUR</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1128,12 +1128,12 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>04:56:11</t>
+          <t>04:48:57</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>06:14</t>
+          <t>06:13</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1142,7 +1142,7 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -1153,21 +1153,21 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>04:48:57</t>
+          <t>05:21:16</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>06:20</t>
+          <t>06:14</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>225_HARAS DEL SUR</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>92</v>
+        <v>53</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1178,12 +1178,12 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>04:56:11</t>
+          <t>04:48:57</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>06:21</t>
+          <t>06:20</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1192,7 +1192,7 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1203,21 +1203,21 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>04:48:57</t>
+          <t>05:21:16</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>06:26</t>
+          <t>06:21</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>98</v>
+        <v>60</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1228,12 +1228,12 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>04:56:11</t>
+          <t>04:48:57</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>06:27</t>
+          <t>06:26</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1242,7 +1242,7 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1253,21 +1253,21 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>04:48:57</t>
+          <t>05:21:16</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>06:29</t>
+          <t>06:27</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>86_EST CHICA-ESC AGRARIA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>101</v>
+        <v>66</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -1278,12 +1278,12 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>04:56:11</t>
+          <t>04:48:57</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>06:30</t>
+          <t>06:29</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1292,7 +1292,7 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -1303,21 +1303,21 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>04:56:11</t>
+          <t>05:21:16</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>06:31</t>
+          <t>06:30</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>86_EST CHICA-ESC AGRARIA</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -1328,21 +1328,21 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>04:48:57</t>
+          <t>05:21:16</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>06:43</t>
+          <t>06:31</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>115</v>
+        <v>70</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -1353,12 +1353,12 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>04:56:11</t>
+          <t>04:48:57</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>06:44</t>
+          <t>06:43</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1367,7 +1367,7 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -1378,21 +1378,21 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>04:48:57</t>
+          <t>05:21:16</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>06:46</t>
+          <t>06:44</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>225_C ROCA-H SUR</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>118</v>
+        <v>83</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -1403,23 +1403,173 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
+          <t>05:21:16</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>06:46</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>85</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
           <t>04:56:11</t>
         </is>
       </c>
-      <c r="B43" t="inlineStr">
+      <c r="B44" t="inlineStr">
         <is>
           <t>06:47</t>
         </is>
       </c>
-      <c r="C43" t="inlineStr">
+      <c r="C44" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D43" t="n">
+      <c r="D44" t="n">
         <v>111</v>
       </c>
-      <c r="E43" t="inlineStr">
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>05:21:16</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>99</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>05:21:16</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>07:05</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>104</v>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>05:21:16</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>07:07</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>106</v>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>05:21:16</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>07:11</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>110</v>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>05:21:16</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>07:16</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>115</v>
+      </c>
+      <c r="E49" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1436,7 +1586,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1454,14 +1604,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:56:11</t>
+          <t>Última actualización: 05:21:16</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 11</t>
+          <t>Total filas: 12</t>
         </is>
       </c>
     </row>
@@ -1670,7 +1820,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>04:56:11</t>
+          <t>05:21:16</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1684,7 +1834,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -1695,7 +1845,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>04:56:11</t>
+          <t>05:21:16</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1709,7 +1859,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -1720,7 +1870,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>04:48:57</t>
+          <t>05:21:16</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1734,7 +1884,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>118</v>
+        <v>85</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -1762,6 +1912,31 @@
         <v>111</v>
       </c>
       <c r="E16" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>05:21:16</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>07:11</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>110</v>
+      </c>
+      <c r="E17" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1778,7 +1953,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1796,14 +1971,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:56:11</t>
+          <t>Última actualización: 05:21:16</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 7</t>
+          <t>Total filas: 8</t>
         </is>
       </c>
     </row>
@@ -1887,7 +2062,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>04:56:11</t>
+          <t>05:21:16</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -1901,7 +2076,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -1937,7 +2112,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>04:56:11</t>
+          <t>05:21:16</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1951,7 +2126,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>73</v>
+        <v>48</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -1987,7 +2162,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>04:56:11</t>
+          <t>05:21:16</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -2001,11 +2176,36 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>97</v>
+        <v>72</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>05:21:16</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>99</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 821
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-23.xlsx
+++ b/data/horarios-141-2026-01-23.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 05:21:16</t>
+          <t>Última actualización: 05:52:07</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 44</t>
+          <t>Total filas: 54</t>
         </is>
       </c>
     </row>
@@ -1053,7 +1053,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>05:21:16</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1067,7 +1067,7 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>33</v>
+        <v>2</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1128,21 +1128,21 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>04:48:57</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>06:13</t>
+          <t>06:12</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>225_HARAS DEL SUR</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>85</v>
+        <v>20</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -1153,12 +1153,12 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>05:21:16</t>
+          <t>04:48:57</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>06:14</t>
+          <t>06:13</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1167,7 +1167,7 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1178,21 +1178,21 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>04:48:57</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>06:20</t>
+          <t>06:14</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>225_HARAS DEL SUR</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>92</v>
+        <v>22</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1203,12 +1203,12 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>05:21:16</t>
+          <t>04:48:57</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>06:21</t>
+          <t>06:20</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1217,7 +1217,7 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>60</v>
+        <v>92</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1228,21 +1228,21 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>04:48:57</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>06:26</t>
+          <t>06:21</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>98</v>
+        <v>29</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1253,12 +1253,12 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>05:21:16</t>
+          <t>04:48:57</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>06:27</t>
+          <t>06:26</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1267,7 +1267,7 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>66</v>
+        <v>98</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -1278,21 +1278,21 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>04:48:57</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>06:29</t>
+          <t>06:27</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>86_EST CHICA-ESC AGRARIA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>101</v>
+        <v>35</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -1303,12 +1303,12 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>05:21:16</t>
+          <t>04:48:57</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>06:30</t>
+          <t>06:29</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1317,7 +1317,7 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>69</v>
+        <v>101</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -1328,21 +1328,21 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>05:21:16</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>06:31</t>
+          <t>06:30</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>86_EST CHICA-ESC AGRARIA</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>70</v>
+        <v>38</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -1353,21 +1353,21 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>04:48:57</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>06:43</t>
+          <t>06:31</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>115</v>
+        <v>39</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -1378,12 +1378,12 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>05:21:16</t>
+          <t>04:48:57</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>06:44</t>
+          <t>06:43</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1392,7 +1392,7 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>83</v>
+        <v>115</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -1403,21 +1403,21 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>05:21:16</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>06:46</t>
+          <t>06:44</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>225_C ROCA-H SUR</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>85</v>
+        <v>52</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -1428,12 +1428,12 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>04:56:11</t>
+          <t>05:21:16</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>06:47</t>
+          <t>06:46</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1442,7 +1442,7 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>111</v>
+        <v>85</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -1453,21 +1453,21 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>05:21:16</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>06:47</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>99</v>
+        <v>55</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -1478,21 +1478,21 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>05:21:16</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>07:05</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>104</v>
+        <v>68</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -1503,21 +1503,21 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>05:21:16</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>07:07</t>
+          <t>07:05</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>106</v>
+        <v>73</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -1528,21 +1528,21 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>05:21:16</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>07:11</t>
+          <t>07:05</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>110</v>
+        <v>73</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -1553,23 +1553,273 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
+          <t>05:52:07</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>07:07</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>75</v>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
           <t>05:21:16</t>
         </is>
       </c>
-      <c r="B49" t="inlineStr">
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>07:11</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>110</v>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>05:52:07</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>07:12</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>80</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>05:52:07</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
         <is>
           <t>07:16</t>
         </is>
       </c>
-      <c r="C49" t="inlineStr">
+      <c r="C52" t="inlineStr">
         <is>
           <t>11_ETCHEVERRY</t>
         </is>
       </c>
-      <c r="D49" t="n">
-        <v>115</v>
-      </c>
-      <c r="E49" t="inlineStr">
+      <c r="D52" t="n">
+        <v>84</v>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>05:52:07</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>07:21</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>89</v>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>05:52:07</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>07:23</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>91</v>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>05:52:07</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>07:32</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>100</v>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>05:52:07</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>07:32</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>100</v>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>05:52:07</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>07:32</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>100</v>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>05:52:07</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>07:37</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>105</v>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>05:52:07</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>07:48</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>116</v>
+      </c>
+      <c r="E59" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1586,7 +1836,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1604,14 +1854,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 05:21:16</t>
+          <t>Última actualización: 05:52:07</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 12</t>
+          <t>Total filas: 14</t>
         </is>
       </c>
     </row>
@@ -1870,21 +2120,21 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>05:21:16</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>06:46</t>
+          <t>06:12</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>85</v>
+        <v>20</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -1895,12 +2145,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>04:56:11</t>
+          <t>05:21:16</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>06:47</t>
+          <t>06:46</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1909,7 +2159,7 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>111</v>
+        <v>85</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -1920,23 +2170,73 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
+          <t>05:52:07</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>06:47</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>55</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
           <t>05:21:16</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="B18" t="inlineStr">
         <is>
           <t>07:11</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="C18" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D17" t="n">
+      <c r="D18" t="n">
         <v>110</v>
       </c>
-      <c r="E17" t="inlineStr">
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>05:52:07</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>07:12</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>80</v>
+      </c>
+      <c r="E19" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1953,7 +2253,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1971,14 +2271,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 05:21:16</t>
+          <t>Última actualización: 05:52:07</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 8</t>
+          <t>Total filas: 10</t>
         </is>
       </c>
     </row>
@@ -2137,37 +2437,37 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>04:48:57</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>06:32</t>
+          <t>06:13</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>104</v>
+        <v>21</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>L6203</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>05:21:16</t>
+          <t>04:48:57</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>06:33</t>
+          <t>06:32</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -2176,7 +2476,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>72</v>
+        <v>104</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -2187,23 +2487,73 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>05:21:16</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
+          <t>06:33</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>41</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>05:52:07</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
           <t>07:00</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C14" t="inlineStr">
         <is>
           <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
-      <c r="D13" t="n">
-        <v>99</v>
-      </c>
-      <c r="E13" t="inlineStr">
+      <c r="D14" t="n">
+        <v>68</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>05:52:07</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>07:35</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>103</v>
+      </c>
+      <c r="E15" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 822
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-23.xlsx
+++ b/data/horarios-141-2026-01-23.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E59"/>
+  <dimension ref="A1:E69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 05:52:07</t>
+          <t>Última actualización: 06:21:22</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 54</t>
+          <t>Total filas: 64</t>
         </is>
       </c>
     </row>
@@ -1228,7 +1228,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:21:22</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1242,7 +1242,7 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1303,7 +1303,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>04:48:57</t>
+          <t>06:21:22</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1317,7 +1317,7 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>101</v>
+        <v>8</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -1328,21 +1328,21 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:21:22</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>06:30</t>
+          <t>06:29</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>86_EST CHICA-ESC AGRARIA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -1358,16 +1358,16 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>06:31</t>
+          <t>06:30</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>86_EST CHICA-ESC AGRARIA</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -1378,21 +1378,21 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>04:48:57</t>
+          <t>06:21:22</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>06:43</t>
+          <t>06:31</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>115</v>
+        <v>10</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -1403,12 +1403,12 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>04:48:57</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>06:44</t>
+          <t>06:43</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1417,7 +1417,7 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>52</v>
+        <v>115</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -1428,21 +1428,21 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>05:21:16</t>
+          <t>06:21:22</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>06:46</t>
+          <t>06:44</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>225_C ROCA-H SUR</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>85</v>
+        <v>23</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -1453,12 +1453,12 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:21:22</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>06:47</t>
+          <t>06:46</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1467,7 +1467,7 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -1483,16 +1483,16 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>06:47</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -1503,21 +1503,21 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:21:22</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>07:05</t>
+          <t>06:59</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>73</v>
+        <v>38</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -1533,16 +1533,16 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>07:05</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -1553,21 +1553,21 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:21:22</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>07:07</t>
+          <t>07:01</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>75</v>
+        <v>40</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -1578,21 +1578,21 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>05:21:16</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>07:11</t>
+          <t>07:05</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>110</v>
+        <v>73</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -1603,21 +1603,21 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:21:22</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>07:12</t>
+          <t>07:05</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>80</v>
+        <v>44</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -1628,21 +1628,21 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:21:22</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>07:16</t>
+          <t>07:07</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>84</v>
+        <v>46</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -1653,21 +1653,21 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:21:22</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>07:21</t>
+          <t>07:11</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>89</v>
+        <v>50</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -1683,16 +1683,16 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>07:23</t>
+          <t>07:12</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D54" t="n">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -1703,21 +1703,21 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:21:22</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>07:32</t>
+          <t>07:15</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>100</v>
+        <v>54</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1733,16 +1733,16 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>07:32</t>
+          <t>07:16</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1753,21 +1753,21 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:21:22</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>07:32</t>
+          <t>07:21</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -1778,21 +1778,21 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:21:22</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>07:37</t>
+          <t>07:23</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>105</v>
+        <v>62</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -1803,23 +1803,273 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
+          <t>06:21:22</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>07:31</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>70</v>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
           <t>05:52:07</t>
         </is>
       </c>
-      <c r="B59" t="inlineStr">
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>07:32</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>100</v>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>06:21:22</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>07:32</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>71</v>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>05:52:07</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>07:32</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>100</v>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>06:21:22</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>07:37</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>76</v>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>06:21:22</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>07:39</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>78</v>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>06:21:22</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>07:47</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>86</v>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>05:52:07</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
         <is>
           <t>07:48</t>
         </is>
       </c>
-      <c r="C59" t="inlineStr">
+      <c r="C66" t="inlineStr">
         <is>
           <t>14_ABASTO</t>
         </is>
       </c>
-      <c r="D59" t="n">
+      <c r="D66" t="n">
         <v>116</v>
       </c>
-      <c r="E59" t="inlineStr">
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>06:21:22</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>07:51</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>215D_EL PATO</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>90</v>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>06:21:22</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>08:01</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>100</v>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>06:21:22</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>08:12</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>111</v>
+      </c>
+      <c r="E69" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1836,7 +2086,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1854,14 +2104,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 05:52:07</t>
+          <t>Última actualización: 06:21:22</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 14</t>
+          <t>Total filas: 15</t>
         </is>
       </c>
     </row>
@@ -2145,7 +2395,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>05:21:16</t>
+          <t>06:21:22</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -2159,7 +2409,7 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>85</v>
+        <v>25</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -2195,7 +2445,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>05:21:16</t>
+          <t>06:21:22</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -2209,7 +2459,7 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>110</v>
+        <v>50</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -2237,6 +2487,31 @@
         <v>80</v>
       </c>
       <c r="E19" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>06:21:22</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>07:51</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>215D_EL PATO</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>90</v>
+      </c>
+      <c r="E20" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2253,7 +2528,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2271,14 +2546,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 05:52:07</t>
+          <t>Última actualización: 06:21:22</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 10</t>
+          <t>Total filas: 11</t>
         </is>
       </c>
     </row>
@@ -2487,7 +2762,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:21:22</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -2501,7 +2776,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>41</v>
+        <v>12</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -2512,7 +2787,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:21:22</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -2526,7 +2801,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>68</v>
+        <v>39</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -2537,7 +2812,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:21:22</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -2551,11 +2826,36 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>103</v>
+        <v>74</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
           <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>06:21:22</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>08:07</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>106</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 823
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-23.xlsx
+++ b/data/horarios-141-2026-01-23.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E69"/>
+  <dimension ref="A1:E78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:21:22</t>
+          <t>Última actualización: 06:49:33</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 64</t>
+          <t>Total filas: 73</t>
         </is>
       </c>
     </row>
@@ -1503,7 +1503,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>06:21:22</t>
+          <t>06:49:33</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -1517,7 +1517,7 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -1553,7 +1553,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>06:21:22</t>
+          <t>06:49:33</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -1567,7 +1567,7 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -1578,12 +1578,12 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:49:33</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>07:05</t>
+          <t>07:04</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -1592,7 +1592,7 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>73</v>
+        <v>15</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -1603,7 +1603,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>06:21:22</t>
+          <t>06:49:33</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -1617,7 +1617,7 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -1628,21 +1628,21 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>06:21:22</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>07:07</t>
+          <t>07:05</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>46</v>
+        <v>73</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -1653,21 +1653,21 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>06:21:22</t>
+          <t>06:49:33</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>07:11</t>
+          <t>07:07</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>50</v>
+        <v>18</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -1678,12 +1678,12 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:49:33</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>07:12</t>
+          <t>07:11</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -1692,7 +1692,7 @@
         </is>
       </c>
       <c r="D54" t="n">
-        <v>80</v>
+        <v>22</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -1703,21 +1703,21 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>06:21:22</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>07:15</t>
+          <t>07:12</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>54</v>
+        <v>80</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1728,12 +1728,12 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:49:33</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>07:16</t>
+          <t>07:15</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -1742,7 +1742,7 @@
         </is>
       </c>
       <c r="D56" t="n">
-        <v>84</v>
+        <v>26</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1753,21 +1753,21 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>06:21:22</t>
+          <t>06:49:33</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>07:21</t>
+          <t>07:16</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -1778,21 +1778,21 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>06:21:22</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>07:23</t>
+          <t>07:16</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>62</v>
+        <v>84</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -1803,21 +1803,21 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>06:21:22</t>
+          <t>06:49:33</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>07:31</t>
+          <t>07:21</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>70</v>
+        <v>32</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -1828,21 +1828,21 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:49:33</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>07:32</t>
+          <t>07:23</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D60" t="n">
-        <v>100</v>
+        <v>34</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -1853,21 +1853,21 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>06:21:22</t>
+          <t>06:49:33</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>07:32</t>
+          <t>07:31</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D61" t="n">
-        <v>71</v>
+        <v>42</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -1888,7 +1888,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D62" t="n">
@@ -1903,21 +1903,21 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>06:21:22</t>
+          <t>06:49:33</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>07:37</t>
+          <t>07:32</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D63" t="n">
-        <v>76</v>
+        <v>43</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -1928,21 +1928,21 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>06:21:22</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>07:39</t>
+          <t>07:32</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>78</v>
+        <v>100</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -1953,21 +1953,21 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>06:21:22</t>
+          <t>06:49:33</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>07:47</t>
+          <t>07:36</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>86</v>
+        <v>47</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -1978,21 +1978,21 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:21:22</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>07:48</t>
+          <t>07:37</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>116</v>
+        <v>76</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2003,21 +2003,21 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>06:21:22</t>
+          <t>06:49:33</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>07:51</t>
+          <t>07:39</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2028,21 +2028,21 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>06:21:22</t>
+          <t>06:49:33</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>08:01</t>
+          <t>07:47</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D68" t="n">
-        <v>100</v>
+        <v>58</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -2053,23 +2053,248 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
+          <t>05:52:07</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>07:48</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>116</v>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>06:49:33</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>07:51</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>215D_EL PATO</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>62</v>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
           <t>06:21:22</t>
         </is>
       </c>
-      <c r="B69" t="inlineStr">
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>08:01</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>100</v>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>06:49:33</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>08:06</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>77</v>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>06:49:33</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
         <is>
           <t>08:12</t>
         </is>
       </c>
-      <c r="C69" t="inlineStr">
+      <c r="C73" t="inlineStr">
         <is>
           <t>15_ABASTO</t>
         </is>
       </c>
-      <c r="D69" t="n">
-        <v>111</v>
-      </c>
-      <c r="E69" t="inlineStr">
+      <c r="D73" t="n">
+        <v>83</v>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>06:49:33</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>08:21</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>92</v>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>06:49:33</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>08:22</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>93</v>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>06:49:33</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>08:23</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>94</v>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>06:49:33</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>08:27</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>98</v>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>06:49:33</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>08:42</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>113</v>
+      </c>
+      <c r="E78" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2086,7 +2311,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2104,14 +2329,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:21:22</t>
+          <t>Última actualización: 06:49:33</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 15</t>
+          <t>Total filas: 16</t>
         </is>
       </c>
     </row>
@@ -2445,7 +2670,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>06:21:22</t>
+          <t>06:49:33</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -2459,7 +2684,7 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -2495,7 +2720,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>06:21:22</t>
+          <t>06:49:33</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -2509,9 +2734,34 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>90</v>
+        <v>62</v>
       </c>
       <c r="E20" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>06:49:33</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>08:23</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>94</v>
+      </c>
+      <c r="E21" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2528,7 +2778,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2546,14 +2796,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:21:22</t>
+          <t>Última actualización: 06:49:33</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 11</t>
+          <t>Total filas: 12</t>
         </is>
       </c>
     </row>
@@ -2787,7 +3037,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>06:21:22</t>
+          <t>06:49:33</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -2801,7 +3051,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -2812,7 +3062,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>06:21:22</t>
+          <t>06:49:33</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -2826,7 +3076,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>74</v>
+        <v>46</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -2837,7 +3087,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>06:21:22</t>
+          <t>06:49:33</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -2851,11 +3101,36 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>106</v>
+        <v>78</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>06:49:33</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>08:33</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>104</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 824
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-23.xlsx
+++ b/data/horarios-141-2026-01-23.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E78"/>
+  <dimension ref="A1:E81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:49:33</t>
+          <t>Última actualización: 06:59:37</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 73</t>
+          <t>Total filas: 76</t>
         </is>
       </c>
     </row>
@@ -1313,7 +1313,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>86_EST CHICA-ESC AGRARIA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1338,7 +1338,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>86_EST CHICA-ESC AGRARIA</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1503,7 +1503,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>06:49:33</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -1513,11 +1513,11 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -1528,12 +1528,12 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>06:59</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1542,7 +1542,7 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>68</v>
+        <v>0</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -1553,21 +1553,21 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>06:49:33</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>07:01</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>12</v>
+        <v>68</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -1583,16 +1583,16 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>07:04</t>
+          <t>07:01</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -1608,16 +1608,16 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>07:05</t>
+          <t>07:04</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -1628,7 +1628,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1638,11 +1638,11 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>73</v>
+        <v>6</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -1653,21 +1653,21 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>06:49:33</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>07:07</t>
+          <t>07:05</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>18</v>
+        <v>73</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -1678,21 +1678,21 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>06:49:33</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>07:11</t>
+          <t>07:07</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D54" t="n">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -1703,12 +1703,12 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>07:12</t>
+          <t>07:11</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -1717,7 +1717,7 @@
         </is>
       </c>
       <c r="D55" t="n">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1728,21 +1728,21 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>06:49:33</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>07:15</t>
+          <t>07:12</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>26</v>
+        <v>80</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1753,21 +1753,21 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>06:49:33</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>07:16</t>
+          <t>07:15</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -1803,21 +1803,21 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>06:49:33</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>07:21</t>
+          <t>07:16</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -1828,21 +1828,21 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>06:49:33</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>07:23</t>
+          <t>07:21</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D60" t="n">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -1853,21 +1853,21 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>06:49:33</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>07:31</t>
+          <t>07:23</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D61" t="n">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -1878,21 +1878,21 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>07:32</t>
+          <t>07:31</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D62" t="n">
-        <v>100</v>
+        <v>32</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -1903,21 +1903,21 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>06:49:33</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>07:32</t>
+          <t>07:31</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D63" t="n">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -1928,7 +1928,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -1938,11 +1938,11 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>100</v>
+        <v>33</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -1953,21 +1953,21 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>06:49:33</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>07:36</t>
+          <t>07:32</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>47</v>
+        <v>100</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -1978,21 +1978,21 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>06:21:22</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>07:37</t>
+          <t>07:32</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>76</v>
+        <v>100</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2003,21 +2003,21 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>06:49:33</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>07:39</t>
+          <t>07:36</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2028,21 +2028,21 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>06:49:33</t>
+          <t>06:21:22</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>07:47</t>
+          <t>07:37</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D68" t="n">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -2053,21 +2053,21 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>07:48</t>
+          <t>07:39</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D69" t="n">
-        <v>116</v>
+        <v>40</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -2078,21 +2078,21 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>06:49:33</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>07:51</t>
+          <t>07:47</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D70" t="n">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -2103,21 +2103,21 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>06:21:22</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>08:01</t>
+          <t>07:48</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -2128,21 +2128,21 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>06:49:33</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>08:06</t>
+          <t>07:51</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -2153,21 +2153,21 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>06:49:33</t>
+          <t>06:21:22</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>08:12</t>
+          <t>08:01</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D73" t="n">
-        <v>83</v>
+        <v>100</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -2178,21 +2178,21 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>06:49:33</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>08:21</t>
+          <t>08:06</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D74" t="n">
-        <v>92</v>
+        <v>67</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -2203,21 +2203,21 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>06:49:33</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>08:22</t>
+          <t>08:12</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2228,21 +2228,21 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>06:49:33</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>08:23</t>
+          <t>08:21</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2253,21 +2253,21 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>06:49:33</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>08:27</t>
+          <t>08:22</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2278,23 +2278,98 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>06:49:33</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
+          <t>08:23</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>84</v>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>06:59:37</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>08:27</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>88</v>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>06:59:37</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
           <t>08:42</t>
         </is>
       </c>
-      <c r="C78" t="inlineStr">
+      <c r="C80" t="inlineStr">
         <is>
           <t>81_EL PELIGRO</t>
         </is>
       </c>
-      <c r="D78" t="n">
-        <v>113</v>
-      </c>
-      <c r="E78" t="inlineStr">
+      <c r="D80" t="n">
+        <v>103</v>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>06:59:37</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>08:54</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>115</v>
+      </c>
+      <c r="E81" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2329,7 +2404,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:49:33</t>
+          <t>Última actualización: 06:59:37</t>
         </is>
       </c>
     </row>
@@ -2670,7 +2745,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>06:49:33</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -2684,7 +2759,7 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -2720,7 +2795,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>06:49:33</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -2734,7 +2809,7 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -2745,7 +2820,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>06:49:33</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -2759,7 +2834,7 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -2778,7 +2853,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2796,14 +2871,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:49:33</t>
+          <t>Última actualización: 06:59:37</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 12</t>
+          <t>Total filas: 15</t>
         </is>
       </c>
     </row>
@@ -3037,12 +3112,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>06:49:33</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>06:59</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -3051,7 +3126,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -3067,16 +3142,16 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>07:35</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>46</v>
+        <v>11</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -3087,48 +3162,123 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>06:49:33</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>08:07</t>
+          <t>07:35</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>78</v>
+        <v>36</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>L6203</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
+          <t>06:59:37</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>08:06</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>67</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
           <t>06:49:33</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>08:07</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>78</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>06:49:33</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
         <is>
           <t>08:33</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="C19" t="inlineStr">
         <is>
           <t>215A_LA PLATA</t>
         </is>
       </c>
-      <c r="D17" t="n">
+      <c r="D19" t="n">
         <v>104</v>
       </c>
-      <c r="E17" t="inlineStr">
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>06:59:37</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>08:38</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>99</v>
+      </c>
+      <c r="E20" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 825
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-23.xlsx
+++ b/data/horarios-141-2026-01-23.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E81"/>
+  <dimension ref="A1:E96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:59:37</t>
+          <t>Última actualización: 07:28:14</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 76</t>
+          <t>Total filas: 91</t>
         </is>
       </c>
     </row>
@@ -1313,7 +1313,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>86_EST CHICA-ESC AGRARIA</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1338,7 +1338,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>86_EST CHICA-ESC AGRARIA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1513,7 +1513,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -1538,7 +1538,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -1628,7 +1628,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1638,11 +1638,11 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>6</v>
+        <v>73</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -1653,7 +1653,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1663,11 +1663,11 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>73</v>
+        <v>6</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -1778,7 +1778,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1788,11 +1788,11 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -1803,7 +1803,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1813,11 +1813,11 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>17</v>
+        <v>84</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -1878,12 +1878,12 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>07:31</t>
+          <t>07:30</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -1892,7 +1892,7 @@
         </is>
       </c>
       <c r="D62" t="n">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -1933,16 +1933,16 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>07:32</t>
+          <t>07:31</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -1953,7 +1953,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1963,11 +1963,11 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -1988,7 +1988,7 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D66" t="n">
@@ -2003,21 +2003,21 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>07:36</t>
+          <t>07:32</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>37</v>
+        <v>100</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2028,21 +2028,21 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>06:21:22</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>07:37</t>
+          <t>07:35</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D68" t="n">
-        <v>76</v>
+        <v>7</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -2058,16 +2058,16 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>07:39</t>
+          <t>07:36</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D69" t="n">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -2078,21 +2078,21 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>07:47</t>
+          <t>07:37</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D70" t="n">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -2103,21 +2103,21 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>07:48</t>
+          <t>07:39</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>116</v>
+        <v>11</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -2133,16 +2133,16 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>07:51</t>
+          <t>07:47</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -2153,21 +2153,21 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>06:21:22</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>08:01</t>
+          <t>07:47</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D73" t="n">
-        <v>100</v>
+        <v>19</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -2178,21 +2178,21 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>08:06</t>
+          <t>07:48</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D74" t="n">
-        <v>67</v>
+        <v>20</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -2203,21 +2203,21 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>08:12</t>
+          <t>07:51</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>73</v>
+        <v>23</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2228,21 +2228,21 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>08:21</t>
+          <t>07:55</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>82</v>
+        <v>27</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2253,21 +2253,21 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>08:22</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>83</v>
+        <v>32</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2278,21 +2278,21 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>06:21:22</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>08:23</t>
+          <t>08:01</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2303,21 +2303,21 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>08:27</t>
+          <t>08:03</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>88</v>
+        <v>35</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -2333,16 +2333,16 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>08:42</t>
+          <t>08:06</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>103</v>
+        <v>67</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -2353,23 +2353,398 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
+          <t>07:28:14</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>08:11</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>43</v>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>07:28:14</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>08:12</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>44</v>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>07:28:14</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>08:21</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>53</v>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
           <t>06:59:37</t>
         </is>
       </c>
-      <c r="B81" t="inlineStr">
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>08:22</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>83</v>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>07:28:14</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>08:23</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>55</v>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>07:28:14</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>08:23</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>55</v>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>07:28:14</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>08:27</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>59</v>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>07:28:14</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>08:42</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>74</v>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>07:28:14</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>08:44</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>76</v>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>07:28:14</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
         <is>
           <t>08:54</t>
         </is>
       </c>
-      <c r="C81" t="inlineStr">
+      <c r="C90" t="inlineStr">
         <is>
           <t>17_ROMERO</t>
         </is>
       </c>
-      <c r="D81" t="n">
+      <c r="D90" t="n">
+        <v>86</v>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>07:28:14</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>09:02</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>94</v>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>07:28:14</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>09:11</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>103</v>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>07:28:14</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>09:17</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>109</v>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>07:28:14</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>09:21</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>113</v>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>07:28:14</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>09:23</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
         <v>115</v>
       </c>
-      <c r="E81" t="inlineStr">
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>07:28:14</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>09:24</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>116</v>
+      </c>
+      <c r="E96" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2386,7 +2761,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2404,14 +2779,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:59:37</t>
+          <t>Última actualización: 07:28:14</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 16</t>
+          <t>Total filas: 17</t>
         </is>
       </c>
     </row>
@@ -2795,7 +3170,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -2809,7 +3184,7 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>52</v>
+        <v>23</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -2820,7 +3195,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -2834,9 +3209,34 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>84</v>
+        <v>55</v>
       </c>
       <c r="E21" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>07:28:14</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>09:02</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>94</v>
+      </c>
+      <c r="E22" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2853,7 +3253,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2871,14 +3271,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:59:37</t>
+          <t>Última actualización: 07:28:14</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 15</t>
+          <t>Total filas: 17</t>
         </is>
       </c>
     </row>
@@ -3162,7 +3562,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -3176,7 +3576,7 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -3237,50 +3637,100 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>06:49:33</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>08:33</t>
+          <t>08:10</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>104</v>
+        <v>42</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>L6173</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>06:49:33</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
+          <t>08:33</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>104</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>07:28:14</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
           <t>08:38</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="C21" t="inlineStr">
         <is>
           <t>215A_LA PLATA</t>
         </is>
       </c>
-      <c r="D20" t="n">
-        <v>99</v>
-      </c>
-      <c r="E20" t="inlineStr">
+      <c r="D21" t="n">
+        <v>70</v>
+      </c>
+      <c r="E21" t="inlineStr">
         <is>
           <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>07:28:14</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>09:09</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>215D_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>101</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 826
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-23.xlsx
+++ b/data/horarios-141-2026-01-23.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E96"/>
+  <dimension ref="A1:E112"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 07:28:14</t>
+          <t>Última actualización: 07:51:34</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 91</t>
+          <t>Total filas: 107</t>
         </is>
       </c>
     </row>
@@ -1313,7 +1313,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>86_EST CHICA-ESC AGRARIA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1338,7 +1338,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>86_EST CHICA-ESC AGRARIA</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1778,7 +1778,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1788,11 +1788,11 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>17</v>
+        <v>84</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -1803,7 +1803,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1813,11 +1813,11 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D63" t="n">
@@ -1938,7 +1938,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -1953,7 +1953,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1963,11 +1963,11 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -1978,7 +1978,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -1988,11 +1988,11 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2203,7 +2203,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>07:51:34</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2217,7 +2217,7 @@
         </is>
       </c>
       <c r="D75" t="n">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2228,12 +2228,12 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>07:51:34</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>07:55</t>
+          <t>07:51</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -2242,7 +2242,7 @@
         </is>
       </c>
       <c r="D76" t="n">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2258,16 +2258,16 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>07:55</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2278,12 +2278,12 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>06:21:22</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>08:01</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -2292,7 +2292,7 @@
         </is>
       </c>
       <c r="D78" t="n">
-        <v>100</v>
+        <v>32</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2303,21 +2303,21 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>07:51:34</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>08:03</t>
+          <t>08:01</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -2328,21 +2328,21 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>07:51:34</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>08:06</t>
+          <t>08:03</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>67</v>
+        <v>12</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -2353,21 +2353,21 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>08:11</t>
+          <t>08:06</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D81" t="n">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -2378,21 +2378,21 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>07:51:34</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>08:12</t>
+          <t>08:10</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D82" t="n">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -2408,16 +2408,16 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>08:21</t>
+          <t>08:11</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D83" t="n">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -2428,21 +2428,21 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>07:51:34</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>08:22</t>
+          <t>08:12</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D84" t="n">
-        <v>83</v>
+        <v>21</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -2453,21 +2453,21 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>07:51:34</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>08:23</t>
+          <t>08:13</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2478,21 +2478,21 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>07:51:34</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>08:23</t>
+          <t>08:21</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2503,21 +2503,21 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>07:51:34</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>08:27</t>
+          <t>08:22</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D87" t="n">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -2528,21 +2528,21 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>07:51:34</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>08:42</t>
+          <t>08:23</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>74</v>
+        <v>32</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -2558,16 +2558,16 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>08:44</t>
+          <t>08:23</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -2578,21 +2578,21 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>07:51:34</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>08:54</t>
+          <t>08:27</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D90" t="n">
-        <v>86</v>
+        <v>36</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -2603,21 +2603,21 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>07:51:34</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>09:02</t>
+          <t>08:30</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D91" t="n">
-        <v>94</v>
+        <v>39</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -2628,21 +2628,21 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>07:51:34</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>09:11</t>
+          <t>08:42</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D92" t="n">
-        <v>103</v>
+        <v>51</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -2653,21 +2653,21 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>07:51:34</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>09:17</t>
+          <t>08:43</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D93" t="n">
-        <v>109</v>
+        <v>52</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
@@ -2683,16 +2683,16 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>09:21</t>
+          <t>08:44</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D94" t="n">
-        <v>113</v>
+        <v>76</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
@@ -2703,12 +2703,12 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>07:51:34</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>09:23</t>
+          <t>08:54</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -2717,7 +2717,7 @@
         </is>
       </c>
       <c r="D95" t="n">
-        <v>115</v>
+        <v>63</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -2728,23 +2728,423 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
+          <t>07:51:34</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>09:01</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>70</v>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
           <t>07:28:14</t>
         </is>
       </c>
-      <c r="B96" t="inlineStr">
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>09:02</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D97" t="n">
+        <v>94</v>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>07:51:34</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>09:03</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>72</v>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>07:51:34</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>09:10</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D99" t="n">
+        <v>79</v>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>07:28:14</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>09:11</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D100" t="n">
+        <v>103</v>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>07:51:34</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>09:16</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
+        <v>85</v>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>07:28:14</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>09:17</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D102" t="n">
+        <v>109</v>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>07:51:34</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>09:21</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D103" t="n">
+        <v>90</v>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>07:51:34</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>09:22</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D104" t="n">
+        <v>91</v>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>07:28:14</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>09:23</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D105" t="n">
+        <v>115</v>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>07:51:34</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>09:23</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D106" t="n">
+        <v>92</v>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>07:28:14</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
         <is>
           <t>09:24</t>
         </is>
       </c>
-      <c r="C96" t="inlineStr">
+      <c r="C107" t="inlineStr">
         <is>
           <t>11_ETCHEVERRY</t>
         </is>
       </c>
-      <c r="D96" t="n">
+      <c r="D107" t="n">
         <v>116</v>
       </c>
-      <c r="E96" t="inlineStr">
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>07:51:34</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>09:32</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D108" t="n">
+        <v>101</v>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>07:51:34</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>09:33</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D109" t="n">
+        <v>102</v>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>07:51:34</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>09:34</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D110" t="n">
+        <v>103</v>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>07:51:34</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>09:42</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D111" t="n">
+        <v>111</v>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>07:51:34</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>09:43</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D112" t="n">
+        <v>112</v>
+      </c>
+      <c r="E112" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2761,7 +3161,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2779,14 +3179,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 07:28:14</t>
+          <t>Última actualización: 07:51:34</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 17</t>
+          <t>Total filas: 19</t>
         </is>
       </c>
     </row>
@@ -3170,7 +3570,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>07:51:34</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -3184,7 +3584,7 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -3195,7 +3595,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>07:51:34</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -3209,7 +3609,7 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -3220,23 +3620,73 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
+          <t>07:51:34</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>09:01</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>70</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
           <t>07:28:14</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
+      <c r="B23" t="inlineStr">
         <is>
           <t>09:02</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
+      <c r="C23" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D22" t="n">
+      <c r="D23" t="n">
         <v>94</v>
       </c>
-      <c r="E22" t="inlineStr">
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>07:51:34</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>09:42</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>111</v>
+      </c>
+      <c r="E24" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -3253,7 +3703,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3271,14 +3721,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 07:28:14</t>
+          <t>Última actualización: 07:51:34</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 17</t>
+          <t>Total filas: 19</t>
         </is>
       </c>
     </row>
@@ -3662,37 +4112,37 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>06:49:33</t>
+          <t>07:51:34</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>08:33</t>
+          <t>08:11</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>104</v>
+        <v>20</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>L6173</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>06:49:33</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>08:38</t>
+          <t>08:33</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -3701,7 +4151,7 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -3717,18 +4167,68 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
+          <t>08:38</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>70</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>07:51:34</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>08:40</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>49</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>07:51:34</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
           <t>09:09</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
+      <c r="C24" t="inlineStr">
         <is>
           <t>215D_LA PLATA</t>
         </is>
       </c>
-      <c r="D22" t="n">
-        <v>101</v>
-      </c>
-      <c r="E22" t="inlineStr">
+      <c r="D24" t="n">
+        <v>78</v>
+      </c>
+      <c r="E24" t="inlineStr">
         <is>
           <t>L6203</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 827
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-23.xlsx
+++ b/data/horarios-141-2026-01-23.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E112"/>
+  <dimension ref="A1:E119"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 07:51:34</t>
+          <t>Última actualización: 08:13:38</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 107</t>
+          <t>Total filas: 114</t>
         </is>
       </c>
     </row>
@@ -1313,7 +1313,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>86_EST CHICA-ESC AGRARIA</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1338,7 +1338,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>86_EST CHICA-ESC AGRARIA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1513,7 +1513,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -1538,7 +1538,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -1913,7 +1913,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D63" t="n">
@@ -1938,7 +1938,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -1963,7 +1963,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D65" t="n">
@@ -2013,7 +2013,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D67" t="n">
@@ -2213,7 +2213,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D75" t="n">
@@ -2238,7 +2238,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D76" t="n">
@@ -2478,7 +2478,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>07:51:34</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2492,7 +2492,7 @@
         </is>
       </c>
       <c r="D86" t="n">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2503,7 +2503,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>07:51:34</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -2517,7 +2517,7 @@
         </is>
       </c>
       <c r="D87" t="n">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -2528,7 +2528,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>07:51:34</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -2542,7 +2542,7 @@
         </is>
       </c>
       <c r="D88" t="n">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -2578,7 +2578,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>07:51:34</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -2592,7 +2592,7 @@
         </is>
       </c>
       <c r="D90" t="n">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -2628,21 +2628,21 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>07:51:34</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>08:42</t>
+          <t>08:33</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D92" t="n">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -2653,21 +2653,21 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>07:51:34</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>08:43</t>
+          <t>08:36</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D93" t="n">
-        <v>52</v>
+        <v>23</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
@@ -2678,21 +2678,21 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>08:44</t>
+          <t>08:42</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D94" t="n">
-        <v>76</v>
+        <v>29</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
@@ -2703,21 +2703,21 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>07:51:34</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>08:54</t>
+          <t>08:43</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D95" t="n">
-        <v>63</v>
+        <v>30</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -2728,21 +2728,21 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>07:51:34</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>09:01</t>
+          <t>08:44</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D96" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -2753,21 +2753,21 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>09:02</t>
+          <t>08:53</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D97" t="n">
-        <v>94</v>
+        <v>40</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -2778,21 +2778,21 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>07:51:34</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>09:03</t>
+          <t>08:54</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D98" t="n">
-        <v>72</v>
+        <v>41</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -2803,21 +2803,21 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>07:51:34</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>09:10</t>
+          <t>09:01</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D99" t="n">
-        <v>79</v>
+        <v>48</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -2828,21 +2828,21 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>09:11</t>
+          <t>09:01</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>103</v>
+        <v>48</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -2853,21 +2853,21 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>07:51:34</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>09:16</t>
+          <t>09:02</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D101" t="n">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -2878,21 +2878,21 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>09:17</t>
+          <t>09:03</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D102" t="n">
-        <v>109</v>
+        <v>50</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -2903,21 +2903,21 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>07:51:34</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>09:21</t>
+          <t>09:10</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>90</v>
+        <v>57</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -2928,21 +2928,21 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>07:51:34</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>09:22</t>
+          <t>09:11</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D104" t="n">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -2953,21 +2953,21 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>09:23</t>
+          <t>09:16</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D105" t="n">
-        <v>115</v>
+        <v>63</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -2978,21 +2978,21 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>07:51:34</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>09:23</t>
+          <t>09:17</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D106" t="n">
-        <v>92</v>
+        <v>109</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -3003,21 +3003,21 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>09:24</t>
+          <t>09:21</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D107" t="n">
-        <v>116</v>
+        <v>68</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -3028,21 +3028,21 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>07:51:34</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>09:32</t>
+          <t>09:22</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D108" t="n">
-        <v>101</v>
+        <v>69</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -3053,21 +3053,21 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>07:51:34</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>09:33</t>
+          <t>09:23</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D109" t="n">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -3078,21 +3078,21 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>07:51:34</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>09:34</t>
+          <t>09:23</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D110" t="n">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -3103,21 +3103,21 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>07:51:34</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>09:42</t>
+          <t>09:24</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D111" t="n">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -3128,23 +3128,198 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
+          <t>08:13:38</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>09:32</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D112" t="n">
+        <v>79</v>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>08:13:38</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>09:33</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D113" t="n">
+        <v>80</v>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>08:13:38</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>09:34</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D114" t="n">
+        <v>81</v>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>08:13:38</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>09:41</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D115" t="n">
+        <v>88</v>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
           <t>07:51:34</t>
         </is>
       </c>
-      <c r="B112" t="inlineStr">
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>09:42</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D116" t="n">
+        <v>111</v>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>08:13:38</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
         <is>
           <t>09:43</t>
         </is>
       </c>
-      <c r="C112" t="inlineStr">
+      <c r="C117" t="inlineStr">
         <is>
           <t>14_ABASTO</t>
         </is>
       </c>
-      <c r="D112" t="n">
-        <v>112</v>
-      </c>
-      <c r="E112" t="inlineStr">
+      <c r="D117" t="n">
+        <v>90</v>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>08:13:38</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>09:58</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D118" t="n">
+        <v>105</v>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>08:13:38</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>10:12</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D119" t="n">
+        <v>119</v>
+      </c>
+      <c r="E119" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -3161,7 +3336,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3179,14 +3354,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 07:51:34</t>
+          <t>Última actualización: 08:13:38</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 19</t>
+          <t>Total filas: 20</t>
         </is>
       </c>
     </row>
@@ -3595,7 +3770,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>07:51:34</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -3609,7 +3784,7 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -3620,7 +3795,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>07:51:34</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -3634,7 +3809,7 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -3670,23 +3845,48 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
+          <t>08:13:38</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>09:41</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>88</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
           <t>07:51:34</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
+      <c r="B25" t="inlineStr">
         <is>
           <t>09:42</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
+      <c r="C25" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D24" t="n">
+      <c r="D25" t="n">
         <v>111</v>
       </c>
-      <c r="E24" t="inlineStr">
+      <c r="E25" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -3703,7 +3903,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3721,14 +3921,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 07:51:34</t>
+          <t>Última actualización: 08:13:38</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 19</t>
+          <t>Total filas: 23</t>
         </is>
       </c>
     </row>
@@ -4137,37 +4337,37 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>06:49:33</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>08:33</t>
+          <t>08:16</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>104</v>
+        <v>3</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>L6173</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>06:49:33</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>08:38</t>
+          <t>08:33</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -4176,7 +4376,7 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -4187,12 +4387,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>07:51:34</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>08:40</t>
+          <t>08:38</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -4201,7 +4401,7 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>49</v>
+        <v>70</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -4217,20 +4417,120 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
+          <t>08:40</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>49</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>08:13:38</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>08:45</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>32</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>08:13:38</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>09:08</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>215D_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>55</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>07:51:34</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
           <t>09:09</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
+      <c r="C27" t="inlineStr">
         <is>
           <t>215D_LA PLATA</t>
         </is>
       </c>
-      <c r="D24" t="n">
+      <c r="D27" t="n">
         <v>78</v>
       </c>
-      <c r="E24" t="inlineStr">
+      <c r="E27" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>08:13:38</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>10:03</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-40 Y 115</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>110</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 828
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-23.xlsx
+++ b/data/horarios-141-2026-01-23.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E119"/>
+  <dimension ref="A1:E130"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:13:38</t>
+          <t>Última actualización: 08:34:05</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 114</t>
+          <t>Total filas: 125</t>
         </is>
       </c>
     </row>
@@ -1313,7 +1313,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>86_EST CHICA-ESC AGRARIA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1338,7 +1338,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>86_EST CHICA-ESC AGRARIA</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1513,7 +1513,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -1538,7 +1538,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -1778,7 +1778,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1788,11 +1788,11 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -1803,7 +1803,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1813,11 +1813,11 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>17</v>
+        <v>84</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -1953,7 +1953,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1963,11 +1963,11 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -1978,7 +1978,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -1988,11 +1988,11 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2013,7 +2013,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D67" t="n">
@@ -2213,7 +2213,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D75" t="n">
@@ -2238,7 +2238,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D76" t="n">
@@ -2678,7 +2678,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>08:34:05</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
@@ -2692,7 +2692,7 @@
         </is>
       </c>
       <c r="D94" t="n">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
@@ -2728,7 +2728,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>08:34:05</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -2742,7 +2742,7 @@
         </is>
       </c>
       <c r="D96" t="n">
-        <v>76</v>
+        <v>10</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -2753,7 +2753,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>08:34:05</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -2767,7 +2767,7 @@
         </is>
       </c>
       <c r="D97" t="n">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -2778,7 +2778,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>08:34:05</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -2792,7 +2792,7 @@
         </is>
       </c>
       <c r="D98" t="n">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -2853,7 +2853,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>08:34:05</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -2867,7 +2867,7 @@
         </is>
       </c>
       <c r="D101" t="n">
-        <v>94</v>
+        <v>28</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -2903,21 +2903,21 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>08:34:05</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>09:10</t>
+          <t>09:04</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -2928,21 +2928,21 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>08:34:05</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>09:11</t>
+          <t>09:05</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D104" t="n">
-        <v>103</v>
+        <v>31</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -2958,16 +2958,16 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>09:16</t>
+          <t>09:10</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D105" t="n">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -2978,21 +2978,21 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>08:34:05</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>09:17</t>
+          <t>09:11</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D106" t="n">
-        <v>109</v>
+        <v>37</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -3003,21 +3003,21 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>08:34:05</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>09:21</t>
+          <t>09:13</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D107" t="n">
-        <v>68</v>
+        <v>39</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -3033,16 +3033,16 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>09:22</t>
+          <t>09:16</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D108" t="n">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -3053,21 +3053,21 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>08:34:05</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>09:23</t>
+          <t>09:17</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D109" t="n">
-        <v>115</v>
+        <v>43</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -3078,21 +3078,21 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>08:34:05</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>09:23</t>
+          <t>09:21</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D110" t="n">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -3103,21 +3103,21 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>09:24</t>
+          <t>09:22</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D111" t="n">
-        <v>116</v>
+        <v>69</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -3128,21 +3128,21 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>08:34:05</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>09:32</t>
+          <t>09:23</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3153,21 +3153,21 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>09:33</t>
+          <t>09:23</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>80</v>
+        <v>115</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3183,16 +3183,16 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>09:34</t>
+          <t>09:23</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D114" t="n">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -3203,21 +3203,21 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>08:34:05</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>09:41</t>
+          <t>09:24</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D115" t="n">
-        <v>88</v>
+        <v>50</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -3228,21 +3228,21 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>07:51:34</t>
+          <t>08:34:05</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>09:42</t>
+          <t>09:32</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D116" t="n">
-        <v>111</v>
+        <v>58</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -3253,21 +3253,21 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>08:34:05</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>09:43</t>
+          <t>09:33</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D117" t="n">
-        <v>90</v>
+        <v>59</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -3283,7 +3283,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>09:58</t>
+          <t>09:34</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
@@ -3292,7 +3292,7 @@
         </is>
       </c>
       <c r="D118" t="n">
-        <v>105</v>
+        <v>81</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -3303,23 +3303,298 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
+          <t>08:34:05</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>09:35</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D119" t="n">
+        <v>61</v>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>08:34:05</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>09:35</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D120" t="n">
+        <v>61</v>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
           <t>08:13:38</t>
         </is>
       </c>
-      <c r="B119" t="inlineStr">
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>09:41</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D121" t="n">
+        <v>88</v>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>08:34:05</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>09:42</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D122" t="n">
+        <v>68</v>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>08:13:38</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>09:43</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D123" t="n">
+        <v>90</v>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>08:34:05</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>09:44</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D124" t="n">
+        <v>70</v>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>08:13:38</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>09:58</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D125" t="n">
+        <v>105</v>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>08:34:05</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>10:11</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D126" t="n">
+        <v>97</v>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>08:34:05</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
         <is>
           <t>10:12</t>
         </is>
       </c>
-      <c r="C119" t="inlineStr">
+      <c r="C127" t="inlineStr">
         <is>
           <t>15_ABASTO</t>
         </is>
       </c>
-      <c r="D119" t="n">
-        <v>119</v>
-      </c>
-      <c r="E119" t="inlineStr">
+      <c r="D127" t="n">
+        <v>98</v>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>08:34:05</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>10:21</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D128" t="n">
+        <v>107</v>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>08:34:05</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>10:22</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D129" t="n">
+        <v>108</v>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>08:34:05</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>10:27</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D130" t="n">
+        <v>113</v>
+      </c>
+      <c r="E130" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -3336,7 +3611,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3354,14 +3629,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:13:38</t>
+          <t>Última actualización: 08:34:05</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 20</t>
+          <t>Total filas: 21</t>
         </is>
       </c>
     </row>
@@ -3820,7 +4095,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>08:34:05</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -3834,7 +4109,7 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>94</v>
+        <v>28</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -3870,7 +4145,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>07:51:34</t>
+          <t>08:34:05</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -3884,9 +4159,34 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>111</v>
+        <v>68</v>
       </c>
       <c r="E25" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>08:34:05</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>10:27</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>113</v>
+      </c>
+      <c r="E26" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -3903,7 +4203,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3921,14 +4221,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:13:38</t>
+          <t>Última actualización: 08:34:05</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 23</t>
+          <t>Total filas: 24</t>
         </is>
       </c>
     </row>
@@ -4462,37 +4762,37 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>08:34:05</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>09:08</t>
+          <t>08:46</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>215D_LA PLATA</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>55</v>
+        <v>12</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>L6203</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>07:51:34</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>09:09</t>
+          <t>09:08</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -4501,7 +4801,7 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -4512,23 +4812,48 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>08:34:05</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
+          <t>09:09</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>215D_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>35</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>08:34:05</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
           <t>10:03</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
+      <c r="C29" t="inlineStr">
         <is>
           <t>215B_LP-P MOR-40 Y 115</t>
         </is>
       </c>
-      <c r="D28" t="n">
-        <v>110</v>
-      </c>
-      <c r="E28" t="inlineStr">
+      <c r="D29" t="n">
+        <v>89</v>
+      </c>
+      <c r="E29" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 829
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-23.xlsx
+++ b/data/horarios-141-2026-01-23.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E130"/>
+  <dimension ref="A1:E133"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:34:05</t>
+          <t>Última actualización: 08:48:01</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 125</t>
+          <t>Total filas: 128</t>
         </is>
       </c>
     </row>
@@ -1313,7 +1313,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>86_EST CHICA-ESC AGRARIA</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1338,7 +1338,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>86_EST CHICA-ESC AGRARIA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1513,7 +1513,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -1538,7 +1538,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -1628,7 +1628,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1638,11 +1638,11 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>73</v>
+        <v>6</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -1653,7 +1653,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1663,11 +1663,11 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>6</v>
+        <v>73</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D63" t="n">
@@ -1938,7 +1938,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -1953,7 +1953,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1963,11 +1963,11 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -1988,7 +1988,7 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D66" t="n">
@@ -2003,7 +2003,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -2013,11 +2013,11 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2128,7 +2128,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -2138,11 +2138,11 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -2153,7 +2153,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -2163,11 +2163,11 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D73" t="n">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -2528,7 +2528,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -2538,11 +2538,11 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -2553,7 +2553,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2563,11 +2563,11 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -2753,7 +2753,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>08:34:05</t>
+          <t>08:48:01</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -2767,7 +2767,7 @@
         </is>
       </c>
       <c r="D97" t="n">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -2853,7 +2853,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>08:34:05</t>
+          <t>08:48:01</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -2867,7 +2867,7 @@
         </is>
       </c>
       <c r="D101" t="n">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -2903,7 +2903,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>08:34:05</t>
+          <t>08:48:01</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -2917,7 +2917,7 @@
         </is>
       </c>
       <c r="D103" t="n">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -2928,7 +2928,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>08:34:05</t>
+          <t>08:48:01</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -2942,7 +2942,7 @@
         </is>
       </c>
       <c r="D104" t="n">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -2978,7 +2978,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>08:34:05</t>
+          <t>08:48:01</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -2992,7 +2992,7 @@
         </is>
       </c>
       <c r="D106" t="n">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -3003,7 +3003,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>08:34:05</t>
+          <t>08:48:01</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -3017,7 +3017,7 @@
         </is>
       </c>
       <c r="D107" t="n">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -3053,7 +3053,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>08:34:05</t>
+          <t>08:48:01</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -3067,7 +3067,7 @@
         </is>
       </c>
       <c r="D109" t="n">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -3078,7 +3078,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>08:34:05</t>
+          <t>08:48:01</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -3092,7 +3092,7 @@
         </is>
       </c>
       <c r="D110" t="n">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -3128,7 +3128,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>08:34:05</t>
+          <t>08:48:01</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -3142,7 +3142,7 @@
         </is>
       </c>
       <c r="D112" t="n">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3203,7 +3203,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>08:34:05</t>
+          <t>08:48:01</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
@@ -3217,7 +3217,7 @@
         </is>
       </c>
       <c r="D115" t="n">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -3228,7 +3228,7 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>08:34:05</t>
+          <t>08:48:01</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
@@ -3242,7 +3242,7 @@
         </is>
       </c>
       <c r="D116" t="n">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -3253,7 +3253,7 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>08:34:05</t>
+          <t>08:48:01</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
@@ -3267,7 +3267,7 @@
         </is>
       </c>
       <c r="D117" t="n">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -3303,7 +3303,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>08:34:05</t>
+          <t>08:48:01</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -3313,11 +3313,11 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D119" t="n">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -3328,7 +3328,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>08:34:05</t>
+          <t>08:48:01</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
@@ -3338,11 +3338,11 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D120" t="n">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
@@ -3378,7 +3378,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>08:34:05</t>
+          <t>08:48:01</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
@@ -3392,7 +3392,7 @@
         </is>
       </c>
       <c r="D122" t="n">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -3428,7 +3428,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>08:34:05</t>
+          <t>08:48:01</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
@@ -3442,7 +3442,7 @@
         </is>
       </c>
       <c r="D124" t="n">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -3453,21 +3453,21 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>08:48:01</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>09:58</t>
+          <t>09:52</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D125" t="n">
-        <v>105</v>
+        <v>64</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -3478,21 +3478,21 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>08:34:05</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>10:11</t>
+          <t>09:58</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D126" t="n">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -3503,21 +3503,21 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>08:34:05</t>
+          <t>08:48:01</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>10:12</t>
+          <t>10:11</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D127" t="n">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
@@ -3533,16 +3533,16 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>10:21</t>
+          <t>10:12</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D128" t="n">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -3553,21 +3553,21 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>08:34:05</t>
+          <t>08:48:01</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>10:22</t>
+          <t>10:21</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D129" t="n">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -3578,23 +3578,98 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>08:34:05</t>
+          <t>08:48:01</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
+          <t>10:22</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D130" t="n">
+        <v>94</v>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>08:48:01</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
           <t>10:27</t>
         </is>
       </c>
-      <c r="C130" t="inlineStr">
+      <c r="C131" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D130" t="n">
-        <v>113</v>
-      </c>
-      <c r="E130" t="inlineStr">
+      <c r="D131" t="n">
+        <v>99</v>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>08:48:01</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>10:42</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D132" t="n">
+        <v>114</v>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>08:48:01</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>10:44</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D133" t="n">
+        <v>116</v>
+      </c>
+      <c r="E133" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -3629,7 +3704,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:34:05</t>
+          <t>Última actualización: 08:48:01</t>
         </is>
       </c>
     </row>
@@ -4095,7 +4170,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>08:34:05</t>
+          <t>08:48:01</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -4109,7 +4184,7 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -4145,7 +4220,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>08:34:05</t>
+          <t>08:48:01</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -4159,7 +4234,7 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -4170,7 +4245,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>08:34:05</t>
+          <t>08:48:01</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -4184,7 +4259,7 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -4203,7 +4278,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4221,14 +4296,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:34:05</t>
+          <t>Última actualización: 08:48:01</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 24</t>
+          <t>Total filas: 25</t>
         </is>
       </c>
     </row>
@@ -4837,23 +4912,48 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>08:34:05</t>
+          <t>08:48:01</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
+          <t>09:10</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>215D_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>22</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>08:48:01</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
           <t>10:03</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
+      <c r="C30" t="inlineStr">
         <is>
           <t>215B_LP-P MOR-40 Y 115</t>
         </is>
       </c>
-      <c r="D29" t="n">
-        <v>89</v>
-      </c>
-      <c r="E29" t="inlineStr">
+      <c r="D30" t="n">
+        <v>75</v>
+      </c>
+      <c r="E30" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 830
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-23.xlsx
+++ b/data/horarios-141-2026-01-23.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E133"/>
+  <dimension ref="A1:E139"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:48:01</t>
+          <t>Última actualización: 08:56:26</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 128</t>
+          <t>Total filas: 134</t>
         </is>
       </c>
     </row>
@@ -1313,7 +1313,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>86_EST CHICA-ESC AGRARIA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1338,7 +1338,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>86_EST CHICA-ESC AGRARIA</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1963,7 +1963,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D65" t="n">
@@ -1978,7 +1978,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -1988,11 +1988,11 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2003,7 +2003,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -2013,11 +2013,11 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2128,7 +2128,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -2138,11 +2138,11 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -2153,7 +2153,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -2163,11 +2163,11 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D73" t="n">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -2828,7 +2828,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -2842,7 +2842,7 @@
         </is>
       </c>
       <c r="D100" t="n">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -2878,7 +2878,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -2892,7 +2892,7 @@
         </is>
       </c>
       <c r="D102" t="n">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -2903,7 +2903,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>08:48:01</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -2913,11 +2913,11 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -2933,16 +2933,16 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>09:05</t>
+          <t>09:04</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D104" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -2953,21 +2953,21 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>08:48:01</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>09:10</t>
+          <t>09:05</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D105" t="n">
-        <v>57</v>
+        <v>17</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -2978,12 +2978,12 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>08:48:01</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>09:11</t>
+          <t>09:10</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -2992,7 +2992,7 @@
         </is>
       </c>
       <c r="D106" t="n">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -3008,16 +3008,16 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>09:13</t>
+          <t>09:11</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D107" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -3028,21 +3028,21 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>09:16</t>
+          <t>09:13</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D108" t="n">
-        <v>63</v>
+        <v>17</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -3053,12 +3053,12 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>08:48:01</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>09:17</t>
+          <t>09:16</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -3067,7 +3067,7 @@
         </is>
       </c>
       <c r="D109" t="n">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -3083,16 +3083,16 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>09:21</t>
+          <t>09:17</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D110" t="n">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -3103,21 +3103,21 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>09:22</t>
+          <t>09:21</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D111" t="n">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -3128,21 +3128,21 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>08:48:01</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>09:23</t>
+          <t>09:22</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>35</v>
+        <v>69</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3178,7 +3178,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
@@ -3192,7 +3192,7 @@
         </is>
       </c>
       <c r="D114" t="n">
-        <v>70</v>
+        <v>27</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -3203,21 +3203,21 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>08:48:01</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>09:24</t>
+          <t>09:23</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D115" t="n">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -3233,16 +3233,16 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>09:32</t>
+          <t>09:24</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D116" t="n">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -3253,21 +3253,21 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>08:48:01</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>09:33</t>
+          <t>09:32</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D117" t="n">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -3278,21 +3278,21 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>09:34</t>
+          <t>09:33</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D118" t="n">
-        <v>81</v>
+        <v>37</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -3303,21 +3303,21 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>08:48:01</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>09:35</t>
+          <t>09:34</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D119" t="n">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -3328,21 +3328,21 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>08:48:01</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>09:35</t>
+          <t>09:34</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D120" t="n">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
@@ -3353,21 +3353,21 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>08:48:01</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>09:41</t>
+          <t>09:35</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D121" t="n">
-        <v>88</v>
+        <v>47</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
@@ -3383,16 +3383,16 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>09:42</t>
+          <t>09:35</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D122" t="n">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -3408,16 +3408,16 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>09:43</t>
+          <t>09:41</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D123" t="n">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -3428,21 +3428,21 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>08:48:01</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>09:44</t>
+          <t>09:42</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D124" t="n">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -3453,21 +3453,21 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>08:48:01</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>09:52</t>
+          <t>09:43</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D125" t="n">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -3478,21 +3478,21 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>08:48:01</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>09:58</t>
+          <t>09:44</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D126" t="n">
-        <v>105</v>
+        <v>56</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -3503,21 +3503,21 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>08:48:01</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>10:11</t>
+          <t>09:52</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D127" t="n">
-        <v>83</v>
+        <v>56</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
@@ -3528,21 +3528,21 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>08:34:05</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>10:12</t>
+          <t>09:53</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D128" t="n">
-        <v>98</v>
+        <v>57</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -3553,21 +3553,21 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>08:48:01</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>10:21</t>
+          <t>09:58</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D129" t="n">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -3578,21 +3578,21 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>08:48:01</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>10:22</t>
+          <t>10:10</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D130" t="n">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -3608,16 +3608,16 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>10:27</t>
+          <t>10:11</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D131" t="n">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -3628,21 +3628,21 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>08:48:01</t>
+          <t>08:34:05</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>10:42</t>
+          <t>10:12</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D132" t="n">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -3653,23 +3653,173 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
+          <t>08:56:26</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>10:21</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D133" t="n">
+        <v>85</v>
+      </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>08:56:26</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>10:22</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D134" t="n">
+        <v>86</v>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>08:56:26</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>10:26</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D135" t="n">
+        <v>90</v>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
           <t>08:48:01</t>
         </is>
       </c>
-      <c r="B133" t="inlineStr">
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>10:27</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D136" t="n">
+        <v>99</v>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>08:56:26</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>10:42</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D137" t="n">
+        <v>106</v>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>08:56:26</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>10:43</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D138" t="n">
+        <v>107</v>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>08:48:01</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
         <is>
           <t>10:44</t>
         </is>
       </c>
-      <c r="C133" t="inlineStr">
+      <c r="C139" t="inlineStr">
         <is>
           <t>14_ABASTO</t>
         </is>
       </c>
-      <c r="D133" t="n">
+      <c r="D139" t="n">
         <v>116</v>
       </c>
-      <c r="E133" t="inlineStr">
+      <c r="E139" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -3686,7 +3836,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3704,14 +3854,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:48:01</t>
+          <t>Última actualización: 08:56:26</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 21</t>
+          <t>Total filas: 22</t>
         </is>
       </c>
     </row>
@@ -4145,7 +4295,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -4159,7 +4309,7 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -4220,7 +4370,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>08:48:01</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -4234,7 +4384,7 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -4245,23 +4395,48 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
+          <t>08:56:26</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>10:26</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>90</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
           <t>08:48:01</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr">
+      <c r="B27" t="inlineStr">
         <is>
           <t>10:27</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
+      <c r="C27" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D26" t="n">
+      <c r="D27" t="n">
         <v>99</v>
       </c>
-      <c r="E26" t="inlineStr">
+      <c r="E27" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -4278,7 +4453,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4296,14 +4471,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:48:01</t>
+          <t>Última actualización: 08:56:26</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 25</t>
+          <t>Total filas: 26</t>
         </is>
       </c>
     </row>
@@ -4887,7 +5062,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>08:34:05</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -4901,7 +5076,7 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -4937,7 +5112,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>08:48:01</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -4951,9 +5126,34 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="E30" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>08:56:26</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>10:54</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>118</v>
+      </c>
+      <c r="E31" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 831
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-23.xlsx
+++ b/data/horarios-141-2026-01-23.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E139"/>
+  <dimension ref="A1:E153"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:56:26</t>
+          <t>Última actualización: 09:33:33</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 134</t>
+          <t>Total filas: 148</t>
         </is>
       </c>
     </row>
@@ -1313,7 +1313,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>86_EST CHICA-ESC AGRARIA</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1338,7 +1338,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>86_EST CHICA-ESC AGRARIA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1628,7 +1628,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1638,11 +1638,11 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>6</v>
+        <v>73</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -1653,7 +1653,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1663,11 +1663,11 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>73</v>
+        <v>6</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -1778,7 +1778,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1788,11 +1788,11 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>17</v>
+        <v>84</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -1803,7 +1803,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1813,11 +1813,11 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D63" t="n">
@@ -1938,7 +1938,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -2803,7 +2803,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -2813,11 +2813,11 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D99" t="n">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -2828,7 +2828,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -2838,11 +2838,11 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -3153,7 +3153,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3163,11 +3163,11 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>115</v>
+        <v>27</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3188,7 +3188,7 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D114" t="n">
@@ -3203,7 +3203,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
@@ -3213,11 +3213,11 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D115" t="n">
-        <v>27</v>
+        <v>115</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -3303,12 +3303,12 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>09:33:33</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>09:34</t>
+          <t>09:33</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
@@ -3317,7 +3317,7 @@
         </is>
       </c>
       <c r="D119" t="n">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -3353,12 +3353,12 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>08:48:01</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>09:35</t>
+          <t>09:34</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
@@ -3367,7 +3367,7 @@
         </is>
       </c>
       <c r="D121" t="n">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
@@ -3388,7 +3388,7 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D122" t="n">
@@ -3403,21 +3403,21 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>08:48:01</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>09:41</t>
+          <t>09:35</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D123" t="n">
-        <v>88</v>
+        <v>47</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -3428,12 +3428,12 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>09:42</t>
+          <t>09:41</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
@@ -3442,7 +3442,7 @@
         </is>
       </c>
       <c r="D124" t="n">
-        <v>46</v>
+        <v>88</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -3453,21 +3453,21 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>09:33:33</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>09:43</t>
+          <t>09:42</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D125" t="n">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -3478,12 +3478,12 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>08:48:01</t>
+          <t>09:33:33</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>09:44</t>
+          <t>09:43</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
@@ -3492,7 +3492,7 @@
         </is>
       </c>
       <c r="D126" t="n">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -3503,17 +3503,17 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>08:48:01</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>09:52</t>
+          <t>09:44</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D127" t="n">
@@ -3528,21 +3528,21 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>09:33:33</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>09:53</t>
+          <t>09:46</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D128" t="n">
-        <v>57</v>
+        <v>13</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -3553,21 +3553,21 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>09:33:33</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>09:58</t>
+          <t>09:52</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D129" t="n">
-        <v>105</v>
+        <v>19</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -3578,21 +3578,21 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>09:33:33</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>10:10</t>
+          <t>09:53</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D130" t="n">
-        <v>74</v>
+        <v>20</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -3603,21 +3603,21 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>08:48:01</t>
+          <t>09:33:33</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>10:11</t>
+          <t>09:58</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D131" t="n">
-        <v>83</v>
+        <v>25</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -3628,21 +3628,21 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>08:34:05</t>
+          <t>09:33:33</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>10:12</t>
+          <t>10:03</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D132" t="n">
-        <v>98</v>
+        <v>30</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -3653,21 +3653,21 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>09:33:33</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>10:21</t>
+          <t>10:04</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D133" t="n">
-        <v>85</v>
+        <v>31</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -3678,21 +3678,21 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>09:33:33</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>10:22</t>
+          <t>10:10</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D134" t="n">
-        <v>86</v>
+        <v>37</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -3703,21 +3703,21 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>08:48:01</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>10:26</t>
+          <t>10:11</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D135" t="n">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -3728,21 +3728,21 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>08:48:01</t>
+          <t>08:34:05</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>10:27</t>
+          <t>10:12</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D136" t="n">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -3753,21 +3753,21 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>09:33:33</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>10:42</t>
+          <t>10:13</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D137" t="n">
-        <v>106</v>
+        <v>40</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -3778,21 +3778,21 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>09:33:33</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>10:43</t>
+          <t>10:21</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D138" t="n">
-        <v>107</v>
+        <v>48</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -3803,23 +3803,373 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
+          <t>09:33:33</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>10:22</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D139" t="n">
+        <v>49</v>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>09:33:33</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>10:23</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D140" t="n">
+        <v>50</v>
+      </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>09:33:33</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>10:26</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D141" t="n">
+        <v>53</v>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
           <t>08:48:01</t>
         </is>
       </c>
-      <c r="B139" t="inlineStr">
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>10:27</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D142" t="n">
+        <v>99</v>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>09:33:33</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>10:42</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D143" t="n">
+        <v>69</v>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>09:33:33</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>10:43</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D144" t="n">
+        <v>70</v>
+      </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>08:48:01</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
         <is>
           <t>10:44</t>
         </is>
       </c>
-      <c r="C139" t="inlineStr">
+      <c r="C145" t="inlineStr">
         <is>
           <t>14_ABASTO</t>
         </is>
       </c>
-      <c r="D139" t="n">
+      <c r="D145" t="n">
         <v>116</v>
       </c>
-      <c r="E139" t="inlineStr">
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>09:33:33</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>10:52</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D146" t="n">
+        <v>79</v>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>09:33:33</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>10:56</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D147" t="n">
+        <v>83</v>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>09:33:33</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>11:02</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D148" t="n">
+        <v>89</v>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>09:33:33</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>11:06</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D149" t="n">
+        <v>93</v>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>09:33:33</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>11:19</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>86_EST CHICA-ESC AGRARIA</t>
+        </is>
+      </c>
+      <c r="D150" t="n">
+        <v>106</v>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>09:33:33</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>11:21</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D151" t="n">
+        <v>108</v>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>09:33:33</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>11:27</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>225_C ROCA-H SUR</t>
+        </is>
+      </c>
+      <c r="D152" t="n">
+        <v>114</v>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>09:33:33</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>11:32</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D153" t="n">
+        <v>119</v>
+      </c>
+      <c r="E153" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -3836,7 +4186,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3854,14 +4204,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:56:26</t>
+          <t>Última actualización: 09:33:33</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 22</t>
+          <t>Total filas: 23</t>
         </is>
       </c>
     </row>
@@ -4370,7 +4720,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>09:33:33</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -4384,7 +4734,7 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -4395,7 +4745,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>09:33:33</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -4409,7 +4759,7 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>90</v>
+        <v>53</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -4437,6 +4787,31 @@
         <v>99</v>
       </c>
       <c r="E27" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>09:33:33</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>11:02</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>89</v>
+      </c>
+      <c r="E28" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -4453,7 +4828,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4471,14 +4846,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:56:26</t>
+          <t>Última actualización: 09:33:33</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 26</t>
+          <t>Total filas: 27</t>
         </is>
       </c>
     </row>
@@ -5112,7 +5487,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>09:33:33</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -5126,7 +5501,7 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>67</v>
+        <v>30</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -5137,7 +5512,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>09:33:33</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -5151,11 +5526,36 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>118</v>
+        <v>81</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
           <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>09:33:33</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>11:14</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>101</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 832
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-23.xlsx
+++ b/data/horarios-141-2026-01-23.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E153"/>
+  <dimension ref="A1:E172"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 09:33:33</t>
+          <t>Última actualización: 10:27:29</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 148</t>
+          <t>Total filas: 167</t>
         </is>
       </c>
     </row>
@@ -1513,7 +1513,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -1538,7 +1538,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -1913,7 +1913,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D63" t="n">
@@ -1938,7 +1938,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -1963,7 +1963,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D65" t="n">
@@ -1978,7 +1978,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -1988,11 +1988,11 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2003,7 +2003,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -2013,11 +2013,11 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2528,7 +2528,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -2538,11 +2538,11 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -2553,7 +2553,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2563,11 +2563,11 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -2803,7 +2803,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -2813,11 +2813,11 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D99" t="n">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -2828,7 +2828,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -2838,11 +2838,11 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -3163,7 +3163,7 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D113" t="n">
@@ -3188,7 +3188,7 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D114" t="n">
@@ -3278,7 +3278,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>09:33:33</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -3288,11 +3288,11 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D118" t="n">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -3303,7 +3303,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>09:33:33</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -3313,11 +3313,11 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D119" t="n">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -3388,7 +3388,7 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D122" t="n">
@@ -3413,7 +3413,7 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D123" t="n">
@@ -3878,7 +3878,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>08:48:01</t>
+          <t>10:27:29</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
@@ -3892,7 +3892,7 @@
         </is>
       </c>
       <c r="D142" t="n">
-        <v>99</v>
+        <v>0</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -3903,21 +3903,21 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>09:33:33</t>
+          <t>10:27:29</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>10:42</t>
+          <t>10:29</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D143" t="n">
-        <v>69</v>
+        <v>2</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -3928,21 +3928,21 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>09:33:33</t>
+          <t>10:27:29</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>10:43</t>
+          <t>10:34</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D144" t="n">
-        <v>70</v>
+        <v>7</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -3953,21 +3953,21 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>08:48:01</t>
+          <t>10:27:29</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>10:44</t>
+          <t>10:35</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D145" t="n">
-        <v>116</v>
+        <v>8</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
@@ -3978,21 +3978,21 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>09:33:33</t>
+          <t>10:27:29</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>10:52</t>
+          <t>10:42</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D146" t="n">
-        <v>79</v>
+        <v>15</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -4003,21 +4003,21 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>09:33:33</t>
+          <t>10:27:29</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>10:56</t>
+          <t>10:43</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D147" t="n">
-        <v>83</v>
+        <v>16</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -4028,21 +4028,21 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>09:33:33</t>
+          <t>08:48:01</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>11:02</t>
+          <t>10:44</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D148" t="n">
-        <v>89</v>
+        <v>116</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -4053,21 +4053,21 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>09:33:33</t>
+          <t>10:27:29</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>11:06</t>
+          <t>10:46</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D149" t="n">
-        <v>93</v>
+        <v>19</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
@@ -4078,21 +4078,21 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>09:33:33</t>
+          <t>10:27:29</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>11:19</t>
+          <t>10:52</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>86_EST CHICA-ESC AGRARIA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D150" t="n">
-        <v>106</v>
+        <v>25</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
@@ -4103,21 +4103,21 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>09:33:33</t>
+          <t>10:27:29</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>11:21</t>
+          <t>10:53</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D151" t="n">
-        <v>108</v>
+        <v>26</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -4128,21 +4128,21 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>09:33:33</t>
+          <t>10:27:29</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>11:27</t>
+          <t>10:56</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D152" t="n">
-        <v>114</v>
+        <v>29</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -4153,23 +4153,498 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>09:33:33</t>
+          <t>10:27:29</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
         <is>
+          <t>11:02</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D153" t="n">
+        <v>35</v>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>10:27:29</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>11:03</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D154" t="n">
+        <v>36</v>
+      </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>10:27:29</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>11:04</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D155" t="n">
+        <v>37</v>
+      </c>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>10:27:29</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>11:06</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D156" t="n">
+        <v>39</v>
+      </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>10:27:29</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>11:12</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D157" t="n">
+        <v>45</v>
+      </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>10:27:29</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>11:19</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>86_EST CHICA-ESC AGRARIA</t>
+        </is>
+      </c>
+      <c r="D158" t="n">
+        <v>52</v>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>10:27:29</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>11:21</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D159" t="n">
+        <v>54</v>
+      </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>10:27:29</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>11:27</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>225_C ROCA-H SUR</t>
+        </is>
+      </c>
+      <c r="D160" t="n">
+        <v>60</v>
+      </c>
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>10:27:29</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
           <t>11:32</t>
         </is>
       </c>
-      <c r="C153" t="inlineStr">
+      <c r="C161" t="inlineStr">
         <is>
           <t>81_EL PELIGRO</t>
         </is>
       </c>
-      <c r="D153" t="n">
-        <v>119</v>
-      </c>
-      <c r="E153" t="inlineStr">
+      <c r="D161" t="n">
+        <v>65</v>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>10:27:29</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>11:35</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D162" t="n">
+        <v>68</v>
+      </c>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>10:27:29</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>11:42</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D163" t="n">
+        <v>75</v>
+      </c>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>10:27:29</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>11:49</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D164" t="n">
+        <v>82</v>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>10:27:29</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>11:51</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D165" t="n">
+        <v>84</v>
+      </c>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>10:27:29</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>11:59</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D166" t="n">
+        <v>92</v>
+      </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>10:27:29</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>12:02</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D167" t="n">
+        <v>95</v>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>10:27:29</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>12:06</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D168" t="n">
+        <v>99</v>
+      </c>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>10:27:29</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>12:14</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D169" t="n">
+        <v>107</v>
+      </c>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>10:27:29</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>12:17</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D170" t="n">
+        <v>110</v>
+      </c>
+      <c r="E170" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>10:27:29</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>12:20</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D171" t="n">
+        <v>113</v>
+      </c>
+      <c r="E171" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>10:27:29</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>12:21</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D172" t="n">
+        <v>114</v>
+      </c>
+      <c r="E172" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -4186,7 +4661,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4204,14 +4679,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 09:33:33</t>
+          <t>Última actualización: 10:27:29</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 23</t>
+          <t>Total filas: 25</t>
         </is>
       </c>
     </row>
@@ -4770,7 +5245,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>08:48:01</t>
+          <t>10:27:29</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -4784,7 +5259,7 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>99</v>
+        <v>0</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -4795,7 +5270,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>09:33:33</t>
+          <t>10:27:29</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -4809,9 +5284,59 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>89</v>
+        <v>35</v>
       </c>
       <c r="E28" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>10:27:29</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>11:51</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>84</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>10:27:29</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>12:20</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>113</v>
+      </c>
+      <c r="E30" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -4828,7 +5353,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4846,14 +5371,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 09:33:33</t>
+          <t>Última actualización: 10:27:29</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 27</t>
+          <t>Total filas: 28</t>
         </is>
       </c>
     </row>
@@ -5512,7 +6037,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>09:33:33</t>
+          <t>10:27:29</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -5526,7 +6051,7 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>81</v>
+        <v>27</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -5537,7 +6062,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>09:33:33</t>
+          <t>10:27:29</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -5551,11 +6076,36 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>101</v>
+        <v>47</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>10:27:29</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>12:04</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>97</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 833
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-23.xlsx
+++ b/data/horarios-141-2026-01-23.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E172"/>
+  <dimension ref="A1:E183"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 10:27:29</t>
+          <t>Última actualización: 10:57:35</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 167</t>
+          <t>Total filas: 178</t>
         </is>
       </c>
     </row>
@@ -1313,7 +1313,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>86_EST CHICA-ESC AGRARIA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1338,7 +1338,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>86_EST CHICA-ESC AGRARIA</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1628,7 +1628,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1638,11 +1638,11 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>73</v>
+        <v>6</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -1653,7 +1653,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1663,11 +1663,11 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>6</v>
+        <v>73</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -1778,7 +1778,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1788,11 +1788,11 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -1803,7 +1803,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1813,11 +1813,11 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>17</v>
+        <v>84</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D63" t="n">
@@ -1938,7 +1938,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -1963,7 +1963,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D65" t="n">
@@ -1978,7 +1978,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -1988,11 +1988,11 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2003,7 +2003,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -2013,11 +2013,11 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2128,7 +2128,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -2138,11 +2138,11 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -2153,7 +2153,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -2163,11 +2163,11 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D73" t="n">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -2803,7 +2803,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -2813,11 +2813,11 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D99" t="n">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -2828,7 +2828,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -2838,11 +2838,11 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -2903,7 +2903,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>08:48:01</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -2913,11 +2913,11 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -2928,7 +2928,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>08:48:01</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -2938,11 +2938,11 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D104" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -3163,7 +3163,7 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D113" t="n">
@@ -3178,7 +3178,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
@@ -3188,11 +3188,11 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D114" t="n">
-        <v>27</v>
+        <v>115</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -3203,7 +3203,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
@@ -3213,11 +3213,11 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D115" t="n">
-        <v>115</v>
+        <v>27</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -3278,7 +3278,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>09:33:33</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -3288,11 +3288,11 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D118" t="n">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -3303,7 +3303,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>09:33:33</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -3313,11 +3313,11 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D119" t="n">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -3338,7 +3338,7 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D120" t="n">
@@ -3363,7 +3363,7 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D121" t="n">
@@ -3388,7 +3388,7 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D122" t="n">
@@ -3413,7 +3413,7 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D123" t="n">
@@ -4153,21 +4153,21 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>10:27:29</t>
+          <t>10:57:35</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>11:02</t>
+          <t>10:57</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D153" t="n">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -4178,21 +4178,21 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>10:27:29</t>
+          <t>10:57:35</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>11:03</t>
+          <t>10:57</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D154" t="n">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -4203,21 +4203,21 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>10:27:29</t>
+          <t>10:57:35</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>11:04</t>
+          <t>11:02</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D155" t="n">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
@@ -4228,21 +4228,21 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>10:27:29</t>
+          <t>10:57:35</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>11:06</t>
+          <t>11:03</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D156" t="n">
-        <v>39</v>
+        <v>6</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
@@ -4253,21 +4253,21 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>10:27:29</t>
+          <t>10:57:35</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>11:12</t>
+          <t>11:04</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D157" t="n">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
@@ -4278,21 +4278,21 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>10:27:29</t>
+          <t>10:57:35</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>11:19</t>
+          <t>11:06</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>86_EST CHICA-ESC AGRARIA</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D158" t="n">
-        <v>52</v>
+        <v>9</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -4303,21 +4303,21 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>10:27:29</t>
+          <t>10:57:35</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>11:21</t>
+          <t>11:11</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D159" t="n">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
@@ -4328,21 +4328,21 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>10:27:29</t>
+          <t>10:57:35</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>11:27</t>
+          <t>11:12</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D160" t="n">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -4353,21 +4353,21 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>10:27:29</t>
+          <t>10:57:35</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>11:32</t>
+          <t>11:19</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>86_EST CHICA-ESC AGRARIA</t>
         </is>
       </c>
       <c r="D161" t="n">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -4378,21 +4378,21 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>10:27:29</t>
+          <t>10:57:35</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>11:35</t>
+          <t>11:21</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D162" t="n">
-        <v>68</v>
+        <v>24</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -4403,21 +4403,21 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>10:27:29</t>
+          <t>10:57:35</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>11:42</t>
+          <t>11:27</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>225_C ROCA-H SUR</t>
         </is>
       </c>
       <c r="D163" t="n">
-        <v>75</v>
+        <v>30</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
@@ -4428,21 +4428,21 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>10:27:29</t>
+          <t>10:57:35</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>11:49</t>
+          <t>11:32</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D164" t="n">
-        <v>82</v>
+        <v>35</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
@@ -4453,21 +4453,21 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>10:27:29</t>
+          <t>10:57:35</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>11:51</t>
+          <t>11:34</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D165" t="n">
-        <v>84</v>
+        <v>37</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -4478,21 +4478,21 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>10:27:29</t>
+          <t>10:57:35</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>11:59</t>
+          <t>11:35</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D166" t="n">
-        <v>92</v>
+        <v>38</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -4503,21 +4503,21 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>10:27:29</t>
+          <t>10:57:35</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>12:02</t>
+          <t>11:42</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D167" t="n">
-        <v>95</v>
+        <v>45</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -4528,21 +4528,21 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>10:27:29</t>
+          <t>10:57:35</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>12:06</t>
+          <t>11:43</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D168" t="n">
-        <v>99</v>
+        <v>46</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
@@ -4558,16 +4558,16 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>12:14</t>
+          <t>11:49</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D169" t="n">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -4578,21 +4578,21 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>10:27:29</t>
+          <t>10:57:35</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>12:17</t>
+          <t>11:51</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D170" t="n">
-        <v>110</v>
+        <v>54</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -4603,21 +4603,21 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>10:27:29</t>
+          <t>10:57:35</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>12:20</t>
+          <t>11:52</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D171" t="n">
-        <v>113</v>
+        <v>55</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -4628,23 +4628,298 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
+          <t>10:57:35</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>11:59</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D172" t="n">
+        <v>62</v>
+      </c>
+      <c r="E172" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>10:57:35</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>12:02</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D173" t="n">
+        <v>65</v>
+      </c>
+      <c r="E173" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>10:57:35</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>12:06</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D174" t="n">
+        <v>69</v>
+      </c>
+      <c r="E174" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>10:57:35</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>12:06</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D175" t="n">
+        <v>69</v>
+      </c>
+      <c r="E175" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>10:57:35</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>12:14</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D176" t="n">
+        <v>77</v>
+      </c>
+      <c r="E176" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>10:57:35</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>12:14</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D177" t="n">
+        <v>77</v>
+      </c>
+      <c r="E177" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
           <t>10:27:29</t>
         </is>
       </c>
-      <c r="B172" t="inlineStr">
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>12:17</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D178" t="n">
+        <v>110</v>
+      </c>
+      <c r="E178" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>10:57:35</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>12:20</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D179" t="n">
+        <v>83</v>
+      </c>
+      <c r="E179" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>10:57:35</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>12:20</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D180" t="n">
+        <v>83</v>
+      </c>
+      <c r="E180" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>10:57:35</t>
+        </is>
+      </c>
+      <c r="B181" t="inlineStr">
         <is>
           <t>12:21</t>
         </is>
       </c>
-      <c r="C172" t="inlineStr">
+      <c r="C181" t="inlineStr">
         <is>
           <t>26_HERNANDEZ</t>
         </is>
       </c>
-      <c r="D172" t="n">
-        <v>114</v>
-      </c>
-      <c r="E172" t="inlineStr">
+      <c r="D181" t="n">
+        <v>84</v>
+      </c>
+      <c r="E181" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>10:57:35</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>12:36</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D182" t="n">
+        <v>99</v>
+      </c>
+      <c r="E182" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>10:57:35</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>12:38</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>17_179 Y 38</t>
+        </is>
+      </c>
+      <c r="D183" t="n">
+        <v>101</v>
+      </c>
+      <c r="E183" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -4679,7 +4954,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 10:27:29</t>
+          <t>Última actualización: 10:57:35</t>
         </is>
       </c>
     </row>
@@ -5270,7 +5545,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>10:27:29</t>
+          <t>10:57:35</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -5284,7 +5559,7 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -5295,7 +5570,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>10:27:29</t>
+          <t>10:57:35</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -5309,7 +5584,7 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>84</v>
+        <v>54</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -5320,7 +5595,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>10:27:29</t>
+          <t>10:57:35</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -5334,7 +5609,7 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>113</v>
+        <v>83</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -5353,7 +5628,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5371,14 +5646,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 10:27:29</t>
+          <t>Última actualización: 10:57:35</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 28</t>
+          <t>Total filas: 30</t>
         </is>
       </c>
     </row>
@@ -6062,12 +6337,12 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>10:27:29</t>
+          <t>10:57:35</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>11:14</t>
+          <t>11:13</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -6076,7 +6351,7 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -6092,20 +6367,70 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
+          <t>11:14</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>47</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>10:57:35</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
           <t>12:04</t>
         </is>
       </c>
-      <c r="C33" t="inlineStr">
+      <c r="C34" t="inlineStr">
         <is>
           <t>215A_LA PLATA</t>
         </is>
       </c>
-      <c r="D33" t="n">
-        <v>97</v>
-      </c>
-      <c r="E33" t="inlineStr">
+      <c r="D34" t="n">
+        <v>67</v>
+      </c>
+      <c r="E34" t="inlineStr">
         <is>
           <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>10:57:35</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>12:53</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>116</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 834
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-23.xlsx
+++ b/data/horarios-141-2026-01-23.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E183"/>
+  <dimension ref="A1:E196"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 10:57:35</t>
+          <t>Última actualización: 11:22:44</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 178</t>
+          <t>Total filas: 191</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1638,11 +1638,11 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>6</v>
+        <v>73</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -1653,7 +1653,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1663,11 +1663,11 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>73</v>
+        <v>6</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -1778,7 +1778,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1788,11 +1788,11 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>17</v>
+        <v>84</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -1803,7 +1803,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1813,11 +1813,11 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D63" t="n">
@@ -1938,7 +1938,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -1978,7 +1978,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -1988,11 +1988,11 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2003,7 +2003,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -2013,11 +2013,11 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2803,7 +2803,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -2813,11 +2813,11 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D99" t="n">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -2828,7 +2828,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -2838,11 +2838,11 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -3163,7 +3163,7 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D113" t="n">
@@ -3178,7 +3178,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
@@ -3188,11 +3188,11 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D114" t="n">
-        <v>115</v>
+        <v>27</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -3203,7 +3203,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
@@ -3213,11 +3213,11 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D115" t="n">
-        <v>27</v>
+        <v>115</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -3278,7 +3278,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>09:33:33</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -3288,11 +3288,11 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D118" t="n">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -3303,7 +3303,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>09:33:33</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -3313,11 +3313,11 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D119" t="n">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -3338,7 +3338,7 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D120" t="n">
@@ -3363,7 +3363,7 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D121" t="n">
@@ -3388,7 +3388,7 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D122" t="n">
@@ -3413,7 +3413,7 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D123" t="n">
@@ -4403,21 +4403,21 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>10:57:35</t>
+          <t>11:22:44</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>11:27</t>
+          <t>11:22</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D163" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
@@ -4428,21 +4428,21 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>10:57:35</t>
+          <t>11:22:44</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>11:32</t>
+          <t>11:22</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D164" t="n">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
@@ -4453,21 +4453,21 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>10:57:35</t>
+          <t>11:22:44</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>11:34</t>
+          <t>11:23</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_C ROCA-H SUR</t>
         </is>
       </c>
       <c r="D165" t="n">
-        <v>37</v>
+        <v>1</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -4483,16 +4483,16 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>11:35</t>
+          <t>11:27</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>225_C ROCA-H SUR</t>
         </is>
       </c>
       <c r="D166" t="n">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -4503,21 +4503,21 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>10:57:35</t>
+          <t>11:22:44</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>11:42</t>
+          <t>11:32</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D167" t="n">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -4528,21 +4528,21 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>10:57:35</t>
+          <t>11:22:44</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>11:43</t>
+          <t>11:34</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D168" t="n">
-        <v>46</v>
+        <v>12</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
@@ -4553,21 +4553,21 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>10:27:29</t>
+          <t>11:22:44</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>11:49</t>
+          <t>11:35</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D169" t="n">
-        <v>82</v>
+        <v>13</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -4578,21 +4578,21 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>10:57:35</t>
+          <t>11:22:44</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>11:51</t>
+          <t>11:41</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D170" t="n">
-        <v>54</v>
+        <v>19</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -4608,16 +4608,16 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>11:52</t>
+          <t>11:42</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D171" t="n">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -4628,21 +4628,21 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>10:57:35</t>
+          <t>11:22:44</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>11:59</t>
+          <t>11:43</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D172" t="n">
-        <v>62</v>
+        <v>21</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
@@ -4653,21 +4653,21 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>10:57:35</t>
+          <t>11:22:44</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>12:02</t>
+          <t>11:46</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D173" t="n">
-        <v>65</v>
+        <v>24</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
@@ -4678,21 +4678,21 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>10:57:35</t>
+          <t>10:27:29</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>12:06</t>
+          <t>11:49</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D174" t="n">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
@@ -4703,21 +4703,21 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>10:57:35</t>
+          <t>11:22:44</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>12:06</t>
+          <t>11:51</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D175" t="n">
-        <v>69</v>
+        <v>29</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
@@ -4728,21 +4728,21 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>10:57:35</t>
+          <t>11:22:44</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>12:14</t>
+          <t>11:52</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D176" t="n">
-        <v>77</v>
+        <v>30</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -4753,21 +4753,21 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>10:57:35</t>
+          <t>11:22:44</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>12:14</t>
+          <t>11:59</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D177" t="n">
-        <v>77</v>
+        <v>37</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -4778,21 +4778,21 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>10:27:29</t>
+          <t>11:22:44</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>12:17</t>
+          <t>12:02</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D178" t="n">
-        <v>110</v>
+        <v>40</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -4803,21 +4803,21 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>10:57:35</t>
+          <t>11:22:44</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>12:20</t>
+          <t>12:04</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D179" t="n">
-        <v>83</v>
+        <v>42</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -4828,12 +4828,12 @@
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>10:57:35</t>
+          <t>11:22:44</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>12:20</t>
+          <t>12:06</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
@@ -4842,7 +4842,7 @@
         </is>
       </c>
       <c r="D180" t="n">
-        <v>83</v>
+        <v>44</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
@@ -4853,21 +4853,21 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>10:57:35</t>
+          <t>11:22:44</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>12:21</t>
+          <t>12:06</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D181" t="n">
-        <v>84</v>
+        <v>44</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
@@ -4878,21 +4878,21 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>10:57:35</t>
+          <t>11:22:44</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>12:36</t>
+          <t>12:13</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D182" t="n">
-        <v>99</v>
+        <v>51</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
@@ -4908,18 +4908,343 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
+          <t>12:14</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D183" t="n">
+        <v>77</v>
+      </c>
+      <c r="E183" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>11:22:44</t>
+        </is>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>12:14</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D184" t="n">
+        <v>52</v>
+      </c>
+      <c r="E184" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>10:27:29</t>
+        </is>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>12:17</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D185" t="n">
+        <v>110</v>
+      </c>
+      <c r="E185" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>11:22:44</t>
+        </is>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>12:20</t>
+        </is>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D186" t="n">
+        <v>58</v>
+      </c>
+      <c r="E186" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>11:22:44</t>
+        </is>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>12:20</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D187" t="n">
+        <v>58</v>
+      </c>
+      <c r="E187" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>11:22:44</t>
+        </is>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>12:21</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D188" t="n">
+        <v>59</v>
+      </c>
+      <c r="E188" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>11:22:44</t>
+        </is>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>12:36</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D189" t="n">
+        <v>74</v>
+      </c>
+      <c r="E189" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>11:22:44</t>
+        </is>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
           <t>12:38</t>
         </is>
       </c>
-      <c r="C183" t="inlineStr">
+      <c r="C190" t="inlineStr">
         <is>
           <t>17_179 Y 38</t>
         </is>
       </c>
-      <c r="D183" t="n">
-        <v>101</v>
-      </c>
-      <c r="E183" t="inlineStr">
+      <c r="D190" t="n">
+        <v>76</v>
+      </c>
+      <c r="E190" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>11:22:44</t>
+        </is>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>12:48</t>
+        </is>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D191" t="n">
+        <v>86</v>
+      </c>
+      <c r="E191" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>11:22:44</t>
+        </is>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>12:50</t>
+        </is>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D192" t="n">
+        <v>88</v>
+      </c>
+      <c r="E192" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>11:22:44</t>
+        </is>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>13:06</t>
+        </is>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D193" t="n">
+        <v>104</v>
+      </c>
+      <c r="E193" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>11:22:44</t>
+        </is>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>13:10</t>
+        </is>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D194" t="n">
+        <v>108</v>
+      </c>
+      <c r="E194" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>11:22:44</t>
+        </is>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>13:13</t>
+        </is>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>215D_EL PATO</t>
+        </is>
+      </c>
+      <c r="D195" t="n">
+        <v>111</v>
+      </c>
+      <c r="E195" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>11:22:44</t>
+        </is>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>13:20</t>
+        </is>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D196" t="n">
+        <v>118</v>
+      </c>
+      <c r="E196" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -4936,7 +5261,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4954,14 +5279,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 10:57:35</t>
+          <t>Última actualización: 11:22:44</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 25</t>
+          <t>Total filas: 26</t>
         </is>
       </c>
     </row>
@@ -5570,7 +5895,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>10:57:35</t>
+          <t>11:22:44</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -5584,7 +5909,7 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -5595,7 +5920,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>10:57:35</t>
+          <t>11:22:44</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -5609,9 +5934,34 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="E30" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>11:22:44</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>13:13</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>215D_EL PATO</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>111</v>
+      </c>
+      <c r="E31" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -5646,7 +5996,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 10:57:35</t>
+          <t>Última actualización: 11:22:44</t>
         </is>
       </c>
     </row>
@@ -6387,7 +6737,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>10:57:35</t>
+          <t>11:22:44</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -6401,7 +6751,7 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -6412,7 +6762,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>10:57:35</t>
+          <t>11:22:44</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -6426,7 +6776,7 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>116</v>
+        <v>91</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 835
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-23.xlsx
+++ b/data/horarios-141-2026-01-23.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E196"/>
+  <dimension ref="A1:E208"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:22:44</t>
+          <t>Última actualización: 11:49:24</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 191</t>
+          <t>Total filas: 203</t>
         </is>
       </c>
     </row>
@@ -2528,7 +2528,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -2538,11 +2538,11 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -2553,7 +2553,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2563,11 +2563,11 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -2903,7 +2903,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>08:48:01</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -2913,11 +2913,11 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -2928,7 +2928,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>08:48:01</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -2938,11 +2938,11 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D104" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -4413,7 +4413,7 @@
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D163" t="n">
@@ -4438,7 +4438,7 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D164" t="n">
@@ -4703,7 +4703,7 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>11:22:44</t>
+          <t>11:49:23</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
@@ -4717,7 +4717,7 @@
         </is>
       </c>
       <c r="D175" t="n">
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
@@ -4753,7 +4753,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>11:22:44</t>
+          <t>11:49:23</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
@@ -4767,7 +4767,7 @@
         </is>
       </c>
       <c r="D177" t="n">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -4778,7 +4778,7 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>11:22:44</t>
+          <t>11:49:23</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
@@ -4792,7 +4792,7 @@
         </is>
       </c>
       <c r="D178" t="n">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -4803,7 +4803,7 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>11:22:44</t>
+          <t>11:49:23</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
@@ -4817,7 +4817,7 @@
         </is>
       </c>
       <c r="D179" t="n">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -4853,7 +4853,7 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>11:22:44</t>
+          <t>11:49:23</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
@@ -4867,7 +4867,7 @@
         </is>
       </c>
       <c r="D181" t="n">
-        <v>44</v>
+        <v>17</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
@@ -4878,7 +4878,7 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>11:22:44</t>
+          <t>11:49:23</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
@@ -4892,7 +4892,7 @@
         </is>
       </c>
       <c r="D182" t="n">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
@@ -4903,7 +4903,7 @@
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>10:57:35</t>
+          <t>11:49:23</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
@@ -4913,11 +4913,11 @@
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D183" t="n">
-        <v>77</v>
+        <v>25</v>
       </c>
       <c r="E183" t="inlineStr">
         <is>
@@ -4928,7 +4928,7 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>11:22:44</t>
+          <t>10:57:35</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
@@ -4938,11 +4938,11 @@
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D184" t="n">
-        <v>52</v>
+        <v>77</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -4953,21 +4953,21 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>10:27:29</t>
+          <t>11:49:23</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>12:17</t>
+          <t>12:16</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D185" t="n">
-        <v>110</v>
+        <v>27</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -4978,12 +4978,12 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>11:22:44</t>
+          <t>10:27:29</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>12:20</t>
+          <t>12:17</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
@@ -4992,7 +4992,7 @@
         </is>
       </c>
       <c r="D186" t="n">
-        <v>58</v>
+        <v>110</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -5003,7 +5003,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>11:22:44</t>
+          <t>11:49:23</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
@@ -5013,11 +5013,11 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D187" t="n">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -5028,21 +5028,21 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>11:22:44</t>
+          <t>11:49:23</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>12:21</t>
+          <t>12:20</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D188" t="n">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5053,21 +5053,21 @@
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>11:22:44</t>
+          <t>11:49:23</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>12:36</t>
+          <t>12:21</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D189" t="n">
-        <v>74</v>
+        <v>32</v>
       </c>
       <c r="E189" t="inlineStr">
         <is>
@@ -5078,21 +5078,21 @@
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>11:22:44</t>
+          <t>11:49:23</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>12:38</t>
+          <t>12:34</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>17_179 Y 38</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D190" t="n">
-        <v>76</v>
+        <v>45</v>
       </c>
       <c r="E190" t="inlineStr">
         <is>
@@ -5103,21 +5103,21 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>11:22:44</t>
+          <t>11:49:23</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>12:48</t>
+          <t>12:34</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D191" t="n">
-        <v>86</v>
+        <v>45</v>
       </c>
       <c r="E191" t="inlineStr">
         <is>
@@ -5133,16 +5133,16 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>12:50</t>
+          <t>12:36</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D192" t="n">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="E192" t="inlineStr">
         <is>
@@ -5153,21 +5153,21 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>11:22:44</t>
+          <t>11:49:23</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>13:06</t>
+          <t>12:37</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D193" t="n">
-        <v>104</v>
+        <v>48</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
@@ -5178,21 +5178,21 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>11:22:44</t>
+          <t>11:49:23</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>13:10</t>
+          <t>12:38</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_179 Y 38</t>
         </is>
       </c>
       <c r="D194" t="n">
-        <v>108</v>
+        <v>49</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -5203,21 +5203,21 @@
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>11:22:44</t>
+          <t>11:49:23</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>13:13</t>
+          <t>12:41</t>
         </is>
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D195" t="n">
-        <v>111</v>
+        <v>52</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
@@ -5228,23 +5228,323 @@
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
+          <t>11:49:23</t>
+        </is>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>12:45</t>
+        </is>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D196" t="n">
+        <v>56</v>
+      </c>
+      <c r="E196" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>11:49:23</t>
+        </is>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>12:48</t>
+        </is>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D197" t="n">
+        <v>59</v>
+      </c>
+      <c r="E197" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
           <t>11:22:44</t>
         </is>
       </c>
-      <c r="B196" t="inlineStr">
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>12:50</t>
+        </is>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D198" t="n">
+        <v>88</v>
+      </c>
+      <c r="E198" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>11:49:23</t>
+        </is>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>13:02</t>
+        </is>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D199" t="n">
+        <v>73</v>
+      </c>
+      <c r="E199" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>11:49:23</t>
+        </is>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>13:06</t>
+        </is>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D200" t="n">
+        <v>77</v>
+      </c>
+      <c r="E200" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>11:22:44</t>
+        </is>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>13:10</t>
+        </is>
+      </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D201" t="n">
+        <v>108</v>
+      </c>
+      <c r="E201" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>11:22:44</t>
+        </is>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>13:13</t>
+        </is>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>215D_EL PATO</t>
+        </is>
+      </c>
+      <c r="D202" t="n">
+        <v>111</v>
+      </c>
+      <c r="E202" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>11:49:23</t>
+        </is>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>13:14</t>
+        </is>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>215D_EL PATO</t>
+        </is>
+      </c>
+      <c r="D203" t="n">
+        <v>85</v>
+      </c>
+      <c r="E203" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>11:49:23</t>
+        </is>
+      </c>
+      <c r="B204" t="inlineStr">
         <is>
           <t>13:20</t>
         </is>
       </c>
-      <c r="C196" t="inlineStr">
+      <c r="C204" t="inlineStr">
         <is>
           <t>10_OLMOS</t>
         </is>
       </c>
-      <c r="D196" t="n">
-        <v>118</v>
-      </c>
-      <c r="E196" t="inlineStr">
+      <c r="D204" t="n">
+        <v>91</v>
+      </c>
+      <c r="E204" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>11:49:23</t>
+        </is>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>13:21</t>
+        </is>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D205" t="n">
+        <v>92</v>
+      </c>
+      <c r="E205" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>11:49:23</t>
+        </is>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>13:26</t>
+        </is>
+      </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D206" t="n">
+        <v>97</v>
+      </c>
+      <c r="E206" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>11:49:23</t>
+        </is>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>13:26</t>
+        </is>
+      </c>
+      <c r="C207" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D207" t="n">
+        <v>97</v>
+      </c>
+      <c r="E207" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>11:49:23</t>
+        </is>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>13:46</t>
+        </is>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D208" t="n">
+        <v>117</v>
+      </c>
+      <c r="E208" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -5261,7 +5561,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5279,14 +5579,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:22:44</t>
+          <t>Última actualización: 11:49:24</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 26</t>
+          <t>Total filas: 27</t>
         </is>
       </c>
     </row>
@@ -5895,7 +6195,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>11:22:44</t>
+          <t>11:49:23</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -5909,7 +6209,7 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -5920,7 +6220,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>11:22:44</t>
+          <t>11:49:23</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -5934,7 +6234,7 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -5962,6 +6262,31 @@
         <v>111</v>
       </c>
       <c r="E31" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>11:49:23</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>13:14</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>215D_EL PATO</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>85</v>
+      </c>
+      <c r="E32" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -5978,7 +6303,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5996,14 +6321,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:22:44</t>
+          <t>Última actualización: 11:49:24</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 30</t>
+          <t>Total filas: 32</t>
         </is>
       </c>
     </row>
@@ -6737,7 +7062,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>11:22:44</t>
+          <t>11:49:23</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -6751,7 +7076,7 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -6781,6 +7106,56 @@
       <c r="E35" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>11:49:23</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>12:54</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>65</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>11:49:23</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>13:31</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>102</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 836
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-23.xlsx
+++ b/data/horarios-141-2026-01-23.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E208"/>
+  <dimension ref="A1:E216"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:49:24</t>
+          <t>Última actualización: 12:02:21</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 203</t>
+          <t>Total filas: 211</t>
         </is>
       </c>
     </row>
@@ -1313,7 +1313,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>86_EST CHICA-ESC AGRARIA</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1338,7 +1338,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>86_EST CHICA-ESC AGRARIA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1628,7 +1628,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1638,11 +1638,11 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>73</v>
+        <v>6</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -1653,7 +1653,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1663,11 +1663,11 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>6</v>
+        <v>73</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -1778,7 +1778,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1788,11 +1788,11 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -1803,7 +1803,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1813,11 +1813,11 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>17</v>
+        <v>84</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D63" t="n">
@@ -1938,7 +1938,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -1953,7 +1953,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1963,11 +1963,11 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -1988,7 +1988,7 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D66" t="n">
@@ -2003,7 +2003,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -2013,11 +2013,11 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2128,7 +2128,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -2138,11 +2138,11 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -2153,7 +2153,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -2163,11 +2163,11 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D73" t="n">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -2213,7 +2213,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D75" t="n">
@@ -2238,7 +2238,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D76" t="n">
@@ -2528,7 +2528,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -2538,11 +2538,11 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -2553,7 +2553,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2563,11 +2563,11 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -2903,7 +2903,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>08:48:01</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -2913,11 +2913,11 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -2928,7 +2928,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>08:48:01</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -2938,11 +2938,11 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D104" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -3153,7 +3153,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3163,11 +3163,11 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>27</v>
+        <v>115</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3188,7 +3188,7 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D114" t="n">
@@ -3203,7 +3203,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
@@ -3213,11 +3213,11 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D115" t="n">
-        <v>115</v>
+        <v>27</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -3278,7 +3278,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>09:33:33</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -3288,11 +3288,11 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D118" t="n">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -3303,7 +3303,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>09:33:33</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -3313,11 +3313,11 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D119" t="n">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -3338,7 +3338,7 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D120" t="n">
@@ -3363,7 +3363,7 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D121" t="n">
@@ -3388,7 +3388,7 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D122" t="n">
@@ -3413,7 +3413,7 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D123" t="n">
@@ -4778,7 +4778,7 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>11:49:23</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
@@ -4792,7 +4792,7 @@
         </is>
       </c>
       <c r="D178" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -4828,21 +4828,21 @@
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>11:22:44</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>12:06</t>
+          <t>12:05</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D180" t="n">
-        <v>44</v>
+        <v>3</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
@@ -4853,7 +4853,7 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>11:49:23</t>
+          <t>11:22:44</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
@@ -4863,11 +4863,11 @@
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D181" t="n">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
@@ -4878,21 +4878,21 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>11:49:23</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>12:13</t>
+          <t>12:06</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D182" t="n">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
@@ -4903,21 +4903,21 @@
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>11:49:23</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>12:14</t>
+          <t>12:13</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D183" t="n">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="E183" t="inlineStr">
         <is>
@@ -4928,7 +4928,7 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>10:57:35</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
@@ -4938,11 +4938,11 @@
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D184" t="n">
-        <v>77</v>
+        <v>12</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -4953,21 +4953,21 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>11:49:23</t>
+          <t>10:57:35</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>12:16</t>
+          <t>12:14</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D185" t="n">
-        <v>27</v>
+        <v>77</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -4978,21 +4978,21 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>10:27:29</t>
+          <t>11:49:23</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>12:17</t>
+          <t>12:16</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D186" t="n">
-        <v>110</v>
+        <v>27</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -5003,12 +5003,12 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>11:49:23</t>
+          <t>10:27:29</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>12:20</t>
+          <t>12:17</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
@@ -5017,7 +5017,7 @@
         </is>
       </c>
       <c r="D187" t="n">
-        <v>31</v>
+        <v>110</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -5028,21 +5028,21 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>11:49:23</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>12:20</t>
+          <t>12:17</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D188" t="n">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5053,21 +5053,21 @@
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>11:49:23</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>12:21</t>
+          <t>12:20</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D189" t="n">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="E189" t="inlineStr">
         <is>
@@ -5078,21 +5078,21 @@
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>11:49:23</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>12:34</t>
+          <t>12:20</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D190" t="n">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="E190" t="inlineStr">
         <is>
@@ -5103,21 +5103,21 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>11:49:23</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>12:34</t>
+          <t>12:21</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D191" t="n">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="E191" t="inlineStr">
         <is>
@@ -5128,21 +5128,21 @@
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>11:22:44</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>12:36</t>
+          <t>12:27</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D192" t="n">
-        <v>74</v>
+        <v>25</v>
       </c>
       <c r="E192" t="inlineStr">
         <is>
@@ -5158,16 +5158,16 @@
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>12:37</t>
+          <t>12:34</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D193" t="n">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
@@ -5178,21 +5178,21 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>11:49:23</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>12:38</t>
+          <t>12:34</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>17_179 Y 38</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D194" t="n">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -5203,21 +5203,21 @@
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>11:49:23</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>12:41</t>
+          <t>12:35</t>
         </is>
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D195" t="n">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
@@ -5228,21 +5228,21 @@
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>11:49:23</t>
+          <t>11:22:44</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>12:45</t>
+          <t>12:36</t>
         </is>
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D196" t="n">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="E196" t="inlineStr">
         <is>
@@ -5253,21 +5253,21 @@
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>11:49:23</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>12:48</t>
+          <t>12:37</t>
         </is>
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D197" t="n">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
@@ -5278,21 +5278,21 @@
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>11:22:44</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>12:50</t>
+          <t>12:38</t>
         </is>
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>17_179 Y 38</t>
         </is>
       </c>
       <c r="D198" t="n">
-        <v>88</v>
+        <v>36</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
@@ -5303,21 +5303,21 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>11:49:23</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>13:02</t>
+          <t>12:41</t>
         </is>
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D199" t="n">
-        <v>73</v>
+        <v>39</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
@@ -5333,16 +5333,16 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>13:06</t>
+          <t>12:45</t>
         </is>
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D200" t="n">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
@@ -5353,21 +5353,21 @@
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>11:22:44</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>13:10</t>
+          <t>12:48</t>
         </is>
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D201" t="n">
-        <v>108</v>
+        <v>46</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
@@ -5378,21 +5378,21 @@
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>11:22:44</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>13:13</t>
+          <t>12:50</t>
         </is>
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D202" t="n">
-        <v>111</v>
+        <v>48</v>
       </c>
       <c r="E202" t="inlineStr">
         <is>
@@ -5403,21 +5403,21 @@
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>11:49:23</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>13:14</t>
+          <t>13:02</t>
         </is>
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D203" t="n">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
@@ -5428,21 +5428,21 @@
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>11:49:23</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>13:20</t>
+          <t>13:06</t>
         </is>
       </c>
       <c r="C204" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D204" t="n">
-        <v>91</v>
+        <v>64</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
@@ -5453,21 +5453,21 @@
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>11:49:23</t>
+          <t>11:22:44</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>13:21</t>
+          <t>13:10</t>
         </is>
       </c>
       <c r="C205" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D205" t="n">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="E205" t="inlineStr">
         <is>
@@ -5478,21 +5478,21 @@
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>11:49:23</t>
+          <t>11:22:44</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>13:26</t>
+          <t>13:13</t>
         </is>
       </c>
       <c r="C206" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D206" t="n">
-        <v>97</v>
+        <v>111</v>
       </c>
       <c r="E206" t="inlineStr">
         <is>
@@ -5503,21 +5503,21 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>11:49:23</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>13:26</t>
+          <t>13:14</t>
         </is>
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D207" t="n">
-        <v>97</v>
+        <v>72</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -5533,18 +5533,218 @@
       </c>
       <c r="B208" t="inlineStr">
         <is>
+          <t>13:20</t>
+        </is>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D208" t="n">
+        <v>91</v>
+      </c>
+      <c r="E208" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>12:02:21</t>
+        </is>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>13:21</t>
+        </is>
+      </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D209" t="n">
+        <v>79</v>
+      </c>
+      <c r="E209" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>12:02:21</t>
+        </is>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>13:23</t>
+        </is>
+      </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D210" t="n">
+        <v>81</v>
+      </c>
+      <c r="E210" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>12:02:21</t>
+        </is>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>13:26</t>
+        </is>
+      </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D211" t="n">
+        <v>84</v>
+      </c>
+      <c r="E211" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>11:49:23</t>
+        </is>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>13:26</t>
+        </is>
+      </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D212" t="n">
+        <v>97</v>
+      </c>
+      <c r="E212" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>12:02:21</t>
+        </is>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
           <t>13:46</t>
         </is>
       </c>
-      <c r="C208" t="inlineStr">
+      <c r="C213" t="inlineStr">
         <is>
           <t>17_ROMERO</t>
         </is>
       </c>
-      <c r="D208" t="n">
-        <v>117</v>
-      </c>
-      <c r="E208" t="inlineStr">
+      <c r="D213" t="n">
+        <v>104</v>
+      </c>
+      <c r="E213" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>12:02:21</t>
+        </is>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>13:50</t>
+        </is>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D214" t="n">
+        <v>108</v>
+      </c>
+      <c r="E214" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>12:02:21</t>
+        </is>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>13:56</t>
+        </is>
+      </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D215" t="n">
+        <v>114</v>
+      </c>
+      <c r="E215" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>12:02:21</t>
+        </is>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>13:56</t>
+        </is>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D216" t="n">
+        <v>114</v>
+      </c>
+      <c r="E216" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -5561,7 +5761,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5579,14 +5779,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:49:24</t>
+          <t>Última actualización: 12:02:21</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 27</t>
+          <t>Total filas: 28</t>
         </is>
       </c>
     </row>
@@ -6220,7 +6420,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>11:49:23</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -6234,7 +6434,7 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -6270,7 +6470,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>11:49:23</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -6284,9 +6484,34 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="E32" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>12:02:21</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>13:50</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>108</v>
+      </c>
+      <c r="E33" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -6303,7 +6528,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6321,14 +6546,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:49:24</t>
+          <t>Última actualización: 12:02:21</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 32</t>
+          <t>Total filas: 33</t>
         </is>
       </c>
     </row>
@@ -7062,12 +7287,12 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>11:49:23</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>12:04</t>
+          <t>12:03</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -7076,7 +7301,7 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -7087,37 +7312,37 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>11:22:44</t>
+          <t>11:49:23</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>12:53</t>
+          <t>12:04</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>91</v>
+        <v>15</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>L6203</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>11:49:23</t>
+          <t>11:22:44</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>12:54</t>
+          <t>12:53</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -7126,7 +7351,7 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>65</v>
+        <v>91</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -7137,23 +7362,48 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>11:49:23</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
+          <t>12:54</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>52</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>12:02:21</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
           <t>13:31</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr">
+      <c r="C38" t="inlineStr">
         <is>
           <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
-      <c r="D37" t="n">
-        <v>102</v>
-      </c>
-      <c r="E37" t="inlineStr">
+      <c r="D38" t="n">
+        <v>89</v>
+      </c>
+      <c r="E38" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 837
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-23.xlsx
+++ b/data/horarios-141-2026-01-23.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E216"/>
+  <dimension ref="A1:E233"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:02:21</t>
+          <t>Última actualización: 12:37:00</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 211</t>
+          <t>Total filas: 228</t>
         </is>
       </c>
     </row>
@@ -1513,7 +1513,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -1538,7 +1538,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -1778,7 +1778,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1788,11 +1788,11 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>17</v>
+        <v>84</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -1803,7 +1803,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1813,11 +1813,11 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -2128,7 +2128,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -2138,11 +2138,11 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -2153,7 +2153,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -2163,11 +2163,11 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D73" t="n">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -2213,7 +2213,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D75" t="n">
@@ -2238,7 +2238,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D76" t="n">
@@ -2528,7 +2528,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -2538,11 +2538,11 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -2553,7 +2553,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2563,11 +2563,11 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -2803,7 +2803,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -2813,11 +2813,11 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D99" t="n">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -2828,7 +2828,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -2838,11 +2838,11 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -3153,7 +3153,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3163,11 +3163,11 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>115</v>
+        <v>27</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3178,7 +3178,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
@@ -3188,11 +3188,11 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D114" t="n">
-        <v>27</v>
+        <v>115</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -3388,7 +3388,7 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D122" t="n">
@@ -3413,7 +3413,7 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D123" t="n">
@@ -4163,7 +4163,7 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D153" t="n">
@@ -4188,7 +4188,7 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D154" t="n">
@@ -4413,7 +4413,7 @@
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D163" t="n">
@@ -4438,7 +4438,7 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D164" t="n">
@@ -4928,7 +4928,7 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>10:57:35</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
@@ -4938,11 +4938,11 @@
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D184" t="n">
-        <v>12</v>
+        <v>77</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -4953,7 +4953,7 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>10:57:35</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
@@ -4963,11 +4963,11 @@
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D185" t="n">
-        <v>77</v>
+        <v>12</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -5003,7 +5003,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>10:27:29</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
@@ -5013,11 +5013,11 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D187" t="n">
-        <v>110</v>
+        <v>15</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -5028,7 +5028,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>10:27:29</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -5038,11 +5038,11 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D188" t="n">
-        <v>15</v>
+        <v>110</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5153,7 +5153,7 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>11:49:23</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
@@ -5163,11 +5163,11 @@
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D193" t="n">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
@@ -5178,7 +5178,7 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>11:49:23</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
@@ -5188,11 +5188,11 @@
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D194" t="n">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -5253,7 +5253,7 @@
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>12:37:00</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
@@ -5267,7 +5267,7 @@
         </is>
       </c>
       <c r="D197" t="n">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
@@ -5278,7 +5278,7 @@
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>12:37:00</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
@@ -5288,11 +5288,11 @@
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>17_179 Y 38</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D198" t="n">
-        <v>36</v>
+        <v>1</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
@@ -5303,21 +5303,21 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>12:37:00</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>12:41</t>
+          <t>12:38</t>
         </is>
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_179 Y 38</t>
         </is>
       </c>
       <c r="D199" t="n">
-        <v>39</v>
+        <v>1</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
@@ -5328,21 +5328,21 @@
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>11:49:23</t>
+          <t>12:37:00</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>12:45</t>
+          <t>12:38</t>
         </is>
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D200" t="n">
-        <v>56</v>
+        <v>1</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
@@ -5358,16 +5358,16 @@
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>12:48</t>
+          <t>12:41</t>
         </is>
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D201" t="n">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
@@ -5378,21 +5378,21 @@
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>11:49:23</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>12:50</t>
+          <t>12:45</t>
         </is>
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D202" t="n">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="E202" t="inlineStr">
         <is>
@@ -5403,21 +5403,21 @@
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>12:37:00</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>13:02</t>
+          <t>12:47</t>
         </is>
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D203" t="n">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
@@ -5433,16 +5433,16 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>13:06</t>
+          <t>12:48</t>
         </is>
       </c>
       <c r="C204" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D204" t="n">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
@@ -5453,21 +5453,21 @@
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>11:22:44</t>
+          <t>12:37:00</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>13:10</t>
+          <t>12:49</t>
         </is>
       </c>
       <c r="C205" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D205" t="n">
-        <v>108</v>
+        <v>12</v>
       </c>
       <c r="E205" t="inlineStr">
         <is>
@@ -5478,21 +5478,21 @@
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>11:22:44</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>13:13</t>
+          <t>12:50</t>
         </is>
       </c>
       <c r="C206" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D206" t="n">
-        <v>111</v>
+        <v>48</v>
       </c>
       <c r="E206" t="inlineStr">
         <is>
@@ -5503,21 +5503,21 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>12:37:00</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>13:14</t>
+          <t>12:55</t>
         </is>
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D207" t="n">
-        <v>72</v>
+        <v>18</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -5528,21 +5528,21 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>11:49:23</t>
+          <t>12:37:00</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>13:20</t>
+          <t>13:02</t>
         </is>
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D208" t="n">
-        <v>91</v>
+        <v>25</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -5553,21 +5553,21 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>12:37:00</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>13:21</t>
+          <t>13:03</t>
         </is>
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D209" t="n">
-        <v>79</v>
+        <v>26</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -5578,21 +5578,21 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>12:37:00</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>13:23</t>
+          <t>13:06</t>
         </is>
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D210" t="n">
-        <v>81</v>
+        <v>29</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
@@ -5608,16 +5608,16 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>13:26</t>
+          <t>13:06</t>
         </is>
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D211" t="n">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="E211" t="inlineStr">
         <is>
@@ -5628,21 +5628,21 @@
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>11:49:23</t>
+          <t>12:37:00</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>13:26</t>
+          <t>13:07</t>
         </is>
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D212" t="n">
-        <v>97</v>
+        <v>30</v>
       </c>
       <c r="E212" t="inlineStr">
         <is>
@@ -5653,21 +5653,21 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>12:37:00</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>13:46</t>
+          <t>13:08</t>
         </is>
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D213" t="n">
-        <v>104</v>
+        <v>31</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -5678,17 +5678,17 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>11:22:44</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>13:50</t>
+          <t>13:10</t>
         </is>
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D214" t="n">
@@ -5703,21 +5703,21 @@
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>11:22:44</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>13:56</t>
+          <t>13:13</t>
         </is>
       </c>
       <c r="C215" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D215" t="n">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
@@ -5728,23 +5728,448 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
+          <t>12:37:00</t>
+        </is>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>13:14</t>
+        </is>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>215D_EL PATO</t>
+        </is>
+      </c>
+      <c r="D216" t="n">
+        <v>37</v>
+      </c>
+      <c r="E216" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>12:37:00</t>
+        </is>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>13:15</t>
+        </is>
+      </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D217" t="n">
+        <v>38</v>
+      </c>
+      <c r="E217" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>12:37:00</t>
+        </is>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>13:20</t>
+        </is>
+      </c>
+      <c r="C218" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D218" t="n">
+        <v>43</v>
+      </c>
+      <c r="E218" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>12:37:00</t>
+        </is>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>13:21</t>
+        </is>
+      </c>
+      <c r="C219" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D219" t="n">
+        <v>44</v>
+      </c>
+      <c r="E219" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
           <t>12:02:21</t>
         </is>
       </c>
-      <c r="B216" t="inlineStr">
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>13:23</t>
+        </is>
+      </c>
+      <c r="C220" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D220" t="n">
+        <v>81</v>
+      </c>
+      <c r="E220" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>12:02:21</t>
+        </is>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>13:26</t>
+        </is>
+      </c>
+      <c r="C221" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D221" t="n">
+        <v>84</v>
+      </c>
+      <c r="E221" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>12:37:00</t>
+        </is>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>13:26</t>
+        </is>
+      </c>
+      <c r="C222" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D222" t="n">
+        <v>49</v>
+      </c>
+      <c r="E222" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>12:37:00</t>
+        </is>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>13:27</t>
+        </is>
+      </c>
+      <c r="C223" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D223" t="n">
+        <v>50</v>
+      </c>
+      <c r="E223" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t>12:37:00</t>
+        </is>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>13:46</t>
+        </is>
+      </c>
+      <c r="C224" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D224" t="n">
+        <v>69</v>
+      </c>
+      <c r="E224" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>12:02:21</t>
+        </is>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>13:50</t>
+        </is>
+      </c>
+      <c r="C225" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D225" t="n">
+        <v>108</v>
+      </c>
+      <c r="E225" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
+          <t>12:37:00</t>
+        </is>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>13:51</t>
+        </is>
+      </c>
+      <c r="C226" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D226" t="n">
+        <v>74</v>
+      </c>
+      <c r="E226" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
+          <t>12:37:00</t>
+        </is>
+      </c>
+      <c r="B227" t="inlineStr">
         <is>
           <t>13:56</t>
         </is>
       </c>
-      <c r="C216" t="inlineStr">
+      <c r="C227" t="inlineStr">
         <is>
           <t>225_GOMEZ</t>
         </is>
       </c>
-      <c r="D216" t="n">
+      <c r="D227" t="n">
+        <v>79</v>
+      </c>
+      <c r="E227" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>12:02:21</t>
+        </is>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>13:56</t>
+        </is>
+      </c>
+      <c r="C228" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D228" t="n">
         <v>114</v>
       </c>
-      <c r="E216" t="inlineStr">
+      <c r="E228" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>12:37:00</t>
+        </is>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>13:57</t>
+        </is>
+      </c>
+      <c r="C229" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D229" t="n">
+        <v>80</v>
+      </c>
+      <c r="E229" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t>12:37:00</t>
+        </is>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>14:04</t>
+        </is>
+      </c>
+      <c r="C230" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D230" t="n">
+        <v>87</v>
+      </c>
+      <c r="E230" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>12:37:00</t>
+        </is>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>14:17</t>
+        </is>
+      </c>
+      <c r="C231" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D231" t="n">
+        <v>100</v>
+      </c>
+      <c r="E231" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>12:37:00</t>
+        </is>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>14:20</t>
+        </is>
+      </c>
+      <c r="C232" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D232" t="n">
+        <v>103</v>
+      </c>
+      <c r="E232" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>12:37:00</t>
+        </is>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>14:21</t>
+        </is>
+      </c>
+      <c r="C233" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D233" t="n">
+        <v>104</v>
+      </c>
+      <c r="E233" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -5761,7 +6186,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5779,14 +6204,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:02:21</t>
+          <t>Última actualización: 12:37:00</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 28</t>
+          <t>Total filas: 30</t>
         </is>
       </c>
     </row>
@@ -6470,7 +6895,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>12:37:00</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -6484,7 +6909,7 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>72</v>
+        <v>37</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -6512,6 +6937,56 @@
         <v>108</v>
       </c>
       <c r="E33" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>12:37:00</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>13:51</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>74</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>12:37:00</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>14:20</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>103</v>
+      </c>
+      <c r="E35" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -6528,7 +7003,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6546,14 +7021,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:02:21</t>
+          <t>Última actualización: 12:37:00</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 33</t>
+          <t>Total filas: 34</t>
         </is>
       </c>
     </row>
@@ -7362,7 +7837,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>12:37:00</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -7376,7 +7851,7 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -7387,7 +7862,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>12:37:00</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -7401,9 +7876,34 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>89</v>
+        <v>54</v>
       </c>
       <c r="E38" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>12:37:00</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>14:09</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>92</v>
+      </c>
+      <c r="E39" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 838
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-23.xlsx
+++ b/data/horarios-141-2026-01-23.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E233"/>
+  <dimension ref="A1:E242"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:37:00</t>
+          <t>Última actualización: 12:54:24</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 228</t>
+          <t>Total filas: 237</t>
         </is>
       </c>
     </row>
@@ -1513,7 +1513,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -1538,7 +1538,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -1913,7 +1913,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D63" t="n">
@@ -1938,7 +1938,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -2213,7 +2213,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D75" t="n">
@@ -2238,7 +2238,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D76" t="n">
@@ -2528,7 +2528,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -2538,11 +2538,11 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -2553,7 +2553,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2563,11 +2563,11 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -2803,7 +2803,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -2813,11 +2813,11 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D99" t="n">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -2828,7 +2828,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -2838,11 +2838,11 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -3163,7 +3163,7 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D113" t="n">
@@ -3178,7 +3178,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
@@ -3188,11 +3188,11 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D114" t="n">
-        <v>115</v>
+        <v>27</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -3203,7 +3203,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
@@ -3213,11 +3213,11 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D115" t="n">
-        <v>27</v>
+        <v>115</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -3338,7 +3338,7 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D120" t="n">
@@ -3363,7 +3363,7 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D121" t="n">
@@ -4413,7 +4413,7 @@
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D163" t="n">
@@ -4438,7 +4438,7 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D164" t="n">
@@ -5288,7 +5288,7 @@
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_179 Y 38</t>
         </is>
       </c>
       <c r="D198" t="n">
@@ -5313,7 +5313,7 @@
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>17_179 Y 38</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D199" t="n">
@@ -5503,21 +5503,21 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>12:54:24</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>12:55</t>
+          <t>12:54</t>
         </is>
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D207" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -5528,21 +5528,21 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>12:54:24</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>13:02</t>
+          <t>12:55</t>
         </is>
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D208" t="n">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -5558,16 +5558,16 @@
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>13:03</t>
+          <t>12:55</t>
         </is>
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D209" t="n">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -5583,16 +5583,16 @@
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>13:06</t>
+          <t>13:02</t>
         </is>
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D210" t="n">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
@@ -5603,21 +5603,21 @@
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>12:37:00</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>13:06</t>
+          <t>13:03</t>
         </is>
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D211" t="n">
-        <v>64</v>
+        <v>26</v>
       </c>
       <c r="E211" t="inlineStr">
         <is>
@@ -5628,21 +5628,21 @@
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>12:54:24</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>13:07</t>
+          <t>13:05</t>
         </is>
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D212" t="n">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="E212" t="inlineStr">
         <is>
@@ -5658,16 +5658,16 @@
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>13:08</t>
+          <t>13:06</t>
         </is>
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D213" t="n">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -5678,21 +5678,21 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>11:22:44</t>
+          <t>12:54:24</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>13:10</t>
+          <t>13:06</t>
         </is>
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D214" t="n">
-        <v>108</v>
+        <v>12</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
@@ -5703,21 +5703,21 @@
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>11:22:44</t>
+          <t>12:37:00</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>13:13</t>
+          <t>13:07</t>
         </is>
       </c>
       <c r="C215" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D215" t="n">
-        <v>111</v>
+        <v>30</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
@@ -5728,21 +5728,21 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>12:54:24</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>13:14</t>
+          <t>13:08</t>
         </is>
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D216" t="n">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
@@ -5753,21 +5753,21 @@
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>11:22:44</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>13:15</t>
+          <t>13:10</t>
         </is>
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D217" t="n">
-        <v>38</v>
+        <v>108</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
@@ -5778,21 +5778,21 @@
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>11:22:44</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>13:20</t>
+          <t>13:13</t>
         </is>
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D218" t="n">
-        <v>43</v>
+        <v>111</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
@@ -5803,21 +5803,21 @@
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>12:54:24</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>13:21</t>
+          <t>13:14</t>
         </is>
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D219" t="n">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
@@ -5828,21 +5828,21 @@
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>12:54:24</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>13:23</t>
+          <t>13:14</t>
         </is>
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D220" t="n">
-        <v>81</v>
+        <v>20</v>
       </c>
       <c r="E220" t="inlineStr">
         <is>
@@ -5853,21 +5853,21 @@
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>12:37:00</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>13:26</t>
+          <t>13:15</t>
         </is>
       </c>
       <c r="C221" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D221" t="n">
-        <v>84</v>
+        <v>38</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
@@ -5878,21 +5878,21 @@
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>12:54:24</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>13:26</t>
+          <t>13:19</t>
         </is>
       </c>
       <c r="C222" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D222" t="n">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
@@ -5908,16 +5908,16 @@
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>13:27</t>
+          <t>13:20</t>
         </is>
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D223" t="n">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -5928,21 +5928,21 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>12:54:24</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>13:46</t>
+          <t>13:21</t>
         </is>
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D224" t="n">
-        <v>69</v>
+        <v>27</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -5958,16 +5958,16 @@
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>13:50</t>
+          <t>13:23</t>
         </is>
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D225" t="n">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -5978,21 +5978,21 @@
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>12:54:24</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>13:51</t>
+          <t>13:26</t>
         </is>
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D226" t="n">
-        <v>74</v>
+        <v>32</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
@@ -6003,21 +6003,21 @@
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>12:54:24</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>13:56</t>
+          <t>13:26</t>
         </is>
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D227" t="n">
-        <v>79</v>
+        <v>32</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
@@ -6028,21 +6028,21 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>12:37:00</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>13:56</t>
+          <t>13:27</t>
         </is>
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D228" t="n">
-        <v>114</v>
+        <v>50</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -6053,21 +6053,21 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>12:54:24</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>13:57</t>
+          <t>13:34</t>
         </is>
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D229" t="n">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -6078,21 +6078,21 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>12:54:24</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>14:04</t>
+          <t>13:36</t>
         </is>
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D230" t="n">
-        <v>87</v>
+        <v>42</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -6103,21 +6103,21 @@
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>12:54:24</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>14:17</t>
+          <t>13:46</t>
         </is>
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D231" t="n">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -6128,21 +6128,21 @@
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>12:54:24</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>14:20</t>
+          <t>13:50</t>
         </is>
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D232" t="n">
-        <v>103</v>
+        <v>56</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -6153,23 +6153,248 @@
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
+          <t>12:54:24</t>
+        </is>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>13:50</t>
+        </is>
+      </c>
+      <c r="C233" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D233" t="n">
+        <v>56</v>
+      </c>
+      <c r="E233" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
           <t>12:37:00</t>
         </is>
       </c>
-      <c r="B233" t="inlineStr">
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>13:51</t>
+        </is>
+      </c>
+      <c r="C234" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D234" t="n">
+        <v>74</v>
+      </c>
+      <c r="E234" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>12:54:24</t>
+        </is>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>13:56</t>
+        </is>
+      </c>
+      <c r="C235" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D235" t="n">
+        <v>62</v>
+      </c>
+      <c r="E235" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>12:54:24</t>
+        </is>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>13:56</t>
+        </is>
+      </c>
+      <c r="C236" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D236" t="n">
+        <v>62</v>
+      </c>
+      <c r="E236" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>12:37:00</t>
+        </is>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>13:57</t>
+        </is>
+      </c>
+      <c r="C237" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D237" t="n">
+        <v>80</v>
+      </c>
+      <c r="E237" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>12:54:24</t>
+        </is>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>14:04</t>
+        </is>
+      </c>
+      <c r="C238" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D238" t="n">
+        <v>70</v>
+      </c>
+      <c r="E238" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>12:54:24</t>
+        </is>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>14:17</t>
+        </is>
+      </c>
+      <c r="C239" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D239" t="n">
+        <v>83</v>
+      </c>
+      <c r="E239" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>12:54:24</t>
+        </is>
+      </c>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>14:20</t>
+        </is>
+      </c>
+      <c r="C240" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D240" t="n">
+        <v>86</v>
+      </c>
+      <c r="E240" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>12:54:24</t>
+        </is>
+      </c>
+      <c r="B241" t="inlineStr">
         <is>
           <t>14:21</t>
         </is>
       </c>
-      <c r="C233" t="inlineStr">
+      <c r="C241" t="inlineStr">
         <is>
           <t>26_HERNANDEZ</t>
         </is>
       </c>
-      <c r="D233" t="n">
-        <v>104</v>
-      </c>
-      <c r="E233" t="inlineStr">
+      <c r="D241" t="n">
+        <v>87</v>
+      </c>
+      <c r="E241" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>12:54:24</t>
+        </is>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>14:39</t>
+        </is>
+      </c>
+      <c r="C242" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D242" t="n">
+        <v>105</v>
+      </c>
+      <c r="E242" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -6204,7 +6429,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:37:00</t>
+          <t>Última actualización: 12:54:24</t>
         </is>
       </c>
     </row>
@@ -6895,7 +7120,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>12:54:24</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -6909,7 +7134,7 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -6920,7 +7145,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>12:54:24</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -6934,7 +7159,7 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>108</v>
+        <v>56</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -6970,7 +7195,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>12:54:24</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -6984,7 +7209,7 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -7003,7 +7228,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7021,14 +7246,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:37:00</t>
+          <t>Última actualización: 12:54:24</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 34</t>
+          <t>Total filas: 35</t>
         </is>
       </c>
     </row>
@@ -7837,7 +8062,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>12:54:24</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -7851,7 +8076,7 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -7862,7 +8087,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>12:54:24</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -7876,7 +8101,7 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -7887,7 +8112,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>12:54:24</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -7901,11 +8126,36 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
           <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>12:54:24</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>14:53</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>215D_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>119</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 839
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-23.xlsx
+++ b/data/horarios-141-2026-01-23.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E242"/>
+  <dimension ref="A1:E253"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:54:24</t>
+          <t>Última actualización: 13:18:32</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 237</t>
+          <t>Total filas: 248</t>
         </is>
       </c>
     </row>
@@ -1313,7 +1313,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>86_EST CHICA-ESC AGRARIA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1338,7 +1338,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>86_EST CHICA-ESC AGRARIA</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1913,7 +1913,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D63" t="n">
@@ -1938,7 +1938,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -1953,7 +1953,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1963,11 +1963,11 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -1988,7 +1988,7 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D66" t="n">
@@ -2003,7 +2003,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -2013,11 +2013,11 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2128,7 +2128,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -2138,11 +2138,11 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -2153,7 +2153,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -2163,11 +2163,11 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D73" t="n">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -2528,7 +2528,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -2538,11 +2538,11 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -2553,7 +2553,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2563,11 +2563,11 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -4163,7 +4163,7 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D153" t="n">
@@ -4188,7 +4188,7 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D154" t="n">
@@ -4413,7 +4413,7 @@
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D163" t="n">
@@ -4438,7 +4438,7 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D164" t="n">
@@ -4928,7 +4928,7 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>10:57:35</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
@@ -4938,11 +4938,11 @@
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D184" t="n">
-        <v>77</v>
+        <v>12</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -4953,7 +4953,7 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>10:57:35</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
@@ -4963,11 +4963,11 @@
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D185" t="n">
-        <v>12</v>
+        <v>77</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -5063,7 +5063,7 @@
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D189" t="n">
@@ -5088,7 +5088,7 @@
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D190" t="n">
@@ -5153,7 +5153,7 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>11:49:23</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
@@ -5163,11 +5163,11 @@
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D193" t="n">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
@@ -5178,7 +5178,7 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>11:49:23</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
@@ -5188,11 +5188,11 @@
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D194" t="n">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -5288,7 +5288,7 @@
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>17_179 Y 38</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D198" t="n">
@@ -5313,7 +5313,7 @@
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_179 Y 38</t>
         </is>
       </c>
       <c r="D199" t="n">
@@ -5338,7 +5338,7 @@
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D200" t="n">
@@ -5813,7 +5813,7 @@
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D219" t="n">
@@ -5838,7 +5838,7 @@
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D220" t="n">
@@ -5928,7 +5928,7 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>12:54:24</t>
+          <t>13:18:32</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
@@ -5942,7 +5942,7 @@
         </is>
       </c>
       <c r="D224" t="n">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -5978,7 +5978,7 @@
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>12:54:24</t>
+          <t>13:18:32</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
@@ -5992,7 +5992,7 @@
         </is>
       </c>
       <c r="D226" t="n">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
@@ -6003,7 +6003,7 @@
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>12:54:24</t>
+          <t>13:18:32</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
@@ -6017,7 +6017,7 @@
         </is>
       </c>
       <c r="D227" t="n">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
@@ -6053,21 +6053,21 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>12:54:24</t>
+          <t>13:18:32</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>13:34</t>
+          <t>13:33</t>
         </is>
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D229" t="n">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -6078,21 +6078,21 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>12:54:24</t>
+          <t>13:18:32</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>13:36</t>
+          <t>13:34</t>
         </is>
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D230" t="n">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -6103,21 +6103,21 @@
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>12:54:24</t>
+          <t>13:18:32</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>13:46</t>
+          <t>13:36</t>
         </is>
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D231" t="n">
-        <v>52</v>
+        <v>18</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -6128,21 +6128,21 @@
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>12:54:24</t>
+          <t>13:18:32</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>13:50</t>
+          <t>13:46</t>
         </is>
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D232" t="n">
-        <v>56</v>
+        <v>28</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -6153,21 +6153,21 @@
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>12:54:24</t>
+          <t>13:18:32</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>13:50</t>
+          <t>13:46</t>
         </is>
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D233" t="n">
-        <v>56</v>
+        <v>28</v>
       </c>
       <c r="E233" t="inlineStr">
         <is>
@@ -6178,21 +6178,21 @@
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>13:18:32</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>13:51</t>
+          <t>13:50</t>
         </is>
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D234" t="n">
-        <v>74</v>
+        <v>32</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
@@ -6203,21 +6203,21 @@
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>12:54:24</t>
+          <t>13:18:32</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>13:56</t>
+          <t>13:50</t>
         </is>
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D235" t="n">
-        <v>62</v>
+        <v>32</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
@@ -6228,21 +6228,21 @@
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>12:54:24</t>
+          <t>12:37:00</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>13:56</t>
+          <t>13:51</t>
         </is>
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D236" t="n">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -6253,21 +6253,21 @@
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>13:18:32</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>13:57</t>
+          <t>13:55</t>
         </is>
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D237" t="n">
-        <v>80</v>
+        <v>37</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
@@ -6278,21 +6278,21 @@
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>12:54:24</t>
+          <t>13:18:32</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>14:04</t>
+          <t>13:56</t>
         </is>
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D238" t="n">
-        <v>70</v>
+        <v>38</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -6303,21 +6303,21 @@
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>12:54:24</t>
+          <t>13:18:32</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>14:17</t>
+          <t>13:56</t>
         </is>
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D239" t="n">
-        <v>83</v>
+        <v>38</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
@@ -6328,21 +6328,21 @@
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>12:54:24</t>
+          <t>12:37:00</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>14:20</t>
+          <t>13:57</t>
         </is>
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D240" t="n">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -6353,21 +6353,21 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>12:54:24</t>
+          <t>13:18:32</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>14:21</t>
+          <t>14:04</t>
         </is>
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D241" t="n">
-        <v>87</v>
+        <v>46</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -6378,23 +6378,298 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
+          <t>13:18:32</t>
+        </is>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>14:04</t>
+        </is>
+      </c>
+      <c r="C242" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D242" t="n">
+        <v>46</v>
+      </c>
+      <c r="E242" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>13:18:32</t>
+        </is>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>14:16</t>
+        </is>
+      </c>
+      <c r="C243" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D243" t="n">
+        <v>58</v>
+      </c>
+      <c r="E243" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
           <t>12:54:24</t>
         </is>
       </c>
-      <c r="B242" t="inlineStr">
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>14:17</t>
+        </is>
+      </c>
+      <c r="C244" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D244" t="n">
+        <v>83</v>
+      </c>
+      <c r="E244" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>13:18:32</t>
+        </is>
+      </c>
+      <c r="B245" t="inlineStr">
+        <is>
+          <t>14:20</t>
+        </is>
+      </c>
+      <c r="C245" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D245" t="n">
+        <v>62</v>
+      </c>
+      <c r="E245" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t>13:18:32</t>
+        </is>
+      </c>
+      <c r="B246" t="inlineStr">
+        <is>
+          <t>14:21</t>
+        </is>
+      </c>
+      <c r="C246" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D246" t="n">
+        <v>63</v>
+      </c>
+      <c r="E246" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>12:54:24</t>
+        </is>
+      </c>
+      <c r="B247" t="inlineStr">
         <is>
           <t>14:39</t>
         </is>
       </c>
-      <c r="C242" t="inlineStr">
+      <c r="C247" t="inlineStr">
         <is>
           <t>14_ABASTO</t>
         </is>
       </c>
-      <c r="D242" t="n">
+      <c r="D247" t="n">
         <v>105</v>
       </c>
-      <c r="E242" t="inlineStr">
+      <c r="E247" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>13:18:32</t>
+        </is>
+      </c>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t>14:44</t>
+        </is>
+      </c>
+      <c r="C248" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D248" t="n">
+        <v>86</v>
+      </c>
+      <c r="E248" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t>13:18:32</t>
+        </is>
+      </c>
+      <c r="B249" t="inlineStr">
+        <is>
+          <t>14:56</t>
+        </is>
+      </c>
+      <c r="C249" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D249" t="n">
+        <v>98</v>
+      </c>
+      <c r="E249" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t>13:18:32</t>
+        </is>
+      </c>
+      <c r="B250" t="inlineStr">
+        <is>
+          <t>14:58</t>
+        </is>
+      </c>
+      <c r="C250" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D250" t="n">
+        <v>100</v>
+      </c>
+      <c r="E250" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>13:18:32</t>
+        </is>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="C251" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D251" t="n">
+        <v>102</v>
+      </c>
+      <c r="E251" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>13:18:32</t>
+        </is>
+      </c>
+      <c r="B252" t="inlineStr">
+        <is>
+          <t>15:05</t>
+        </is>
+      </c>
+      <c r="C252" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D252" t="n">
+        <v>107</v>
+      </c>
+      <c r="E252" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t>13:18:32</t>
+        </is>
+      </c>
+      <c r="B253" t="inlineStr">
+        <is>
+          <t>15:13</t>
+        </is>
+      </c>
+      <c r="C253" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D253" t="n">
+        <v>115</v>
+      </c>
+      <c r="E253" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -6411,7 +6686,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6429,14 +6704,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:54:24</t>
+          <t>Última actualización: 13:18:32</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 30</t>
+          <t>Total filas: 31</t>
         </is>
       </c>
     </row>
@@ -7145,7 +7420,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>12:54:24</t>
+          <t>13:18:32</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -7159,7 +7434,7 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -7195,7 +7470,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>12:54:24</t>
+          <t>13:18:32</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -7209,9 +7484,34 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>86</v>
+        <v>62</v>
       </c>
       <c r="E35" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>13:18:32</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>14:58</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>100</v>
+      </c>
+      <c r="E36" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -7246,7 +7546,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:54:24</t>
+          <t>Última actualización: 13:18:32</t>
         </is>
       </c>
     </row>
@@ -8087,7 +8387,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>12:54:24</t>
+          <t>13:18:32</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -8101,7 +8401,7 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -8112,7 +8412,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>12:54:24</t>
+          <t>13:18:32</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -8126,7 +8426,7 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -8137,7 +8437,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>12:54:24</t>
+          <t>13:18:32</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -8151,7 +8451,7 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>119</v>
+        <v>95</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 840
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-23.xlsx
+++ b/data/horarios-141-2026-01-23.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E253"/>
+  <dimension ref="A1:E268"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 13:18:32</t>
+          <t>Última actualización: 13:51:20</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 248</t>
+          <t>Total filas: 263</t>
         </is>
       </c>
     </row>
@@ -1313,7 +1313,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>86_EST CHICA-ESC AGRARIA</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1338,7 +1338,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>86_EST CHICA-ESC AGRARIA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1513,7 +1513,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -1538,7 +1538,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -1628,7 +1628,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1638,11 +1638,11 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>6</v>
+        <v>73</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -1653,7 +1653,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1663,11 +1663,11 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>73</v>
+        <v>6</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D63" t="n">
@@ -1938,7 +1938,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -1953,7 +1953,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1963,11 +1963,11 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -2003,7 +2003,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -2013,11 +2013,11 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2128,7 +2128,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -2138,11 +2138,11 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -2153,7 +2153,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -2163,11 +2163,11 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D73" t="n">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -2213,7 +2213,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D75" t="n">
@@ -2238,7 +2238,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D76" t="n">
@@ -2528,7 +2528,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -2538,11 +2538,11 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -2553,7 +2553,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2563,11 +2563,11 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -2803,7 +2803,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -2813,11 +2813,11 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D99" t="n">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -2828,7 +2828,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -2838,11 +2838,11 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -2903,7 +2903,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>08:48:01</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -2913,11 +2913,11 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -2928,7 +2928,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>08:48:01</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -2938,11 +2938,11 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D104" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -3153,7 +3153,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3163,11 +3163,11 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>27</v>
+        <v>115</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3203,7 +3203,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
@@ -3213,11 +3213,11 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D115" t="n">
-        <v>115</v>
+        <v>27</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -3338,7 +3338,7 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D120" t="n">
@@ -3363,7 +3363,7 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D121" t="n">
@@ -4413,7 +4413,7 @@
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D163" t="n">
@@ -4438,7 +4438,7 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D164" t="n">
@@ -4853,7 +4853,7 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>11:22:44</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
@@ -4863,11 +4863,11 @@
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D181" t="n">
-        <v>44</v>
+        <v>4</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
@@ -4878,7 +4878,7 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>11:22:44</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
@@ -4888,11 +4888,11 @@
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D182" t="n">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
@@ -4928,7 +4928,7 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>10:57:35</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
@@ -4938,11 +4938,11 @@
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D184" t="n">
-        <v>12</v>
+        <v>77</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -4953,7 +4953,7 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>10:57:35</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
@@ -4963,11 +4963,11 @@
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D185" t="n">
-        <v>77</v>
+        <v>12</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -5003,7 +5003,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>10:27:29</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
@@ -5013,11 +5013,11 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D187" t="n">
-        <v>15</v>
+        <v>110</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -5028,7 +5028,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>10:27:29</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -5038,11 +5038,11 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D188" t="n">
-        <v>110</v>
+        <v>15</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5063,7 +5063,7 @@
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D189" t="n">
@@ -5088,7 +5088,7 @@
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D190" t="n">
@@ -5288,7 +5288,7 @@
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D198" t="n">
@@ -5313,7 +5313,7 @@
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>17_179 Y 38</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D199" t="n">
@@ -5338,7 +5338,7 @@
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_179 Y 38</t>
         </is>
       </c>
       <c r="D200" t="n">
@@ -6228,7 +6228,7 @@
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>13:51:20</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
@@ -6242,7 +6242,7 @@
         </is>
       </c>
       <c r="D236" t="n">
-        <v>74</v>
+        <v>0</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -6253,21 +6253,21 @@
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>13:18:32</t>
+          <t>13:51:20</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>13:55</t>
+          <t>13:51</t>
         </is>
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D237" t="n">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
@@ -6283,16 +6283,16 @@
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>13:56</t>
+          <t>13:55</t>
         </is>
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D238" t="n">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -6303,7 +6303,7 @@
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>13:18:32</t>
+          <t>13:51:20</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
@@ -6313,11 +6313,11 @@
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D239" t="n">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
@@ -6328,21 +6328,21 @@
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>13:51:20</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>13:57</t>
+          <t>13:56</t>
         </is>
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D240" t="n">
-        <v>80</v>
+        <v>5</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -6353,21 +6353,21 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>13:18:32</t>
+          <t>13:51:20</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>14:04</t>
+          <t>13:57</t>
         </is>
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D241" t="n">
-        <v>46</v>
+        <v>6</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -6378,21 +6378,21 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>13:18:32</t>
+          <t>12:37:00</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>14:04</t>
+          <t>13:57</t>
         </is>
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D242" t="n">
-        <v>46</v>
+        <v>80</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -6403,21 +6403,21 @@
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>13:18:32</t>
+          <t>13:51:20</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>14:16</t>
+          <t>14:04</t>
         </is>
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D243" t="n">
-        <v>58</v>
+        <v>13</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -6428,21 +6428,21 @@
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>12:54:24</t>
+          <t>13:18:32</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>14:17</t>
+          <t>14:04</t>
         </is>
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D244" t="n">
-        <v>83</v>
+        <v>46</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -6453,21 +6453,21 @@
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>13:18:32</t>
+          <t>13:51:20</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>14:20</t>
+          <t>14:05</t>
         </is>
       </c>
       <c r="C245" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D245" t="n">
-        <v>62</v>
+        <v>14</v>
       </c>
       <c r="E245" t="inlineStr">
         <is>
@@ -6478,21 +6478,21 @@
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>13:18:32</t>
+          <t>13:51:20</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>14:21</t>
+          <t>14:07</t>
         </is>
       </c>
       <c r="C246" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D246" t="n">
-        <v>63</v>
+        <v>16</v>
       </c>
       <c r="E246" t="inlineStr">
         <is>
@@ -6503,21 +6503,21 @@
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>12:54:24</t>
+          <t>13:51:20</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>14:39</t>
+          <t>14:12</t>
         </is>
       </c>
       <c r="C247" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D247" t="n">
-        <v>105</v>
+        <v>21</v>
       </c>
       <c r="E247" t="inlineStr">
         <is>
@@ -6533,16 +6533,16 @@
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>14:44</t>
+          <t>14:16</t>
         </is>
       </c>
       <c r="C248" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D248" t="n">
-        <v>86</v>
+        <v>58</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
@@ -6553,21 +6553,21 @@
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>13:18:32</t>
+          <t>13:51:20</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>14:56</t>
+          <t>14:17</t>
         </is>
       </c>
       <c r="C249" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D249" t="n">
-        <v>98</v>
+        <v>26</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
@@ -6578,21 +6578,21 @@
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>13:18:32</t>
+          <t>13:51:20</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>14:58</t>
+          <t>14:20</t>
         </is>
       </c>
       <c r="C250" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D250" t="n">
-        <v>100</v>
+        <v>29</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -6603,21 +6603,21 @@
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>13:18:32</t>
+          <t>13:51:20</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>14:21</t>
         </is>
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D251" t="n">
-        <v>102</v>
+        <v>30</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -6628,21 +6628,21 @@
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>13:18:32</t>
+          <t>13:51:20</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>15:05</t>
+          <t>14:30</t>
         </is>
       </c>
       <c r="C252" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D252" t="n">
-        <v>107</v>
+        <v>39</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
@@ -6653,23 +6653,398 @@
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>13:18:32</t>
+          <t>12:54:24</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
         <is>
+          <t>14:39</t>
+        </is>
+      </c>
+      <c r="C253" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D253" t="n">
+        <v>105</v>
+      </c>
+      <c r="E253" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t>13:51:20</t>
+        </is>
+      </c>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t>14:44</t>
+        </is>
+      </c>
+      <c r="C254" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D254" t="n">
+        <v>53</v>
+      </c>
+      <c r="E254" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>13:51:20</t>
+        </is>
+      </c>
+      <c r="B255" t="inlineStr">
+        <is>
+          <t>14:56</t>
+        </is>
+      </c>
+      <c r="C255" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D255" t="n">
+        <v>65</v>
+      </c>
+      <c r="E255" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>13:51:20</t>
+        </is>
+      </c>
+      <c r="B256" t="inlineStr">
+        <is>
+          <t>14:58</t>
+        </is>
+      </c>
+      <c r="C256" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D256" t="n">
+        <v>67</v>
+      </c>
+      <c r="E256" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>13:51:20</t>
+        </is>
+      </c>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="C257" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D257" t="n">
+        <v>69</v>
+      </c>
+      <c r="E257" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
+          <t>13:51:20</t>
+        </is>
+      </c>
+      <c r="B258" t="inlineStr">
+        <is>
+          <t>15:05</t>
+        </is>
+      </c>
+      <c r="C258" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D258" t="n">
+        <v>74</v>
+      </c>
+      <c r="E258" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t>13:51:20</t>
+        </is>
+      </c>
+      <c r="B259" t="inlineStr">
+        <is>
+          <t>15:10</t>
+        </is>
+      </c>
+      <c r="C259" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D259" t="n">
+        <v>79</v>
+      </c>
+      <c r="E259" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>13:51:20</t>
+        </is>
+      </c>
+      <c r="B260" t="inlineStr">
+        <is>
           <t>15:13</t>
         </is>
       </c>
-      <c r="C253" t="inlineStr">
+      <c r="C260" t="inlineStr">
         <is>
           <t>11_ETCHEVERRY</t>
         </is>
       </c>
-      <c r="D253" t="n">
+      <c r="D260" t="n">
+        <v>82</v>
+      </c>
+      <c r="E260" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>13:51:20</t>
+        </is>
+      </c>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t>15:20</t>
+        </is>
+      </c>
+      <c r="C261" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D261" t="n">
+        <v>89</v>
+      </c>
+      <c r="E261" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>13:51:20</t>
+        </is>
+      </c>
+      <c r="B262" t="inlineStr">
+        <is>
+          <t>15:21</t>
+        </is>
+      </c>
+      <c r="C262" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D262" t="n">
+        <v>90</v>
+      </c>
+      <c r="E262" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>13:51:20</t>
+        </is>
+      </c>
+      <c r="B263" t="inlineStr">
+        <is>
+          <t>15:32</t>
+        </is>
+      </c>
+      <c r="C263" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D263" t="n">
+        <v>101</v>
+      </c>
+      <c r="E263" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>13:51:20</t>
+        </is>
+      </c>
+      <c r="B264" t="inlineStr">
+        <is>
+          <t>15:35</t>
+        </is>
+      </c>
+      <c r="C264" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D264" t="n">
+        <v>104</v>
+      </c>
+      <c r="E264" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>13:51:20</t>
+        </is>
+      </c>
+      <c r="B265" t="inlineStr">
+        <is>
+          <t>15:37</t>
+        </is>
+      </c>
+      <c r="C265" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D265" t="n">
+        <v>106</v>
+      </c>
+      <c r="E265" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t>13:51:20</t>
+        </is>
+      </c>
+      <c r="B266" t="inlineStr">
+        <is>
+          <t>15:38</t>
+        </is>
+      </c>
+      <c r="C266" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D266" t="n">
+        <v>107</v>
+      </c>
+      <c r="E266" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>13:51:20</t>
+        </is>
+      </c>
+      <c r="B267" t="inlineStr">
+        <is>
+          <t>15:44</t>
+        </is>
+      </c>
+      <c r="C267" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D267" t="n">
+        <v>113</v>
+      </c>
+      <c r="E267" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
+          <t>13:51:20</t>
+        </is>
+      </c>
+      <c r="B268" t="inlineStr">
+        <is>
+          <t>15:46</t>
+        </is>
+      </c>
+      <c r="C268" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D268" t="n">
         <v>115</v>
       </c>
-      <c r="E253" t="inlineStr">
+      <c r="E268" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -6686,7 +7061,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6704,14 +7079,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 13:18:32</t>
+          <t>Última actualización: 13:51:20</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 31</t>
+          <t>Total filas: 32</t>
         </is>
       </c>
     </row>
@@ -7445,7 +7820,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>13:51:20</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -7459,7 +7834,7 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>74</v>
+        <v>0</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -7470,7 +7845,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>13:18:32</t>
+          <t>13:51:20</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -7484,7 +7859,7 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>62</v>
+        <v>29</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -7495,7 +7870,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>13:18:32</t>
+          <t>13:51:20</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -7509,9 +7884,34 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>100</v>
+        <v>67</v>
       </c>
       <c r="E36" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>13:51:20</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>15:38</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>107</v>
+      </c>
+      <c r="E37" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -7528,7 +7928,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7546,14 +7946,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 13:18:32</t>
+          <t>Última actualización: 13:51:20</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 35</t>
+          <t>Total filas: 36</t>
         </is>
       </c>
     </row>
@@ -8412,7 +8812,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>13:18:32</t>
+          <t>13:51:20</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -8426,7 +8826,7 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -8437,7 +8837,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>13:18:32</t>
+          <t>13:51:20</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -8451,11 +8851,36 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>95</v>
+        <v>62</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>13:51:20</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>15:34</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>103</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 841
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-23.xlsx
+++ b/data/horarios-141-2026-01-23.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E268"/>
+  <dimension ref="A1:E279"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 13:51:20</t>
+          <t>Última actualización: 14:19:39</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 263</t>
+          <t>Total filas: 274</t>
         </is>
       </c>
     </row>
@@ -1313,7 +1313,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>86_EST CHICA-ESC AGRARIA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1338,7 +1338,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>86_EST CHICA-ESC AGRARIA</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1953,7 +1953,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1963,11 +1963,11 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -1978,7 +1978,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -1988,11 +1988,11 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2128,7 +2128,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -2138,11 +2138,11 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -2153,7 +2153,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -2163,11 +2163,11 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D73" t="n">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -2213,7 +2213,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D75" t="n">
@@ -2238,7 +2238,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D76" t="n">
@@ -2528,7 +2528,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -2538,11 +2538,11 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -2553,7 +2553,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2563,11 +2563,11 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -3188,7 +3188,7 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D114" t="n">
@@ -3213,7 +3213,7 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D115" t="n">
@@ -3278,7 +3278,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>09:33:33</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -3288,11 +3288,11 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D118" t="n">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -3303,7 +3303,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>09:33:33</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -3313,11 +3313,11 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D119" t="n">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -4163,7 +4163,7 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D153" t="n">
@@ -4188,7 +4188,7 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D154" t="n">
@@ -5153,7 +5153,7 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>11:49:23</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
@@ -5163,11 +5163,11 @@
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D193" t="n">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
@@ -5178,7 +5178,7 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>11:49:23</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
@@ -5188,11 +5188,11 @@
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D194" t="n">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -5313,7 +5313,7 @@
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_179 Y 38</t>
         </is>
       </c>
       <c r="D199" t="n">
@@ -5338,7 +5338,7 @@
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>17_179 Y 38</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D200" t="n">
@@ -5988,7 +5988,7 @@
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D226" t="n">
@@ -6013,7 +6013,7 @@
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D227" t="n">
@@ -6238,7 +6238,7 @@
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D236" t="n">
@@ -6263,7 +6263,7 @@
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D237" t="n">
@@ -6403,7 +6403,7 @@
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>13:51:20</t>
+          <t>13:18:32</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
@@ -6413,11 +6413,11 @@
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D243" t="n">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -6428,7 +6428,7 @@
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>13:18:32</t>
+          <t>13:51:20</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
@@ -6438,11 +6438,11 @@
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D244" t="n">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -6578,12 +6578,12 @@
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>13:51:20</t>
+          <t>14:19:39</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>14:20</t>
+          <t>14:19</t>
         </is>
       </c>
       <c r="C250" t="inlineStr">
@@ -6592,7 +6592,7 @@
         </is>
       </c>
       <c r="D250" t="n">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -6608,16 +6608,16 @@
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>14:21</t>
+          <t>14:20</t>
         </is>
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D251" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -6628,21 +6628,21 @@
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>13:51:20</t>
+          <t>14:19:39</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>14:30</t>
+          <t>14:21</t>
         </is>
       </c>
       <c r="C252" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D252" t="n">
-        <v>39</v>
+        <v>2</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
@@ -6653,12 +6653,12 @@
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>12:54:24</t>
+          <t>14:19:39</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>14:39</t>
+          <t>14:22</t>
         </is>
       </c>
       <c r="C253" t="inlineStr">
@@ -6667,7 +6667,7 @@
         </is>
       </c>
       <c r="D253" t="n">
-        <v>105</v>
+        <v>3</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -6678,21 +6678,21 @@
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>13:51:20</t>
+          <t>14:19:39</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>14:44</t>
+          <t>14:28</t>
         </is>
       </c>
       <c r="C254" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D254" t="n">
-        <v>53</v>
+        <v>9</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
@@ -6708,16 +6708,16 @@
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>14:56</t>
+          <t>14:30</t>
         </is>
       </c>
       <c r="C255" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D255" t="n">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="E255" t="inlineStr">
         <is>
@@ -6728,21 +6728,21 @@
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>13:51:20</t>
+          <t>14:19:39</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>14:58</t>
+          <t>14:34</t>
         </is>
       </c>
       <c r="C256" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D256" t="n">
-        <v>67</v>
+        <v>15</v>
       </c>
       <c r="E256" t="inlineStr">
         <is>
@@ -6753,21 +6753,21 @@
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>13:51:20</t>
+          <t>12:54:24</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>14:39</t>
         </is>
       </c>
       <c r="C257" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D257" t="n">
-        <v>69</v>
+        <v>105</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
@@ -6778,21 +6778,21 @@
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>13:51:20</t>
+          <t>14:19:39</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>15:05</t>
+          <t>14:44</t>
         </is>
       </c>
       <c r="C258" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D258" t="n">
-        <v>74</v>
+        <v>25</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
@@ -6803,21 +6803,21 @@
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>13:51:20</t>
+          <t>14:19:39</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>15:10</t>
+          <t>14:46</t>
         </is>
       </c>
       <c r="C259" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D259" t="n">
-        <v>79</v>
+        <v>27</v>
       </c>
       <c r="E259" t="inlineStr">
         <is>
@@ -6828,21 +6828,21 @@
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>13:51:20</t>
+          <t>14:19:39</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>15:13</t>
+          <t>14:56</t>
         </is>
       </c>
       <c r="C260" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D260" t="n">
-        <v>82</v>
+        <v>37</v>
       </c>
       <c r="E260" t="inlineStr">
         <is>
@@ -6853,21 +6853,21 @@
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>13:51:20</t>
+          <t>14:19:39</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>15:20</t>
+          <t>14:58</t>
         </is>
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D261" t="n">
-        <v>89</v>
+        <v>39</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
@@ -6878,21 +6878,21 @@
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>13:51:20</t>
+          <t>14:19:39</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>15:21</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="C262" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D262" t="n">
-        <v>90</v>
+        <v>41</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -6903,21 +6903,21 @@
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>13:51:20</t>
+          <t>14:19:39</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>15:32</t>
+          <t>15:05</t>
         </is>
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D263" t="n">
-        <v>101</v>
+        <v>46</v>
       </c>
       <c r="E263" t="inlineStr">
         <is>
@@ -6928,21 +6928,21 @@
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>13:51:20</t>
+          <t>14:19:39</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>15:35</t>
+          <t>15:06</t>
         </is>
       </c>
       <c r="C264" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D264" t="n">
-        <v>104</v>
+        <v>47</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
@@ -6953,21 +6953,21 @@
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>13:51:20</t>
+          <t>14:19:39</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>15:37</t>
+          <t>15:10</t>
         </is>
       </c>
       <c r="C265" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D265" t="n">
-        <v>106</v>
+        <v>51</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
@@ -6978,21 +6978,21 @@
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>13:51:20</t>
+          <t>14:19:39</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>15:38</t>
+          <t>15:13</t>
         </is>
       </c>
       <c r="C266" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D266" t="n">
-        <v>107</v>
+        <v>54</v>
       </c>
       <c r="E266" t="inlineStr">
         <is>
@@ -7003,21 +7003,21 @@
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>13:51:20</t>
+          <t>14:19:39</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>15:44</t>
+          <t>15:20</t>
         </is>
       </c>
       <c r="C267" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D267" t="n">
-        <v>113</v>
+        <v>61</v>
       </c>
       <c r="E267" t="inlineStr">
         <is>
@@ -7028,23 +7028,298 @@
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
+          <t>14:19:39</t>
+        </is>
+      </c>
+      <c r="B268" t="inlineStr">
+        <is>
+          <t>15:21</t>
+        </is>
+      </c>
+      <c r="C268" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D268" t="n">
+        <v>62</v>
+      </c>
+      <c r="E268" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>14:19:39</t>
+        </is>
+      </c>
+      <c r="B269" t="inlineStr">
+        <is>
+          <t>15:32</t>
+        </is>
+      </c>
+      <c r="C269" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D269" t="n">
+        <v>73</v>
+      </c>
+      <c r="E269" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>14:19:39</t>
+        </is>
+      </c>
+      <c r="B270" t="inlineStr">
+        <is>
+          <t>15:34</t>
+        </is>
+      </c>
+      <c r="C270" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D270" t="n">
+        <v>75</v>
+      </c>
+      <c r="E270" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
           <t>13:51:20</t>
         </is>
       </c>
-      <c r="B268" t="inlineStr">
+      <c r="B271" t="inlineStr">
+        <is>
+          <t>15:35</t>
+        </is>
+      </c>
+      <c r="C271" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D271" t="n">
+        <v>104</v>
+      </c>
+      <c r="E271" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>14:19:39</t>
+        </is>
+      </c>
+      <c r="B272" t="inlineStr">
+        <is>
+          <t>15:37</t>
+        </is>
+      </c>
+      <c r="C272" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D272" t="n">
+        <v>78</v>
+      </c>
+      <c r="E272" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t>14:19:39</t>
+        </is>
+      </c>
+      <c r="B273" t="inlineStr">
+        <is>
+          <t>15:38</t>
+        </is>
+      </c>
+      <c r="C273" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D273" t="n">
+        <v>79</v>
+      </c>
+      <c r="E273" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>13:51:20</t>
+        </is>
+      </c>
+      <c r="B274" t="inlineStr">
+        <is>
+          <t>15:44</t>
+        </is>
+      </c>
+      <c r="C274" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D274" t="n">
+        <v>113</v>
+      </c>
+      <c r="E274" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>14:19:39</t>
+        </is>
+      </c>
+      <c r="B275" t="inlineStr">
         <is>
           <t>15:46</t>
         </is>
       </c>
-      <c r="C268" t="inlineStr">
+      <c r="C275" t="inlineStr">
         <is>
           <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
-      <c r="D268" t="n">
-        <v>115</v>
-      </c>
-      <c r="E268" t="inlineStr">
+      <c r="D275" t="n">
+        <v>87</v>
+      </c>
+      <c r="E275" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>14:19:39</t>
+        </is>
+      </c>
+      <c r="B276" t="inlineStr">
+        <is>
+          <t>15:53</t>
+        </is>
+      </c>
+      <c r="C276" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D276" t="n">
+        <v>94</v>
+      </c>
+      <c r="E276" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>14:19:39</t>
+        </is>
+      </c>
+      <c r="B277" t="inlineStr">
+        <is>
+          <t>15:53</t>
+        </is>
+      </c>
+      <c r="C277" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D277" t="n">
+        <v>94</v>
+      </c>
+      <c r="E277" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="inlineStr">
+        <is>
+          <t>14:19:39</t>
+        </is>
+      </c>
+      <c r="B278" t="inlineStr">
+        <is>
+          <t>15:55</t>
+        </is>
+      </c>
+      <c r="C278" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D278" t="n">
+        <v>96</v>
+      </c>
+      <c r="E278" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="inlineStr">
+        <is>
+          <t>14:19:39</t>
+        </is>
+      </c>
+      <c r="B279" t="inlineStr">
+        <is>
+          <t>16:15</t>
+        </is>
+      </c>
+      <c r="C279" t="inlineStr">
+        <is>
+          <t>225_C ROCA-H SUR</t>
+        </is>
+      </c>
+      <c r="D279" t="n">
+        <v>116</v>
+      </c>
+      <c r="E279" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -7061,7 +7336,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7079,14 +7354,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 13:51:20</t>
+          <t>Última actualización: 14:19:39</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 32</t>
+          <t>Total filas: 33</t>
         </is>
       </c>
     </row>
@@ -7845,12 +8120,12 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>13:51:20</t>
+          <t>14:19:39</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>14:20</t>
+          <t>14:19</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -7859,7 +8134,7 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -7875,16 +8150,16 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>14:58</t>
+          <t>14:20</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>67</v>
+        <v>29</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -7895,23 +8170,48 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>13:51:20</t>
+          <t>14:19:39</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
+          <t>14:58</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>39</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>14:19:39</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
           <t>15:38</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr">
+      <c r="C38" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D37" t="n">
-        <v>107</v>
-      </c>
-      <c r="E37" t="inlineStr">
+      <c r="D38" t="n">
+        <v>79</v>
+      </c>
+      <c r="E38" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -7928,7 +8228,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7946,14 +8246,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 13:51:20</t>
+          <t>Última actualización: 14:19:39</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 36</t>
+          <t>Total filas: 39</t>
         </is>
       </c>
     </row>
@@ -8837,12 +9137,12 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>13:51:20</t>
+          <t>14:19:39</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>14:53</t>
+          <t>14:52</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -8851,7 +9151,7 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>62</v>
+        <v>33</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -8867,20 +9167,95 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
+          <t>14:53</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>215D_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>62</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>13:51:20</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
           <t>15:34</t>
         </is>
       </c>
-      <c r="C41" t="inlineStr">
+      <c r="C42" t="inlineStr">
         <is>
           <t>215A_LA PLATA</t>
         </is>
       </c>
-      <c r="D41" t="n">
+      <c r="D42" t="n">
         <v>103</v>
       </c>
-      <c r="E41" t="inlineStr">
+      <c r="E42" t="inlineStr">
         <is>
           <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>14:19:39</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>15:35</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>76</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>14:19:39</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>16:13</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>114</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 842
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-23.xlsx
+++ b/data/horarios-141-2026-01-23.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E279"/>
+  <dimension ref="A1:E296"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:19:39</t>
+          <t>Última actualización: 14:45:15</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 274</t>
+          <t>Total filas: 291</t>
         </is>
       </c>
     </row>
@@ -1313,7 +1313,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>86_EST CHICA-ESC AGRARIA</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1338,7 +1338,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>86_EST CHICA-ESC AGRARIA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -2213,7 +2213,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D75" t="n">
@@ -2238,7 +2238,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D76" t="n">
@@ -3188,7 +3188,7 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D114" t="n">
@@ -3213,7 +3213,7 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D115" t="n">
@@ -3278,7 +3278,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>09:33:33</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -3288,11 +3288,11 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D118" t="n">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -3303,7 +3303,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>09:33:33</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -3313,11 +3313,11 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D119" t="n">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -4413,7 +4413,7 @@
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D163" t="n">
@@ -4438,7 +4438,7 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D164" t="n">
@@ -4928,7 +4928,7 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>10:57:35</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
@@ -4938,11 +4938,11 @@
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D184" t="n">
-        <v>77</v>
+        <v>12</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -4953,7 +4953,7 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>10:57:35</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
@@ -4963,11 +4963,11 @@
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D185" t="n">
-        <v>12</v>
+        <v>77</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -5063,7 +5063,7 @@
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D189" t="n">
@@ -5088,7 +5088,7 @@
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D190" t="n">
@@ -5288,7 +5288,7 @@
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_179 Y 38</t>
         </is>
       </c>
       <c r="D198" t="n">
@@ -5313,7 +5313,7 @@
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>17_179 Y 38</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D199" t="n">
@@ -5653,7 +5653,7 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>12:54:24</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
@@ -5663,11 +5663,11 @@
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D213" t="n">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -5678,7 +5678,7 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>12:54:24</t>
+          <t>12:37:00</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
@@ -5688,11 +5688,11 @@
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D214" t="n">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
@@ -5813,7 +5813,7 @@
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D219" t="n">
@@ -5838,7 +5838,7 @@
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D220" t="n">
@@ -6353,7 +6353,7 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>13:51:20</t>
+          <t>12:37:00</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
@@ -6363,11 +6363,11 @@
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D241" t="n">
-        <v>6</v>
+        <v>80</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -6378,7 +6378,7 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>13:51:20</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
@@ -6388,11 +6388,11 @@
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D242" t="n">
-        <v>80</v>
+        <v>6</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -6403,7 +6403,7 @@
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>13:18:32</t>
+          <t>13:51:20</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
@@ -6413,11 +6413,11 @@
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D243" t="n">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -6428,7 +6428,7 @@
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>13:51:20</t>
+          <t>13:18:32</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
@@ -6438,11 +6438,11 @@
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D244" t="n">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -6853,21 +6853,21 @@
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>14:19:39</t>
+          <t>14:45:15</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>14:58</t>
+          <t>14:57</t>
         </is>
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D261" t="n">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
@@ -6878,21 +6878,21 @@
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>14:19:39</t>
+          <t>14:45:15</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>14:58</t>
         </is>
       </c>
       <c r="C262" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D262" t="n">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -6903,21 +6903,21 @@
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>14:19:39</t>
+          <t>14:45:15</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>15:05</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D263" t="n">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="E263" t="inlineStr">
         <is>
@@ -6928,21 +6928,21 @@
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>14:19:39</t>
+          <t>14:45:15</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>15:06</t>
+          <t>15:05</t>
         </is>
       </c>
       <c r="C264" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D264" t="n">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
@@ -6958,16 +6958,16 @@
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>15:10</t>
+          <t>15:06</t>
         </is>
       </c>
       <c r="C265" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D265" t="n">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
@@ -6978,21 +6978,21 @@
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>14:19:39</t>
+          <t>14:45:15</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>15:13</t>
+          <t>15:07</t>
         </is>
       </c>
       <c r="C266" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D266" t="n">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="E266" t="inlineStr">
         <is>
@@ -7003,21 +7003,21 @@
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>14:19:39</t>
+          <t>14:45:15</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>15:20</t>
+          <t>15:10</t>
         </is>
       </c>
       <c r="C267" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D267" t="n">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="E267" t="inlineStr">
         <is>
@@ -7033,16 +7033,16 @@
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>15:21</t>
+          <t>15:13</t>
         </is>
       </c>
       <c r="C268" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D268" t="n">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="E268" t="inlineStr">
         <is>
@@ -7053,21 +7053,21 @@
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>14:19:39</t>
+          <t>14:45:15</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>15:32</t>
+          <t>15:14</t>
         </is>
       </c>
       <c r="C269" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D269" t="n">
-        <v>73</v>
+        <v>29</v>
       </c>
       <c r="E269" t="inlineStr">
         <is>
@@ -7078,21 +7078,21 @@
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>14:19:39</t>
+          <t>14:45:15</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>15:34</t>
+          <t>15:17</t>
         </is>
       </c>
       <c r="C270" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D270" t="n">
-        <v>75</v>
+        <v>32</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
@@ -7103,21 +7103,21 @@
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>13:51:20</t>
+          <t>14:45:15</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>15:35</t>
+          <t>15:20</t>
         </is>
       </c>
       <c r="C271" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D271" t="n">
-        <v>104</v>
+        <v>35</v>
       </c>
       <c r="E271" t="inlineStr">
         <is>
@@ -7128,21 +7128,21 @@
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>14:19:39</t>
+          <t>14:45:15</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>15:37</t>
+          <t>15:21</t>
         </is>
       </c>
       <c r="C272" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D272" t="n">
-        <v>78</v>
+        <v>36</v>
       </c>
       <c r="E272" t="inlineStr">
         <is>
@@ -7153,21 +7153,21 @@
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>14:19:39</t>
+          <t>14:45:15</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>15:38</t>
+          <t>15:32</t>
         </is>
       </c>
       <c r="C273" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D273" t="n">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="E273" t="inlineStr">
         <is>
@@ -7178,21 +7178,21 @@
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>13:51:20</t>
+          <t>14:19:39</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>15:44</t>
+          <t>15:34</t>
         </is>
       </c>
       <c r="C274" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D274" t="n">
-        <v>113</v>
+        <v>75</v>
       </c>
       <c r="E274" t="inlineStr">
         <is>
@@ -7203,21 +7203,21 @@
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>14:19:39</t>
+          <t>14:45:15</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>15:46</t>
+          <t>15:35</t>
         </is>
       </c>
       <c r="C275" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D275" t="n">
-        <v>87</v>
+        <v>50</v>
       </c>
       <c r="E275" t="inlineStr">
         <is>
@@ -7228,21 +7228,21 @@
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>14:19:39</t>
+          <t>14:45:15</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>15:53</t>
+          <t>15:37</t>
         </is>
       </c>
       <c r="C276" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D276" t="n">
-        <v>94</v>
+        <v>52</v>
       </c>
       <c r="E276" t="inlineStr">
         <is>
@@ -7258,16 +7258,16 @@
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>15:53</t>
+          <t>15:38</t>
         </is>
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D277" t="n">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="E277" t="inlineStr">
         <is>
@@ -7278,21 +7278,21 @@
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>14:19:39</t>
+          <t>14:45:15</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>15:55</t>
+          <t>15:39</t>
         </is>
       </c>
       <c r="C278" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D278" t="n">
-        <v>96</v>
+        <v>54</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
@@ -7303,23 +7303,448 @@
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
+          <t>13:51:20</t>
+        </is>
+      </c>
+      <c r="B279" t="inlineStr">
+        <is>
+          <t>15:44</t>
+        </is>
+      </c>
+      <c r="C279" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D279" t="n">
+        <v>113</v>
+      </c>
+      <c r="E279" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
           <t>14:19:39</t>
         </is>
       </c>
-      <c r="B279" t="inlineStr">
+      <c r="B280" t="inlineStr">
+        <is>
+          <t>15:46</t>
+        </is>
+      </c>
+      <c r="C280" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D280" t="n">
+        <v>87</v>
+      </c>
+      <c r="E280" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr">
+        <is>
+          <t>14:45:15</t>
+        </is>
+      </c>
+      <c r="B281" t="inlineStr">
+        <is>
+          <t>15:46</t>
+        </is>
+      </c>
+      <c r="C281" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D281" t="n">
+        <v>61</v>
+      </c>
+      <c r="E281" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
+          <t>14:45:15</t>
+        </is>
+      </c>
+      <c r="B282" t="inlineStr">
+        <is>
+          <t>15:47</t>
+        </is>
+      </c>
+      <c r="C282" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D282" t="n">
+        <v>62</v>
+      </c>
+      <c r="E282" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr">
+        <is>
+          <t>14:19:39</t>
+        </is>
+      </c>
+      <c r="B283" t="inlineStr">
+        <is>
+          <t>15:53</t>
+        </is>
+      </c>
+      <c r="C283" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D283" t="n">
+        <v>94</v>
+      </c>
+      <c r="E283" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr">
+        <is>
+          <t>14:19:39</t>
+        </is>
+      </c>
+      <c r="B284" t="inlineStr">
+        <is>
+          <t>15:53</t>
+        </is>
+      </c>
+      <c r="C284" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D284" t="n">
+        <v>94</v>
+      </c>
+      <c r="E284" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="inlineStr">
+        <is>
+          <t>14:45:15</t>
+        </is>
+      </c>
+      <c r="B285" t="inlineStr">
+        <is>
+          <t>15:54</t>
+        </is>
+      </c>
+      <c r="C285" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D285" t="n">
+        <v>69</v>
+      </c>
+      <c r="E285" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="inlineStr">
+        <is>
+          <t>14:19:39</t>
+        </is>
+      </c>
+      <c r="B286" t="inlineStr">
+        <is>
+          <t>15:55</t>
+        </is>
+      </c>
+      <c r="C286" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D286" t="n">
+        <v>96</v>
+      </c>
+      <c r="E286" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="inlineStr">
+        <is>
+          <t>14:45:15</t>
+        </is>
+      </c>
+      <c r="B287" t="inlineStr">
+        <is>
+          <t>15:56</t>
+        </is>
+      </c>
+      <c r="C287" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D287" t="n">
+        <v>71</v>
+      </c>
+      <c r="E287" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="inlineStr">
+        <is>
+          <t>14:45:15</t>
+        </is>
+      </c>
+      <c r="B288" t="inlineStr">
+        <is>
+          <t>15:57</t>
+        </is>
+      </c>
+      <c r="C288" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D288" t="n">
+        <v>72</v>
+      </c>
+      <c r="E288" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="inlineStr">
+        <is>
+          <t>14:45:15</t>
+        </is>
+      </c>
+      <c r="B289" t="inlineStr">
+        <is>
+          <t>16:09</t>
+        </is>
+      </c>
+      <c r="C289" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D289" t="n">
+        <v>84</v>
+      </c>
+      <c r="E289" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="inlineStr">
+        <is>
+          <t>14:45:15</t>
+        </is>
+      </c>
+      <c r="B290" t="inlineStr">
+        <is>
+          <t>16:09</t>
+        </is>
+      </c>
+      <c r="C290" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D290" t="n">
+        <v>84</v>
+      </c>
+      <c r="E290" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="inlineStr">
+        <is>
+          <t>14:45:15</t>
+        </is>
+      </c>
+      <c r="B291" t="inlineStr">
         <is>
           <t>16:15</t>
         </is>
       </c>
-      <c r="C279" t="inlineStr">
+      <c r="C291" t="inlineStr">
         <is>
           <t>225_C ROCA-H SUR</t>
         </is>
       </c>
-      <c r="D279" t="n">
-        <v>116</v>
-      </c>
-      <c r="E279" t="inlineStr">
+      <c r="D291" t="n">
+        <v>90</v>
+      </c>
+      <c r="E291" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="inlineStr">
+        <is>
+          <t>14:45:15</t>
+        </is>
+      </c>
+      <c r="B292" t="inlineStr">
+        <is>
+          <t>16:20</t>
+        </is>
+      </c>
+      <c r="C292" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D292" t="n">
+        <v>95</v>
+      </c>
+      <c r="E292" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="inlineStr">
+        <is>
+          <t>14:45:15</t>
+        </is>
+      </c>
+      <c r="B293" t="inlineStr">
+        <is>
+          <t>16:21</t>
+        </is>
+      </c>
+      <c r="C293" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D293" t="n">
+        <v>96</v>
+      </c>
+      <c r="E293" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="inlineStr">
+        <is>
+          <t>14:45:15</t>
+        </is>
+      </c>
+      <c r="B294" t="inlineStr">
+        <is>
+          <t>16:30</t>
+        </is>
+      </c>
+      <c r="C294" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D294" t="n">
+        <v>105</v>
+      </c>
+      <c r="E294" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="inlineStr">
+        <is>
+          <t>14:45:15</t>
+        </is>
+      </c>
+      <c r="B295" t="inlineStr">
+        <is>
+          <t>16:43</t>
+        </is>
+      </c>
+      <c r="C295" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D295" t="n">
+        <v>118</v>
+      </c>
+      <c r="E295" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="inlineStr">
+        <is>
+          <t>14:45:15</t>
+        </is>
+      </c>
+      <c r="B296" t="inlineStr">
+        <is>
+          <t>16:43</t>
+        </is>
+      </c>
+      <c r="C296" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D296" t="n">
+        <v>118</v>
+      </c>
+      <c r="E296" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -7336,7 +7761,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7354,14 +7779,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:19:39</t>
+          <t>Última actualización: 14:45:15</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 33</t>
+          <t>Total filas: 35</t>
         </is>
       </c>
     </row>
@@ -8170,7 +8595,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>14:19:39</t>
+          <t>14:45:15</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -8184,7 +8609,7 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -8212,6 +8637,56 @@
         <v>79</v>
       </c>
       <c r="E38" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>14:45:15</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>15:39</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>54</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>14:45:15</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>16:20</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>95</v>
+      </c>
+      <c r="E40" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -8228,7 +8703,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8246,14 +8721,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:19:39</t>
+          <t>Última actualización: 14:45:15</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 39</t>
+          <t>Total filas: 41</t>
         </is>
       </c>
     </row>
@@ -9162,7 +9637,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>13:51:20</t>
+          <t>14:45:15</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -9176,7 +9651,7 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>62</v>
+        <v>8</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -9237,23 +9712,73 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
+          <t>14:45:15</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>15:38</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>53</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
           <t>14:19:39</t>
         </is>
       </c>
-      <c r="B44" t="inlineStr">
+      <c r="B45" t="inlineStr">
         <is>
           <t>16:13</t>
         </is>
       </c>
-      <c r="C44" t="inlineStr">
+      <c r="C45" t="inlineStr">
         <is>
           <t>215C_LA PLATA</t>
         </is>
       </c>
-      <c r="D44" t="n">
+      <c r="D45" t="n">
         <v>114</v>
       </c>
-      <c r="E44" t="inlineStr">
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>14:45:15</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>16:14</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>89</v>
+      </c>
+      <c r="E46" t="inlineStr">
         <is>
           <t>L6203</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 843
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-23.xlsx
+++ b/data/horarios-141-2026-01-23.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E296"/>
+  <dimension ref="A1:E305"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:45:15</t>
+          <t>Última actualización: 14:55:42</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 291</t>
+          <t>Total filas: 300</t>
         </is>
       </c>
     </row>
@@ -1313,7 +1313,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>86_EST CHICA-ESC AGRARIA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1338,7 +1338,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>86_EST CHICA-ESC AGRARIA</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1628,7 +1628,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1638,11 +1638,11 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>73</v>
+        <v>6</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -1653,7 +1653,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1663,11 +1663,11 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>6</v>
+        <v>73</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -2803,7 +2803,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -2813,11 +2813,11 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D99" t="n">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -2828,7 +2828,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -2838,11 +2838,11 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -3153,7 +3153,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3163,11 +3163,11 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>115</v>
+        <v>27</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3188,7 +3188,7 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D114" t="n">
@@ -3203,7 +3203,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
@@ -3213,11 +3213,11 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D115" t="n">
-        <v>27</v>
+        <v>115</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -3278,7 +3278,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>09:33:33</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -3288,11 +3288,11 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D118" t="n">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -3303,7 +3303,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>09:33:33</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -3313,11 +3313,11 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D119" t="n">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -3338,7 +3338,7 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D120" t="n">
@@ -3363,7 +3363,7 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D121" t="n">
@@ -3388,7 +3388,7 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D122" t="n">
@@ -3413,7 +3413,7 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D123" t="n">
@@ -4163,7 +4163,7 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D153" t="n">
@@ -4188,7 +4188,7 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D154" t="n">
@@ -4413,7 +4413,7 @@
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D163" t="n">
@@ -4438,7 +4438,7 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D164" t="n">
@@ -4853,7 +4853,7 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>11:22:44</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
@@ -4863,11 +4863,11 @@
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D181" t="n">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
@@ -4878,7 +4878,7 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>11:22:44</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
@@ -4888,11 +4888,11 @@
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D182" t="n">
-        <v>44</v>
+        <v>4</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
@@ -5003,7 +5003,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>10:27:29</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
@@ -5013,11 +5013,11 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D187" t="n">
-        <v>110</v>
+        <v>15</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -5028,7 +5028,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>10:27:29</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -5038,11 +5038,11 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D188" t="n">
-        <v>15</v>
+        <v>110</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5063,7 +5063,7 @@
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D189" t="n">
@@ -5088,7 +5088,7 @@
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D190" t="n">
@@ -5288,7 +5288,7 @@
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>17_179 Y 38</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D198" t="n">
@@ -5338,7 +5338,7 @@
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_179 Y 38</t>
         </is>
       </c>
       <c r="D200" t="n">
@@ -6138,7 +6138,7 @@
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D232" t="n">
@@ -6163,7 +6163,7 @@
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D233" t="n">
@@ -6188,7 +6188,7 @@
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D234" t="n">
@@ -6213,7 +6213,7 @@
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D235" t="n">
@@ -6238,7 +6238,7 @@
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D236" t="n">
@@ -6263,7 +6263,7 @@
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D237" t="n">
@@ -6313,7 +6313,7 @@
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D239" t="n">
@@ -6338,7 +6338,7 @@
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D240" t="n">
@@ -6828,21 +6828,21 @@
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>14:19:39</t>
+          <t>14:55:42</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>14:56</t>
+          <t>14:55</t>
         </is>
       </c>
       <c r="C260" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D260" t="n">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="E260" t="inlineStr">
         <is>
@@ -6853,21 +6853,21 @@
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>14:45:15</t>
+          <t>14:55:42</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>14:57</t>
+          <t>14:55</t>
         </is>
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D261" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
@@ -6878,21 +6878,21 @@
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>14:45:15</t>
+          <t>14:55:42</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>14:58</t>
+          <t>14:56</t>
         </is>
       </c>
       <c r="C262" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D262" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -6908,16 +6908,16 @@
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>14:57</t>
         </is>
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D263" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E263" t="inlineStr">
         <is>
@@ -6933,16 +6933,16 @@
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>15:05</t>
+          <t>14:58</t>
         </is>
       </c>
       <c r="C264" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D264" t="n">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
@@ -6953,21 +6953,21 @@
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>14:19:39</t>
+          <t>14:55:42</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>15:06</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="C265" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D265" t="n">
-        <v>47</v>
+        <v>5</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
@@ -6978,21 +6978,21 @@
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>14:45:15</t>
+          <t>14:55:42</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>15:07</t>
+          <t>15:05</t>
         </is>
       </c>
       <c r="C266" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D266" t="n">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E266" t="inlineStr">
         <is>
@@ -7003,21 +7003,21 @@
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>14:45:15</t>
+          <t>14:55:42</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>15:10</t>
+          <t>15:06</t>
         </is>
       </c>
       <c r="C267" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D267" t="n">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="E267" t="inlineStr">
         <is>
@@ -7028,21 +7028,21 @@
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>14:19:39</t>
+          <t>14:55:42</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>15:13</t>
+          <t>15:06</t>
         </is>
       </c>
       <c r="C268" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D268" t="n">
-        <v>54</v>
+        <v>11</v>
       </c>
       <c r="E268" t="inlineStr">
         <is>
@@ -7058,16 +7058,16 @@
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>15:14</t>
+          <t>15:07</t>
         </is>
       </c>
       <c r="C269" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D269" t="n">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="E269" t="inlineStr">
         <is>
@@ -7078,21 +7078,21 @@
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>14:45:15</t>
+          <t>14:55:42</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>15:17</t>
+          <t>15:10</t>
         </is>
       </c>
       <c r="C270" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D270" t="n">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
@@ -7103,21 +7103,21 @@
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>14:45:15</t>
+          <t>14:55:42</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>15:20</t>
+          <t>15:13</t>
         </is>
       </c>
       <c r="C271" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D271" t="n">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="E271" t="inlineStr">
         <is>
@@ -7133,16 +7133,16 @@
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>15:21</t>
+          <t>15:14</t>
         </is>
       </c>
       <c r="C272" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D272" t="n">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="E272" t="inlineStr">
         <is>
@@ -7153,21 +7153,21 @@
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>14:45:15</t>
+          <t>14:55:42</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>15:32</t>
+          <t>15:16</t>
         </is>
       </c>
       <c r="C273" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D273" t="n">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="E273" t="inlineStr">
         <is>
@@ -7178,21 +7178,21 @@
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>14:19:39</t>
+          <t>14:45:15</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>15:34</t>
+          <t>15:17</t>
         </is>
       </c>
       <c r="C274" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D274" t="n">
-        <v>75</v>
+        <v>32</v>
       </c>
       <c r="E274" t="inlineStr">
         <is>
@@ -7203,21 +7203,21 @@
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>14:45:15</t>
+          <t>14:55:42</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>15:35</t>
+          <t>15:20</t>
         </is>
       </c>
       <c r="C275" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D275" t="n">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="E275" t="inlineStr">
         <is>
@@ -7228,21 +7228,21 @@
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>14:45:15</t>
+          <t>14:55:42</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>15:37</t>
+          <t>15:21</t>
         </is>
       </c>
       <c r="C276" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D276" t="n">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="E276" t="inlineStr">
         <is>
@@ -7253,21 +7253,21 @@
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>14:19:39</t>
+          <t>14:55:42</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>15:38</t>
+          <t>15:32</t>
         </is>
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D277" t="n">
-        <v>79</v>
+        <v>37</v>
       </c>
       <c r="E277" t="inlineStr">
         <is>
@@ -7278,21 +7278,21 @@
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>14:45:15</t>
+          <t>14:55:42</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>15:39</t>
+          <t>15:34</t>
         </is>
       </c>
       <c r="C278" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D278" t="n">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
@@ -7303,21 +7303,21 @@
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>13:51:20</t>
+          <t>14:45:15</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>15:44</t>
+          <t>15:35</t>
         </is>
       </c>
       <c r="C279" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D279" t="n">
-        <v>113</v>
+        <v>50</v>
       </c>
       <c r="E279" t="inlineStr">
         <is>
@@ -7328,21 +7328,21 @@
     <row r="280">
       <c r="A280" t="inlineStr">
         <is>
-          <t>14:19:39</t>
+          <t>14:55:42</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>15:46</t>
+          <t>15:37</t>
         </is>
       </c>
       <c r="C280" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D280" t="n">
-        <v>87</v>
+        <v>42</v>
       </c>
       <c r="E280" t="inlineStr">
         <is>
@@ -7353,21 +7353,21 @@
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>14:45:15</t>
+          <t>14:55:42</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>15:46</t>
+          <t>15:38</t>
         </is>
       </c>
       <c r="C281" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D281" t="n">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
@@ -7383,16 +7383,16 @@
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>15:47</t>
+          <t>15:39</t>
         </is>
       </c>
       <c r="C282" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D282" t="n">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="E282" t="inlineStr">
         <is>
@@ -7403,21 +7403,21 @@
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>14:19:39</t>
+          <t>13:51:20</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>15:53</t>
+          <t>15:44</t>
         </is>
       </c>
       <c r="C283" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D283" t="n">
-        <v>94</v>
+        <v>113</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
@@ -7428,21 +7428,21 @@
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>14:19:39</t>
+          <t>14:55:42</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>15:53</t>
+          <t>15:45</t>
         </is>
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D284" t="n">
-        <v>94</v>
+        <v>50</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
@@ -7458,16 +7458,16 @@
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>15:54</t>
+          <t>15:46</t>
         </is>
       </c>
       <c r="C285" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D285" t="n">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
@@ -7478,21 +7478,21 @@
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>14:19:39</t>
+          <t>14:55:42</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>15:55</t>
+          <t>15:46</t>
         </is>
       </c>
       <c r="C286" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D286" t="n">
-        <v>96</v>
+        <v>51</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
@@ -7508,16 +7508,16 @@
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>15:56</t>
+          <t>15:47</t>
         </is>
       </c>
       <c r="C287" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D287" t="n">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
@@ -7528,12 +7528,12 @@
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>14:45:15</t>
+          <t>14:19:39</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>15:57</t>
+          <t>15:53</t>
         </is>
       </c>
       <c r="C288" t="inlineStr">
@@ -7542,7 +7542,7 @@
         </is>
       </c>
       <c r="D288" t="n">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="E288" t="inlineStr">
         <is>
@@ -7553,21 +7553,21 @@
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>14:45:15</t>
+          <t>14:55:42</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>16:09</t>
+          <t>15:53</t>
         </is>
       </c>
       <c r="C289" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D289" t="n">
-        <v>84</v>
+        <v>58</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
@@ -7583,16 +7583,16 @@
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>16:09</t>
+          <t>15:54</t>
         </is>
       </c>
       <c r="C290" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D290" t="n">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
@@ -7603,21 +7603,21 @@
     <row r="291">
       <c r="A291" t="inlineStr">
         <is>
-          <t>14:45:15</t>
+          <t>14:55:42</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>16:15</t>
+          <t>15:55</t>
         </is>
       </c>
       <c r="C291" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D291" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E291" t="inlineStr">
         <is>
@@ -7633,16 +7633,16 @@
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>16:20</t>
+          <t>15:56</t>
         </is>
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D292" t="n">
-        <v>95</v>
+        <v>71</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
@@ -7653,21 +7653,21 @@
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>14:45:15</t>
+          <t>14:55:42</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>16:21</t>
+          <t>15:56</t>
         </is>
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D293" t="n">
-        <v>96</v>
+        <v>61</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
@@ -7683,16 +7683,16 @@
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>16:30</t>
+          <t>15:57</t>
         </is>
       </c>
       <c r="C294" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D294" t="n">
-        <v>105</v>
+        <v>72</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
@@ -7703,21 +7703,21 @@
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>14:45:15</t>
+          <t>14:55:42</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>16:43</t>
+          <t>16:08</t>
         </is>
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D295" t="n">
-        <v>118</v>
+        <v>73</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
@@ -7733,18 +7733,243 @@
       </c>
       <c r="B296" t="inlineStr">
         <is>
+          <t>16:09</t>
+        </is>
+      </c>
+      <c r="C296" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D296" t="n">
+        <v>84</v>
+      </c>
+      <c r="E296" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="inlineStr">
+        <is>
+          <t>14:45:15</t>
+        </is>
+      </c>
+      <c r="B297" t="inlineStr">
+        <is>
+          <t>16:09</t>
+        </is>
+      </c>
+      <c r="C297" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D297" t="n">
+        <v>84</v>
+      </c>
+      <c r="E297" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="inlineStr">
+        <is>
+          <t>14:55:42</t>
+        </is>
+      </c>
+      <c r="B298" t="inlineStr">
+        <is>
+          <t>16:15</t>
+        </is>
+      </c>
+      <c r="C298" t="inlineStr">
+        <is>
+          <t>225_C ROCA-H SUR</t>
+        </is>
+      </c>
+      <c r="D298" t="n">
+        <v>80</v>
+      </c>
+      <c r="E298" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="inlineStr">
+        <is>
+          <t>14:55:42</t>
+        </is>
+      </c>
+      <c r="B299" t="inlineStr">
+        <is>
+          <t>16:19</t>
+        </is>
+      </c>
+      <c r="C299" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D299" t="n">
+        <v>84</v>
+      </c>
+      <c r="E299" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="inlineStr">
+        <is>
+          <t>14:45:15</t>
+        </is>
+      </c>
+      <c r="B300" t="inlineStr">
+        <is>
+          <t>16:20</t>
+        </is>
+      </c>
+      <c r="C300" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D300" t="n">
+        <v>95</v>
+      </c>
+      <c r="E300" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="inlineStr">
+        <is>
+          <t>14:55:42</t>
+        </is>
+      </c>
+      <c r="B301" t="inlineStr">
+        <is>
+          <t>16:21</t>
+        </is>
+      </c>
+      <c r="C301" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D301" t="n">
+        <v>86</v>
+      </c>
+      <c r="E301" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>14:55:42</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>16:30</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D302" t="n">
+        <v>95</v>
+      </c>
+      <c r="E302" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>14:55:42</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>16:42</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D303" t="n">
+        <v>107</v>
+      </c>
+      <c r="E303" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>14:45:15</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
           <t>16:43</t>
         </is>
       </c>
-      <c r="C296" t="inlineStr">
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D304" t="n">
+        <v>118</v>
+      </c>
+      <c r="E304" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>14:55:42</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>16:43</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
         <is>
           <t>225_GOMEZ</t>
         </is>
       </c>
-      <c r="D296" t="n">
-        <v>118</v>
-      </c>
-      <c r="E296" t="inlineStr">
+      <c r="D305" t="n">
+        <v>108</v>
+      </c>
+      <c r="E305" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -7761,7 +7986,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7779,14 +8004,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:45:15</t>
+          <t>Última actualización: 14:55:42</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 35</t>
+          <t>Total filas: 37</t>
         </is>
       </c>
     </row>
@@ -8595,12 +8820,12 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>14:45:15</t>
+          <t>14:55:42</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>14:58</t>
+          <t>14:55</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -8609,7 +8834,7 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -8620,21 +8845,21 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>14:19:39</t>
+          <t>14:45:15</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>15:38</t>
+          <t>14:58</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>79</v>
+        <v>13</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -8645,12 +8870,12 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>14:45:15</t>
+          <t>14:55:42</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>15:39</t>
+          <t>15:38</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -8659,7 +8884,7 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -8675,18 +8900,68 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
+          <t>15:39</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>54</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>14:55:42</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>16:19</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>84</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>14:45:15</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
           <t>16:20</t>
         </is>
       </c>
-      <c r="C40" t="inlineStr">
+      <c r="C42" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D40" t="n">
+      <c r="D42" t="n">
         <v>95</v>
       </c>
-      <c r="E40" t="inlineStr">
+      <c r="E42" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -8703,7 +8978,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E46"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8721,14 +8996,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:45:15</t>
+          <t>Última actualización: 14:55:42</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 41</t>
+          <t>Total filas: 42</t>
         </is>
       </c>
     </row>
@@ -9687,7 +9962,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>14:19:39</t>
+          <t>14:55:42</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -9701,7 +9976,7 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -9737,7 +10012,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>14:19:39</t>
+          <t>14:55:42</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -9751,7 +10026,7 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>114</v>
+        <v>78</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -9781,6 +10056,31 @@
       <c r="E46" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>14:55:42</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>16:52</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-40 Y 115</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>117</v>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 844
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-23.xlsx
+++ b/data/horarios-141-2026-01-23.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E305"/>
+  <dimension ref="A1:E314"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:55:42</t>
+          <t>Última actualización: 15:21:03</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 300</t>
+          <t>Total filas: 309</t>
         </is>
       </c>
     </row>
@@ -1513,7 +1513,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -1538,7 +1538,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -1778,7 +1778,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1788,11 +1788,11 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -1803,7 +1803,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1813,11 +1813,11 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>17</v>
+        <v>84</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D63" t="n">
@@ -1938,7 +1938,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -2213,7 +2213,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D75" t="n">
@@ -2238,7 +2238,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D76" t="n">
@@ -2528,7 +2528,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -2538,11 +2538,11 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -2553,7 +2553,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2563,11 +2563,11 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -2903,7 +2903,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>08:48:01</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -2913,11 +2913,11 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -2928,7 +2928,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>08:48:01</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -2938,11 +2938,11 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D104" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -3338,7 +3338,7 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D120" t="n">
@@ -3363,7 +3363,7 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D121" t="n">
@@ -3388,7 +3388,7 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D122" t="n">
@@ -3413,7 +3413,7 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D123" t="n">
@@ -4928,7 +4928,7 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>10:57:35</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
@@ -4938,11 +4938,11 @@
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D184" t="n">
-        <v>12</v>
+        <v>77</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -4953,7 +4953,7 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>10:57:35</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
@@ -4963,11 +4963,11 @@
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D185" t="n">
-        <v>77</v>
+        <v>12</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -5003,7 +5003,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>10:27:29</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
@@ -5013,11 +5013,11 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D187" t="n">
-        <v>15</v>
+        <v>110</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -5028,7 +5028,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>10:27:29</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -5038,11 +5038,11 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D188" t="n">
-        <v>110</v>
+        <v>15</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5288,7 +5288,7 @@
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_179 Y 38</t>
         </is>
       </c>
       <c r="D198" t="n">
@@ -5338,7 +5338,7 @@
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>17_179 Y 38</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D200" t="n">
@@ -5653,7 +5653,7 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>12:54:24</t>
+          <t>12:37:00</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
@@ -5663,11 +5663,11 @@
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D213" t="n">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -5678,7 +5678,7 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>12:54:24</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
@@ -5688,11 +5688,11 @@
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D214" t="n">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
@@ -5813,7 +5813,7 @@
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D219" t="n">
@@ -5838,7 +5838,7 @@
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D220" t="n">
@@ -5988,7 +5988,7 @@
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D226" t="n">
@@ -6013,7 +6013,7 @@
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D227" t="n">
@@ -6138,7 +6138,7 @@
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D232" t="n">
@@ -6163,7 +6163,7 @@
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D233" t="n">
@@ -6188,7 +6188,7 @@
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D234" t="n">
@@ -6213,7 +6213,7 @@
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D235" t="n">
@@ -6313,7 +6313,7 @@
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D239" t="n">
@@ -6338,7 +6338,7 @@
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D240" t="n">
@@ -6353,7 +6353,7 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>13:51:20</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
@@ -6363,11 +6363,11 @@
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D241" t="n">
-        <v>80</v>
+        <v>6</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -6378,7 +6378,7 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>13:51:20</t>
+          <t>12:37:00</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
@@ -6388,11 +6388,11 @@
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D242" t="n">
-        <v>6</v>
+        <v>80</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -6403,7 +6403,7 @@
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>13:51:20</t>
+          <t>13:18:32</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
@@ -6413,11 +6413,11 @@
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D243" t="n">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -6428,7 +6428,7 @@
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>13:18:32</t>
+          <t>13:51:20</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
@@ -6438,11 +6438,11 @@
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D244" t="n">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -7013,7 +7013,7 @@
       </c>
       <c r="C267" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D267" t="n">
@@ -7038,7 +7038,7 @@
       </c>
       <c r="C268" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D268" t="n">
@@ -7228,7 +7228,7 @@
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>14:55:42</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
@@ -7238,11 +7238,11 @@
       </c>
       <c r="C276" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D276" t="n">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="E276" t="inlineStr">
         <is>
@@ -7253,21 +7253,21 @@
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>14:55:42</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>15:32</t>
+          <t>15:21</t>
         </is>
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D277" t="n">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="E277" t="inlineStr">
         <is>
@@ -7278,21 +7278,21 @@
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>14:55:42</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>15:34</t>
+          <t>15:32</t>
         </is>
       </c>
       <c r="C278" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D278" t="n">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
@@ -7303,12 +7303,12 @@
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>14:45:15</t>
+          <t>14:55:42</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>15:35</t>
+          <t>15:34</t>
         </is>
       </c>
       <c r="C279" t="inlineStr">
@@ -7317,7 +7317,7 @@
         </is>
       </c>
       <c r="D279" t="n">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="E279" t="inlineStr">
         <is>
@@ -7328,21 +7328,21 @@
     <row r="280">
       <c r="A280" t="inlineStr">
         <is>
-          <t>14:55:42</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>15:37</t>
+          <t>15:35</t>
         </is>
       </c>
       <c r="C280" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D280" t="n">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="E280" t="inlineStr">
         <is>
@@ -7353,21 +7353,21 @@
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>14:55:42</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>15:38</t>
+          <t>15:37</t>
         </is>
       </c>
       <c r="C281" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D281" t="n">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
@@ -7378,12 +7378,12 @@
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>14:45:15</t>
+          <t>14:55:42</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>15:39</t>
+          <t>15:38</t>
         </is>
       </c>
       <c r="C282" t="inlineStr">
@@ -7392,7 +7392,7 @@
         </is>
       </c>
       <c r="D282" t="n">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="E282" t="inlineStr">
         <is>
@@ -7403,21 +7403,21 @@
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>13:51:20</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>15:44</t>
+          <t>15:39</t>
         </is>
       </c>
       <c r="C283" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D283" t="n">
-        <v>113</v>
+        <v>18</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
@@ -7428,12 +7428,12 @@
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>14:55:42</t>
+          <t>13:51:20</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>15:45</t>
+          <t>15:44</t>
         </is>
       </c>
       <c r="C284" t="inlineStr">
@@ -7442,7 +7442,7 @@
         </is>
       </c>
       <c r="D284" t="n">
-        <v>50</v>
+        <v>113</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
@@ -7453,12 +7453,12 @@
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>14:45:15</t>
+          <t>14:55:42</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>15:46</t>
+          <t>15:45</t>
         </is>
       </c>
       <c r="C285" t="inlineStr">
@@ -7467,7 +7467,7 @@
         </is>
       </c>
       <c r="D285" t="n">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
@@ -7503,21 +7503,21 @@
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>14:45:15</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>15:47</t>
+          <t>15:46</t>
         </is>
       </c>
       <c r="C287" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D287" t="n">
-        <v>62</v>
+        <v>25</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
@@ -7528,21 +7528,21 @@
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>14:19:39</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>15:53</t>
+          <t>15:47</t>
         </is>
       </c>
       <c r="C288" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D288" t="n">
-        <v>94</v>
+        <v>26</v>
       </c>
       <c r="E288" t="inlineStr">
         <is>
@@ -7578,21 +7578,21 @@
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>14:45:15</t>
+          <t>14:19:39</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>15:54</t>
+          <t>15:53</t>
         </is>
       </c>
       <c r="C290" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D290" t="n">
-        <v>69</v>
+        <v>94</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
@@ -7603,21 +7603,21 @@
     <row r="291">
       <c r="A291" t="inlineStr">
         <is>
-          <t>14:55:42</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>15:55</t>
+          <t>15:54</t>
         </is>
       </c>
       <c r="C291" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D291" t="n">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="E291" t="inlineStr">
         <is>
@@ -7628,12 +7628,12 @@
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>14:45:15</t>
+          <t>14:55:42</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>15:56</t>
+          <t>15:55</t>
         </is>
       </c>
       <c r="C292" t="inlineStr">
@@ -7642,7 +7642,7 @@
         </is>
       </c>
       <c r="D292" t="n">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
@@ -7653,21 +7653,21 @@
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>14:55:42</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>15:56</t>
+          <t>15:55</t>
         </is>
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D293" t="n">
-        <v>61</v>
+        <v>34</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
@@ -7678,12 +7678,12 @@
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>14:45:15</t>
+          <t>14:55:42</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>15:57</t>
+          <t>15:56</t>
         </is>
       </c>
       <c r="C294" t="inlineStr">
@@ -7692,7 +7692,7 @@
         </is>
       </c>
       <c r="D294" t="n">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
@@ -7703,21 +7703,21 @@
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>14:55:42</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>16:08</t>
+          <t>15:56</t>
         </is>
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D295" t="n">
-        <v>73</v>
+        <v>35</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
@@ -7728,21 +7728,21 @@
     <row r="296">
       <c r="A296" t="inlineStr">
         <is>
-          <t>14:45:15</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>16:09</t>
+          <t>15:57</t>
         </is>
       </c>
       <c r="C296" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D296" t="n">
-        <v>84</v>
+        <v>36</v>
       </c>
       <c r="E296" t="inlineStr">
         <is>
@@ -7753,21 +7753,21 @@
     <row r="297">
       <c r="A297" t="inlineStr">
         <is>
-          <t>14:45:15</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>16:09</t>
+          <t>16:05</t>
         </is>
       </c>
       <c r="C297" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D297" t="n">
-        <v>84</v>
+        <v>44</v>
       </c>
       <c r="E297" t="inlineStr">
         <is>
@@ -7783,16 +7783,16 @@
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>16:15</t>
+          <t>16:08</t>
         </is>
       </c>
       <c r="C298" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D298" t="n">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E298" t="inlineStr">
         <is>
@@ -7803,21 +7803,21 @@
     <row r="299">
       <c r="A299" t="inlineStr">
         <is>
-          <t>14:55:42</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>16:19</t>
+          <t>16:09</t>
         </is>
       </c>
       <c r="C299" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D299" t="n">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="E299" t="inlineStr">
         <is>
@@ -7833,16 +7833,16 @@
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>16:20</t>
+          <t>16:09</t>
         </is>
       </c>
       <c r="C300" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D300" t="n">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="E300" t="inlineStr">
         <is>
@@ -7853,21 +7853,21 @@
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>14:55:42</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>16:21</t>
+          <t>16:15</t>
         </is>
       </c>
       <c r="C301" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>225_C ROCA-H SUR</t>
         </is>
       </c>
       <c r="D301" t="n">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="E301" t="inlineStr">
         <is>
@@ -7878,21 +7878,21 @@
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>14:55:42</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>16:30</t>
+          <t>16:15</t>
         </is>
       </c>
       <c r="C302" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D302" t="n">
-        <v>95</v>
+        <v>54</v>
       </c>
       <c r="E302" t="inlineStr">
         <is>
@@ -7908,16 +7908,16 @@
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>16:42</t>
+          <t>16:19</t>
         </is>
       </c>
       <c r="C303" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D303" t="n">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="E303" t="inlineStr">
         <is>
@@ -7928,21 +7928,21 @@
     <row r="304">
       <c r="A304" t="inlineStr">
         <is>
-          <t>14:45:15</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>16:43</t>
+          <t>16:20</t>
         </is>
       </c>
       <c r="C304" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D304" t="n">
-        <v>118</v>
+        <v>59</v>
       </c>
       <c r="E304" t="inlineStr">
         <is>
@@ -7953,23 +7953,248 @@
     <row r="305">
       <c r="A305" t="inlineStr">
         <is>
+          <t>15:21:03</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>16:21</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D305" t="n">
+        <v>60</v>
+      </c>
+      <c r="E305" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>15:21:03</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>16:30</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D306" t="n">
+        <v>69</v>
+      </c>
+      <c r="E306" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>15:21:03</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>16:37</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D307" t="n">
+        <v>76</v>
+      </c>
+      <c r="E307" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>15:21:03</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>16:40</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D308" t="n">
+        <v>79</v>
+      </c>
+      <c r="E308" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
           <t>14:55:42</t>
         </is>
       </c>
-      <c r="B305" t="inlineStr">
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>16:42</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D309" t="n">
+        <v>107</v>
+      </c>
+      <c r="E309" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>15:21:03</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
         <is>
           <t>16:43</t>
         </is>
       </c>
-      <c r="C305" t="inlineStr">
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D310" t="n">
+        <v>82</v>
+      </c>
+      <c r="E310" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>15:21:03</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>16:43</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
         <is>
           <t>225_GOMEZ</t>
         </is>
       </c>
-      <c r="D305" t="n">
-        <v>108</v>
-      </c>
-      <c r="E305" t="inlineStr">
+      <c r="D311" t="n">
+        <v>82</v>
+      </c>
+      <c r="E311" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>15:21:03</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>16:48</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D312" t="n">
+        <v>87</v>
+      </c>
+      <c r="E312" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>15:21:03</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>16:56</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>17_179 Y 38</t>
+        </is>
+      </c>
+      <c r="D313" t="n">
+        <v>95</v>
+      </c>
+      <c r="E313" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>15:21:03</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>17:05</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D314" t="n">
+        <v>104</v>
+      </c>
+      <c r="E314" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -7986,7 +8211,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8004,14 +8229,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:55:42</t>
+          <t>Última actualización: 15:21:03</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 37</t>
+          <t>Total filas: 38</t>
         </is>
       </c>
     </row>
@@ -8895,7 +9120,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>14:45:15</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -8909,7 +9134,7 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -8945,7 +9170,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>14:45:15</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -8959,9 +9184,34 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>95</v>
+        <v>59</v>
       </c>
       <c r="E42" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>15:21:03</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>17:05</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>104</v>
+      </c>
+      <c r="E43" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -8978,7 +9228,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8996,14 +9246,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:55:42</t>
+          <t>Última actualización: 15:21:03</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 42</t>
+          <t>Total filas: 45</t>
         </is>
       </c>
     </row>
@@ -9987,12 +10237,12 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>14:45:15</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>15:38</t>
+          <t>15:36</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -10001,7 +10251,7 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -10012,37 +10262,37 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>14:55:42</t>
+          <t>14:45:15</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>16:13</t>
+          <t>15:38</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>78</v>
+        <v>53</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>L6203</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>14:45:15</t>
+          <t>14:55:42</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>16:14</t>
+          <t>16:13</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -10051,7 +10301,7 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -10062,23 +10312,98 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
+          <t>15:21:03</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>16:14</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>53</v>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
           <t>14:55:42</t>
         </is>
       </c>
-      <c r="B47" t="inlineStr">
+      <c r="B48" t="inlineStr">
         <is>
           <t>16:52</t>
         </is>
       </c>
-      <c r="C47" t="inlineStr">
+      <c r="C48" t="inlineStr">
         <is>
           <t>215B_LP-P MOR-40 Y 115</t>
         </is>
       </c>
-      <c r="D47" t="n">
+      <c r="D48" t="n">
         <v>117</v>
       </c>
-      <c r="E47" t="inlineStr">
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>15:21:03</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>16:53</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-40 Y 115</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>92</v>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>15:21:03</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>17:14</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>113</v>
+      </c>
+      <c r="E50" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 845
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-23.xlsx
+++ b/data/horarios-141-2026-01-23.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E314"/>
+  <dimension ref="A1:E338"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 15:21:03</t>
+          <t>Última actualización: 15:55:57</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 309</t>
+          <t>Total filas: 333</t>
         </is>
       </c>
     </row>
@@ -1513,7 +1513,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -1538,7 +1538,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -1628,7 +1628,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1638,11 +1638,11 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>6</v>
+        <v>73</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -1653,7 +1653,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1663,11 +1663,11 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>73</v>
+        <v>6</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -1778,7 +1778,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1788,11 +1788,11 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>17</v>
+        <v>84</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -1803,7 +1803,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1813,11 +1813,11 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D63" t="n">
@@ -1938,7 +1938,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -1953,7 +1953,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1963,11 +1963,11 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -1978,7 +1978,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -1988,11 +1988,11 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2213,7 +2213,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D75" t="n">
@@ -2238,7 +2238,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D76" t="n">
@@ -2528,7 +2528,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -2538,11 +2538,11 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -2553,7 +2553,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2563,11 +2563,11 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -2803,7 +2803,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -2813,11 +2813,11 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D99" t="n">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -2828,7 +2828,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -2838,11 +2838,11 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -2903,7 +2903,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>08:48:01</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -2913,11 +2913,11 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -2928,7 +2928,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>08:48:01</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -2938,11 +2938,11 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D104" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -3388,7 +3388,7 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D122" t="n">
@@ -3413,7 +3413,7 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D123" t="n">
@@ -4163,7 +4163,7 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D153" t="n">
@@ -4188,7 +4188,7 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D154" t="n">
@@ -4928,7 +4928,7 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>10:57:35</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
@@ -4938,11 +4938,11 @@
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D184" t="n">
-        <v>77</v>
+        <v>12</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -4953,7 +4953,7 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>10:57:35</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
@@ -4963,11 +4963,11 @@
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D185" t="n">
-        <v>12</v>
+        <v>77</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -5003,7 +5003,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>10:27:29</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
@@ -5013,11 +5013,11 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D187" t="n">
-        <v>110</v>
+        <v>15</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -5028,7 +5028,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>10:27:29</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -5038,11 +5038,11 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D188" t="n">
-        <v>15</v>
+        <v>110</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5063,7 +5063,7 @@
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D189" t="n">
@@ -5088,7 +5088,7 @@
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D190" t="n">
@@ -5153,7 +5153,7 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>11:49:23</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
@@ -5163,11 +5163,11 @@
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D193" t="n">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
@@ -5178,7 +5178,7 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>11:49:23</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
@@ -5188,11 +5188,11 @@
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D194" t="n">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -5813,7 +5813,7 @@
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D219" t="n">
@@ -5838,7 +5838,7 @@
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D220" t="n">
@@ -6188,7 +6188,7 @@
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D234" t="n">
@@ -6213,7 +6213,7 @@
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D235" t="n">
@@ -6313,7 +6313,7 @@
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D239" t="n">
@@ -6338,7 +6338,7 @@
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D240" t="n">
@@ -6403,7 +6403,7 @@
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>13:18:32</t>
+          <t>13:51:20</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
@@ -6413,11 +6413,11 @@
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D243" t="n">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -6428,7 +6428,7 @@
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>13:51:20</t>
+          <t>13:18:32</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
@@ -6438,11 +6438,11 @@
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D244" t="n">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -6838,7 +6838,7 @@
       </c>
       <c r="C260" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D260" t="n">
@@ -6863,7 +6863,7 @@
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D261" t="n">
@@ -7478,7 +7478,7 @@
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>14:55:42</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
@@ -7488,11 +7488,11 @@
       </c>
       <c r="C286" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D286" t="n">
-        <v>51</v>
+        <v>25</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
@@ -7503,7 +7503,7 @@
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>14:55:42</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
@@ -7513,11 +7513,11 @@
       </c>
       <c r="C287" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D287" t="n">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
@@ -7628,7 +7628,7 @@
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>14:55:42</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
@@ -7642,7 +7642,7 @@
         </is>
       </c>
       <c r="D292" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
@@ -7678,7 +7678,7 @@
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>14:55:42</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
@@ -7692,7 +7692,7 @@
         </is>
       </c>
       <c r="D294" t="n">
-        <v>61</v>
+        <v>1</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
@@ -7753,21 +7753,21 @@
     <row r="297">
       <c r="A297" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>16:05</t>
+          <t>15:57</t>
         </is>
       </c>
       <c r="C297" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D297" t="n">
-        <v>44</v>
+        <v>2</v>
       </c>
       <c r="E297" t="inlineStr">
         <is>
@@ -7778,21 +7778,21 @@
     <row r="298">
       <c r="A298" t="inlineStr">
         <is>
-          <t>14:55:42</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>16:08</t>
+          <t>16:04</t>
         </is>
       </c>
       <c r="C298" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D298" t="n">
-        <v>73</v>
+        <v>9</v>
       </c>
       <c r="E298" t="inlineStr">
         <is>
@@ -7808,16 +7808,16 @@
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>16:09</t>
+          <t>16:05</t>
         </is>
       </c>
       <c r="C299" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D299" t="n">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E299" t="inlineStr">
         <is>
@@ -7828,21 +7828,21 @@
     <row r="300">
       <c r="A300" t="inlineStr">
         <is>
-          <t>14:45:15</t>
+          <t>14:55:42</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>16:09</t>
+          <t>16:08</t>
         </is>
       </c>
       <c r="C300" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D300" t="n">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="E300" t="inlineStr">
         <is>
@@ -7853,21 +7853,21 @@
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>14:45:15</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>16:15</t>
+          <t>16:09</t>
         </is>
       </c>
       <c r="C301" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D301" t="n">
-        <v>54</v>
+        <v>84</v>
       </c>
       <c r="E301" t="inlineStr">
         <is>
@@ -7883,16 +7883,16 @@
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>16:15</t>
+          <t>16:09</t>
         </is>
       </c>
       <c r="C302" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D302" t="n">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E302" t="inlineStr">
         <is>
@@ -7903,21 +7903,21 @@
     <row r="303">
       <c r="A303" t="inlineStr">
         <is>
-          <t>14:55:42</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>16:19</t>
+          <t>16:10</t>
         </is>
       </c>
       <c r="C303" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D303" t="n">
-        <v>84</v>
+        <v>15</v>
       </c>
       <c r="E303" t="inlineStr">
         <is>
@@ -7928,21 +7928,21 @@
     <row r="304">
       <c r="A304" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>16:20</t>
+          <t>16:14</t>
         </is>
       </c>
       <c r="C304" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>225_C ROCA-H SUR</t>
         </is>
       </c>
       <c r="D304" t="n">
-        <v>59</v>
+        <v>19</v>
       </c>
       <c r="E304" t="inlineStr">
         <is>
@@ -7958,16 +7958,16 @@
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>16:21</t>
+          <t>16:15</t>
         </is>
       </c>
       <c r="C305" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D305" t="n">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E305" t="inlineStr">
         <is>
@@ -7983,16 +7983,16 @@
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>16:30</t>
+          <t>16:15</t>
         </is>
       </c>
       <c r="C306" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>225_C ROCA-H SUR</t>
         </is>
       </c>
       <c r="D306" t="n">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="E306" t="inlineStr">
         <is>
@@ -8003,21 +8003,21 @@
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>16:37</t>
+          <t>16:19</t>
         </is>
       </c>
       <c r="C307" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D307" t="n">
-        <v>76</v>
+        <v>24</v>
       </c>
       <c r="E307" t="inlineStr">
         <is>
@@ -8033,16 +8033,16 @@
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>16:40</t>
+          <t>16:20</t>
         </is>
       </c>
       <c r="C308" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D308" t="n">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="E308" t="inlineStr">
         <is>
@@ -8053,21 +8053,21 @@
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>14:55:42</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>16:42</t>
+          <t>16:20</t>
         </is>
       </c>
       <c r="C309" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D309" t="n">
-        <v>107</v>
+        <v>25</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
@@ -8083,16 +8083,16 @@
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>16:43</t>
+          <t>16:21</t>
         </is>
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D310" t="n">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="E310" t="inlineStr">
         <is>
@@ -8103,21 +8103,21 @@
     <row r="311">
       <c r="A311" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>16:43</t>
+          <t>16:26</t>
         </is>
       </c>
       <c r="C311" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D311" t="n">
-        <v>82</v>
+        <v>31</v>
       </c>
       <c r="E311" t="inlineStr">
         <is>
@@ -8128,21 +8128,21 @@
     <row r="312">
       <c r="A312" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>16:48</t>
+          <t>16:28</t>
         </is>
       </c>
       <c r="C312" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D312" t="n">
-        <v>87</v>
+        <v>33</v>
       </c>
       <c r="E312" t="inlineStr">
         <is>
@@ -8153,21 +8153,21 @@
     <row r="313">
       <c r="A313" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>16:56</t>
+          <t>16:29</t>
         </is>
       </c>
       <c r="C313" t="inlineStr">
         <is>
-          <t>17_179 Y 38</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D313" t="n">
-        <v>95</v>
+        <v>34</v>
       </c>
       <c r="E313" t="inlineStr">
         <is>
@@ -8183,18 +8183,618 @@
       </c>
       <c r="B314" t="inlineStr">
         <is>
+          <t>16:30</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D314" t="n">
+        <v>69</v>
+      </c>
+      <c r="E314" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>15:55:57</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>16:34</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D315" t="n">
+        <v>39</v>
+      </c>
+      <c r="E315" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>15:55:57</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>16:36</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D316" t="n">
+        <v>41</v>
+      </c>
+      <c r="E316" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>15:21:03</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>16:37</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D317" t="n">
+        <v>76</v>
+      </c>
+      <c r="E317" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>15:55:57</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>16:39</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D318" t="n">
+        <v>44</v>
+      </c>
+      <c r="E318" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>15:21:03</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>16:40</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D319" t="n">
+        <v>79</v>
+      </c>
+      <c r="E319" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>15:55:57</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>16:42</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D320" t="n">
+        <v>47</v>
+      </c>
+      <c r="E320" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>15:55:57</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>16:42</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D321" t="n">
+        <v>47</v>
+      </c>
+      <c r="E321" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>15:21:03</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>16:43</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D322" t="n">
+        <v>82</v>
+      </c>
+      <c r="E322" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>15:21:03</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>16:43</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D323" t="n">
+        <v>82</v>
+      </c>
+      <c r="E323" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>15:55:57</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>16:47</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D324" t="n">
+        <v>52</v>
+      </c>
+      <c r="E324" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>15:21:03</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>16:48</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D325" t="n">
+        <v>87</v>
+      </c>
+      <c r="E325" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>15:55:57</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>16:50</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D326" t="n">
+        <v>55</v>
+      </c>
+      <c r="E326" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>15:55:57</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>16:55</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>17_179 Y 38</t>
+        </is>
+      </c>
+      <c r="D327" t="n">
+        <v>60</v>
+      </c>
+      <c r="E327" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>15:21:03</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>16:56</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>17_179 Y 38</t>
+        </is>
+      </c>
+      <c r="D328" t="n">
+        <v>95</v>
+      </c>
+      <c r="E328" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>15:55:57</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>17:04</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D329" t="n">
+        <v>69</v>
+      </c>
+      <c r="E329" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>15:55:57</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>17:04</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D330" t="n">
+        <v>69</v>
+      </c>
+      <c r="E330" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>15:21:03</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
           <t>17:05</t>
         </is>
       </c>
-      <c r="C314" t="inlineStr">
+      <c r="C331" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D314" t="n">
+      <c r="D331" t="n">
         <v>104</v>
       </c>
-      <c r="E314" t="inlineStr">
+      <c r="E331" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>15:55:57</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>17:20</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D332" t="n">
+        <v>85</v>
+      </c>
+      <c r="E332" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>15:55:57</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>17:23</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D333" t="n">
+        <v>88</v>
+      </c>
+      <c r="E333" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>15:55:57</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>17:28</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D334" t="n">
+        <v>93</v>
+      </c>
+      <c r="E334" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>15:55:57</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>17:31</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D335" t="n">
+        <v>96</v>
+      </c>
+      <c r="E335" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>15:55:57</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>17:39</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D336" t="n">
+        <v>104</v>
+      </c>
+      <c r="E336" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>15:55:57</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>17:50</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D337" t="n">
+        <v>115</v>
+      </c>
+      <c r="E337" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>15:55:57</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>17:51</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D338" t="n">
+        <v>116</v>
+      </c>
+      <c r="E338" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -8211,7 +8811,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8229,14 +8829,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 15:21:03</t>
+          <t>Última actualización: 15:55:57</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 38</t>
+          <t>Total filas: 40</t>
         </is>
       </c>
     </row>
@@ -9145,7 +9745,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>14:55:42</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -9159,7 +9759,7 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>84</v>
+        <v>24</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -9195,23 +9795,73 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
+          <t>15:55:57</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>17:04</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>69</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
           <t>15:21:03</t>
         </is>
       </c>
-      <c r="B43" t="inlineStr">
+      <c r="B44" t="inlineStr">
         <is>
           <t>17:05</t>
         </is>
       </c>
-      <c r="C43" t="inlineStr">
+      <c r="C44" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D43" t="n">
+      <c r="D44" t="n">
         <v>104</v>
       </c>
-      <c r="E43" t="inlineStr">
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>15:55:57</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>17:39</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>104</v>
+      </c>
+      <c r="E45" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -9246,7 +9896,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 15:21:03</t>
+          <t>Última actualización: 15:55:57</t>
         </is>
       </c>
     </row>
@@ -10287,7 +10937,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>14:55:42</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -10301,7 +10951,7 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>78</v>
+        <v>18</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -10337,7 +10987,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>14:55:42</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -10351,7 +11001,7 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>117</v>
+        <v>57</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -10387,7 +11037,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -10401,7 +11051,7 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>113</v>
+        <v>79</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 846
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-23.xlsx
+++ b/data/horarios-141-2026-01-23.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E338"/>
+  <dimension ref="A1:E350"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 15:55:57</t>
+          <t>Última actualización: 16:19:36</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 333</t>
+          <t>Total filas: 345</t>
         </is>
       </c>
     </row>
@@ -1313,7 +1313,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>86_EST CHICA-ESC AGRARIA</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1338,7 +1338,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>86_EST CHICA-ESC AGRARIA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1628,7 +1628,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1638,11 +1638,11 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>73</v>
+        <v>6</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -1653,7 +1653,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1663,11 +1663,11 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>6</v>
+        <v>73</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -1953,7 +1953,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1963,11 +1963,11 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -1978,7 +1978,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -1988,11 +1988,11 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2803,7 +2803,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -2813,11 +2813,11 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D99" t="n">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -2828,7 +2828,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -2838,11 +2838,11 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -3163,7 +3163,7 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D113" t="n">
@@ -3188,7 +3188,7 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D114" t="n">
@@ -3278,7 +3278,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>09:33:33</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -3288,11 +3288,11 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D118" t="n">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -3303,7 +3303,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>09:33:33</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -3313,11 +3313,11 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D119" t="n">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -3388,7 +3388,7 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D122" t="n">
@@ -3413,7 +3413,7 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D123" t="n">
@@ -4163,7 +4163,7 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D153" t="n">
@@ -4188,7 +4188,7 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D154" t="n">
@@ -4413,7 +4413,7 @@
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D163" t="n">
@@ -4438,7 +4438,7 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D164" t="n">
@@ -5003,7 +5003,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>10:27:29</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
@@ -5013,11 +5013,11 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D187" t="n">
-        <v>15</v>
+        <v>110</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -5028,7 +5028,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>10:27:29</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -5038,11 +5038,11 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D188" t="n">
-        <v>110</v>
+        <v>15</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5063,7 +5063,7 @@
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D189" t="n">
@@ -5088,7 +5088,7 @@
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D190" t="n">
@@ -5288,7 +5288,7 @@
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>17_179 Y 38</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D198" t="n">
@@ -5313,7 +5313,7 @@
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_179 Y 38</t>
         </is>
       </c>
       <c r="D199" t="n">
@@ -5653,7 +5653,7 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>12:54:24</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
@@ -5663,11 +5663,11 @@
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D213" t="n">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -5678,7 +5678,7 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>12:54:24</t>
+          <t>12:37:00</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
@@ -5688,11 +5688,11 @@
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D214" t="n">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
@@ -5813,7 +5813,7 @@
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D219" t="n">
@@ -5838,7 +5838,7 @@
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D220" t="n">
@@ -6138,7 +6138,7 @@
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D232" t="n">
@@ -6163,7 +6163,7 @@
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D233" t="n">
@@ -6188,7 +6188,7 @@
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D234" t="n">
@@ -6213,7 +6213,7 @@
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D235" t="n">
@@ -6353,7 +6353,7 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>13:51:20</t>
+          <t>12:37:00</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
@@ -6363,11 +6363,11 @@
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D241" t="n">
-        <v>6</v>
+        <v>80</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -6378,7 +6378,7 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>13:51:20</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
@@ -6388,11 +6388,11 @@
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D242" t="n">
-        <v>80</v>
+        <v>6</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -7013,7 +7013,7 @@
       </c>
       <c r="C267" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D267" t="n">
@@ -7038,7 +7038,7 @@
       </c>
       <c r="C268" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D268" t="n">
@@ -7238,7 +7238,7 @@
       </c>
       <c r="C276" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D276" t="n">
@@ -7263,7 +7263,7 @@
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D277" t="n">
@@ -7553,7 +7553,7 @@
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>14:55:42</t>
+          <t>14:19:39</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
@@ -7563,11 +7563,11 @@
       </c>
       <c r="C289" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D289" t="n">
-        <v>58</v>
+        <v>94</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
@@ -7578,7 +7578,7 @@
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>14:19:39</t>
+          <t>14:55:42</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
@@ -7588,11 +7588,11 @@
       </c>
       <c r="C290" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D290" t="n">
-        <v>94</v>
+        <v>58</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
@@ -7628,7 +7628,7 @@
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
@@ -7638,11 +7638,11 @@
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D292" t="n">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
@@ -7653,7 +7653,7 @@
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
@@ -7663,11 +7663,11 @@
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D293" t="n">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
@@ -7678,7 +7678,7 @@
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
@@ -7688,11 +7688,11 @@
       </c>
       <c r="C294" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D294" t="n">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
@@ -7703,7 +7703,7 @@
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
@@ -7713,11 +7713,11 @@
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D295" t="n">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
@@ -7853,7 +7853,7 @@
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>14:45:15</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
@@ -7863,11 +7863,11 @@
       </c>
       <c r="C301" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D301" t="n">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="E301" t="inlineStr">
         <is>
@@ -7878,7 +7878,7 @@
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>14:45:15</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
@@ -7888,11 +7888,11 @@
       </c>
       <c r="C302" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D302" t="n">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="E302" t="inlineStr">
         <is>
@@ -7963,7 +7963,7 @@
       </c>
       <c r="C305" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>225_C ROCA-H SUR</t>
         </is>
       </c>
       <c r="D305" t="n">
@@ -7988,7 +7988,7 @@
       </c>
       <c r="C306" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D306" t="n">
@@ -8003,7 +8003,7 @@
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:19:35</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
@@ -8013,11 +8013,11 @@
       </c>
       <c r="C307" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D307" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="E307" t="inlineStr">
         <is>
@@ -8028,12 +8028,12 @@
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>16:20</t>
+          <t>16:19</t>
         </is>
       </c>
       <c r="C308" t="inlineStr">
@@ -8042,7 +8042,7 @@
         </is>
       </c>
       <c r="D308" t="n">
-        <v>59</v>
+        <v>24</v>
       </c>
       <c r="E308" t="inlineStr">
         <is>
@@ -8078,21 +8078,21 @@
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>16:19:35</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>16:21</t>
+          <t>16:20</t>
         </is>
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D310" t="n">
-        <v>60</v>
+        <v>1</v>
       </c>
       <c r="E310" t="inlineStr">
         <is>
@@ -8103,21 +8103,21 @@
     <row r="311">
       <c r="A311" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:19:35</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>16:26</t>
+          <t>16:20</t>
         </is>
       </c>
       <c r="C311" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D311" t="n">
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="E311" t="inlineStr">
         <is>
@@ -8128,21 +8128,21 @@
     <row r="312">
       <c r="A312" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:19:35</t>
         </is>
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>16:28</t>
+          <t>16:21</t>
         </is>
       </c>
       <c r="C312" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D312" t="n">
-        <v>33</v>
+        <v>2</v>
       </c>
       <c r="E312" t="inlineStr">
         <is>
@@ -8158,16 +8158,16 @@
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>16:29</t>
+          <t>16:26</t>
         </is>
       </c>
       <c r="C313" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D313" t="n">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E313" t="inlineStr">
         <is>
@@ -8178,21 +8178,21 @@
     <row r="314">
       <c r="A314" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>16:30</t>
+          <t>16:28</t>
         </is>
       </c>
       <c r="C314" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D314" t="n">
-        <v>69</v>
+        <v>33</v>
       </c>
       <c r="E314" t="inlineStr">
         <is>
@@ -8208,16 +8208,16 @@
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>16:34</t>
+          <t>16:29</t>
         </is>
       </c>
       <c r="C315" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D315" t="n">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E315" t="inlineStr">
         <is>
@@ -8228,21 +8228,21 @@
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:19:35</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>16:36</t>
+          <t>16:29</t>
         </is>
       </c>
       <c r="C316" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D316" t="n">
-        <v>41</v>
+        <v>10</v>
       </c>
       <c r="E316" t="inlineStr">
         <is>
@@ -8253,21 +8253,21 @@
     <row r="317">
       <c r="A317" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>16:19:35</t>
         </is>
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>16:37</t>
+          <t>16:30</t>
         </is>
       </c>
       <c r="C317" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D317" t="n">
-        <v>76</v>
+        <v>11</v>
       </c>
       <c r="E317" t="inlineStr">
         <is>
@@ -8278,21 +8278,21 @@
     <row r="318">
       <c r="A318" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:19:35</t>
         </is>
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>16:39</t>
+          <t>16:34</t>
         </is>
       </c>
       <c r="C318" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D318" t="n">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="E318" t="inlineStr">
         <is>
@@ -8303,21 +8303,21 @@
     <row r="319">
       <c r="A319" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>16:19:35</t>
         </is>
       </c>
       <c r="B319" t="inlineStr">
         <is>
-          <t>16:40</t>
+          <t>16:36</t>
         </is>
       </c>
       <c r="C319" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D319" t="n">
-        <v>79</v>
+        <v>17</v>
       </c>
       <c r="E319" t="inlineStr">
         <is>
@@ -8328,21 +8328,21 @@
     <row r="320">
       <c r="A320" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B320" t="inlineStr">
         <is>
-          <t>16:42</t>
+          <t>16:37</t>
         </is>
       </c>
       <c r="C320" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D320" t="n">
-        <v>47</v>
+        <v>76</v>
       </c>
       <c r="E320" t="inlineStr">
         <is>
@@ -8358,16 +8358,16 @@
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>16:42</t>
+          <t>16:39</t>
         </is>
       </c>
       <c r="C321" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D321" t="n">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E321" t="inlineStr">
         <is>
@@ -8378,21 +8378,21 @@
     <row r="322">
       <c r="A322" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>16:19:35</t>
         </is>
       </c>
       <c r="B322" t="inlineStr">
         <is>
-          <t>16:43</t>
+          <t>16:40</t>
         </is>
       </c>
       <c r="C322" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D322" t="n">
-        <v>82</v>
+        <v>21</v>
       </c>
       <c r="E322" t="inlineStr">
         <is>
@@ -8403,12 +8403,12 @@
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
         <is>
-          <t>16:43</t>
+          <t>16:42</t>
         </is>
       </c>
       <c r="C323" t="inlineStr">
@@ -8417,7 +8417,7 @@
         </is>
       </c>
       <c r="D323" t="n">
-        <v>82</v>
+        <v>47</v>
       </c>
       <c r="E323" t="inlineStr">
         <is>
@@ -8428,21 +8428,21 @@
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:19:35</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>16:47</t>
+          <t>16:42</t>
         </is>
       </c>
       <c r="C324" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D324" t="n">
-        <v>52</v>
+        <v>23</v>
       </c>
       <c r="E324" t="inlineStr">
         <is>
@@ -8453,21 +8453,21 @@
     <row r="325">
       <c r="A325" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>16:19:35</t>
         </is>
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>16:48</t>
+          <t>16:43</t>
         </is>
       </c>
       <c r="C325" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D325" t="n">
-        <v>87</v>
+        <v>24</v>
       </c>
       <c r="E325" t="inlineStr">
         <is>
@@ -8478,21 +8478,21 @@
     <row r="326">
       <c r="A326" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>16:50</t>
+          <t>16:43</t>
         </is>
       </c>
       <c r="C326" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D326" t="n">
-        <v>55</v>
+        <v>82</v>
       </c>
       <c r="E326" t="inlineStr">
         <is>
@@ -8508,16 +8508,16 @@
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t>16:55</t>
+          <t>16:47</t>
         </is>
       </c>
       <c r="C327" t="inlineStr">
         <is>
-          <t>17_179 Y 38</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D327" t="n">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="E327" t="inlineStr">
         <is>
@@ -8528,21 +8528,21 @@
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>16:19:35</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
         <is>
-          <t>16:56</t>
+          <t>16:48</t>
         </is>
       </c>
       <c r="C328" t="inlineStr">
         <is>
-          <t>17_179 Y 38</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D328" t="n">
-        <v>95</v>
+        <v>29</v>
       </c>
       <c r="E328" t="inlineStr">
         <is>
@@ -8553,21 +8553,21 @@
     <row r="329">
       <c r="A329" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:19:35</t>
         </is>
       </c>
       <c r="B329" t="inlineStr">
         <is>
-          <t>17:04</t>
+          <t>16:50</t>
         </is>
       </c>
       <c r="C329" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D329" t="n">
-        <v>69</v>
+        <v>31</v>
       </c>
       <c r="E329" t="inlineStr">
         <is>
@@ -8583,16 +8583,16 @@
       </c>
       <c r="B330" t="inlineStr">
         <is>
-          <t>17:04</t>
+          <t>16:55</t>
         </is>
       </c>
       <c r="C330" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_179 Y 38</t>
         </is>
       </c>
       <c r="D330" t="n">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="E330" t="inlineStr">
         <is>
@@ -8603,21 +8603,21 @@
     <row r="331">
       <c r="A331" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>16:19:35</t>
         </is>
       </c>
       <c r="B331" t="inlineStr">
         <is>
-          <t>17:05</t>
+          <t>16:56</t>
         </is>
       </c>
       <c r="C331" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>17_179 Y 38</t>
         </is>
       </c>
       <c r="D331" t="n">
-        <v>104</v>
+        <v>37</v>
       </c>
       <c r="E331" t="inlineStr">
         <is>
@@ -8628,21 +8628,21 @@
     <row r="332">
       <c r="A332" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:19:35</t>
         </is>
       </c>
       <c r="B332" t="inlineStr">
         <is>
-          <t>17:20</t>
+          <t>16:57</t>
         </is>
       </c>
       <c r="C332" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D332" t="n">
-        <v>85</v>
+        <v>38</v>
       </c>
       <c r="E332" t="inlineStr">
         <is>
@@ -8653,21 +8653,21 @@
     <row r="333">
       <c r="A333" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:19:35</t>
         </is>
       </c>
       <c r="B333" t="inlineStr">
         <is>
-          <t>17:23</t>
+          <t>17:04</t>
         </is>
       </c>
       <c r="C333" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D333" t="n">
-        <v>88</v>
+        <v>45</v>
       </c>
       <c r="E333" t="inlineStr">
         <is>
@@ -8678,21 +8678,21 @@
     <row r="334">
       <c r="A334" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:19:35</t>
         </is>
       </c>
       <c r="B334" t="inlineStr">
         <is>
-          <t>17:28</t>
+          <t>17:04</t>
         </is>
       </c>
       <c r="C334" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D334" t="n">
-        <v>93</v>
+        <v>45</v>
       </c>
       <c r="E334" t="inlineStr">
         <is>
@@ -8703,21 +8703,21 @@
     <row r="335">
       <c r="A335" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B335" t="inlineStr">
         <is>
-          <t>17:31</t>
+          <t>17:05</t>
         </is>
       </c>
       <c r="C335" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D335" t="n">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="E335" t="inlineStr">
         <is>
@@ -8728,21 +8728,21 @@
     <row r="336">
       <c r="A336" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:19:35</t>
         </is>
       </c>
       <c r="B336" t="inlineStr">
         <is>
-          <t>17:39</t>
+          <t>17:16</t>
         </is>
       </c>
       <c r="C336" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D336" t="n">
-        <v>104</v>
+        <v>57</v>
       </c>
       <c r="E336" t="inlineStr">
         <is>
@@ -8758,16 +8758,16 @@
       </c>
       <c r="B337" t="inlineStr">
         <is>
-          <t>17:50</t>
+          <t>17:20</t>
         </is>
       </c>
       <c r="C337" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D337" t="n">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="E337" t="inlineStr">
         <is>
@@ -8778,23 +8778,323 @@
     <row r="338">
       <c r="A338" t="inlineStr">
         <is>
+          <t>16:19:35</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>17:20</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D338" t="n">
+        <v>61</v>
+      </c>
+      <c r="E338" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>16:19:35</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>17:21</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D339" t="n">
+        <v>62</v>
+      </c>
+      <c r="E339" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
           <t>15:55:57</t>
         </is>
       </c>
-      <c r="B338" t="inlineStr">
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>17:23</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D340" t="n">
+        <v>88</v>
+      </c>
+      <c r="E340" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>16:19:35</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>17:24</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D341" t="n">
+        <v>65</v>
+      </c>
+      <c r="E341" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>16:19:35</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>17:26</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D342" t="n">
+        <v>67</v>
+      </c>
+      <c r="E342" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>15:55:57</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>17:28</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D343" t="n">
+        <v>93</v>
+      </c>
+      <c r="E343" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>15:55:57</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>17:31</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D344" t="n">
+        <v>96</v>
+      </c>
+      <c r="E344" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>15:55:57</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>17:39</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D345" t="n">
+        <v>104</v>
+      </c>
+      <c r="E345" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>16:19:35</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>17:40</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D346" t="n">
+        <v>81</v>
+      </c>
+      <c r="E346" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>16:19:35</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>17:50</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D347" t="n">
+        <v>91</v>
+      </c>
+      <c r="E347" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>15:55:57</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
         <is>
           <t>17:51</t>
         </is>
       </c>
-      <c r="C338" t="inlineStr">
+      <c r="C348" t="inlineStr">
         <is>
           <t>81_EL PELIGRO</t>
         </is>
       </c>
-      <c r="D338" t="n">
+      <c r="D348" t="n">
         <v>116</v>
       </c>
-      <c r="E338" t="inlineStr">
+      <c r="E348" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>16:19:35</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>17:52</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D349" t="n">
+        <v>93</v>
+      </c>
+      <c r="E349" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>16:19:35</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>18:04</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D350" t="n">
+        <v>105</v>
+      </c>
+      <c r="E350" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -8811,7 +9111,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8829,14 +9129,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 15:55:57</t>
+          <t>Última actualización: 16:19:36</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 40</t>
+          <t>Total filas: 41</t>
         </is>
       </c>
     </row>
@@ -9770,7 +10070,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>16:19:35</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -9784,7 +10084,7 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -9795,7 +10095,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:19:35</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -9809,7 +10109,7 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -9862,6 +10162,31 @@
         <v>104</v>
       </c>
       <c r="E45" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>16:19:35</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>17:40</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>81</v>
+      </c>
+      <c r="E46" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -9878,7 +10203,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9896,14 +10221,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 15:55:57</t>
+          <t>Última actualización: 16:19:36</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 45</t>
+          <t>Total filas: 46</t>
         </is>
       </c>
     </row>
@@ -11012,7 +11337,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>16:19:35</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -11026,7 +11351,7 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>92</v>
+        <v>34</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -11037,7 +11362,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:19:35</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -11051,11 +11376,36 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>79</v>
+        <v>55</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
           <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>16:19:35</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>18:03</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>104</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 847
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-23.xlsx
+++ b/data/horarios-141-2026-01-23.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E350"/>
+  <dimension ref="A1:E359"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:19:36</t>
+          <t>Última actualización: 16:36:35</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 345</t>
+          <t>Total filas: 354</t>
         </is>
       </c>
     </row>
@@ -1513,7 +1513,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -1538,7 +1538,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -1628,7 +1628,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1638,11 +1638,11 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>6</v>
+        <v>73</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -1653,7 +1653,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1663,11 +1663,11 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>73</v>
+        <v>6</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -1953,7 +1953,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1963,11 +1963,11 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -1978,7 +1978,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -1988,11 +1988,11 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2013,7 +2013,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D67" t="n">
@@ -2213,7 +2213,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D75" t="n">
@@ -2238,7 +2238,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D76" t="n">
@@ -2803,7 +2803,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -2813,11 +2813,11 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D99" t="n">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -2828,7 +2828,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -2838,11 +2838,11 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -3338,7 +3338,7 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D120" t="n">
@@ -3363,7 +3363,7 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D121" t="n">
@@ -4163,7 +4163,7 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D153" t="n">
@@ -4188,7 +4188,7 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D154" t="n">
@@ -5063,7 +5063,7 @@
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D189" t="n">
@@ -5088,7 +5088,7 @@
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D190" t="n">
@@ -5653,7 +5653,7 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>12:54:24</t>
+          <t>12:37:00</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
@@ -5663,11 +5663,11 @@
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D213" t="n">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -5678,7 +5678,7 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>12:54:24</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
@@ -5688,11 +5688,11 @@
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D214" t="n">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
@@ -5813,7 +5813,7 @@
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D219" t="n">
@@ -5838,7 +5838,7 @@
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D220" t="n">
@@ -5988,7 +5988,7 @@
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D226" t="n">
@@ -6013,7 +6013,7 @@
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D227" t="n">
@@ -6138,7 +6138,7 @@
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D232" t="n">
@@ -6163,7 +6163,7 @@
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D233" t="n">
@@ -6188,7 +6188,7 @@
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D234" t="n">
@@ -6213,7 +6213,7 @@
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D235" t="n">
@@ -6238,7 +6238,7 @@
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D236" t="n">
@@ -6263,7 +6263,7 @@
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D237" t="n">
@@ -6403,7 +6403,7 @@
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>13:51:20</t>
+          <t>13:18:32</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
@@ -6413,11 +6413,11 @@
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D243" t="n">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -6428,7 +6428,7 @@
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>13:18:32</t>
+          <t>13:51:20</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
@@ -6438,11 +6438,11 @@
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D244" t="n">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -7238,7 +7238,7 @@
       </c>
       <c r="C276" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D276" t="n">
@@ -7263,7 +7263,7 @@
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D277" t="n">
@@ -7553,7 +7553,7 @@
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>14:19:39</t>
+          <t>14:55:42</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
@@ -7563,11 +7563,11 @@
       </c>
       <c r="C289" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D289" t="n">
-        <v>94</v>
+        <v>58</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
@@ -7578,7 +7578,7 @@
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>14:55:42</t>
+          <t>14:19:39</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
@@ -7588,11 +7588,11 @@
       </c>
       <c r="C290" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D290" t="n">
-        <v>58</v>
+        <v>94</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
@@ -7678,7 +7678,7 @@
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
@@ -7688,11 +7688,11 @@
       </c>
       <c r="C294" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D294" t="n">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
@@ -7703,7 +7703,7 @@
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
@@ -7713,11 +7713,11 @@
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D295" t="n">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
@@ -7728,7 +7728,7 @@
     <row r="296">
       <c r="A296" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
@@ -7738,11 +7738,11 @@
       </c>
       <c r="C296" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D296" t="n">
-        <v>36</v>
+        <v>2</v>
       </c>
       <c r="E296" t="inlineStr">
         <is>
@@ -7753,7 +7753,7 @@
     <row r="297">
       <c r="A297" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
@@ -7763,11 +7763,11 @@
       </c>
       <c r="C297" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D297" t="n">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="E297" t="inlineStr">
         <is>
@@ -7853,7 +7853,7 @@
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>14:45:15</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
@@ -7863,11 +7863,11 @@
       </c>
       <c r="C301" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D301" t="n">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="E301" t="inlineStr">
         <is>
@@ -7878,7 +7878,7 @@
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>14:45:15</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
@@ -7888,11 +7888,11 @@
       </c>
       <c r="C302" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D302" t="n">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="E302" t="inlineStr">
         <is>
@@ -7963,7 +7963,7 @@
       </c>
       <c r="C305" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D305" t="n">
@@ -7988,7 +7988,7 @@
       </c>
       <c r="C306" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>225_C ROCA-H SUR</t>
         </is>
       </c>
       <c r="D306" t="n">
@@ -8053,7 +8053,7 @@
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:19:35</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
@@ -8063,11 +8063,11 @@
       </c>
       <c r="C309" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D309" t="n">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
@@ -8088,7 +8088,7 @@
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D310" t="n">
@@ -8103,7 +8103,7 @@
     <row r="311">
       <c r="A311" t="inlineStr">
         <is>
-          <t>16:19:35</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
@@ -8113,11 +8113,11 @@
       </c>
       <c r="C311" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D311" t="n">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="E311" t="inlineStr">
         <is>
@@ -8203,7 +8203,7 @@
     <row r="315">
       <c r="A315" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:19:35</t>
         </is>
       </c>
       <c r="B315" t="inlineStr">
@@ -8213,11 +8213,11 @@
       </c>
       <c r="C315" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D315" t="n">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="E315" t="inlineStr">
         <is>
@@ -8228,7 +8228,7 @@
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
-          <t>16:19:35</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
@@ -8238,11 +8238,11 @@
       </c>
       <c r="C316" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D316" t="n">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="E316" t="inlineStr">
         <is>
@@ -8378,7 +8378,7 @@
     <row r="322">
       <c r="A322" t="inlineStr">
         <is>
-          <t>16:19:35</t>
+          <t>16:36:35</t>
         </is>
       </c>
       <c r="B322" t="inlineStr">
@@ -8392,7 +8392,7 @@
         </is>
       </c>
       <c r="D322" t="n">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="E322" t="inlineStr">
         <is>
@@ -8403,7 +8403,7 @@
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:36:35</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
@@ -8413,11 +8413,11 @@
       </c>
       <c r="C323" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D323" t="n">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="E323" t="inlineStr">
         <is>
@@ -8428,7 +8428,7 @@
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>16:19:35</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
@@ -8438,11 +8438,11 @@
       </c>
       <c r="C324" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D324" t="n">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="E324" t="inlineStr">
         <is>
@@ -8453,7 +8453,7 @@
     <row r="325">
       <c r="A325" t="inlineStr">
         <is>
-          <t>16:19:35</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B325" t="inlineStr">
@@ -8463,11 +8463,11 @@
       </c>
       <c r="C325" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D325" t="n">
-        <v>24</v>
+        <v>82</v>
       </c>
       <c r="E325" t="inlineStr">
         <is>
@@ -8478,7 +8478,7 @@
     <row r="326">
       <c r="A326" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>16:36:35</t>
         </is>
       </c>
       <c r="B326" t="inlineStr">
@@ -8488,11 +8488,11 @@
       </c>
       <c r="C326" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D326" t="n">
-        <v>82</v>
+        <v>7</v>
       </c>
       <c r="E326" t="inlineStr">
         <is>
@@ -8528,7 +8528,7 @@
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>16:19:35</t>
+          <t>16:36:35</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
@@ -8542,7 +8542,7 @@
         </is>
       </c>
       <c r="D328" t="n">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="E328" t="inlineStr">
         <is>
@@ -8553,7 +8553,7 @@
     <row r="329">
       <c r="A329" t="inlineStr">
         <is>
-          <t>16:19:35</t>
+          <t>16:36:35</t>
         </is>
       </c>
       <c r="B329" t="inlineStr">
@@ -8567,7 +8567,7 @@
         </is>
       </c>
       <c r="D329" t="n">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="E329" t="inlineStr">
         <is>
@@ -8603,7 +8603,7 @@
     <row r="331">
       <c r="A331" t="inlineStr">
         <is>
-          <t>16:19:35</t>
+          <t>16:36:35</t>
         </is>
       </c>
       <c r="B331" t="inlineStr">
@@ -8617,7 +8617,7 @@
         </is>
       </c>
       <c r="D331" t="n">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="E331" t="inlineStr">
         <is>
@@ -8628,7 +8628,7 @@
     <row r="332">
       <c r="A332" t="inlineStr">
         <is>
-          <t>16:19:35</t>
+          <t>16:36:35</t>
         </is>
       </c>
       <c r="B332" t="inlineStr">
@@ -8642,7 +8642,7 @@
         </is>
       </c>
       <c r="D332" t="n">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="E332" t="inlineStr">
         <is>
@@ -8653,7 +8653,7 @@
     <row r="333">
       <c r="A333" t="inlineStr">
         <is>
-          <t>16:19:35</t>
+          <t>16:36:35</t>
         </is>
       </c>
       <c r="B333" t="inlineStr">
@@ -8667,7 +8667,7 @@
         </is>
       </c>
       <c r="D333" t="n">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="E333" t="inlineStr">
         <is>
@@ -8678,7 +8678,7 @@
     <row r="334">
       <c r="A334" t="inlineStr">
         <is>
-          <t>16:19:35</t>
+          <t>16:36:35</t>
         </is>
       </c>
       <c r="B334" t="inlineStr">
@@ -8692,7 +8692,7 @@
         </is>
       </c>
       <c r="D334" t="n">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="E334" t="inlineStr">
         <is>
@@ -8728,21 +8728,21 @@
     <row r="336">
       <c r="A336" t="inlineStr">
         <is>
-          <t>16:19:35</t>
+          <t>16:36:35</t>
         </is>
       </c>
       <c r="B336" t="inlineStr">
         <is>
-          <t>17:16</t>
+          <t>17:10</t>
         </is>
       </c>
       <c r="C336" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D336" t="n">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="E336" t="inlineStr">
         <is>
@@ -8753,21 +8753,21 @@
     <row r="337">
       <c r="A337" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:36:35</t>
         </is>
       </c>
       <c r="B337" t="inlineStr">
         <is>
-          <t>17:20</t>
+          <t>17:16</t>
         </is>
       </c>
       <c r="C337" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D337" t="n">
-        <v>85</v>
+        <v>40</v>
       </c>
       <c r="E337" t="inlineStr">
         <is>
@@ -8778,21 +8778,21 @@
     <row r="338">
       <c r="A338" t="inlineStr">
         <is>
-          <t>16:19:35</t>
+          <t>16:36:35</t>
         </is>
       </c>
       <c r="B338" t="inlineStr">
         <is>
-          <t>17:20</t>
+          <t>17:16</t>
         </is>
       </c>
       <c r="C338" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D338" t="n">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="E338" t="inlineStr">
         <is>
@@ -8803,12 +8803,12 @@
     <row r="339">
       <c r="A339" t="inlineStr">
         <is>
-          <t>16:19:35</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B339" t="inlineStr">
         <is>
-          <t>17:21</t>
+          <t>17:20</t>
         </is>
       </c>
       <c r="C339" t="inlineStr">
@@ -8817,7 +8817,7 @@
         </is>
       </c>
       <c r="D339" t="n">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="E339" t="inlineStr">
         <is>
@@ -8828,21 +8828,21 @@
     <row r="340">
       <c r="A340" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:36:35</t>
         </is>
       </c>
       <c r="B340" t="inlineStr">
         <is>
-          <t>17:23</t>
+          <t>17:20</t>
         </is>
       </c>
       <c r="C340" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D340" t="n">
-        <v>88</v>
+        <v>44</v>
       </c>
       <c r="E340" t="inlineStr">
         <is>
@@ -8853,21 +8853,21 @@
     <row r="341">
       <c r="A341" t="inlineStr">
         <is>
-          <t>16:19:35</t>
+          <t>16:36:35</t>
         </is>
       </c>
       <c r="B341" t="inlineStr">
         <is>
-          <t>17:24</t>
+          <t>17:21</t>
         </is>
       </c>
       <c r="C341" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D341" t="n">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="E341" t="inlineStr">
         <is>
@@ -8878,21 +8878,21 @@
     <row r="342">
       <c r="A342" t="inlineStr">
         <is>
-          <t>16:19:35</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B342" t="inlineStr">
         <is>
-          <t>17:26</t>
+          <t>17:23</t>
         </is>
       </c>
       <c r="C342" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D342" t="n">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="E342" t="inlineStr">
         <is>
@@ -8903,21 +8903,21 @@
     <row r="343">
       <c r="A343" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:36:35</t>
         </is>
       </c>
       <c r="B343" t="inlineStr">
         <is>
-          <t>17:28</t>
+          <t>17:24</t>
         </is>
       </c>
       <c r="C343" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D343" t="n">
-        <v>93</v>
+        <v>48</v>
       </c>
       <c r="E343" t="inlineStr">
         <is>
@@ -8928,12 +8928,12 @@
     <row r="344">
       <c r="A344" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:19:35</t>
         </is>
       </c>
       <c r="B344" t="inlineStr">
         <is>
-          <t>17:31</t>
+          <t>17:26</t>
         </is>
       </c>
       <c r="C344" t="inlineStr">
@@ -8942,7 +8942,7 @@
         </is>
       </c>
       <c r="D344" t="n">
-        <v>96</v>
+        <v>67</v>
       </c>
       <c r="E344" t="inlineStr">
         <is>
@@ -8953,21 +8953,21 @@
     <row r="345">
       <c r="A345" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:36:35</t>
         </is>
       </c>
       <c r="B345" t="inlineStr">
         <is>
-          <t>17:39</t>
+          <t>17:28</t>
         </is>
       </c>
       <c r="C345" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D345" t="n">
-        <v>104</v>
+        <v>52</v>
       </c>
       <c r="E345" t="inlineStr">
         <is>
@@ -8978,21 +8978,21 @@
     <row r="346">
       <c r="A346" t="inlineStr">
         <is>
-          <t>16:19:35</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B346" t="inlineStr">
         <is>
-          <t>17:40</t>
+          <t>17:31</t>
         </is>
       </c>
       <c r="C346" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D346" t="n">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="E346" t="inlineStr">
         <is>
@@ -9003,21 +9003,21 @@
     <row r="347">
       <c r="A347" t="inlineStr">
         <is>
-          <t>16:19:35</t>
+          <t>16:36:35</t>
         </is>
       </c>
       <c r="B347" t="inlineStr">
         <is>
-          <t>17:50</t>
+          <t>17:34</t>
         </is>
       </c>
       <c r="C347" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D347" t="n">
-        <v>91</v>
+        <v>58</v>
       </c>
       <c r="E347" t="inlineStr">
         <is>
@@ -9028,21 +9028,21 @@
     <row r="348">
       <c r="A348" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:36:35</t>
         </is>
       </c>
       <c r="B348" t="inlineStr">
         <is>
-          <t>17:51</t>
+          <t>17:36</t>
         </is>
       </c>
       <c r="C348" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D348" t="n">
-        <v>116</v>
+        <v>60</v>
       </c>
       <c r="E348" t="inlineStr">
         <is>
@@ -9053,21 +9053,21 @@
     <row r="349">
       <c r="A349" t="inlineStr">
         <is>
-          <t>16:19:35</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B349" t="inlineStr">
         <is>
-          <t>17:52</t>
+          <t>17:39</t>
         </is>
       </c>
       <c r="C349" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D349" t="n">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="E349" t="inlineStr">
         <is>
@@ -9078,23 +9078,248 @@
     <row r="350">
       <c r="A350" t="inlineStr">
         <is>
-          <t>16:19:35</t>
+          <t>16:36:35</t>
         </is>
       </c>
       <c r="B350" t="inlineStr">
         <is>
+          <t>17:40</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D350" t="n">
+        <v>64</v>
+      </c>
+      <c r="E350" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>16:36:35</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>17:40</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D351" t="n">
+        <v>64</v>
+      </c>
+      <c r="E351" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>16:36:35</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>17:45</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D352" t="n">
+        <v>69</v>
+      </c>
+      <c r="E352" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>16:36:35</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>17:50</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D353" t="n">
+        <v>74</v>
+      </c>
+      <c r="E353" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>15:55:57</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>17:51</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D354" t="n">
+        <v>116</v>
+      </c>
+      <c r="E354" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>16:36:35</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>17:52</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D355" t="n">
+        <v>76</v>
+      </c>
+      <c r="E355" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>16:36:35</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
           <t>18:04</t>
         </is>
       </c>
-      <c r="C350" t="inlineStr">
+      <c r="C356" t="inlineStr">
         <is>
           <t>17_ROMERO</t>
         </is>
       </c>
-      <c r="D350" t="n">
+      <c r="D356" t="n">
+        <v>88</v>
+      </c>
+      <c r="E356" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>16:36:35</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>18:21</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D357" t="n">
         <v>105</v>
       </c>
-      <c r="E350" t="inlineStr">
+      <c r="E357" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>16:36:35</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>18:28</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D358" t="n">
+        <v>112</v>
+      </c>
+      <c r="E358" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>16:36:35</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>18:32</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D359" t="n">
+        <v>116</v>
+      </c>
+      <c r="E359" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -9111,7 +9336,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E46"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9129,14 +9354,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:19:36</t>
+          <t>Última actualización: 16:36:35</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 41</t>
+          <t>Total filas: 42</t>
         </is>
       </c>
     </row>
@@ -10095,7 +10320,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>16:19:35</t>
+          <t>16:36:35</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -10109,7 +10334,7 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -10170,7 +10395,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>16:19:35</t>
+          <t>16:36:35</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -10184,9 +10409,34 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="E46" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>16:36:35</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>18:28</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>112</v>
+      </c>
+      <c r="E47" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -10221,7 +10471,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:19:36</t>
+          <t>Última actualización: 16:36:35</t>
         </is>
       </c>
     </row>
@@ -11337,7 +11587,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>16:19:35</t>
+          <t>16:36:35</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -11351,7 +11601,7 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -11362,7 +11612,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>16:19:35</t>
+          <t>16:36:35</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -11376,7 +11626,7 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -11387,7 +11637,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>16:19:35</t>
+          <t>16:36:35</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -11401,7 +11651,7 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>104</v>
+        <v>87</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 848
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-23.xlsx
+++ b/data/horarios-141-2026-01-23.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E359"/>
+  <dimension ref="A1:E362"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:36:35</t>
+          <t>Última actualización: 16:46:26</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 354</t>
+          <t>Total filas: 357</t>
         </is>
       </c>
     </row>
@@ -1513,7 +1513,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -1538,7 +1538,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -1628,7 +1628,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1638,11 +1638,11 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>73</v>
+        <v>6</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -1653,7 +1653,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1663,11 +1663,11 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>6</v>
+        <v>73</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -1778,7 +1778,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1788,11 +1788,11 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -1803,7 +1803,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1813,11 +1813,11 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>17</v>
+        <v>84</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D63" t="n">
@@ -1938,7 +1938,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -1988,7 +1988,7 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D66" t="n">
@@ -2013,7 +2013,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D67" t="n">
@@ -2128,7 +2128,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -2138,11 +2138,11 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -2153,7 +2153,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -2163,11 +2163,11 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D73" t="n">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -2213,7 +2213,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D75" t="n">
@@ -2238,7 +2238,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D76" t="n">
@@ -2528,7 +2528,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -2538,11 +2538,11 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -2553,7 +2553,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2563,11 +2563,11 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -2803,7 +2803,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -2813,11 +2813,11 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D99" t="n">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -2828,7 +2828,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -2838,11 +2838,11 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -3153,7 +3153,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3163,11 +3163,11 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>27</v>
+        <v>115</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3203,7 +3203,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
@@ -3213,11 +3213,11 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D115" t="n">
-        <v>115</v>
+        <v>27</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -3338,7 +3338,7 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D120" t="n">
@@ -3363,7 +3363,7 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D121" t="n">
@@ -4163,7 +4163,7 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D153" t="n">
@@ -4188,7 +4188,7 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D154" t="n">
@@ -4928,7 +4928,7 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>10:57:35</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
@@ -4938,11 +4938,11 @@
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D184" t="n">
-        <v>12</v>
+        <v>77</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -4953,7 +4953,7 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>10:57:35</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
@@ -4963,11 +4963,11 @@
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D185" t="n">
-        <v>77</v>
+        <v>12</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -5003,7 +5003,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>10:27:29</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
@@ -5013,11 +5013,11 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D187" t="n">
-        <v>110</v>
+        <v>15</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -5028,7 +5028,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>10:27:29</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -5038,11 +5038,11 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D188" t="n">
-        <v>15</v>
+        <v>110</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5288,7 +5288,7 @@
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_179 Y 38</t>
         </is>
       </c>
       <c r="D198" t="n">
@@ -5313,7 +5313,7 @@
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>17_179 Y 38</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D199" t="n">
@@ -5338,7 +5338,7 @@
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D200" t="n">
@@ -6138,7 +6138,7 @@
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D232" t="n">
@@ -6163,7 +6163,7 @@
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D233" t="n">
@@ -6188,7 +6188,7 @@
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D234" t="n">
@@ -6213,7 +6213,7 @@
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D235" t="n">
@@ -6313,7 +6313,7 @@
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D239" t="n">
@@ -6338,7 +6338,7 @@
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D240" t="n">
@@ -7013,7 +7013,7 @@
       </c>
       <c r="C267" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D267" t="n">
@@ -7038,7 +7038,7 @@
       </c>
       <c r="C268" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D268" t="n">
@@ -7478,7 +7478,7 @@
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>14:55:42</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
@@ -7488,11 +7488,11 @@
       </c>
       <c r="C286" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D286" t="n">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
@@ -7503,7 +7503,7 @@
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>14:55:42</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
@@ -7513,11 +7513,11 @@
       </c>
       <c r="C287" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D287" t="n">
-        <v>51</v>
+        <v>25</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
@@ -7553,7 +7553,7 @@
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>14:55:42</t>
+          <t>14:19:39</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
@@ -7563,11 +7563,11 @@
       </c>
       <c r="C289" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D289" t="n">
-        <v>58</v>
+        <v>94</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
@@ -7578,7 +7578,7 @@
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>14:19:39</t>
+          <t>14:55:42</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
@@ -7588,11 +7588,11 @@
       </c>
       <c r="C290" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D290" t="n">
-        <v>94</v>
+        <v>58</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
@@ -7678,7 +7678,7 @@
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
@@ -7688,11 +7688,11 @@
       </c>
       <c r="C294" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D294" t="n">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
@@ -7703,7 +7703,7 @@
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
@@ -7713,11 +7713,11 @@
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D295" t="n">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
@@ -7853,7 +7853,7 @@
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>14:45:15</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
@@ -7863,11 +7863,11 @@
       </c>
       <c r="C301" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D301" t="n">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="E301" t="inlineStr">
         <is>
@@ -7878,7 +7878,7 @@
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>14:45:15</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
@@ -7888,11 +7888,11 @@
       </c>
       <c r="C302" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D302" t="n">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="E302" t="inlineStr">
         <is>
@@ -7963,7 +7963,7 @@
       </c>
       <c r="C305" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>225_C ROCA-H SUR</t>
         </is>
       </c>
       <c r="D305" t="n">
@@ -7988,7 +7988,7 @@
       </c>
       <c r="C306" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D306" t="n">
@@ -8063,7 +8063,7 @@
       </c>
       <c r="C309" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D309" t="n">
@@ -8088,7 +8088,7 @@
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D310" t="n">
@@ -8203,7 +8203,7 @@
     <row r="315">
       <c r="A315" t="inlineStr">
         <is>
-          <t>16:19:35</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B315" t="inlineStr">
@@ -8213,11 +8213,11 @@
       </c>
       <c r="C315" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D315" t="n">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="E315" t="inlineStr">
         <is>
@@ -8228,7 +8228,7 @@
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:19:35</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
@@ -8238,11 +8238,11 @@
       </c>
       <c r="C316" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D316" t="n">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="E316" t="inlineStr">
         <is>
@@ -8403,7 +8403,7 @@
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>16:36:35</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
@@ -8413,11 +8413,11 @@
       </c>
       <c r="C323" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D323" t="n">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="E323" t="inlineStr">
         <is>
@@ -8428,7 +8428,7 @@
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:36:35</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
@@ -8438,11 +8438,11 @@
       </c>
       <c r="C324" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D324" t="n">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="E324" t="inlineStr">
         <is>
@@ -8528,7 +8528,7 @@
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>16:36:35</t>
+          <t>16:46:26</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
@@ -8538,11 +8538,11 @@
       </c>
       <c r="C328" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D328" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="E328" t="inlineStr">
         <is>
@@ -8558,16 +8558,16 @@
       </c>
       <c r="B329" t="inlineStr">
         <is>
-          <t>16:50</t>
+          <t>16:48</t>
         </is>
       </c>
       <c r="C329" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D329" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E329" t="inlineStr">
         <is>
@@ -8578,21 +8578,21 @@
     <row r="330">
       <c r="A330" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:36:35</t>
         </is>
       </c>
       <c r="B330" t="inlineStr">
         <is>
-          <t>16:55</t>
+          <t>16:50</t>
         </is>
       </c>
       <c r="C330" t="inlineStr">
         <is>
-          <t>17_179 Y 38</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D330" t="n">
-        <v>60</v>
+        <v>14</v>
       </c>
       <c r="E330" t="inlineStr">
         <is>
@@ -8603,12 +8603,12 @@
     <row r="331">
       <c r="A331" t="inlineStr">
         <is>
-          <t>16:36:35</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B331" t="inlineStr">
         <is>
-          <t>16:56</t>
+          <t>16:55</t>
         </is>
       </c>
       <c r="C331" t="inlineStr">
@@ -8617,7 +8617,7 @@
         </is>
       </c>
       <c r="D331" t="n">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E331" t="inlineStr">
         <is>
@@ -8628,21 +8628,21 @@
     <row r="332">
       <c r="A332" t="inlineStr">
         <is>
-          <t>16:36:35</t>
+          <t>16:46:26</t>
         </is>
       </c>
       <c r="B332" t="inlineStr">
         <is>
-          <t>16:57</t>
+          <t>16:56</t>
         </is>
       </c>
       <c r="C332" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_179 Y 38</t>
         </is>
       </c>
       <c r="D332" t="n">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="E332" t="inlineStr">
         <is>
@@ -8653,21 +8653,21 @@
     <row r="333">
       <c r="A333" t="inlineStr">
         <is>
-          <t>16:36:35</t>
+          <t>16:46:26</t>
         </is>
       </c>
       <c r="B333" t="inlineStr">
         <is>
-          <t>17:04</t>
+          <t>16:57</t>
         </is>
       </c>
       <c r="C333" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D333" t="n">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="E333" t="inlineStr">
         <is>
@@ -8678,7 +8678,7 @@
     <row r="334">
       <c r="A334" t="inlineStr">
         <is>
-          <t>16:36:35</t>
+          <t>16:46:26</t>
         </is>
       </c>
       <c r="B334" t="inlineStr">
@@ -8692,7 +8692,7 @@
         </is>
       </c>
       <c r="D334" t="n">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="E334" t="inlineStr">
         <is>
@@ -8703,21 +8703,21 @@
     <row r="335">
       <c r="A335" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>16:46:26</t>
         </is>
       </c>
       <c r="B335" t="inlineStr">
         <is>
-          <t>17:05</t>
+          <t>17:04</t>
         </is>
       </c>
       <c r="C335" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D335" t="n">
-        <v>104</v>
+        <v>18</v>
       </c>
       <c r="E335" t="inlineStr">
         <is>
@@ -8728,21 +8728,21 @@
     <row r="336">
       <c r="A336" t="inlineStr">
         <is>
-          <t>16:36:35</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B336" t="inlineStr">
         <is>
-          <t>17:10</t>
+          <t>17:05</t>
         </is>
       </c>
       <c r="C336" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D336" t="n">
-        <v>34</v>
+        <v>104</v>
       </c>
       <c r="E336" t="inlineStr">
         <is>
@@ -8753,21 +8753,21 @@
     <row r="337">
       <c r="A337" t="inlineStr">
         <is>
-          <t>16:36:35</t>
+          <t>16:46:26</t>
         </is>
       </c>
       <c r="B337" t="inlineStr">
         <is>
-          <t>17:16</t>
+          <t>17:10</t>
         </is>
       </c>
       <c r="C337" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D337" t="n">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="E337" t="inlineStr">
         <is>
@@ -8778,7 +8778,7 @@
     <row r="338">
       <c r="A338" t="inlineStr">
         <is>
-          <t>16:36:35</t>
+          <t>16:46:26</t>
         </is>
       </c>
       <c r="B338" t="inlineStr">
@@ -8788,11 +8788,11 @@
       </c>
       <c r="C338" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D338" t="n">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="E338" t="inlineStr">
         <is>
@@ -8803,21 +8803,21 @@
     <row r="339">
       <c r="A339" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:46:26</t>
         </is>
       </c>
       <c r="B339" t="inlineStr">
         <is>
-          <t>17:20</t>
+          <t>17:16</t>
         </is>
       </c>
       <c r="C339" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D339" t="n">
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="E339" t="inlineStr">
         <is>
@@ -8828,7 +8828,7 @@
     <row r="340">
       <c r="A340" t="inlineStr">
         <is>
-          <t>16:36:35</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B340" t="inlineStr">
@@ -8838,11 +8838,11 @@
       </c>
       <c r="C340" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D340" t="n">
-        <v>44</v>
+        <v>85</v>
       </c>
       <c r="E340" t="inlineStr">
         <is>
@@ -8853,21 +8853,21 @@
     <row r="341">
       <c r="A341" t="inlineStr">
         <is>
-          <t>16:36:35</t>
+          <t>16:46:26</t>
         </is>
       </c>
       <c r="B341" t="inlineStr">
         <is>
-          <t>17:21</t>
+          <t>17:20</t>
         </is>
       </c>
       <c r="C341" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D341" t="n">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="E341" t="inlineStr">
         <is>
@@ -8878,21 +8878,21 @@
     <row r="342">
       <c r="A342" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:46:26</t>
         </is>
       </c>
       <c r="B342" t="inlineStr">
         <is>
-          <t>17:23</t>
+          <t>17:21</t>
         </is>
       </c>
       <c r="C342" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D342" t="n">
-        <v>88</v>
+        <v>35</v>
       </c>
       <c r="E342" t="inlineStr">
         <is>
@@ -8903,12 +8903,12 @@
     <row r="343">
       <c r="A343" t="inlineStr">
         <is>
-          <t>16:36:35</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B343" t="inlineStr">
         <is>
-          <t>17:24</t>
+          <t>17:23</t>
         </is>
       </c>
       <c r="C343" t="inlineStr">
@@ -8917,7 +8917,7 @@
         </is>
       </c>
       <c r="D343" t="n">
-        <v>48</v>
+        <v>88</v>
       </c>
       <c r="E343" t="inlineStr">
         <is>
@@ -8928,21 +8928,21 @@
     <row r="344">
       <c r="A344" t="inlineStr">
         <is>
-          <t>16:19:35</t>
+          <t>16:46:26</t>
         </is>
       </c>
       <c r="B344" t="inlineStr">
         <is>
-          <t>17:26</t>
+          <t>17:24</t>
         </is>
       </c>
       <c r="C344" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D344" t="n">
-        <v>67</v>
+        <v>38</v>
       </c>
       <c r="E344" t="inlineStr">
         <is>
@@ -8953,21 +8953,21 @@
     <row r="345">
       <c r="A345" t="inlineStr">
         <is>
-          <t>16:36:35</t>
+          <t>16:19:35</t>
         </is>
       </c>
       <c r="B345" t="inlineStr">
         <is>
-          <t>17:28</t>
+          <t>17:26</t>
         </is>
       </c>
       <c r="C345" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D345" t="n">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="E345" t="inlineStr">
         <is>
@@ -8978,21 +8978,21 @@
     <row r="346">
       <c r="A346" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:46:26</t>
         </is>
       </c>
       <c r="B346" t="inlineStr">
         <is>
-          <t>17:31</t>
+          <t>17:28</t>
         </is>
       </c>
       <c r="C346" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D346" t="n">
-        <v>96</v>
+        <v>42</v>
       </c>
       <c r="E346" t="inlineStr">
         <is>
@@ -9003,21 +9003,21 @@
     <row r="347">
       <c r="A347" t="inlineStr">
         <is>
-          <t>16:36:35</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B347" t="inlineStr">
         <is>
-          <t>17:34</t>
+          <t>17:31</t>
         </is>
       </c>
       <c r="C347" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D347" t="n">
-        <v>58</v>
+        <v>96</v>
       </c>
       <c r="E347" t="inlineStr">
         <is>
@@ -9028,21 +9028,21 @@
     <row r="348">
       <c r="A348" t="inlineStr">
         <is>
-          <t>16:36:35</t>
+          <t>16:46:26</t>
         </is>
       </c>
       <c r="B348" t="inlineStr">
         <is>
-          <t>17:36</t>
+          <t>17:34</t>
         </is>
       </c>
       <c r="C348" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D348" t="n">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="E348" t="inlineStr">
         <is>
@@ -9053,21 +9053,21 @@
     <row r="349">
       <c r="A349" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:46:26</t>
         </is>
       </c>
       <c r="B349" t="inlineStr">
         <is>
-          <t>17:39</t>
+          <t>17:36</t>
         </is>
       </c>
       <c r="C349" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D349" t="n">
-        <v>104</v>
+        <v>50</v>
       </c>
       <c r="E349" t="inlineStr">
         <is>
@@ -9078,21 +9078,21 @@
     <row r="350">
       <c r="A350" t="inlineStr">
         <is>
-          <t>16:36:35</t>
+          <t>16:46:26</t>
         </is>
       </c>
       <c r="B350" t="inlineStr">
         <is>
-          <t>17:40</t>
+          <t>17:38</t>
         </is>
       </c>
       <c r="C350" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D350" t="n">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="E350" t="inlineStr">
         <is>
@@ -9103,21 +9103,21 @@
     <row r="351">
       <c r="A351" t="inlineStr">
         <is>
-          <t>16:36:35</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B351" t="inlineStr">
         <is>
-          <t>17:40</t>
+          <t>17:39</t>
         </is>
       </c>
       <c r="C351" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D351" t="n">
-        <v>64</v>
+        <v>104</v>
       </c>
       <c r="E351" t="inlineStr">
         <is>
@@ -9128,21 +9128,21 @@
     <row r="352">
       <c r="A352" t="inlineStr">
         <is>
-          <t>16:36:35</t>
+          <t>16:46:26</t>
         </is>
       </c>
       <c r="B352" t="inlineStr">
         <is>
-          <t>17:45</t>
+          <t>17:40</t>
         </is>
       </c>
       <c r="C352" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D352" t="n">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="E352" t="inlineStr">
         <is>
@@ -9153,21 +9153,21 @@
     <row r="353">
       <c r="A353" t="inlineStr">
         <is>
-          <t>16:36:35</t>
+          <t>16:46:26</t>
         </is>
       </c>
       <c r="B353" t="inlineStr">
         <is>
-          <t>17:50</t>
+          <t>17:40</t>
         </is>
       </c>
       <c r="C353" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D353" t="n">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="E353" t="inlineStr">
         <is>
@@ -9178,21 +9178,21 @@
     <row r="354">
       <c r="A354" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:46:26</t>
         </is>
       </c>
       <c r="B354" t="inlineStr">
         <is>
-          <t>17:51</t>
+          <t>17:45</t>
         </is>
       </c>
       <c r="C354" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D354" t="n">
-        <v>116</v>
+        <v>59</v>
       </c>
       <c r="E354" t="inlineStr">
         <is>
@@ -9203,21 +9203,21 @@
     <row r="355">
       <c r="A355" t="inlineStr">
         <is>
-          <t>16:36:35</t>
+          <t>16:46:26</t>
         </is>
       </c>
       <c r="B355" t="inlineStr">
         <is>
-          <t>17:52</t>
+          <t>17:50</t>
         </is>
       </c>
       <c r="C355" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D355" t="n">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="E355" t="inlineStr">
         <is>
@@ -9228,21 +9228,21 @@
     <row r="356">
       <c r="A356" t="inlineStr">
         <is>
-          <t>16:36:35</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B356" t="inlineStr">
         <is>
-          <t>18:04</t>
+          <t>17:51</t>
         </is>
       </c>
       <c r="C356" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D356" t="n">
-        <v>88</v>
+        <v>116</v>
       </c>
       <c r="E356" t="inlineStr">
         <is>
@@ -9253,21 +9253,21 @@
     <row r="357">
       <c r="A357" t="inlineStr">
         <is>
-          <t>16:36:35</t>
+          <t>16:46:26</t>
         </is>
       </c>
       <c r="B357" t="inlineStr">
         <is>
-          <t>18:21</t>
+          <t>17:52</t>
         </is>
       </c>
       <c r="C357" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D357" t="n">
-        <v>105</v>
+        <v>66</v>
       </c>
       <c r="E357" t="inlineStr">
         <is>
@@ -9278,21 +9278,21 @@
     <row r="358">
       <c r="A358" t="inlineStr">
         <is>
-          <t>16:36:35</t>
+          <t>16:46:26</t>
         </is>
       </c>
       <c r="B358" t="inlineStr">
         <is>
-          <t>18:28</t>
+          <t>18:04</t>
         </is>
       </c>
       <c r="C358" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D358" t="n">
-        <v>112</v>
+        <v>78</v>
       </c>
       <c r="E358" t="inlineStr">
         <is>
@@ -9303,23 +9303,98 @@
     <row r="359">
       <c r="A359" t="inlineStr">
         <is>
-          <t>16:36:35</t>
+          <t>16:46:26</t>
         </is>
       </c>
       <c r="B359" t="inlineStr">
         <is>
+          <t>18:21</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D359" t="n">
+        <v>95</v>
+      </c>
+      <c r="E359" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>16:46:26</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>18:28</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D360" t="n">
+        <v>102</v>
+      </c>
+      <c r="E360" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>16:46:26</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
           <t>18:32</t>
         </is>
       </c>
-      <c r="C359" t="inlineStr">
+      <c r="C361" t="inlineStr">
         <is>
           <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
-      <c r="D359" t="n">
-        <v>116</v>
-      </c>
-      <c r="E359" t="inlineStr">
+      <c r="D361" t="n">
+        <v>106</v>
+      </c>
+      <c r="E361" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>16:46:26</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>18:40</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D362" t="n">
+        <v>114</v>
+      </c>
+      <c r="E362" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -9354,7 +9429,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:36:35</t>
+          <t>Última actualización: 16:46:26</t>
         </is>
       </c>
     </row>
@@ -10320,7 +10395,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>16:36:35</t>
+          <t>16:46:26</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -10334,7 +10409,7 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -10395,7 +10470,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>16:36:35</t>
+          <t>16:46:26</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -10409,7 +10484,7 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -10420,7 +10495,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>16:36:35</t>
+          <t>16:46:26</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -10434,7 +10509,7 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -10453,7 +10528,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10471,14 +10546,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:36:35</t>
+          <t>Última actualización: 16:46:26</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 46</t>
+          <t>Total filas: 48</t>
         </is>
       </c>
     </row>
@@ -11562,12 +11637,12 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:46:26</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>16:52</t>
+          <t>16:48</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -11576,7 +11651,7 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>57</v>
+        <v>2</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -11587,12 +11662,12 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>16:36:35</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>16:53</t>
+          <t>16:52</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -11601,7 +11676,7 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -11617,16 +11692,16 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>17:14</t>
+          <t>16:53</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215B_LP-P MOR-40 Y 115</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -11637,23 +11712,73 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
+          <t>16:46:26</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>17:14</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>28</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
           <t>16:36:35</t>
         </is>
       </c>
-      <c r="B51" t="inlineStr">
+      <c r="B52" t="inlineStr">
         <is>
           <t>18:03</t>
         </is>
       </c>
-      <c r="C51" t="inlineStr">
+      <c r="C52" t="inlineStr">
         <is>
           <t>215C_LA PLATA</t>
         </is>
       </c>
-      <c r="D51" t="n">
+      <c r="D52" t="n">
         <v>87</v>
       </c>
-      <c r="E51" t="inlineStr">
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>16:46:26</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>18:04</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>78</v>
+      </c>
+      <c r="E53" t="inlineStr">
         <is>
           <t>L6203</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 849
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-23.xlsx
+++ b/data/horarios-141-2026-01-23.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E362"/>
+  <dimension ref="A1:E375"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:46:26</t>
+          <t>Última actualización: 16:53:56</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 357</t>
+          <t>Total filas: 370</t>
         </is>
       </c>
     </row>
@@ -1513,7 +1513,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -1538,7 +1538,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -1628,7 +1628,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1638,11 +1638,11 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>6</v>
+        <v>73</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -1653,7 +1653,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1663,11 +1663,11 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>73</v>
+        <v>6</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -1953,7 +1953,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1963,11 +1963,11 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -2003,7 +2003,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -2013,11 +2013,11 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2128,7 +2128,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -2138,11 +2138,11 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -2153,7 +2153,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -2163,11 +2163,11 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D73" t="n">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -2213,7 +2213,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D75" t="n">
@@ -2238,7 +2238,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D76" t="n">
@@ -2528,7 +2528,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -2538,11 +2538,11 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -2553,7 +2553,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2563,11 +2563,11 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -2903,7 +2903,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>08:48:01</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -2913,11 +2913,11 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -2928,7 +2928,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>08:48:01</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -2938,11 +2938,11 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D104" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -3153,7 +3153,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3163,11 +3163,11 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>115</v>
+        <v>27</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3188,7 +3188,7 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D114" t="n">
@@ -3203,7 +3203,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
@@ -3213,11 +3213,11 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D115" t="n">
-        <v>27</v>
+        <v>115</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -3338,7 +3338,7 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D120" t="n">
@@ -3363,7 +3363,7 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D121" t="n">
@@ -3388,7 +3388,7 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D122" t="n">
@@ -3413,7 +3413,7 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D123" t="n">
@@ -4413,7 +4413,7 @@
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D163" t="n">
@@ -4438,7 +4438,7 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D164" t="n">
@@ -5063,7 +5063,7 @@
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D189" t="n">
@@ -5088,7 +5088,7 @@
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D190" t="n">
@@ -5153,7 +5153,7 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>11:49:23</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
@@ -5163,11 +5163,11 @@
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D193" t="n">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
@@ -5178,7 +5178,7 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>11:49:23</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
@@ -5188,11 +5188,11 @@
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D194" t="n">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -5653,7 +5653,7 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>12:54:24</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
@@ -5663,11 +5663,11 @@
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D213" t="n">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -5678,7 +5678,7 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>12:54:24</t>
+          <t>12:37:00</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
@@ -5688,11 +5688,11 @@
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D214" t="n">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
@@ -5813,7 +5813,7 @@
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D219" t="n">
@@ -5838,7 +5838,7 @@
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D220" t="n">
@@ -5988,7 +5988,7 @@
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D226" t="n">
@@ -6013,7 +6013,7 @@
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D227" t="n">
@@ -6188,7 +6188,7 @@
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D234" t="n">
@@ -6213,7 +6213,7 @@
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D235" t="n">
@@ -6313,7 +6313,7 @@
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D239" t="n">
@@ -6338,7 +6338,7 @@
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D240" t="n">
@@ -6838,7 +6838,7 @@
       </c>
       <c r="C260" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D260" t="n">
@@ -6863,7 +6863,7 @@
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D261" t="n">
@@ -7013,7 +7013,7 @@
       </c>
       <c r="C267" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D267" t="n">
@@ -7038,7 +7038,7 @@
       </c>
       <c r="C268" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D268" t="n">
@@ -7478,7 +7478,7 @@
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>14:55:42</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
@@ -7488,11 +7488,11 @@
       </c>
       <c r="C286" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D286" t="n">
-        <v>51</v>
+        <v>25</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
@@ -7503,7 +7503,7 @@
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>14:55:42</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
@@ -7513,11 +7513,11 @@
       </c>
       <c r="C287" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D287" t="n">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
@@ -7553,7 +7553,7 @@
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>14:19:39</t>
+          <t>14:55:42</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
@@ -7563,11 +7563,11 @@
       </c>
       <c r="C289" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D289" t="n">
-        <v>94</v>
+        <v>58</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
@@ -7578,7 +7578,7 @@
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>14:55:42</t>
+          <t>14:19:39</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
@@ -7588,11 +7588,11 @@
       </c>
       <c r="C290" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D290" t="n">
-        <v>58</v>
+        <v>94</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
@@ -7963,7 +7963,7 @@
       </c>
       <c r="C305" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D305" t="n">
@@ -7988,7 +7988,7 @@
       </c>
       <c r="C306" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>225_C ROCA-H SUR</t>
         </is>
       </c>
       <c r="D306" t="n">
@@ -8078,7 +8078,7 @@
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>16:19:35</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
@@ -8088,11 +8088,11 @@
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D310" t="n">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="E310" t="inlineStr">
         <is>
@@ -8103,7 +8103,7 @@
     <row r="311">
       <c r="A311" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:19:35</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
@@ -8113,11 +8113,11 @@
       </c>
       <c r="C311" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D311" t="n">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="E311" t="inlineStr">
         <is>
@@ -8528,7 +8528,7 @@
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>16:46:26</t>
+          <t>16:36:35</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
@@ -8538,11 +8538,11 @@
       </c>
       <c r="C328" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D328" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E328" t="inlineStr">
         <is>
@@ -8553,7 +8553,7 @@
     <row r="329">
       <c r="A329" t="inlineStr">
         <is>
-          <t>16:36:35</t>
+          <t>16:46:26</t>
         </is>
       </c>
       <c r="B329" t="inlineStr">
@@ -8563,11 +8563,11 @@
       </c>
       <c r="C329" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D329" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="E329" t="inlineStr">
         <is>
@@ -8603,21 +8603,21 @@
     <row r="331">
       <c r="A331" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:53:56</t>
         </is>
       </c>
       <c r="B331" t="inlineStr">
         <is>
-          <t>16:55</t>
+          <t>16:53</t>
         </is>
       </c>
       <c r="C331" t="inlineStr">
         <is>
-          <t>17_179 Y 38</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D331" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="E331" t="inlineStr">
         <is>
@@ -8628,12 +8628,12 @@
     <row r="332">
       <c r="A332" t="inlineStr">
         <is>
-          <t>16:46:26</t>
+          <t>16:53:56</t>
         </is>
       </c>
       <c r="B332" t="inlineStr">
         <is>
-          <t>16:56</t>
+          <t>16:55</t>
         </is>
       </c>
       <c r="C332" t="inlineStr">
@@ -8642,7 +8642,7 @@
         </is>
       </c>
       <c r="D332" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E332" t="inlineStr">
         <is>
@@ -8653,12 +8653,12 @@
     <row r="333">
       <c r="A333" t="inlineStr">
         <is>
-          <t>16:46:26</t>
+          <t>16:53:56</t>
         </is>
       </c>
       <c r="B333" t="inlineStr">
         <is>
-          <t>16:57</t>
+          <t>16:56</t>
         </is>
       </c>
       <c r="C333" t="inlineStr">
@@ -8667,7 +8667,7 @@
         </is>
       </c>
       <c r="D333" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="E333" t="inlineStr">
         <is>
@@ -8683,16 +8683,16 @@
       </c>
       <c r="B334" t="inlineStr">
         <is>
-          <t>17:04</t>
+          <t>16:56</t>
         </is>
       </c>
       <c r="C334" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>17_179 Y 38</t>
         </is>
       </c>
       <c r="D334" t="n">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="E334" t="inlineStr">
         <is>
@@ -8708,16 +8708,16 @@
       </c>
       <c r="B335" t="inlineStr">
         <is>
-          <t>17:04</t>
+          <t>16:57</t>
         </is>
       </c>
       <c r="C335" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D335" t="n">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E335" t="inlineStr">
         <is>
@@ -8728,21 +8728,21 @@
     <row r="336">
       <c r="A336" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>16:53:56</t>
         </is>
       </c>
       <c r="B336" t="inlineStr">
         <is>
-          <t>17:05</t>
+          <t>17:04</t>
         </is>
       </c>
       <c r="C336" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D336" t="n">
-        <v>104</v>
+        <v>11</v>
       </c>
       <c r="E336" t="inlineStr">
         <is>
@@ -8753,21 +8753,21 @@
     <row r="337">
       <c r="A337" t="inlineStr">
         <is>
-          <t>16:46:26</t>
+          <t>16:53:56</t>
         </is>
       </c>
       <c r="B337" t="inlineStr">
         <is>
-          <t>17:10</t>
+          <t>17:04</t>
         </is>
       </c>
       <c r="C337" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D337" t="n">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="E337" t="inlineStr">
         <is>
@@ -8778,21 +8778,21 @@
     <row r="338">
       <c r="A338" t="inlineStr">
         <is>
-          <t>16:46:26</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B338" t="inlineStr">
         <is>
-          <t>17:16</t>
+          <t>17:05</t>
         </is>
       </c>
       <c r="C338" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D338" t="n">
-        <v>30</v>
+        <v>104</v>
       </c>
       <c r="E338" t="inlineStr">
         <is>
@@ -8803,21 +8803,21 @@
     <row r="339">
       <c r="A339" t="inlineStr">
         <is>
-          <t>16:46:26</t>
+          <t>16:53:56</t>
         </is>
       </c>
       <c r="B339" t="inlineStr">
         <is>
-          <t>17:16</t>
+          <t>17:09</t>
         </is>
       </c>
       <c r="C339" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D339" t="n">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="E339" t="inlineStr">
         <is>
@@ -8828,21 +8828,21 @@
     <row r="340">
       <c r="A340" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:46:26</t>
         </is>
       </c>
       <c r="B340" t="inlineStr">
         <is>
-          <t>17:20</t>
+          <t>17:10</t>
         </is>
       </c>
       <c r="C340" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D340" t="n">
-        <v>85</v>
+        <v>24</v>
       </c>
       <c r="E340" t="inlineStr">
         <is>
@@ -8853,21 +8853,21 @@
     <row r="341">
       <c r="A341" t="inlineStr">
         <is>
-          <t>16:46:26</t>
+          <t>16:53:56</t>
         </is>
       </c>
       <c r="B341" t="inlineStr">
         <is>
-          <t>17:20</t>
+          <t>17:15</t>
         </is>
       </c>
       <c r="C341" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D341" t="n">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="E341" t="inlineStr">
         <is>
@@ -8883,16 +8883,16 @@
       </c>
       <c r="B342" t="inlineStr">
         <is>
-          <t>17:21</t>
+          <t>17:16</t>
         </is>
       </c>
       <c r="C342" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D342" t="n">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E342" t="inlineStr">
         <is>
@@ -8903,21 +8903,21 @@
     <row r="343">
       <c r="A343" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:53:56</t>
         </is>
       </c>
       <c r="B343" t="inlineStr">
         <is>
-          <t>17:23</t>
+          <t>17:16</t>
         </is>
       </c>
       <c r="C343" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D343" t="n">
-        <v>88</v>
+        <v>23</v>
       </c>
       <c r="E343" t="inlineStr">
         <is>
@@ -8928,21 +8928,21 @@
     <row r="344">
       <c r="A344" t="inlineStr">
         <is>
-          <t>16:46:26</t>
+          <t>16:53:56</t>
         </is>
       </c>
       <c r="B344" t="inlineStr">
         <is>
-          <t>17:24</t>
+          <t>17:20</t>
         </is>
       </c>
       <c r="C344" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D344" t="n">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="E344" t="inlineStr">
         <is>
@@ -8953,21 +8953,21 @@
     <row r="345">
       <c r="A345" t="inlineStr">
         <is>
-          <t>16:19:35</t>
+          <t>16:53:56</t>
         </is>
       </c>
       <c r="B345" t="inlineStr">
         <is>
-          <t>17:26</t>
+          <t>17:20</t>
         </is>
       </c>
       <c r="C345" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D345" t="n">
-        <v>67</v>
+        <v>27</v>
       </c>
       <c r="E345" t="inlineStr">
         <is>
@@ -8983,16 +8983,16 @@
       </c>
       <c r="B346" t="inlineStr">
         <is>
-          <t>17:28</t>
+          <t>17:21</t>
         </is>
       </c>
       <c r="C346" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D346" t="n">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="E346" t="inlineStr">
         <is>
@@ -9003,21 +9003,21 @@
     <row r="347">
       <c r="A347" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:53:56</t>
         </is>
       </c>
       <c r="B347" t="inlineStr">
         <is>
-          <t>17:31</t>
+          <t>17:23</t>
         </is>
       </c>
       <c r="C347" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D347" t="n">
-        <v>96</v>
+        <v>30</v>
       </c>
       <c r="E347" t="inlineStr">
         <is>
@@ -9033,16 +9033,16 @@
       </c>
       <c r="B348" t="inlineStr">
         <is>
-          <t>17:34</t>
+          <t>17:24</t>
         </is>
       </c>
       <c r="C348" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D348" t="n">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="E348" t="inlineStr">
         <is>
@@ -9053,12 +9053,12 @@
     <row r="349">
       <c r="A349" t="inlineStr">
         <is>
-          <t>16:46:26</t>
+          <t>16:19:35</t>
         </is>
       </c>
       <c r="B349" t="inlineStr">
         <is>
-          <t>17:36</t>
+          <t>17:26</t>
         </is>
       </c>
       <c r="C349" t="inlineStr">
@@ -9067,7 +9067,7 @@
         </is>
       </c>
       <c r="D349" t="n">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="E349" t="inlineStr">
         <is>
@@ -9078,21 +9078,21 @@
     <row r="350">
       <c r="A350" t="inlineStr">
         <is>
-          <t>16:46:26</t>
+          <t>16:53:56</t>
         </is>
       </c>
       <c r="B350" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>17:28</t>
         </is>
       </c>
       <c r="C350" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D350" t="n">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="E350" t="inlineStr">
         <is>
@@ -9108,16 +9108,16 @@
       </c>
       <c r="B351" t="inlineStr">
         <is>
-          <t>17:39</t>
+          <t>17:31</t>
         </is>
       </c>
       <c r="C351" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D351" t="n">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="E351" t="inlineStr">
         <is>
@@ -9128,21 +9128,21 @@
     <row r="352">
       <c r="A352" t="inlineStr">
         <is>
-          <t>16:46:26</t>
+          <t>16:53:56</t>
         </is>
       </c>
       <c r="B352" t="inlineStr">
         <is>
-          <t>17:40</t>
+          <t>17:34</t>
         </is>
       </c>
       <c r="C352" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D352" t="n">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="E352" t="inlineStr">
         <is>
@@ -9153,21 +9153,21 @@
     <row r="353">
       <c r="A353" t="inlineStr">
         <is>
-          <t>16:46:26</t>
+          <t>16:53:56</t>
         </is>
       </c>
       <c r="B353" t="inlineStr">
         <is>
-          <t>17:40</t>
+          <t>17:36</t>
         </is>
       </c>
       <c r="C353" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D353" t="n">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="E353" t="inlineStr">
         <is>
@@ -9178,21 +9178,21 @@
     <row r="354">
       <c r="A354" t="inlineStr">
         <is>
-          <t>16:46:26</t>
+          <t>16:53:56</t>
         </is>
       </c>
       <c r="B354" t="inlineStr">
         <is>
-          <t>17:45</t>
+          <t>17:37</t>
         </is>
       </c>
       <c r="C354" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D354" t="n">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="E354" t="inlineStr">
         <is>
@@ -9208,16 +9208,16 @@
       </c>
       <c r="B355" t="inlineStr">
         <is>
-          <t>17:50</t>
+          <t>17:38</t>
         </is>
       </c>
       <c r="C355" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D355" t="n">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="E355" t="inlineStr">
         <is>
@@ -9228,21 +9228,21 @@
     <row r="356">
       <c r="A356" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:53:56</t>
         </is>
       </c>
       <c r="B356" t="inlineStr">
         <is>
-          <t>17:51</t>
+          <t>17:39</t>
         </is>
       </c>
       <c r="C356" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D356" t="n">
-        <v>116</v>
+        <v>46</v>
       </c>
       <c r="E356" t="inlineStr">
         <is>
@@ -9258,16 +9258,16 @@
       </c>
       <c r="B357" t="inlineStr">
         <is>
-          <t>17:52</t>
+          <t>17:40</t>
         </is>
       </c>
       <c r="C357" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D357" t="n">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="E357" t="inlineStr">
         <is>
@@ -9283,16 +9283,16 @@
       </c>
       <c r="B358" t="inlineStr">
         <is>
-          <t>18:04</t>
+          <t>17:40</t>
         </is>
       </c>
       <c r="C358" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D358" t="n">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="E358" t="inlineStr">
         <is>
@@ -9303,21 +9303,21 @@
     <row r="359">
       <c r="A359" t="inlineStr">
         <is>
-          <t>16:46:26</t>
+          <t>16:53:56</t>
         </is>
       </c>
       <c r="B359" t="inlineStr">
         <is>
-          <t>18:21</t>
+          <t>17:44</t>
         </is>
       </c>
       <c r="C359" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D359" t="n">
-        <v>95</v>
+        <v>51</v>
       </c>
       <c r="E359" t="inlineStr">
         <is>
@@ -9333,16 +9333,16 @@
       </c>
       <c r="B360" t="inlineStr">
         <is>
-          <t>18:28</t>
+          <t>17:45</t>
         </is>
       </c>
       <c r="C360" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D360" t="n">
-        <v>102</v>
+        <v>59</v>
       </c>
       <c r="E360" t="inlineStr">
         <is>
@@ -9353,21 +9353,21 @@
     <row r="361">
       <c r="A361" t="inlineStr">
         <is>
-          <t>16:46:26</t>
+          <t>16:53:56</t>
         </is>
       </c>
       <c r="B361" t="inlineStr">
         <is>
-          <t>18:32</t>
+          <t>17:50</t>
         </is>
       </c>
       <c r="C361" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D361" t="n">
-        <v>106</v>
+        <v>57</v>
       </c>
       <c r="E361" t="inlineStr">
         <is>
@@ -9378,23 +9378,348 @@
     <row r="362">
       <c r="A362" t="inlineStr">
         <is>
+          <t>16:53:56</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>17:51</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D362" t="n">
+        <v>58</v>
+      </c>
+      <c r="E362" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
           <t>16:46:26</t>
         </is>
       </c>
-      <c r="B362" t="inlineStr">
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>17:52</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D363" t="n">
+        <v>66</v>
+      </c>
+      <c r="E363" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>16:53:56</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>18:03</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D364" t="n">
+        <v>70</v>
+      </c>
+      <c r="E364" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>16:46:26</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>18:04</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D365" t="n">
+        <v>78</v>
+      </c>
+      <c r="E365" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>16:53:56</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>18:08</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D366" t="n">
+        <v>75</v>
+      </c>
+      <c r="E366" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>16:53:56</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>18:20</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D367" t="n">
+        <v>87</v>
+      </c>
+      <c r="E367" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>16:46:26</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>18:21</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D368" t="n">
+        <v>95</v>
+      </c>
+      <c r="E368" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>16:53:56</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>18:27</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D369" t="n">
+        <v>94</v>
+      </c>
+      <c r="E369" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>16:46:26</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>18:28</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D370" t="n">
+        <v>102</v>
+      </c>
+      <c r="E370" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>16:53:56</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>18:31</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D371" t="n">
+        <v>98</v>
+      </c>
+      <c r="E371" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>16:46:26</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>18:32</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D372" t="n">
+        <v>106</v>
+      </c>
+      <c r="E372" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>16:53:56</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>18:39</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D373" t="n">
+        <v>106</v>
+      </c>
+      <c r="E373" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>16:46:26</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
         <is>
           <t>18:40</t>
         </is>
       </c>
-      <c r="C362" t="inlineStr">
+      <c r="C374" t="inlineStr">
         <is>
           <t>15_ABASTO</t>
         </is>
       </c>
-      <c r="D362" t="n">
+      <c r="D374" t="n">
         <v>114</v>
       </c>
-      <c r="E362" t="inlineStr">
+      <c r="E374" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>16:53:56</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>18:47</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="D375" t="n">
+        <v>114</v>
+      </c>
+      <c r="E375" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -9411,7 +9736,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9429,14 +9754,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:46:26</t>
+          <t>Última actualización: 16:53:56</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 42</t>
+          <t>Total filas: 43</t>
         </is>
       </c>
     </row>
@@ -10395,7 +10720,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>16:46:26</t>
+          <t>16:53:56</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -10409,7 +10734,7 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -10445,7 +10770,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:53:56</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -10459,7 +10784,7 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>104</v>
+        <v>46</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -10495,23 +10820,48 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
+          <t>16:53:56</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>18:27</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>94</v>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
           <t>16:46:26</t>
         </is>
       </c>
-      <c r="B47" t="inlineStr">
+      <c r="B48" t="inlineStr">
         <is>
           <t>18:28</t>
         </is>
       </c>
-      <c r="C47" t="inlineStr">
+      <c r="C48" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D47" t="n">
+      <c r="D48" t="n">
         <v>102</v>
       </c>
-      <c r="E47" t="inlineStr">
+      <c r="E48" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -10528,7 +10878,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E53"/>
+  <dimension ref="A1:E55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10546,14 +10896,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:46:26</t>
+          <t>Última actualización: 16:53:56</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 48</t>
+          <t>Total filas: 50</t>
         </is>
       </c>
     </row>
@@ -11687,7 +12037,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>16:36:35</t>
+          <t>16:53:56</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -11701,7 +12051,7 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -11712,12 +12062,12 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>16:46:26</t>
+          <t>16:53:56</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>17:14</t>
+          <t>17:13</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -11726,7 +12076,7 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -11737,50 +12087,100 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>16:36:35</t>
+          <t>16:46:26</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>18:03</t>
+          <t>17:14</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>87</v>
+        <v>28</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>L6203</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
+          <t>16:53:56</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>18:03</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>70</v>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
           <t>16:46:26</t>
         </is>
       </c>
-      <c r="B53" t="inlineStr">
+      <c r="B54" t="inlineStr">
         <is>
           <t>18:04</t>
         </is>
       </c>
-      <c r="C53" t="inlineStr">
+      <c r="C54" t="inlineStr">
         <is>
           <t>215C_LA PLATA</t>
         </is>
       </c>
-      <c r="D53" t="n">
+      <c r="D54" t="n">
         <v>78</v>
       </c>
-      <c r="E53" t="inlineStr">
+      <c r="E54" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>16:53:56</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>18:51</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>118</v>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 850
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-23.xlsx
+++ b/data/horarios-141-2026-01-23.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E375"/>
+  <dimension ref="A1:E382"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:53:56</t>
+          <t>Última actualización: 17:15:32</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 370</t>
+          <t>Total filas: 377</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1638,11 +1638,11 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>73</v>
+        <v>6</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -1653,7 +1653,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1663,11 +1663,11 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>6</v>
+        <v>73</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -1778,7 +1778,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1788,11 +1788,11 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>17</v>
+        <v>84</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -1803,7 +1803,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1813,11 +1813,11 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D63" t="n">
@@ -1938,7 +1938,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -1978,7 +1978,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -1988,11 +1988,11 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2003,7 +2003,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -2013,11 +2013,11 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2528,7 +2528,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -2538,11 +2538,11 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -2553,7 +2553,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2563,11 +2563,11 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -2903,7 +2903,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>08:48:01</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -2913,11 +2913,11 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -2928,7 +2928,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>08:48:01</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -2938,11 +2938,11 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D104" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -3163,7 +3163,7 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D113" t="n">
@@ -3188,7 +3188,7 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D114" t="n">
@@ -3338,7 +3338,7 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D120" t="n">
@@ -3363,7 +3363,7 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D121" t="n">
@@ -3388,7 +3388,7 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D122" t="n">
@@ -3413,7 +3413,7 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D123" t="n">
@@ -4163,7 +4163,7 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D153" t="n">
@@ -4188,7 +4188,7 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D154" t="n">
@@ -4853,7 +4853,7 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>11:22:44</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
@@ -4863,11 +4863,11 @@
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D181" t="n">
-        <v>44</v>
+        <v>4</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
@@ -4878,7 +4878,7 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>11:22:44</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
@@ -4888,11 +4888,11 @@
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D182" t="n">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
@@ -5003,7 +5003,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>10:27:29</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
@@ -5013,11 +5013,11 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D187" t="n">
-        <v>15</v>
+        <v>110</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -5028,7 +5028,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>10:27:29</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -5038,11 +5038,11 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D188" t="n">
-        <v>110</v>
+        <v>15</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5288,7 +5288,7 @@
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>17_179 Y 38</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D198" t="n">
@@ -5313,7 +5313,7 @@
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D199" t="n">
@@ -5338,7 +5338,7 @@
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_179 Y 38</t>
         </is>
       </c>
       <c r="D200" t="n">
@@ -5528,7 +5528,7 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>12:54:24</t>
+          <t>12:37:00</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
@@ -5538,11 +5538,11 @@
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D208" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -5553,7 +5553,7 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>12:54:24</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
@@ -5563,11 +5563,11 @@
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D209" t="n">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -5653,7 +5653,7 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>12:54:24</t>
+          <t>12:37:00</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
@@ -5663,11 +5663,11 @@
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D213" t="n">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -5678,7 +5678,7 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>12:54:24</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
@@ -5688,11 +5688,11 @@
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D214" t="n">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
@@ -5813,7 +5813,7 @@
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D219" t="n">
@@ -5838,7 +5838,7 @@
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D220" t="n">
@@ -6188,7 +6188,7 @@
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D234" t="n">
@@ -6213,7 +6213,7 @@
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D235" t="n">
@@ -6238,7 +6238,7 @@
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D236" t="n">
@@ -6263,7 +6263,7 @@
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D237" t="n">
@@ -6353,7 +6353,7 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>13:51:20</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
@@ -6363,11 +6363,11 @@
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D241" t="n">
-        <v>80</v>
+        <v>6</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -6378,7 +6378,7 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>13:51:20</t>
+          <t>12:37:00</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
@@ -6388,11 +6388,11 @@
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D242" t="n">
-        <v>6</v>
+        <v>80</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -6838,7 +6838,7 @@
       </c>
       <c r="C260" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D260" t="n">
@@ -6863,7 +6863,7 @@
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D261" t="n">
@@ -7013,7 +7013,7 @@
       </c>
       <c r="C267" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D267" t="n">
@@ -7038,7 +7038,7 @@
       </c>
       <c r="C268" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D268" t="n">
@@ -7238,7 +7238,7 @@
       </c>
       <c r="C276" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D276" t="n">
@@ -7263,7 +7263,7 @@
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D277" t="n">
@@ -7553,7 +7553,7 @@
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>14:55:42</t>
+          <t>14:19:39</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
@@ -7563,11 +7563,11 @@
       </c>
       <c r="C289" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D289" t="n">
-        <v>58</v>
+        <v>94</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
@@ -7578,7 +7578,7 @@
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>14:19:39</t>
+          <t>14:55:42</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
@@ -7588,11 +7588,11 @@
       </c>
       <c r="C290" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D290" t="n">
-        <v>94</v>
+        <v>58</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
@@ -7628,7 +7628,7 @@
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
@@ -7638,11 +7638,11 @@
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D292" t="n">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
@@ -7653,7 +7653,7 @@
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
@@ -7663,11 +7663,11 @@
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D293" t="n">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
@@ -7963,7 +7963,7 @@
       </c>
       <c r="C305" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>225_C ROCA-H SUR</t>
         </is>
       </c>
       <c r="D305" t="n">
@@ -7988,7 +7988,7 @@
       </c>
       <c r="C306" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D306" t="n">
@@ -8053,7 +8053,7 @@
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>16:19:35</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
@@ -8063,11 +8063,11 @@
       </c>
       <c r="C309" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D309" t="n">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
@@ -8078,7 +8078,7 @@
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:19:35</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
@@ -8088,11 +8088,11 @@
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D310" t="n">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="E310" t="inlineStr">
         <is>
@@ -8113,7 +8113,7 @@
       </c>
       <c r="C311" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D311" t="n">
@@ -8403,7 +8403,7 @@
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:36:35</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
@@ -8413,11 +8413,11 @@
       </c>
       <c r="C323" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D323" t="n">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="E323" t="inlineStr">
         <is>
@@ -8428,7 +8428,7 @@
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>16:36:35</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
@@ -8438,11 +8438,11 @@
       </c>
       <c r="C324" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D324" t="n">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="E324" t="inlineStr">
         <is>
@@ -8528,7 +8528,7 @@
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>16:36:35</t>
+          <t>16:46:26</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
@@ -8538,11 +8538,11 @@
       </c>
       <c r="C328" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D328" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="E328" t="inlineStr">
         <is>
@@ -8553,7 +8553,7 @@
     <row r="329">
       <c r="A329" t="inlineStr">
         <is>
-          <t>16:46:26</t>
+          <t>16:36:35</t>
         </is>
       </c>
       <c r="B329" t="inlineStr">
@@ -8563,11 +8563,11 @@
       </c>
       <c r="C329" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D329" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E329" t="inlineStr">
         <is>
@@ -8653,7 +8653,7 @@
     <row r="333">
       <c r="A333" t="inlineStr">
         <is>
-          <t>16:53:56</t>
+          <t>16:46:26</t>
         </is>
       </c>
       <c r="B333" t="inlineStr">
@@ -8663,11 +8663,11 @@
       </c>
       <c r="C333" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_179 Y 38</t>
         </is>
       </c>
       <c r="D333" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E333" t="inlineStr">
         <is>
@@ -8678,7 +8678,7 @@
     <row r="334">
       <c r="A334" t="inlineStr">
         <is>
-          <t>16:46:26</t>
+          <t>16:53:56</t>
         </is>
       </c>
       <c r="B334" t="inlineStr">
@@ -8688,11 +8688,11 @@
       </c>
       <c r="C334" t="inlineStr">
         <is>
-          <t>17_179 Y 38</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D334" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E334" t="inlineStr">
         <is>
@@ -8738,7 +8738,7 @@
       </c>
       <c r="C336" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D336" t="n">
@@ -8763,7 +8763,7 @@
       </c>
       <c r="C337" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D337" t="n">
@@ -8878,7 +8878,7 @@
     <row r="342">
       <c r="A342" t="inlineStr">
         <is>
-          <t>16:46:26</t>
+          <t>17:15:32</t>
         </is>
       </c>
       <c r="B342" t="inlineStr">
@@ -8888,11 +8888,11 @@
       </c>
       <c r="C342" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D342" t="n">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="E342" t="inlineStr">
         <is>
@@ -8903,7 +8903,7 @@
     <row r="343">
       <c r="A343" t="inlineStr">
         <is>
-          <t>16:53:56</t>
+          <t>17:15:32</t>
         </is>
       </c>
       <c r="B343" t="inlineStr">
@@ -8913,11 +8913,11 @@
       </c>
       <c r="C343" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D343" t="n">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="E343" t="inlineStr">
         <is>
@@ -8928,12 +8928,12 @@
     <row r="344">
       <c r="A344" t="inlineStr">
         <is>
-          <t>16:53:56</t>
+          <t>17:15:32</t>
         </is>
       </c>
       <c r="B344" t="inlineStr">
         <is>
-          <t>17:20</t>
+          <t>17:16</t>
         </is>
       </c>
       <c r="C344" t="inlineStr">
@@ -8942,7 +8942,7 @@
         </is>
       </c>
       <c r="D344" t="n">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="E344" t="inlineStr">
         <is>
@@ -8978,21 +8978,21 @@
     <row r="346">
       <c r="A346" t="inlineStr">
         <is>
-          <t>16:46:26</t>
+          <t>16:53:56</t>
         </is>
       </c>
       <c r="B346" t="inlineStr">
         <is>
-          <t>17:21</t>
+          <t>17:20</t>
         </is>
       </c>
       <c r="C346" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D346" t="n">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="E346" t="inlineStr">
         <is>
@@ -9003,21 +9003,21 @@
     <row r="347">
       <c r="A347" t="inlineStr">
         <is>
-          <t>16:53:56</t>
+          <t>17:15:32</t>
         </is>
       </c>
       <c r="B347" t="inlineStr">
         <is>
-          <t>17:23</t>
+          <t>17:21</t>
         </is>
       </c>
       <c r="C347" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D347" t="n">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="E347" t="inlineStr">
         <is>
@@ -9028,21 +9028,21 @@
     <row r="348">
       <c r="A348" t="inlineStr">
         <is>
-          <t>16:46:26</t>
+          <t>17:15:32</t>
         </is>
       </c>
       <c r="B348" t="inlineStr">
         <is>
-          <t>17:24</t>
+          <t>17:22</t>
         </is>
       </c>
       <c r="C348" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D348" t="n">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="E348" t="inlineStr">
         <is>
@@ -9053,21 +9053,21 @@
     <row r="349">
       <c r="A349" t="inlineStr">
         <is>
-          <t>16:19:35</t>
+          <t>16:53:56</t>
         </is>
       </c>
       <c r="B349" t="inlineStr">
         <is>
-          <t>17:26</t>
+          <t>17:23</t>
         </is>
       </c>
       <c r="C349" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D349" t="n">
-        <v>67</v>
+        <v>30</v>
       </c>
       <c r="E349" t="inlineStr">
         <is>
@@ -9078,21 +9078,21 @@
     <row r="350">
       <c r="A350" t="inlineStr">
         <is>
-          <t>16:53:56</t>
+          <t>17:15:32</t>
         </is>
       </c>
       <c r="B350" t="inlineStr">
         <is>
-          <t>17:28</t>
+          <t>17:24</t>
         </is>
       </c>
       <c r="C350" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D350" t="n">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="E350" t="inlineStr">
         <is>
@@ -9103,12 +9103,12 @@
     <row r="351">
       <c r="A351" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:19:35</t>
         </is>
       </c>
       <c r="B351" t="inlineStr">
         <is>
-          <t>17:31</t>
+          <t>17:26</t>
         </is>
       </c>
       <c r="C351" t="inlineStr">
@@ -9117,7 +9117,7 @@
         </is>
       </c>
       <c r="D351" t="n">
-        <v>96</v>
+        <v>67</v>
       </c>
       <c r="E351" t="inlineStr">
         <is>
@@ -9128,21 +9128,21 @@
     <row r="352">
       <c r="A352" t="inlineStr">
         <is>
-          <t>16:53:56</t>
+          <t>17:15:32</t>
         </is>
       </c>
       <c r="B352" t="inlineStr">
         <is>
-          <t>17:34</t>
+          <t>17:28</t>
         </is>
       </c>
       <c r="C352" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D352" t="n">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="E352" t="inlineStr">
         <is>
@@ -9153,12 +9153,12 @@
     <row r="353">
       <c r="A353" t="inlineStr">
         <is>
-          <t>16:53:56</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B353" t="inlineStr">
         <is>
-          <t>17:36</t>
+          <t>17:31</t>
         </is>
       </c>
       <c r="C353" t="inlineStr">
@@ -9167,7 +9167,7 @@
         </is>
       </c>
       <c r="D353" t="n">
-        <v>43</v>
+        <v>96</v>
       </c>
       <c r="E353" t="inlineStr">
         <is>
@@ -9178,21 +9178,21 @@
     <row r="354">
       <c r="A354" t="inlineStr">
         <is>
-          <t>16:53:56</t>
+          <t>17:15:32</t>
         </is>
       </c>
       <c r="B354" t="inlineStr">
         <is>
-          <t>17:37</t>
+          <t>17:34</t>
         </is>
       </c>
       <c r="C354" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D354" t="n">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="E354" t="inlineStr">
         <is>
@@ -9203,21 +9203,21 @@
     <row r="355">
       <c r="A355" t="inlineStr">
         <is>
-          <t>16:46:26</t>
+          <t>17:15:32</t>
         </is>
       </c>
       <c r="B355" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>17:34</t>
         </is>
       </c>
       <c r="C355" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D355" t="n">
-        <v>52</v>
+        <v>19</v>
       </c>
       <c r="E355" t="inlineStr">
         <is>
@@ -9228,21 +9228,21 @@
     <row r="356">
       <c r="A356" t="inlineStr">
         <is>
-          <t>16:53:56</t>
+          <t>17:15:32</t>
         </is>
       </c>
       <c r="B356" t="inlineStr">
         <is>
-          <t>17:39</t>
+          <t>17:36</t>
         </is>
       </c>
       <c r="C356" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D356" t="n">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="E356" t="inlineStr">
         <is>
@@ -9253,21 +9253,21 @@
     <row r="357">
       <c r="A357" t="inlineStr">
         <is>
-          <t>16:46:26</t>
+          <t>16:53:56</t>
         </is>
       </c>
       <c r="B357" t="inlineStr">
         <is>
-          <t>17:40</t>
+          <t>17:37</t>
         </is>
       </c>
       <c r="C357" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D357" t="n">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="E357" t="inlineStr">
         <is>
@@ -9278,21 +9278,21 @@
     <row r="358">
       <c r="A358" t="inlineStr">
         <is>
-          <t>16:46:26</t>
+          <t>17:15:32</t>
         </is>
       </c>
       <c r="B358" t="inlineStr">
         <is>
-          <t>17:40</t>
+          <t>17:38</t>
         </is>
       </c>
       <c r="C358" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D358" t="n">
-        <v>54</v>
+        <v>23</v>
       </c>
       <c r="E358" t="inlineStr">
         <is>
@@ -9308,16 +9308,16 @@
       </c>
       <c r="B359" t="inlineStr">
         <is>
-          <t>17:44</t>
+          <t>17:39</t>
         </is>
       </c>
       <c r="C359" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D359" t="n">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E359" t="inlineStr">
         <is>
@@ -9328,21 +9328,21 @@
     <row r="360">
       <c r="A360" t="inlineStr">
         <is>
-          <t>16:46:26</t>
+          <t>17:15:32</t>
         </is>
       </c>
       <c r="B360" t="inlineStr">
         <is>
-          <t>17:45</t>
+          <t>17:40</t>
         </is>
       </c>
       <c r="C360" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D360" t="n">
-        <v>59</v>
+        <v>25</v>
       </c>
       <c r="E360" t="inlineStr">
         <is>
@@ -9353,21 +9353,21 @@
     <row r="361">
       <c r="A361" t="inlineStr">
         <is>
-          <t>16:53:56</t>
+          <t>17:15:32</t>
         </is>
       </c>
       <c r="B361" t="inlineStr">
         <is>
-          <t>17:50</t>
+          <t>17:40</t>
         </is>
       </c>
       <c r="C361" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D361" t="n">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="E361" t="inlineStr">
         <is>
@@ -9383,16 +9383,16 @@
       </c>
       <c r="B362" t="inlineStr">
         <is>
-          <t>17:51</t>
+          <t>17:44</t>
         </is>
       </c>
       <c r="C362" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D362" t="n">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="E362" t="inlineStr">
         <is>
@@ -9403,21 +9403,21 @@
     <row r="363">
       <c r="A363" t="inlineStr">
         <is>
-          <t>16:46:26</t>
+          <t>17:15:32</t>
         </is>
       </c>
       <c r="B363" t="inlineStr">
         <is>
-          <t>17:52</t>
+          <t>17:45</t>
         </is>
       </c>
       <c r="C363" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D363" t="n">
-        <v>66</v>
+        <v>30</v>
       </c>
       <c r="E363" t="inlineStr">
         <is>
@@ -9428,21 +9428,21 @@
     <row r="364">
       <c r="A364" t="inlineStr">
         <is>
-          <t>16:53:56</t>
+          <t>17:15:32</t>
         </is>
       </c>
       <c r="B364" t="inlineStr">
         <is>
-          <t>18:03</t>
+          <t>17:50</t>
         </is>
       </c>
       <c r="C364" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D364" t="n">
-        <v>70</v>
+        <v>35</v>
       </c>
       <c r="E364" t="inlineStr">
         <is>
@@ -9453,21 +9453,21 @@
     <row r="365">
       <c r="A365" t="inlineStr">
         <is>
-          <t>16:46:26</t>
+          <t>16:53:56</t>
         </is>
       </c>
       <c r="B365" t="inlineStr">
         <is>
-          <t>18:04</t>
+          <t>17:51</t>
         </is>
       </c>
       <c r="C365" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D365" t="n">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="E365" t="inlineStr">
         <is>
@@ -9478,21 +9478,21 @@
     <row r="366">
       <c r="A366" t="inlineStr">
         <is>
-          <t>16:53:56</t>
+          <t>17:15:32</t>
         </is>
       </c>
       <c r="B366" t="inlineStr">
         <is>
-          <t>18:08</t>
+          <t>17:52</t>
         </is>
       </c>
       <c r="C366" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D366" t="n">
-        <v>75</v>
+        <v>37</v>
       </c>
       <c r="E366" t="inlineStr">
         <is>
@@ -9508,16 +9508,16 @@
       </c>
       <c r="B367" t="inlineStr">
         <is>
-          <t>18:20</t>
+          <t>18:03</t>
         </is>
       </c>
       <c r="C367" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D367" t="n">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="E367" t="inlineStr">
         <is>
@@ -9528,21 +9528,21 @@
     <row r="368">
       <c r="A368" t="inlineStr">
         <is>
-          <t>16:46:26</t>
+          <t>17:15:32</t>
         </is>
       </c>
       <c r="B368" t="inlineStr">
         <is>
-          <t>18:21</t>
+          <t>18:04</t>
         </is>
       </c>
       <c r="C368" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D368" t="n">
-        <v>95</v>
+        <v>49</v>
       </c>
       <c r="E368" t="inlineStr">
         <is>
@@ -9553,21 +9553,21 @@
     <row r="369">
       <c r="A369" t="inlineStr">
         <is>
-          <t>16:53:56</t>
+          <t>17:15:32</t>
         </is>
       </c>
       <c r="B369" t="inlineStr">
         <is>
-          <t>18:27</t>
+          <t>18:08</t>
         </is>
       </c>
       <c r="C369" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D369" t="n">
-        <v>94</v>
+        <v>53</v>
       </c>
       <c r="E369" t="inlineStr">
         <is>
@@ -9578,21 +9578,21 @@
     <row r="370">
       <c r="A370" t="inlineStr">
         <is>
-          <t>16:46:26</t>
+          <t>16:53:56</t>
         </is>
       </c>
       <c r="B370" t="inlineStr">
         <is>
-          <t>18:28</t>
+          <t>18:20</t>
         </is>
       </c>
       <c r="C370" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D370" t="n">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="E370" t="inlineStr">
         <is>
@@ -9603,21 +9603,21 @@
     <row r="371">
       <c r="A371" t="inlineStr">
         <is>
-          <t>16:53:56</t>
+          <t>17:15:32</t>
         </is>
       </c>
       <c r="B371" t="inlineStr">
         <is>
-          <t>18:31</t>
+          <t>18:21</t>
         </is>
       </c>
       <c r="C371" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D371" t="n">
-        <v>98</v>
+        <v>66</v>
       </c>
       <c r="E371" t="inlineStr">
         <is>
@@ -9628,21 +9628,21 @@
     <row r="372">
       <c r="A372" t="inlineStr">
         <is>
-          <t>16:46:26</t>
+          <t>16:53:56</t>
         </is>
       </c>
       <c r="B372" t="inlineStr">
         <is>
-          <t>18:32</t>
+          <t>18:27</t>
         </is>
       </c>
       <c r="C372" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D372" t="n">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="E372" t="inlineStr">
         <is>
@@ -9653,21 +9653,21 @@
     <row r="373">
       <c r="A373" t="inlineStr">
         <is>
-          <t>16:53:56</t>
+          <t>17:15:32</t>
         </is>
       </c>
       <c r="B373" t="inlineStr">
         <is>
-          <t>18:39</t>
+          <t>18:28</t>
         </is>
       </c>
       <c r="C373" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D373" t="n">
-        <v>106</v>
+        <v>73</v>
       </c>
       <c r="E373" t="inlineStr">
         <is>
@@ -9678,21 +9678,21 @@
     <row r="374">
       <c r="A374" t="inlineStr">
         <is>
-          <t>16:46:26</t>
+          <t>16:53:56</t>
         </is>
       </c>
       <c r="B374" t="inlineStr">
         <is>
-          <t>18:40</t>
+          <t>18:31</t>
         </is>
       </c>
       <c r="C374" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D374" t="n">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="E374" t="inlineStr">
         <is>
@@ -9703,23 +9703,198 @@
     <row r="375">
       <c r="A375" t="inlineStr">
         <is>
+          <t>17:15:32</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>18:32</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D375" t="n">
+        <v>77</v>
+      </c>
+      <c r="E375" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
           <t>16:53:56</t>
         </is>
       </c>
-      <c r="B375" t="inlineStr">
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>18:39</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D376" t="n">
+        <v>106</v>
+      </c>
+      <c r="E376" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>17:15:32</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>18:40</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D377" t="n">
+        <v>85</v>
+      </c>
+      <c r="E377" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>16:53:56</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
         <is>
           <t>18:47</t>
         </is>
       </c>
-      <c r="C375" t="inlineStr">
+      <c r="C378" t="inlineStr">
         <is>
           <t>14X44_ABASTO</t>
         </is>
       </c>
-      <c r="D375" t="n">
+      <c r="D378" t="n">
         <v>114</v>
       </c>
-      <c r="E375" t="inlineStr">
+      <c r="E378" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>17:15:32</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>18:48</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="D379" t="n">
+        <v>93</v>
+      </c>
+      <c r="E379" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>17:15:32</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>18:58</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D380" t="n">
+        <v>103</v>
+      </c>
+      <c r="E380" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>17:15:32</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>19:04</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D381" t="n">
+        <v>109</v>
+      </c>
+      <c r="E381" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>17:15:32</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>19:10</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D382" t="n">
+        <v>115</v>
+      </c>
+      <c r="E382" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -9736,7 +9911,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E48"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9754,14 +9929,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:53:56</t>
+          <t>Última actualización: 17:15:32</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 43</t>
+          <t>Total filas: 44</t>
         </is>
       </c>
     </row>
@@ -10795,7 +10970,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>16:46:26</t>
+          <t>17:15:32</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -10809,7 +10984,7 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>54</v>
+        <v>25</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -10845,7 +11020,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>16:46:26</t>
+          <t>17:15:32</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -10859,9 +11034,34 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>102</v>
+        <v>73</v>
       </c>
       <c r="E48" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>17:15:32</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>18:58</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>103</v>
+      </c>
+      <c r="E49" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -10878,7 +11078,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E55"/>
+  <dimension ref="A1:E58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10896,14 +11096,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:53:56</t>
+          <t>Última actualización: 17:15:32</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 50</t>
+          <t>Total filas: 53</t>
         </is>
       </c>
     </row>
@@ -12112,37 +12312,37 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>16:53:56</t>
+          <t>17:15:32</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>18:03</t>
+          <t>17:15</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>L6203</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>16:46:26</t>
+          <t>16:53:56</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>18:04</t>
+          <t>18:03</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -12151,7 +12351,7 @@
         </is>
       </c>
       <c r="D54" t="n">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -12162,23 +12362,98 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
+          <t>17:15:32</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>18:04</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>49</v>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
           <t>16:53:56</t>
         </is>
       </c>
-      <c r="B55" t="inlineStr">
+      <c r="B56" t="inlineStr">
         <is>
           <t>18:51</t>
         </is>
       </c>
-      <c r="C55" t="inlineStr">
+      <c r="C56" t="inlineStr">
         <is>
           <t>215A_LA PLATA</t>
         </is>
       </c>
-      <c r="D55" t="n">
+      <c r="D56" t="n">
         <v>118</v>
       </c>
-      <c r="E55" t="inlineStr">
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>17:15:32</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>18:52</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>97</v>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>17:15:32</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>19:04</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>109</v>
+      </c>
+      <c r="E58" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 851
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-23.xlsx
+++ b/data/horarios-141-2026-01-23.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E382"/>
+  <dimension ref="A1:E400"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:15:32</t>
+          <t>Última actualización: 17:42:07</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 377</t>
+          <t>Total filas: 395</t>
         </is>
       </c>
     </row>
@@ -1313,7 +1313,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>86_EST CHICA-ESC AGRARIA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1338,7 +1338,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>86_EST CHICA-ESC AGRARIA</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1513,7 +1513,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -1538,7 +1538,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -1628,7 +1628,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1638,11 +1638,11 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>6</v>
+        <v>73</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -1653,7 +1653,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1663,11 +1663,11 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>73</v>
+        <v>6</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -1778,7 +1778,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1788,11 +1788,11 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -1803,7 +1803,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1813,11 +1813,11 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>17</v>
+        <v>84</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D63" t="n">
@@ -1938,7 +1938,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -1978,7 +1978,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -1988,11 +1988,11 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2003,7 +2003,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -2013,11 +2013,11 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2128,7 +2128,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -2138,11 +2138,11 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -2153,7 +2153,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -2163,11 +2163,11 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D73" t="n">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -2903,7 +2903,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>08:48:01</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -2913,11 +2913,11 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -2928,7 +2928,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>08:48:01</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -2938,11 +2938,11 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D104" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -3278,7 +3278,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>09:33:33</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -3288,11 +3288,11 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D118" t="n">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -3303,7 +3303,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>09:33:33</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -3313,11 +3313,11 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D119" t="n">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -3338,7 +3338,7 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D120" t="n">
@@ -3363,7 +3363,7 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D121" t="n">
@@ -4413,7 +4413,7 @@
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D163" t="n">
@@ -4438,7 +4438,7 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D164" t="n">
@@ -4853,7 +4853,7 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>11:22:44</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
@@ -4863,11 +4863,11 @@
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D181" t="n">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
@@ -4878,7 +4878,7 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>11:22:44</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
@@ -4888,11 +4888,11 @@
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D182" t="n">
-        <v>44</v>
+        <v>4</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
@@ -5153,7 +5153,7 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>11:49:23</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
@@ -5163,11 +5163,11 @@
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D193" t="n">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
@@ -5178,7 +5178,7 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>11:49:23</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
@@ -5188,11 +5188,11 @@
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D194" t="n">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -5288,7 +5288,7 @@
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_179 Y 38</t>
         </is>
       </c>
       <c r="D198" t="n">
@@ -5338,7 +5338,7 @@
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>17_179 Y 38</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D200" t="n">
@@ -5653,7 +5653,7 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>12:54:24</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
@@ -5663,11 +5663,11 @@
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D213" t="n">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -5678,7 +5678,7 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>12:54:24</t>
+          <t>12:37:00</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
@@ -5688,11 +5688,11 @@
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D214" t="n">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
@@ -6138,7 +6138,7 @@
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D232" t="n">
@@ -6163,7 +6163,7 @@
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D233" t="n">
@@ -6313,7 +6313,7 @@
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D239" t="n">
@@ -6338,7 +6338,7 @@
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D240" t="n">
@@ -6403,7 +6403,7 @@
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>13:18:32</t>
+          <t>13:51:20</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
@@ -6413,11 +6413,11 @@
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D243" t="n">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -6428,7 +6428,7 @@
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>13:51:20</t>
+          <t>13:18:32</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
@@ -6438,11 +6438,11 @@
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D244" t="n">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -7013,7 +7013,7 @@
       </c>
       <c r="C267" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D267" t="n">
@@ -7038,7 +7038,7 @@
       </c>
       <c r="C268" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D268" t="n">
@@ -7553,7 +7553,7 @@
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>14:19:39</t>
+          <t>14:55:42</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
@@ -7563,11 +7563,11 @@
       </c>
       <c r="C289" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D289" t="n">
-        <v>94</v>
+        <v>58</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
@@ -7578,7 +7578,7 @@
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>14:55:42</t>
+          <t>14:19:39</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
@@ -7588,11 +7588,11 @@
       </c>
       <c r="C290" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D290" t="n">
-        <v>58</v>
+        <v>94</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
@@ -7628,7 +7628,7 @@
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
@@ -7638,11 +7638,11 @@
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D292" t="n">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
@@ -7653,7 +7653,7 @@
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
@@ -7663,11 +7663,11 @@
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D293" t="n">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
@@ -7678,7 +7678,7 @@
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
@@ -7688,11 +7688,11 @@
       </c>
       <c r="C294" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D294" t="n">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
@@ -7703,7 +7703,7 @@
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
@@ -7713,11 +7713,11 @@
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D295" t="n">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
@@ -7853,7 +7853,7 @@
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>14:45:15</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
@@ -7863,11 +7863,11 @@
       </c>
       <c r="C301" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D301" t="n">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="E301" t="inlineStr">
         <is>
@@ -7878,7 +7878,7 @@
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>14:45:15</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
@@ -7888,11 +7888,11 @@
       </c>
       <c r="C302" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D302" t="n">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="E302" t="inlineStr">
         <is>
@@ -7963,7 +7963,7 @@
       </c>
       <c r="C305" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D305" t="n">
@@ -7988,7 +7988,7 @@
       </c>
       <c r="C306" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>225_C ROCA-H SUR</t>
         </is>
       </c>
       <c r="D306" t="n">
@@ -8003,7 +8003,7 @@
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>16:19:35</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
@@ -8013,11 +8013,11 @@
       </c>
       <c r="C307" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D307" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="E307" t="inlineStr">
         <is>
@@ -8028,7 +8028,7 @@
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:19:35</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
@@ -8038,11 +8038,11 @@
       </c>
       <c r="C308" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D308" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="E308" t="inlineStr">
         <is>
@@ -8403,7 +8403,7 @@
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>16:36:35</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
@@ -8413,11 +8413,11 @@
       </c>
       <c r="C323" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D323" t="n">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="E323" t="inlineStr">
         <is>
@@ -8428,7 +8428,7 @@
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:36:35</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
@@ -8438,11 +8438,11 @@
       </c>
       <c r="C324" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D324" t="n">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="E324" t="inlineStr">
         <is>
@@ -8453,7 +8453,7 @@
     <row r="325">
       <c r="A325" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>16:36:35</t>
         </is>
       </c>
       <c r="B325" t="inlineStr">
@@ -8463,11 +8463,11 @@
       </c>
       <c r="C325" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D325" t="n">
-        <v>82</v>
+        <v>7</v>
       </c>
       <c r="E325" t="inlineStr">
         <is>
@@ -8478,7 +8478,7 @@
     <row r="326">
       <c r="A326" t="inlineStr">
         <is>
-          <t>16:36:35</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B326" t="inlineStr">
@@ -8488,11 +8488,11 @@
       </c>
       <c r="C326" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D326" t="n">
-        <v>7</v>
+        <v>82</v>
       </c>
       <c r="E326" t="inlineStr">
         <is>
@@ -8528,7 +8528,7 @@
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>16:46:26</t>
+          <t>16:36:35</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
@@ -8538,11 +8538,11 @@
       </c>
       <c r="C328" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D328" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E328" t="inlineStr">
         <is>
@@ -8553,7 +8553,7 @@
     <row r="329">
       <c r="A329" t="inlineStr">
         <is>
-          <t>16:36:35</t>
+          <t>16:46:26</t>
         </is>
       </c>
       <c r="B329" t="inlineStr">
@@ -8563,11 +8563,11 @@
       </c>
       <c r="C329" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D329" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="E329" t="inlineStr">
         <is>
@@ -8653,7 +8653,7 @@
     <row r="333">
       <c r="A333" t="inlineStr">
         <is>
-          <t>16:46:26</t>
+          <t>16:53:56</t>
         </is>
       </c>
       <c r="B333" t="inlineStr">
@@ -8663,11 +8663,11 @@
       </c>
       <c r="C333" t="inlineStr">
         <is>
-          <t>17_179 Y 38</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D333" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E333" t="inlineStr">
         <is>
@@ -8678,7 +8678,7 @@
     <row r="334">
       <c r="A334" t="inlineStr">
         <is>
-          <t>16:53:56</t>
+          <t>16:46:26</t>
         </is>
       </c>
       <c r="B334" t="inlineStr">
@@ -8688,11 +8688,11 @@
       </c>
       <c r="C334" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_179 Y 38</t>
         </is>
       </c>
       <c r="D334" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E334" t="inlineStr">
         <is>
@@ -8738,7 +8738,7 @@
       </c>
       <c r="C336" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D336" t="n">
@@ -8763,7 +8763,7 @@
       </c>
       <c r="C337" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D337" t="n">
@@ -8888,7 +8888,7 @@
       </c>
       <c r="C342" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D342" t="n">
@@ -8913,7 +8913,7 @@
       </c>
       <c r="C343" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D343" t="n">
@@ -8938,7 +8938,7 @@
       </c>
       <c r="C344" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D344" t="n">
@@ -8963,7 +8963,7 @@
       </c>
       <c r="C345" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D345" t="n">
@@ -8988,7 +8988,7 @@
       </c>
       <c r="C346" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D346" t="n">
@@ -9188,7 +9188,7 @@
       </c>
       <c r="C354" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D354" t="n">
@@ -9213,7 +9213,7 @@
       </c>
       <c r="C355" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D355" t="n">
@@ -9338,7 +9338,7 @@
       </c>
       <c r="C360" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D360" t="n">
@@ -9363,7 +9363,7 @@
       </c>
       <c r="C361" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D361" t="n">
@@ -9428,21 +9428,21 @@
     <row r="364">
       <c r="A364" t="inlineStr">
         <is>
-          <t>17:15:32</t>
+          <t>17:42:07</t>
         </is>
       </c>
       <c r="B364" t="inlineStr">
         <is>
-          <t>17:50</t>
+          <t>17:49</t>
         </is>
       </c>
       <c r="C364" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D364" t="n">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="E364" t="inlineStr">
         <is>
@@ -9453,21 +9453,21 @@
     <row r="365">
       <c r="A365" t="inlineStr">
         <is>
-          <t>16:53:56</t>
+          <t>17:15:32</t>
         </is>
       </c>
       <c r="B365" t="inlineStr">
         <is>
-          <t>17:51</t>
+          <t>17:50</t>
         </is>
       </c>
       <c r="C365" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D365" t="n">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="E365" t="inlineStr">
         <is>
@@ -9478,12 +9478,12 @@
     <row r="366">
       <c r="A366" t="inlineStr">
         <is>
-          <t>17:15:32</t>
+          <t>16:53:56</t>
         </is>
       </c>
       <c r="B366" t="inlineStr">
         <is>
-          <t>17:52</t>
+          <t>17:51</t>
         </is>
       </c>
       <c r="C366" t="inlineStr">
@@ -9492,7 +9492,7 @@
         </is>
       </c>
       <c r="D366" t="n">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="E366" t="inlineStr">
         <is>
@@ -9503,21 +9503,21 @@
     <row r="367">
       <c r="A367" t="inlineStr">
         <is>
-          <t>16:53:56</t>
+          <t>17:42:07</t>
         </is>
       </c>
       <c r="B367" t="inlineStr">
         <is>
-          <t>18:03</t>
+          <t>17:51</t>
         </is>
       </c>
       <c r="C367" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D367" t="n">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="E367" t="inlineStr">
         <is>
@@ -9528,21 +9528,21 @@
     <row r="368">
       <c r="A368" t="inlineStr">
         <is>
-          <t>17:15:32</t>
+          <t>17:42:07</t>
         </is>
       </c>
       <c r="B368" t="inlineStr">
         <is>
-          <t>18:04</t>
+          <t>17:52</t>
         </is>
       </c>
       <c r="C368" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D368" t="n">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="E368" t="inlineStr">
         <is>
@@ -9553,21 +9553,21 @@
     <row r="369">
       <c r="A369" t="inlineStr">
         <is>
-          <t>17:15:32</t>
+          <t>17:42:07</t>
         </is>
       </c>
       <c r="B369" t="inlineStr">
         <is>
-          <t>18:08</t>
+          <t>17:53</t>
         </is>
       </c>
       <c r="C369" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D369" t="n">
-        <v>53</v>
+        <v>11</v>
       </c>
       <c r="E369" t="inlineStr">
         <is>
@@ -9578,21 +9578,21 @@
     <row r="370">
       <c r="A370" t="inlineStr">
         <is>
-          <t>16:53:56</t>
+          <t>17:42:07</t>
         </is>
       </c>
       <c r="B370" t="inlineStr">
         <is>
-          <t>18:20</t>
+          <t>18:01</t>
         </is>
       </c>
       <c r="C370" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D370" t="n">
-        <v>87</v>
+        <v>19</v>
       </c>
       <c r="E370" t="inlineStr">
         <is>
@@ -9603,21 +9603,21 @@
     <row r="371">
       <c r="A371" t="inlineStr">
         <is>
-          <t>17:15:32</t>
+          <t>16:53:56</t>
         </is>
       </c>
       <c r="B371" t="inlineStr">
         <is>
-          <t>18:21</t>
+          <t>18:03</t>
         </is>
       </c>
       <c r="C371" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D371" t="n">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="E371" t="inlineStr">
         <is>
@@ -9628,21 +9628,21 @@
     <row r="372">
       <c r="A372" t="inlineStr">
         <is>
-          <t>16:53:56</t>
+          <t>17:42:07</t>
         </is>
       </c>
       <c r="B372" t="inlineStr">
         <is>
-          <t>18:27</t>
+          <t>18:04</t>
         </is>
       </c>
       <c r="C372" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D372" t="n">
-        <v>94</v>
+        <v>22</v>
       </c>
       <c r="E372" t="inlineStr">
         <is>
@@ -9653,21 +9653,21 @@
     <row r="373">
       <c r="A373" t="inlineStr">
         <is>
-          <t>17:15:32</t>
+          <t>17:42:07</t>
         </is>
       </c>
       <c r="B373" t="inlineStr">
         <is>
-          <t>18:28</t>
+          <t>18:05</t>
         </is>
       </c>
       <c r="C373" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D373" t="n">
-        <v>73</v>
+        <v>23</v>
       </c>
       <c r="E373" t="inlineStr">
         <is>
@@ -9678,21 +9678,21 @@
     <row r="374">
       <c r="A374" t="inlineStr">
         <is>
-          <t>16:53:56</t>
+          <t>17:15:32</t>
         </is>
       </c>
       <c r="B374" t="inlineStr">
         <is>
-          <t>18:31</t>
+          <t>18:08</t>
         </is>
       </c>
       <c r="C374" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D374" t="n">
-        <v>98</v>
+        <v>53</v>
       </c>
       <c r="E374" t="inlineStr">
         <is>
@@ -9703,21 +9703,21 @@
     <row r="375">
       <c r="A375" t="inlineStr">
         <is>
-          <t>17:15:32</t>
+          <t>17:42:07</t>
         </is>
       </c>
       <c r="B375" t="inlineStr">
         <is>
-          <t>18:32</t>
+          <t>18:09</t>
         </is>
       </c>
       <c r="C375" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D375" t="n">
-        <v>77</v>
+        <v>27</v>
       </c>
       <c r="E375" t="inlineStr">
         <is>
@@ -9728,21 +9728,21 @@
     <row r="376">
       <c r="A376" t="inlineStr">
         <is>
-          <t>16:53:56</t>
+          <t>17:42:07</t>
         </is>
       </c>
       <c r="B376" t="inlineStr">
         <is>
-          <t>18:39</t>
+          <t>18:11</t>
         </is>
       </c>
       <c r="C376" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D376" t="n">
-        <v>106</v>
+        <v>29</v>
       </c>
       <c r="E376" t="inlineStr">
         <is>
@@ -9753,21 +9753,21 @@
     <row r="377">
       <c r="A377" t="inlineStr">
         <is>
-          <t>17:15:32</t>
+          <t>17:42:07</t>
         </is>
       </c>
       <c r="B377" t="inlineStr">
         <is>
-          <t>18:40</t>
+          <t>18:16</t>
         </is>
       </c>
       <c r="C377" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D377" t="n">
-        <v>85</v>
+        <v>34</v>
       </c>
       <c r="E377" t="inlineStr">
         <is>
@@ -9778,21 +9778,21 @@
     <row r="378">
       <c r="A378" t="inlineStr">
         <is>
-          <t>16:53:56</t>
+          <t>17:42:07</t>
         </is>
       </c>
       <c r="B378" t="inlineStr">
         <is>
-          <t>18:47</t>
+          <t>18:16</t>
         </is>
       </c>
       <c r="C378" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D378" t="n">
-        <v>114</v>
+        <v>34</v>
       </c>
       <c r="E378" t="inlineStr">
         <is>
@@ -9803,21 +9803,21 @@
     <row r="379">
       <c r="A379" t="inlineStr">
         <is>
-          <t>17:15:32</t>
+          <t>16:53:56</t>
         </is>
       </c>
       <c r="B379" t="inlineStr">
         <is>
-          <t>18:48</t>
+          <t>18:20</t>
         </is>
       </c>
       <c r="C379" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D379" t="n">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="E379" t="inlineStr">
         <is>
@@ -9828,21 +9828,21 @@
     <row r="380">
       <c r="A380" t="inlineStr">
         <is>
-          <t>17:15:32</t>
+          <t>17:42:07</t>
         </is>
       </c>
       <c r="B380" t="inlineStr">
         <is>
-          <t>18:58</t>
+          <t>18:21</t>
         </is>
       </c>
       <c r="C380" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D380" t="n">
-        <v>103</v>
+        <v>39</v>
       </c>
       <c r="E380" t="inlineStr">
         <is>
@@ -9853,21 +9853,21 @@
     <row r="381">
       <c r="A381" t="inlineStr">
         <is>
-          <t>17:15:32</t>
+          <t>17:42:07</t>
         </is>
       </c>
       <c r="B381" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>18:25</t>
         </is>
       </c>
       <c r="C381" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D381" t="n">
-        <v>109</v>
+        <v>43</v>
       </c>
       <c r="E381" t="inlineStr">
         <is>
@@ -9878,23 +9878,473 @@
     <row r="382">
       <c r="A382" t="inlineStr">
         <is>
+          <t>16:53:56</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>18:27</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D382" t="n">
+        <v>94</v>
+      </c>
+      <c r="E382" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>17:42:07</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>18:28</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D383" t="n">
+        <v>46</v>
+      </c>
+      <c r="E383" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>16:53:56</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>18:31</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D384" t="n">
+        <v>98</v>
+      </c>
+      <c r="E384" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>17:42:07</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>18:32</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D385" t="n">
+        <v>50</v>
+      </c>
+      <c r="E385" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>17:42:07</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>18:35</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D386" t="n">
+        <v>53</v>
+      </c>
+      <c r="E386" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>16:53:56</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>18:39</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D387" t="n">
+        <v>106</v>
+      </c>
+      <c r="E387" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>17:42:07</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>18:40</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D388" t="n">
+        <v>58</v>
+      </c>
+      <c r="E388" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>16:53:56</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>18:47</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="D389" t="n">
+        <v>114</v>
+      </c>
+      <c r="E389" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>17:42:07</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>18:48</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="D390" t="n">
+        <v>66</v>
+      </c>
+      <c r="E390" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
           <t>17:15:32</t>
         </is>
       </c>
-      <c r="B382" t="inlineStr">
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>18:58</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D391" t="n">
+        <v>103</v>
+      </c>
+      <c r="E391" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>17:42:07</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>18:59</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D392" t="n">
+        <v>77</v>
+      </c>
+      <c r="E392" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>17:15:32</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>19:04</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D393" t="n">
+        <v>109</v>
+      </c>
+      <c r="E393" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>17:42:07</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>19:05</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D394" t="n">
+        <v>83</v>
+      </c>
+      <c r="E394" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>17:15:32</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
         <is>
           <t>19:10</t>
         </is>
       </c>
-      <c r="C382" t="inlineStr">
+      <c r="C395" t="inlineStr">
         <is>
           <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
-      <c r="D382" t="n">
+      <c r="D395" t="n">
         <v>115</v>
       </c>
-      <c r="E382" t="inlineStr">
+      <c r="E395" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>17:42:07</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>19:11</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D396" t="n">
+        <v>89</v>
+      </c>
+      <c r="E396" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>17:42:07</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>19:17</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D397" t="n">
+        <v>95</v>
+      </c>
+      <c r="E397" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>17:42:07</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>19:21</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D398" t="n">
+        <v>99</v>
+      </c>
+      <c r="E398" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>17:42:07</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>19:30</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D399" t="n">
+        <v>108</v>
+      </c>
+      <c r="E399" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>17:42:07</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>19:40</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D400" t="n">
+        <v>118</v>
+      </c>
+      <c r="E400" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -9911,7 +10361,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9929,14 +10379,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:15:32</t>
+          <t>Última actualización: 17:42:07</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 44</t>
+          <t>Total filas: 46</t>
         </is>
       </c>
     </row>
@@ -11020,7 +11470,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>17:15:32</t>
+          <t>17:42:07</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -11034,7 +11484,7 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>73</v>
+        <v>46</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -11062,6 +11512,56 @@
         <v>103</v>
       </c>
       <c r="E49" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>17:42:07</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>18:59</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>77</v>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>17:42:07</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>19:40</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>118</v>
+      </c>
+      <c r="E51" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -11096,7 +11596,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:15:32</t>
+          <t>Última actualización: 17:42:07</t>
         </is>
       </c>
     </row>
@@ -12362,7 +12862,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>17:15:32</t>
+          <t>17:42:07</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -12376,7 +12876,7 @@
         </is>
       </c>
       <c r="D55" t="n">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -12412,7 +12912,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>17:15:32</t>
+          <t>17:42:07</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -12426,7 +12926,7 @@
         </is>
       </c>
       <c r="D57" t="n">
-        <v>97</v>
+        <v>70</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -12437,7 +12937,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>17:15:32</t>
+          <t>17:42:07</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -12451,7 +12951,7 @@
         </is>
       </c>
       <c r="D58" t="n">
-        <v>109</v>
+        <v>82</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 852
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-23.xlsx
+++ b/data/horarios-141-2026-01-23.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E400"/>
+  <dimension ref="A1:E411"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:42:07</t>
+          <t>Última actualización: 17:57:31</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 395</t>
+          <t>Total filas: 406</t>
         </is>
       </c>
     </row>
@@ -1313,7 +1313,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>86_EST CHICA-ESC AGRARIA</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1338,7 +1338,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>86_EST CHICA-ESC AGRARIA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1778,7 +1778,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1788,11 +1788,11 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>17</v>
+        <v>84</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -1803,7 +1803,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1813,11 +1813,11 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D63" t="n">
@@ -1938,7 +1938,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -1953,7 +1953,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1963,11 +1963,11 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -1988,7 +1988,7 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D66" t="n">
@@ -2003,7 +2003,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -2013,11 +2013,11 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2128,7 +2128,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -2138,11 +2138,11 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -2153,7 +2153,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -2163,11 +2163,11 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D73" t="n">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -2213,7 +2213,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D75" t="n">
@@ -2238,7 +2238,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D76" t="n">
@@ -2803,7 +2803,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -2813,11 +2813,11 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D99" t="n">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -2828,7 +2828,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -2838,11 +2838,11 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -2903,7 +2903,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>08:48:01</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -2913,11 +2913,11 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -2928,7 +2928,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>08:48:01</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -2938,11 +2938,11 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D104" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -3153,7 +3153,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3163,11 +3163,11 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>27</v>
+        <v>115</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3188,7 +3188,7 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D114" t="n">
@@ -3203,7 +3203,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
@@ -3213,11 +3213,11 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D115" t="n">
-        <v>115</v>
+        <v>27</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -3278,7 +3278,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>09:33:33</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -3288,11 +3288,11 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D118" t="n">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -3303,7 +3303,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>09:33:33</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -3313,11 +3313,11 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D119" t="n">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -3388,7 +3388,7 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D122" t="n">
@@ -3413,7 +3413,7 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D123" t="n">
@@ -4413,7 +4413,7 @@
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D163" t="n">
@@ -4438,7 +4438,7 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D164" t="n">
@@ -5003,7 +5003,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>10:27:29</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
@@ -5013,11 +5013,11 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D187" t="n">
-        <v>110</v>
+        <v>15</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -5028,7 +5028,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>10:27:29</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -5038,11 +5038,11 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D188" t="n">
-        <v>15</v>
+        <v>110</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5063,7 +5063,7 @@
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D189" t="n">
@@ -5088,7 +5088,7 @@
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D190" t="n">
@@ -5153,7 +5153,7 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>11:49:23</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
@@ -5163,11 +5163,11 @@
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D193" t="n">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
@@ -5178,7 +5178,7 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>11:49:23</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
@@ -5188,11 +5188,11 @@
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D194" t="n">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -5528,7 +5528,7 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>12:54:24</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
@@ -5538,11 +5538,11 @@
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D208" t="n">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -5553,7 +5553,7 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>12:54:24</t>
+          <t>12:37:00</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
@@ -5563,11 +5563,11 @@
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D209" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -5653,7 +5653,7 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>12:54:24</t>
+          <t>12:37:00</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
@@ -5663,11 +5663,11 @@
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D213" t="n">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -5678,7 +5678,7 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>12:54:24</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
@@ -5688,11 +5688,11 @@
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D214" t="n">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
@@ -6188,7 +6188,7 @@
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D234" t="n">
@@ -6213,7 +6213,7 @@
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D235" t="n">
@@ -6238,7 +6238,7 @@
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D236" t="n">
@@ -6263,7 +6263,7 @@
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D237" t="n">
@@ -6838,7 +6838,7 @@
       </c>
       <c r="C260" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D260" t="n">
@@ -6863,7 +6863,7 @@
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D261" t="n">
@@ -7013,7 +7013,7 @@
       </c>
       <c r="C267" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D267" t="n">
@@ -7038,7 +7038,7 @@
       </c>
       <c r="C268" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D268" t="n">
@@ -7238,7 +7238,7 @@
       </c>
       <c r="C276" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D276" t="n">
@@ -7263,7 +7263,7 @@
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D277" t="n">
@@ -7628,7 +7628,7 @@
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
@@ -7638,11 +7638,11 @@
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D292" t="n">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
@@ -7653,7 +7653,7 @@
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
@@ -7663,11 +7663,11 @@
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D293" t="n">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
@@ -7678,7 +7678,7 @@
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
@@ -7688,11 +7688,11 @@
       </c>
       <c r="C294" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D294" t="n">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
@@ -7703,7 +7703,7 @@
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
@@ -7713,11 +7713,11 @@
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D295" t="n">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
@@ -7728,7 +7728,7 @@
     <row r="296">
       <c r="A296" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
@@ -7738,11 +7738,11 @@
       </c>
       <c r="C296" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D296" t="n">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="E296" t="inlineStr">
         <is>
@@ -7753,7 +7753,7 @@
     <row r="297">
       <c r="A297" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
@@ -7763,11 +7763,11 @@
       </c>
       <c r="C297" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D297" t="n">
-        <v>36</v>
+        <v>2</v>
       </c>
       <c r="E297" t="inlineStr">
         <is>
@@ -7853,7 +7853,7 @@
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>14:45:15</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
@@ -7863,11 +7863,11 @@
       </c>
       <c r="C301" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D301" t="n">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="E301" t="inlineStr">
         <is>
@@ -7878,7 +7878,7 @@
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>14:45:15</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
@@ -7888,11 +7888,11 @@
       </c>
       <c r="C302" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D302" t="n">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="E302" t="inlineStr">
         <is>
@@ -7963,7 +7963,7 @@
       </c>
       <c r="C305" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>225_C ROCA-H SUR</t>
         </is>
       </c>
       <c r="D305" t="n">
@@ -7988,7 +7988,7 @@
       </c>
       <c r="C306" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D306" t="n">
@@ -8003,7 +8003,7 @@
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:19:35</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
@@ -8013,11 +8013,11 @@
       </c>
       <c r="C307" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D307" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="E307" t="inlineStr">
         <is>
@@ -8028,7 +8028,7 @@
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>16:19:35</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
@@ -8038,11 +8038,11 @@
       </c>
       <c r="C308" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D308" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="E308" t="inlineStr">
         <is>
@@ -8053,7 +8053,7 @@
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:19:35</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
@@ -8063,11 +8063,11 @@
       </c>
       <c r="C309" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D309" t="n">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
@@ -8088,7 +8088,7 @@
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D310" t="n">
@@ -8103,7 +8103,7 @@
     <row r="311">
       <c r="A311" t="inlineStr">
         <is>
-          <t>16:19:35</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
@@ -8113,11 +8113,11 @@
       </c>
       <c r="C311" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D311" t="n">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="E311" t="inlineStr">
         <is>
@@ -8403,7 +8403,7 @@
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:36:35</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
@@ -8413,11 +8413,11 @@
       </c>
       <c r="C323" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D323" t="n">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="E323" t="inlineStr">
         <is>
@@ -8428,7 +8428,7 @@
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>16:36:35</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
@@ -8438,11 +8438,11 @@
       </c>
       <c r="C324" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D324" t="n">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="E324" t="inlineStr">
         <is>
@@ -8653,7 +8653,7 @@
     <row r="333">
       <c r="A333" t="inlineStr">
         <is>
-          <t>16:53:56</t>
+          <t>16:46:26</t>
         </is>
       </c>
       <c r="B333" t="inlineStr">
@@ -8663,11 +8663,11 @@
       </c>
       <c r="C333" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_179 Y 38</t>
         </is>
       </c>
       <c r="D333" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E333" t="inlineStr">
         <is>
@@ -8678,7 +8678,7 @@
     <row r="334">
       <c r="A334" t="inlineStr">
         <is>
-          <t>16:46:26</t>
+          <t>16:53:56</t>
         </is>
       </c>
       <c r="B334" t="inlineStr">
@@ -8688,11 +8688,11 @@
       </c>
       <c r="C334" t="inlineStr">
         <is>
-          <t>17_179 Y 38</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D334" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E334" t="inlineStr">
         <is>
@@ -8738,7 +8738,7 @@
       </c>
       <c r="C336" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D336" t="n">
@@ -8763,7 +8763,7 @@
       </c>
       <c r="C337" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D337" t="n">
@@ -8963,7 +8963,7 @@
       </c>
       <c r="C345" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D345" t="n">
@@ -8988,7 +8988,7 @@
       </c>
       <c r="C346" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D346" t="n">
@@ -9188,7 +9188,7 @@
       </c>
       <c r="C354" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D354" t="n">
@@ -9213,7 +9213,7 @@
       </c>
       <c r="C355" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D355" t="n">
@@ -9338,7 +9338,7 @@
       </c>
       <c r="C360" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D360" t="n">
@@ -9363,7 +9363,7 @@
       </c>
       <c r="C361" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D361" t="n">
@@ -9578,21 +9578,21 @@
     <row r="370">
       <c r="A370" t="inlineStr">
         <is>
-          <t>17:42:07</t>
+          <t>17:57:31</t>
         </is>
       </c>
       <c r="B370" t="inlineStr">
         <is>
-          <t>18:01</t>
+          <t>17:58</t>
         </is>
       </c>
       <c r="C370" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D370" t="n">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="E370" t="inlineStr">
         <is>
@@ -9603,21 +9603,21 @@
     <row r="371">
       <c r="A371" t="inlineStr">
         <is>
-          <t>16:53:56</t>
+          <t>17:42:07</t>
         </is>
       </c>
       <c r="B371" t="inlineStr">
         <is>
-          <t>18:03</t>
+          <t>18:01</t>
         </is>
       </c>
       <c r="C371" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D371" t="n">
-        <v>70</v>
+        <v>19</v>
       </c>
       <c r="E371" t="inlineStr">
         <is>
@@ -9628,12 +9628,12 @@
     <row r="372">
       <c r="A372" t="inlineStr">
         <is>
-          <t>17:42:07</t>
+          <t>16:53:56</t>
         </is>
       </c>
       <c r="B372" t="inlineStr">
         <is>
-          <t>18:04</t>
+          <t>18:03</t>
         </is>
       </c>
       <c r="C372" t="inlineStr">
@@ -9642,7 +9642,7 @@
         </is>
       </c>
       <c r="D372" t="n">
-        <v>22</v>
+        <v>70</v>
       </c>
       <c r="E372" t="inlineStr">
         <is>
@@ -9653,21 +9653,21 @@
     <row r="373">
       <c r="A373" t="inlineStr">
         <is>
-          <t>17:42:07</t>
+          <t>17:57:31</t>
         </is>
       </c>
       <c r="B373" t="inlineStr">
         <is>
-          <t>18:05</t>
+          <t>18:04</t>
         </is>
       </c>
       <c r="C373" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D373" t="n">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="E373" t="inlineStr">
         <is>
@@ -9678,21 +9678,21 @@
     <row r="374">
       <c r="A374" t="inlineStr">
         <is>
-          <t>17:15:32</t>
+          <t>17:57:31</t>
         </is>
       </c>
       <c r="B374" t="inlineStr">
         <is>
-          <t>18:08</t>
+          <t>18:04</t>
         </is>
       </c>
       <c r="C374" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D374" t="n">
-        <v>53</v>
+        <v>7</v>
       </c>
       <c r="E374" t="inlineStr">
         <is>
@@ -9708,16 +9708,16 @@
       </c>
       <c r="B375" t="inlineStr">
         <is>
-          <t>18:09</t>
+          <t>18:05</t>
         </is>
       </c>
       <c r="C375" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D375" t="n">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E375" t="inlineStr">
         <is>
@@ -9728,21 +9728,21 @@
     <row r="376">
       <c r="A376" t="inlineStr">
         <is>
-          <t>17:42:07</t>
+          <t>17:15:32</t>
         </is>
       </c>
       <c r="B376" t="inlineStr">
         <is>
-          <t>18:11</t>
+          <t>18:08</t>
         </is>
       </c>
       <c r="C376" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D376" t="n">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="E376" t="inlineStr">
         <is>
@@ -9758,16 +9758,16 @@
       </c>
       <c r="B377" t="inlineStr">
         <is>
-          <t>18:16</t>
+          <t>18:09</t>
         </is>
       </c>
       <c r="C377" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D377" t="n">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="E377" t="inlineStr">
         <is>
@@ -9778,21 +9778,21 @@
     <row r="378">
       <c r="A378" t="inlineStr">
         <is>
-          <t>17:42:07</t>
+          <t>17:57:31</t>
         </is>
       </c>
       <c r="B378" t="inlineStr">
         <is>
-          <t>18:16</t>
+          <t>18:10</t>
         </is>
       </c>
       <c r="C378" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D378" t="n">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="E378" t="inlineStr">
         <is>
@@ -9803,21 +9803,21 @@
     <row r="379">
       <c r="A379" t="inlineStr">
         <is>
-          <t>16:53:56</t>
+          <t>17:42:07</t>
         </is>
       </c>
       <c r="B379" t="inlineStr">
         <is>
-          <t>18:20</t>
+          <t>18:11</t>
         </is>
       </c>
       <c r="C379" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D379" t="n">
-        <v>87</v>
+        <v>29</v>
       </c>
       <c r="E379" t="inlineStr">
         <is>
@@ -9828,21 +9828,21 @@
     <row r="380">
       <c r="A380" t="inlineStr">
         <is>
-          <t>17:42:07</t>
+          <t>17:57:31</t>
         </is>
       </c>
       <c r="B380" t="inlineStr">
         <is>
-          <t>18:21</t>
+          <t>18:16</t>
         </is>
       </c>
       <c r="C380" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D380" t="n">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="E380" t="inlineStr">
         <is>
@@ -9853,21 +9853,21 @@
     <row r="381">
       <c r="A381" t="inlineStr">
         <is>
-          <t>17:42:07</t>
+          <t>17:57:31</t>
         </is>
       </c>
       <c r="B381" t="inlineStr">
         <is>
-          <t>18:25</t>
+          <t>18:16</t>
         </is>
       </c>
       <c r="C381" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D381" t="n">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="E381" t="inlineStr">
         <is>
@@ -9883,16 +9883,16 @@
       </c>
       <c r="B382" t="inlineStr">
         <is>
-          <t>18:27</t>
+          <t>18:20</t>
         </is>
       </c>
       <c r="C382" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D382" t="n">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="E382" t="inlineStr">
         <is>
@@ -9903,21 +9903,21 @@
     <row r="383">
       <c r="A383" t="inlineStr">
         <is>
-          <t>17:42:07</t>
+          <t>17:57:31</t>
         </is>
       </c>
       <c r="B383" t="inlineStr">
         <is>
-          <t>18:28</t>
+          <t>18:20</t>
         </is>
       </c>
       <c r="C383" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D383" t="n">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="E383" t="inlineStr">
         <is>
@@ -9928,21 +9928,21 @@
     <row r="384">
       <c r="A384" t="inlineStr">
         <is>
-          <t>16:53:56</t>
+          <t>17:57:31</t>
         </is>
       </c>
       <c r="B384" t="inlineStr">
         <is>
-          <t>18:31</t>
+          <t>18:21</t>
         </is>
       </c>
       <c r="C384" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D384" t="n">
-        <v>98</v>
+        <v>24</v>
       </c>
       <c r="E384" t="inlineStr">
         <is>
@@ -9953,21 +9953,21 @@
     <row r="385">
       <c r="A385" t="inlineStr">
         <is>
-          <t>17:42:07</t>
+          <t>17:57:31</t>
         </is>
       </c>
       <c r="B385" t="inlineStr">
         <is>
-          <t>18:32</t>
+          <t>18:24</t>
         </is>
       </c>
       <c r="C385" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D385" t="n">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="E385" t="inlineStr">
         <is>
@@ -9983,16 +9983,16 @@
       </c>
       <c r="B386" t="inlineStr">
         <is>
-          <t>18:35</t>
+          <t>18:25</t>
         </is>
       </c>
       <c r="C386" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D386" t="n">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="E386" t="inlineStr">
         <is>
@@ -10008,16 +10008,16 @@
       </c>
       <c r="B387" t="inlineStr">
         <is>
-          <t>18:39</t>
+          <t>18:27</t>
         </is>
       </c>
       <c r="C387" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D387" t="n">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="E387" t="inlineStr">
         <is>
@@ -10028,21 +10028,21 @@
     <row r="388">
       <c r="A388" t="inlineStr">
         <is>
-          <t>17:42:07</t>
+          <t>17:57:31</t>
         </is>
       </c>
       <c r="B388" t="inlineStr">
         <is>
-          <t>18:40</t>
+          <t>18:28</t>
         </is>
       </c>
       <c r="C388" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D388" t="n">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="E388" t="inlineStr">
         <is>
@@ -10058,16 +10058,16 @@
       </c>
       <c r="B389" t="inlineStr">
         <is>
-          <t>18:47</t>
+          <t>18:31</t>
         </is>
       </c>
       <c r="C389" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D389" t="n">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="E389" t="inlineStr">
         <is>
@@ -10078,21 +10078,21 @@
     <row r="390">
       <c r="A390" t="inlineStr">
         <is>
-          <t>17:42:07</t>
+          <t>17:57:31</t>
         </is>
       </c>
       <c r="B390" t="inlineStr">
         <is>
-          <t>18:48</t>
+          <t>18:32</t>
         </is>
       </c>
       <c r="C390" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D390" t="n">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="E390" t="inlineStr">
         <is>
@@ -10103,21 +10103,21 @@
     <row r="391">
       <c r="A391" t="inlineStr">
         <is>
-          <t>17:15:32</t>
+          <t>17:57:31</t>
         </is>
       </c>
       <c r="B391" t="inlineStr">
         <is>
-          <t>18:58</t>
+          <t>18:34</t>
         </is>
       </c>
       <c r="C391" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D391" t="n">
-        <v>103</v>
+        <v>37</v>
       </c>
       <c r="E391" t="inlineStr">
         <is>
@@ -10133,16 +10133,16 @@
       </c>
       <c r="B392" t="inlineStr">
         <is>
-          <t>18:59</t>
+          <t>18:35</t>
         </is>
       </c>
       <c r="C392" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D392" t="n">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="E392" t="inlineStr">
         <is>
@@ -10153,21 +10153,21 @@
     <row r="393">
       <c r="A393" t="inlineStr">
         <is>
-          <t>17:15:32</t>
+          <t>16:53:56</t>
         </is>
       </c>
       <c r="B393" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>18:39</t>
         </is>
       </c>
       <c r="C393" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D393" t="n">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E393" t="inlineStr">
         <is>
@@ -10178,21 +10178,21 @@
     <row r="394">
       <c r="A394" t="inlineStr">
         <is>
-          <t>17:42:07</t>
+          <t>17:57:31</t>
         </is>
       </c>
       <c r="B394" t="inlineStr">
         <is>
-          <t>19:05</t>
+          <t>18:40</t>
         </is>
       </c>
       <c r="C394" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D394" t="n">
-        <v>83</v>
+        <v>43</v>
       </c>
       <c r="E394" t="inlineStr">
         <is>
@@ -10203,21 +10203,21 @@
     <row r="395">
       <c r="A395" t="inlineStr">
         <is>
-          <t>17:15:32</t>
+          <t>16:53:56</t>
         </is>
       </c>
       <c r="B395" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>18:47</t>
         </is>
       </c>
       <c r="C395" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D395" t="n">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E395" t="inlineStr">
         <is>
@@ -10228,21 +10228,21 @@
     <row r="396">
       <c r="A396" t="inlineStr">
         <is>
-          <t>17:42:07</t>
+          <t>17:57:31</t>
         </is>
       </c>
       <c r="B396" t="inlineStr">
         <is>
-          <t>19:11</t>
+          <t>18:48</t>
         </is>
       </c>
       <c r="C396" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D396" t="n">
-        <v>89</v>
+        <v>51</v>
       </c>
       <c r="E396" t="inlineStr">
         <is>
@@ -10253,21 +10253,21 @@
     <row r="397">
       <c r="A397" t="inlineStr">
         <is>
-          <t>17:42:07</t>
+          <t>17:57:31</t>
         </is>
       </c>
       <c r="B397" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>18:58</t>
         </is>
       </c>
       <c r="C397" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D397" t="n">
-        <v>95</v>
+        <v>61</v>
       </c>
       <c r="E397" t="inlineStr">
         <is>
@@ -10283,16 +10283,16 @@
       </c>
       <c r="B398" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>18:59</t>
         </is>
       </c>
       <c r="C398" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D398" t="n">
-        <v>99</v>
+        <v>77</v>
       </c>
       <c r="E398" t="inlineStr">
         <is>
@@ -10303,21 +10303,21 @@
     <row r="399">
       <c r="A399" t="inlineStr">
         <is>
-          <t>17:42:07</t>
+          <t>17:57:31</t>
         </is>
       </c>
       <c r="B399" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="C399" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D399" t="n">
-        <v>108</v>
+        <v>67</v>
       </c>
       <c r="E399" t="inlineStr">
         <is>
@@ -10333,18 +10333,293 @@
       </c>
       <c r="B400" t="inlineStr">
         <is>
+          <t>19:05</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D400" t="n">
+        <v>83</v>
+      </c>
+      <c r="E400" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>17:57:31</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>19:10</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D401" t="n">
+        <v>73</v>
+      </c>
+      <c r="E401" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>17:42:07</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>19:11</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D402" t="n">
+        <v>89</v>
+      </c>
+      <c r="E402" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>17:57:31</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>19:16</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D403" t="n">
+        <v>79</v>
+      </c>
+      <c r="E403" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>17:42:07</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>19:17</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D404" t="n">
+        <v>95</v>
+      </c>
+      <c r="E404" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>17:57:31</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>19:20</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D405" t="n">
+        <v>83</v>
+      </c>
+      <c r="E405" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>17:57:31</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>19:21</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D406" t="n">
+        <v>84</v>
+      </c>
+      <c r="E406" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>17:57:31</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>19:30</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D407" t="n">
+        <v>93</v>
+      </c>
+      <c r="E407" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>17:57:31</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
           <t>19:40</t>
         </is>
       </c>
-      <c r="C400" t="inlineStr">
+      <c r="C408" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D400" t="n">
-        <v>118</v>
-      </c>
-      <c r="E400" t="inlineStr">
+      <c r="D408" t="n">
+        <v>103</v>
+      </c>
+      <c r="E408" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>17:57:31</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>19:50</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D409" t="n">
+        <v>113</v>
+      </c>
+      <c r="E409" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>17:57:31</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>19:50</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D410" t="n">
+        <v>113</v>
+      </c>
+      <c r="E410" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>17:57:31</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>19:51</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D411" t="n">
+        <v>114</v>
+      </c>
+      <c r="E411" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -10379,7 +10654,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:42:07</t>
+          <t>Última actualización: 17:57:31</t>
         </is>
       </c>
     </row>
@@ -11470,7 +11745,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>17:42:07</t>
+          <t>17:57:31</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -11484,7 +11759,7 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -11495,7 +11770,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>17:15:32</t>
+          <t>17:57:31</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -11509,7 +11784,7 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>103</v>
+        <v>61</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -11545,7 +11820,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>17:42:07</t>
+          <t>17:57:31</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -11559,7 +11834,7 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -11578,7 +11853,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E58"/>
+  <dimension ref="A1:E60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11596,14 +11871,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:42:07</t>
+          <t>Última actualización: 17:57:31</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 53</t>
+          <t>Total filas: 55</t>
         </is>
       </c>
     </row>
@@ -12837,12 +13112,12 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>16:53:56</t>
+          <t>17:57:31</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>18:03</t>
+          <t>18:02</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -12851,7 +13126,7 @@
         </is>
       </c>
       <c r="D54" t="n">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -12862,12 +13137,12 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>17:42:07</t>
+          <t>16:53:56</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>18:04</t>
+          <t>18:03</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -12876,7 +13151,7 @@
         </is>
       </c>
       <c r="D55" t="n">
-        <v>22</v>
+        <v>70</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -12887,37 +13162,37 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>16:53:56</t>
+          <t>17:42:07</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>18:51</t>
+          <t>18:04</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>118</v>
+        <v>22</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>L6173</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>17:42:07</t>
+          <t>16:53:56</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>18:52</t>
+          <t>18:51</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -12926,7 +13201,7 @@
         </is>
       </c>
       <c r="D57" t="n">
-        <v>70</v>
+        <v>118</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -12937,25 +13212,75 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>17:42:07</t>
+          <t>17:57:31</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
+          <t>18:52</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>55</v>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>17:57:31</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
           <t>19:04</t>
         </is>
       </c>
-      <c r="C58" t="inlineStr">
+      <c r="C59" t="inlineStr">
         <is>
           <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
-      <c r="D58" t="n">
-        <v>82</v>
-      </c>
-      <c r="E58" t="inlineStr">
+      <c r="D59" t="n">
+        <v>67</v>
+      </c>
+      <c r="E59" t="inlineStr">
         <is>
           <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>17:57:31</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>19:54</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>117</v>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 853
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-23.xlsx
+++ b/data/horarios-141-2026-01-23.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E411"/>
+  <dimension ref="A1:E428"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:57:31</t>
+          <t>Última actualización: 18:18:12</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 406</t>
+          <t>Total filas: 423</t>
         </is>
       </c>
     </row>
@@ -1313,7 +1313,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>86_EST CHICA-ESC AGRARIA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1338,7 +1338,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>86_EST CHICA-ESC AGRARIA</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1778,7 +1778,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1788,11 +1788,11 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -1803,7 +1803,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1813,11 +1813,11 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>17</v>
+        <v>84</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D63" t="n">
@@ -1938,7 +1938,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -1953,7 +1953,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1963,11 +1963,11 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -1978,7 +1978,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -1988,11 +1988,11 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2213,7 +2213,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D75" t="n">
@@ -2238,7 +2238,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D76" t="n">
@@ -2528,7 +2528,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -2538,11 +2538,11 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -2553,7 +2553,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2563,11 +2563,11 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -2803,7 +2803,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -2813,11 +2813,11 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D99" t="n">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -2828,7 +2828,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -2838,11 +2838,11 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -3153,7 +3153,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3163,11 +3163,11 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>115</v>
+        <v>27</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3203,7 +3203,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
@@ -3213,11 +3213,11 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D115" t="n">
-        <v>27</v>
+        <v>115</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -3338,7 +3338,7 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D120" t="n">
@@ -3363,7 +3363,7 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D121" t="n">
@@ -3388,7 +3388,7 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D122" t="n">
@@ -3413,7 +3413,7 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D123" t="n">
@@ -4163,7 +4163,7 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D153" t="n">
@@ -4188,7 +4188,7 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D154" t="n">
@@ -5063,7 +5063,7 @@
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D189" t="n">
@@ -5088,7 +5088,7 @@
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D190" t="n">
@@ -5153,7 +5153,7 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>11:49:23</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
@@ -5163,11 +5163,11 @@
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D193" t="n">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
@@ -5178,7 +5178,7 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>11:49:23</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
@@ -5188,11 +5188,11 @@
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D194" t="n">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -5288,7 +5288,7 @@
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>17_179 Y 38</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D198" t="n">
@@ -5313,7 +5313,7 @@
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D199" t="n">
@@ -5338,7 +5338,7 @@
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_179 Y 38</t>
         </is>
       </c>
       <c r="D200" t="n">
@@ -5528,7 +5528,7 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>12:54:24</t>
+          <t>12:37:00</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
@@ -5538,11 +5538,11 @@
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D208" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -5553,7 +5553,7 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>12:54:24</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
@@ -5563,11 +5563,11 @@
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D209" t="n">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -5813,7 +5813,7 @@
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D219" t="n">
@@ -5838,7 +5838,7 @@
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D220" t="n">
@@ -6138,7 +6138,7 @@
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D232" t="n">
@@ -6163,7 +6163,7 @@
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D233" t="n">
@@ -6188,7 +6188,7 @@
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D234" t="n">
@@ -6213,7 +6213,7 @@
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D235" t="n">
@@ -6238,7 +6238,7 @@
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D236" t="n">
@@ -6263,7 +6263,7 @@
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D237" t="n">
@@ -6838,7 +6838,7 @@
       </c>
       <c r="C260" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D260" t="n">
@@ -6863,7 +6863,7 @@
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D261" t="n">
@@ -7238,7 +7238,7 @@
       </c>
       <c r="C276" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D276" t="n">
@@ -7263,7 +7263,7 @@
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D277" t="n">
@@ -7478,7 +7478,7 @@
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>14:55:42</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
@@ -7488,11 +7488,11 @@
       </c>
       <c r="C286" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D286" t="n">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
@@ -7503,7 +7503,7 @@
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>14:55:42</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
@@ -7513,11 +7513,11 @@
       </c>
       <c r="C287" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D287" t="n">
-        <v>51</v>
+        <v>25</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
@@ -7553,7 +7553,7 @@
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>14:55:42</t>
+          <t>14:19:39</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
@@ -7563,11 +7563,11 @@
       </c>
       <c r="C289" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D289" t="n">
-        <v>58</v>
+        <v>94</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
@@ -7578,7 +7578,7 @@
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>14:19:39</t>
+          <t>14:55:42</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
@@ -7588,11 +7588,11 @@
       </c>
       <c r="C290" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D290" t="n">
-        <v>94</v>
+        <v>58</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
@@ -7628,7 +7628,7 @@
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
@@ -7638,11 +7638,11 @@
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D292" t="n">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
@@ -7653,7 +7653,7 @@
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
@@ -7663,11 +7663,11 @@
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D293" t="n">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
@@ -7678,7 +7678,7 @@
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
@@ -7688,11 +7688,11 @@
       </c>
       <c r="C294" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D294" t="n">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
@@ -7703,7 +7703,7 @@
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
@@ -7713,11 +7713,11 @@
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D295" t="n">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
@@ -7963,7 +7963,7 @@
       </c>
       <c r="C305" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D305" t="n">
@@ -7988,7 +7988,7 @@
       </c>
       <c r="C306" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>225_C ROCA-H SUR</t>
         </is>
       </c>
       <c r="D306" t="n">
@@ -8078,7 +8078,7 @@
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>16:19:35</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
@@ -8088,11 +8088,11 @@
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D310" t="n">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="E310" t="inlineStr">
         <is>
@@ -8103,7 +8103,7 @@
     <row r="311">
       <c r="A311" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:19:35</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
@@ -8113,11 +8113,11 @@
       </c>
       <c r="C311" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D311" t="n">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="E311" t="inlineStr">
         <is>
@@ -8403,7 +8403,7 @@
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>16:36:35</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
@@ -8413,11 +8413,11 @@
       </c>
       <c r="C323" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D323" t="n">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="E323" t="inlineStr">
         <is>
@@ -8428,7 +8428,7 @@
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:36:35</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
@@ -8438,11 +8438,11 @@
       </c>
       <c r="C324" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D324" t="n">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="E324" t="inlineStr">
         <is>
@@ -8453,7 +8453,7 @@
     <row r="325">
       <c r="A325" t="inlineStr">
         <is>
-          <t>16:36:35</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B325" t="inlineStr">
@@ -8463,11 +8463,11 @@
       </c>
       <c r="C325" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D325" t="n">
-        <v>7</v>
+        <v>82</v>
       </c>
       <c r="E325" t="inlineStr">
         <is>
@@ -8478,7 +8478,7 @@
     <row r="326">
       <c r="A326" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>16:36:35</t>
         </is>
       </c>
       <c r="B326" t="inlineStr">
@@ -8488,11 +8488,11 @@
       </c>
       <c r="C326" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D326" t="n">
-        <v>82</v>
+        <v>7</v>
       </c>
       <c r="E326" t="inlineStr">
         <is>
@@ -8528,7 +8528,7 @@
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>16:36:35</t>
+          <t>16:46:26</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
@@ -8538,11 +8538,11 @@
       </c>
       <c r="C328" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D328" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="E328" t="inlineStr">
         <is>
@@ -8553,7 +8553,7 @@
     <row r="329">
       <c r="A329" t="inlineStr">
         <is>
-          <t>16:46:26</t>
+          <t>16:36:35</t>
         </is>
       </c>
       <c r="B329" t="inlineStr">
@@ -8563,11 +8563,11 @@
       </c>
       <c r="C329" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D329" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E329" t="inlineStr">
         <is>
@@ -8888,7 +8888,7 @@
       </c>
       <c r="C342" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D342" t="n">
@@ -8938,7 +8938,7 @@
       </c>
       <c r="C344" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D344" t="n">
@@ -9188,7 +9188,7 @@
       </c>
       <c r="C354" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D354" t="n">
@@ -9213,7 +9213,7 @@
       </c>
       <c r="C355" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D355" t="n">
@@ -9338,7 +9338,7 @@
       </c>
       <c r="C360" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D360" t="n">
@@ -9363,7 +9363,7 @@
       </c>
       <c r="C361" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D361" t="n">
@@ -9478,7 +9478,7 @@
     <row r="366">
       <c r="A366" t="inlineStr">
         <is>
-          <t>16:53:56</t>
+          <t>17:42:07</t>
         </is>
       </c>
       <c r="B366" t="inlineStr">
@@ -9488,11 +9488,11 @@
       </c>
       <c r="C366" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D366" t="n">
-        <v>58</v>
+        <v>9</v>
       </c>
       <c r="E366" t="inlineStr">
         <is>
@@ -9503,7 +9503,7 @@
     <row r="367">
       <c r="A367" t="inlineStr">
         <is>
-          <t>17:42:07</t>
+          <t>16:53:56</t>
         </is>
       </c>
       <c r="B367" t="inlineStr">
@@ -9513,11 +9513,11 @@
       </c>
       <c r="C367" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D367" t="n">
-        <v>9</v>
+        <v>58</v>
       </c>
       <c r="E367" t="inlineStr">
         <is>
@@ -9838,7 +9838,7 @@
       </c>
       <c r="C380" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D380" t="n">
@@ -9863,7 +9863,7 @@
       </c>
       <c r="C381" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D381" t="n">
@@ -9953,21 +9953,21 @@
     <row r="385">
       <c r="A385" t="inlineStr">
         <is>
-          <t>17:57:31</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B385" t="inlineStr">
         <is>
-          <t>18:24</t>
+          <t>18:22</t>
         </is>
       </c>
       <c r="C385" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D385" t="n">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="E385" t="inlineStr">
         <is>
@@ -9978,12 +9978,12 @@
     <row r="386">
       <c r="A386" t="inlineStr">
         <is>
-          <t>17:42:07</t>
+          <t>17:57:31</t>
         </is>
       </c>
       <c r="B386" t="inlineStr">
         <is>
-          <t>18:25</t>
+          <t>18:24</t>
         </is>
       </c>
       <c r="C386" t="inlineStr">
@@ -9992,7 +9992,7 @@
         </is>
       </c>
       <c r="D386" t="n">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="E386" t="inlineStr">
         <is>
@@ -10003,21 +10003,21 @@
     <row r="387">
       <c r="A387" t="inlineStr">
         <is>
-          <t>16:53:56</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B387" t="inlineStr">
         <is>
-          <t>18:27</t>
+          <t>18:25</t>
         </is>
       </c>
       <c r="C387" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D387" t="n">
-        <v>94</v>
+        <v>7</v>
       </c>
       <c r="E387" t="inlineStr">
         <is>
@@ -10028,12 +10028,12 @@
     <row r="388">
       <c r="A388" t="inlineStr">
         <is>
-          <t>17:57:31</t>
+          <t>16:53:56</t>
         </is>
       </c>
       <c r="B388" t="inlineStr">
         <is>
-          <t>18:28</t>
+          <t>18:27</t>
         </is>
       </c>
       <c r="C388" t="inlineStr">
@@ -10042,7 +10042,7 @@
         </is>
       </c>
       <c r="D388" t="n">
-        <v>31</v>
+        <v>94</v>
       </c>
       <c r="E388" t="inlineStr">
         <is>
@@ -10053,21 +10053,21 @@
     <row r="389">
       <c r="A389" t="inlineStr">
         <is>
-          <t>16:53:56</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B389" t="inlineStr">
         <is>
-          <t>18:31</t>
+          <t>18:28</t>
         </is>
       </c>
       <c r="C389" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D389" t="n">
-        <v>98</v>
+        <v>10</v>
       </c>
       <c r="E389" t="inlineStr">
         <is>
@@ -10078,12 +10078,12 @@
     <row r="390">
       <c r="A390" t="inlineStr">
         <is>
-          <t>17:57:31</t>
+          <t>16:53:56</t>
         </is>
       </c>
       <c r="B390" t="inlineStr">
         <is>
-          <t>18:32</t>
+          <t>18:31</t>
         </is>
       </c>
       <c r="C390" t="inlineStr">
@@ -10092,7 +10092,7 @@
         </is>
       </c>
       <c r="D390" t="n">
-        <v>35</v>
+        <v>98</v>
       </c>
       <c r="E390" t="inlineStr">
         <is>
@@ -10108,16 +10108,16 @@
       </c>
       <c r="B391" t="inlineStr">
         <is>
-          <t>18:34</t>
+          <t>18:32</t>
         </is>
       </c>
       <c r="C391" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D391" t="n">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E391" t="inlineStr">
         <is>
@@ -10128,21 +10128,21 @@
     <row r="392">
       <c r="A392" t="inlineStr">
         <is>
-          <t>17:42:07</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B392" t="inlineStr">
         <is>
-          <t>18:35</t>
+          <t>18:33</t>
         </is>
       </c>
       <c r="C392" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D392" t="n">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="E392" t="inlineStr">
         <is>
@@ -10153,21 +10153,21 @@
     <row r="393">
       <c r="A393" t="inlineStr">
         <is>
-          <t>16:53:56</t>
+          <t>17:57:31</t>
         </is>
       </c>
       <c r="B393" t="inlineStr">
         <is>
-          <t>18:39</t>
+          <t>18:34</t>
         </is>
       </c>
       <c r="C393" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D393" t="n">
-        <v>106</v>
+        <v>37</v>
       </c>
       <c r="E393" t="inlineStr">
         <is>
@@ -10178,21 +10178,21 @@
     <row r="394">
       <c r="A394" t="inlineStr">
         <is>
-          <t>17:57:31</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B394" t="inlineStr">
         <is>
-          <t>18:40</t>
+          <t>18:35</t>
         </is>
       </c>
       <c r="C394" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D394" t="n">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="E394" t="inlineStr">
         <is>
@@ -10208,16 +10208,16 @@
       </c>
       <c r="B395" t="inlineStr">
         <is>
-          <t>18:47</t>
+          <t>18:39</t>
         </is>
       </c>
       <c r="C395" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D395" t="n">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="E395" t="inlineStr">
         <is>
@@ -10233,16 +10233,16 @@
       </c>
       <c r="B396" t="inlineStr">
         <is>
-          <t>18:48</t>
+          <t>18:40</t>
         </is>
       </c>
       <c r="C396" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D396" t="n">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="E396" t="inlineStr">
         <is>
@@ -10253,21 +10253,21 @@
     <row r="397">
       <c r="A397" t="inlineStr">
         <is>
-          <t>17:57:31</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B397" t="inlineStr">
         <is>
-          <t>18:58</t>
+          <t>18:41</t>
         </is>
       </c>
       <c r="C397" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D397" t="n">
-        <v>61</v>
+        <v>23</v>
       </c>
       <c r="E397" t="inlineStr">
         <is>
@@ -10278,21 +10278,21 @@
     <row r="398">
       <c r="A398" t="inlineStr">
         <is>
-          <t>17:42:07</t>
+          <t>16:53:56</t>
         </is>
       </c>
       <c r="B398" t="inlineStr">
         <is>
-          <t>18:59</t>
+          <t>18:47</t>
         </is>
       </c>
       <c r="C398" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D398" t="n">
-        <v>77</v>
+        <v>114</v>
       </c>
       <c r="E398" t="inlineStr">
         <is>
@@ -10308,16 +10308,16 @@
       </c>
       <c r="B399" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>18:48</t>
         </is>
       </c>
       <c r="C399" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D399" t="n">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="E399" t="inlineStr">
         <is>
@@ -10328,21 +10328,21 @@
     <row r="400">
       <c r="A400" t="inlineStr">
         <is>
-          <t>17:42:07</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B400" t="inlineStr">
         <is>
-          <t>19:05</t>
+          <t>18:49</t>
         </is>
       </c>
       <c r="C400" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D400" t="n">
-        <v>83</v>
+        <v>31</v>
       </c>
       <c r="E400" t="inlineStr">
         <is>
@@ -10353,21 +10353,21 @@
     <row r="401">
       <c r="A401" t="inlineStr">
         <is>
-          <t>17:57:31</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B401" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>18:57</t>
         </is>
       </c>
       <c r="C401" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D401" t="n">
-        <v>73</v>
+        <v>39</v>
       </c>
       <c r="E401" t="inlineStr">
         <is>
@@ -10378,21 +10378,21 @@
     <row r="402">
       <c r="A402" t="inlineStr">
         <is>
-          <t>17:42:07</t>
+          <t>17:57:31</t>
         </is>
       </c>
       <c r="B402" t="inlineStr">
         <is>
-          <t>19:11</t>
+          <t>18:58</t>
         </is>
       </c>
       <c r="C402" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D402" t="n">
-        <v>89</v>
+        <v>61</v>
       </c>
       <c r="E402" t="inlineStr">
         <is>
@@ -10403,21 +10403,21 @@
     <row r="403">
       <c r="A403" t="inlineStr">
         <is>
-          <t>17:57:31</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B403" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>18:59</t>
         </is>
       </c>
       <c r="C403" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D403" t="n">
-        <v>79</v>
+        <v>41</v>
       </c>
       <c r="E403" t="inlineStr">
         <is>
@@ -10428,21 +10428,21 @@
     <row r="404">
       <c r="A404" t="inlineStr">
         <is>
-          <t>17:42:07</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B404" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>19:01</t>
         </is>
       </c>
       <c r="C404" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D404" t="n">
-        <v>95</v>
+        <v>43</v>
       </c>
       <c r="E404" t="inlineStr">
         <is>
@@ -10458,16 +10458,16 @@
       </c>
       <c r="B405" t="inlineStr">
         <is>
-          <t>19:20</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="C405" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D405" t="n">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="E405" t="inlineStr">
         <is>
@@ -10478,21 +10478,21 @@
     <row r="406">
       <c r="A406" t="inlineStr">
         <is>
-          <t>17:57:31</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B406" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>19:05</t>
         </is>
       </c>
       <c r="C406" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D406" t="n">
-        <v>84</v>
+        <v>47</v>
       </c>
       <c r="E406" t="inlineStr">
         <is>
@@ -10503,21 +10503,21 @@
     <row r="407">
       <c r="A407" t="inlineStr">
         <is>
-          <t>17:57:31</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B407" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>19:05</t>
         </is>
       </c>
       <c r="C407" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D407" t="n">
-        <v>93</v>
+        <v>47</v>
       </c>
       <c r="E407" t="inlineStr">
         <is>
@@ -10533,16 +10533,16 @@
       </c>
       <c r="B408" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="C408" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D408" t="n">
-        <v>103</v>
+        <v>73</v>
       </c>
       <c r="E408" t="inlineStr">
         <is>
@@ -10553,21 +10553,21 @@
     <row r="409">
       <c r="A409" t="inlineStr">
         <is>
-          <t>17:57:31</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B409" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>19:11</t>
         </is>
       </c>
       <c r="C409" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D409" t="n">
-        <v>113</v>
+        <v>53</v>
       </c>
       <c r="E409" t="inlineStr">
         <is>
@@ -10578,21 +10578,21 @@
     <row r="410">
       <c r="A410" t="inlineStr">
         <is>
-          <t>17:57:31</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B410" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>19:13</t>
         </is>
       </c>
       <c r="C410" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D410" t="n">
-        <v>113</v>
+        <v>55</v>
       </c>
       <c r="E410" t="inlineStr">
         <is>
@@ -10608,18 +10608,443 @@
       </c>
       <c r="B411" t="inlineStr">
         <is>
+          <t>19:16</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D411" t="n">
+        <v>79</v>
+      </c>
+      <c r="E411" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>18:18:12</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>19:17</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D412" t="n">
+        <v>59</v>
+      </c>
+      <c r="E412" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>17:57:31</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>19:20</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D413" t="n">
+        <v>83</v>
+      </c>
+      <c r="E413" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>18:18:12</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>19:21</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D414" t="n">
+        <v>63</v>
+      </c>
+      <c r="E414" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>17:57:31</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>19:21</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D415" t="n">
+        <v>84</v>
+      </c>
+      <c r="E415" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>18:18:12</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>19:22</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D416" t="n">
+        <v>64</v>
+      </c>
+      <c r="E416" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>18:18:12</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>19:29</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D417" t="n">
+        <v>71</v>
+      </c>
+      <c r="E417" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>18:18:12</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>19:30</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D418" t="n">
+        <v>72</v>
+      </c>
+      <c r="E418" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>18:18:12</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>19:40</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D419" t="n">
+        <v>82</v>
+      </c>
+      <c r="E419" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>17:57:31</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>19:50</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D420" t="n">
+        <v>113</v>
+      </c>
+      <c r="E420" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>17:57:31</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>19:50</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D421" t="n">
+        <v>113</v>
+      </c>
+      <c r="E421" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>18:18:12</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
           <t>19:51</t>
         </is>
       </c>
-      <c r="C411" t="inlineStr">
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D422" t="n">
+        <v>93</v>
+      </c>
+      <c r="E422" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>18:18:12</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>19:51</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D423" t="n">
+        <v>93</v>
+      </c>
+      <c r="E423" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>17:57:31</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>19:51</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
         <is>
           <t>81_EL PELIGRO</t>
         </is>
       </c>
-      <c r="D411" t="n">
+      <c r="D424" t="n">
         <v>114</v>
       </c>
-      <c r="E411" t="inlineStr">
+      <c r="E424" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>18:18:12</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>19:52</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D425" t="n">
+        <v>94</v>
+      </c>
+      <c r="E425" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>18:18:12</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D426" t="n">
+        <v>102</v>
+      </c>
+      <c r="E426" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>18:18:12</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>20:10</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D427" t="n">
+        <v>112</v>
+      </c>
+      <c r="E427" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>18:18:12</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>20:11</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D428" t="n">
+        <v>113</v>
+      </c>
+      <c r="E428" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -10654,7 +11079,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:57:31</t>
+          <t>Última actualización: 18:18:12</t>
         </is>
       </c>
     </row>
@@ -11745,7 +12170,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>17:57:31</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -11759,7 +12184,7 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -11795,7 +12220,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>17:42:07</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -11809,7 +12234,7 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>77</v>
+        <v>41</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -11820,7 +12245,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>17:57:31</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -11834,7 +12259,7 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -11871,7 +12296,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:57:31</t>
+          <t>Última actualización: 18:18:12</t>
         </is>
       </c>
     </row>
@@ -13212,7 +13637,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>17:57:31</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -13226,7 +13651,7 @@
         </is>
       </c>
       <c r="D58" t="n">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -13237,7 +13662,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>17:57:31</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -13251,7 +13676,7 @@
         </is>
       </c>
       <c r="D59" t="n">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -13262,7 +13687,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>17:57:31</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -13276,7 +13701,7 @@
         </is>
       </c>
       <c r="D60" t="n">
-        <v>117</v>
+        <v>96</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 854
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-23.xlsx
+++ b/data/horarios-141-2026-01-23.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E428"/>
+  <dimension ref="A1:E447"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:18:12</t>
+          <t>Última actualización: 18:36:52</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 423</t>
+          <t>Total filas: 442</t>
         </is>
       </c>
     </row>
@@ -1313,7 +1313,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>86_EST CHICA-ESC AGRARIA</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1338,7 +1338,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>86_EST CHICA-ESC AGRARIA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1778,7 +1778,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1788,11 +1788,11 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>17</v>
+        <v>84</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -1803,7 +1803,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1813,11 +1813,11 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D63" t="n">
@@ -1938,7 +1938,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -1953,7 +1953,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1963,11 +1963,11 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -1978,7 +1978,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -1988,11 +1988,11 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2528,7 +2528,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -2538,11 +2538,11 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -2553,7 +2553,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2563,11 +2563,11 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -2903,7 +2903,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>08:48:01</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -2913,11 +2913,11 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -2928,7 +2928,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>08:48:01</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -2938,11 +2938,11 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D104" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -3153,7 +3153,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3163,11 +3163,11 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>27</v>
+        <v>115</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3188,7 +3188,7 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D114" t="n">
@@ -3203,7 +3203,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
@@ -3213,11 +3213,11 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D115" t="n">
-        <v>115</v>
+        <v>27</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -3278,7 +3278,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>09:33:33</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -3288,11 +3288,11 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D118" t="n">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -3303,7 +3303,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>09:33:33</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -3313,11 +3313,11 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D119" t="n">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -3388,7 +3388,7 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D122" t="n">
@@ -3413,7 +3413,7 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D123" t="n">
@@ -4853,7 +4853,7 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>11:22:44</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
@@ -4863,11 +4863,11 @@
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D181" t="n">
-        <v>44</v>
+        <v>4</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
@@ -4878,7 +4878,7 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>11:22:44</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
@@ -4888,11 +4888,11 @@
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D182" t="n">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
@@ -4928,7 +4928,7 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>10:57:35</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
@@ -4938,11 +4938,11 @@
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D184" t="n">
-        <v>77</v>
+        <v>12</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -4953,7 +4953,7 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>10:57:35</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
@@ -4963,11 +4963,11 @@
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D185" t="n">
-        <v>12</v>
+        <v>77</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -5003,7 +5003,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>10:27:29</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
@@ -5013,11 +5013,11 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D187" t="n">
-        <v>15</v>
+        <v>110</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -5028,7 +5028,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>10:27:29</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -5038,11 +5038,11 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D188" t="n">
-        <v>110</v>
+        <v>15</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5288,7 +5288,7 @@
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_179 Y 38</t>
         </is>
       </c>
       <c r="D198" t="n">
@@ -5338,7 +5338,7 @@
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>17_179 Y 38</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D200" t="n">
@@ -5528,7 +5528,7 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>12:54:24</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
@@ -5538,11 +5538,11 @@
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D208" t="n">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -5553,7 +5553,7 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>12:54:24</t>
+          <t>12:37:00</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
@@ -5563,11 +5563,11 @@
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D209" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -5813,7 +5813,7 @@
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D219" t="n">
@@ -5838,7 +5838,7 @@
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D220" t="n">
@@ -5988,7 +5988,7 @@
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D226" t="n">
@@ -6013,7 +6013,7 @@
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D227" t="n">
@@ -6238,7 +6238,7 @@
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D236" t="n">
@@ -6263,7 +6263,7 @@
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D237" t="n">
@@ -6313,7 +6313,7 @@
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D239" t="n">
@@ -6338,7 +6338,7 @@
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D240" t="n">
@@ -6353,7 +6353,7 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>13:51:20</t>
+          <t>12:37:00</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
@@ -6363,11 +6363,11 @@
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D241" t="n">
-        <v>6</v>
+        <v>80</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -6378,7 +6378,7 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>13:51:20</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
@@ -6388,11 +6388,11 @@
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D242" t="n">
-        <v>80</v>
+        <v>6</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -6403,7 +6403,7 @@
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>13:51:20</t>
+          <t>13:18:32</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
@@ -6413,11 +6413,11 @@
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D243" t="n">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -6428,7 +6428,7 @@
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>13:18:32</t>
+          <t>13:51:20</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
@@ -6438,11 +6438,11 @@
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D244" t="n">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -7013,7 +7013,7 @@
       </c>
       <c r="C267" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D267" t="n">
@@ -7038,7 +7038,7 @@
       </c>
       <c r="C268" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D268" t="n">
@@ -7238,7 +7238,7 @@
       </c>
       <c r="C276" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D276" t="n">
@@ -7263,7 +7263,7 @@
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D277" t="n">
@@ -7478,7 +7478,7 @@
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>14:55:42</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
@@ -7488,11 +7488,11 @@
       </c>
       <c r="C286" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D286" t="n">
-        <v>51</v>
+        <v>25</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
@@ -7503,7 +7503,7 @@
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>14:55:42</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
@@ -7513,11 +7513,11 @@
       </c>
       <c r="C287" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D287" t="n">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
@@ -7553,7 +7553,7 @@
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>14:19:39</t>
+          <t>14:55:42</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
@@ -7563,11 +7563,11 @@
       </c>
       <c r="C289" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D289" t="n">
-        <v>94</v>
+        <v>58</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
@@ -7578,7 +7578,7 @@
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>14:55:42</t>
+          <t>14:19:39</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
@@ -7588,11 +7588,11 @@
       </c>
       <c r="C290" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D290" t="n">
-        <v>58</v>
+        <v>94</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
@@ -7628,7 +7628,7 @@
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
@@ -7638,11 +7638,11 @@
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D292" t="n">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
@@ -7653,7 +7653,7 @@
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
@@ -7663,11 +7663,11 @@
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D293" t="n">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
@@ -7678,7 +7678,7 @@
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
@@ -7688,11 +7688,11 @@
       </c>
       <c r="C294" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D294" t="n">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
@@ -7703,7 +7703,7 @@
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
@@ -7713,11 +7713,11 @@
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D295" t="n">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
@@ -7853,7 +7853,7 @@
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>14:45:15</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
@@ -7863,11 +7863,11 @@
       </c>
       <c r="C301" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D301" t="n">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="E301" t="inlineStr">
         <is>
@@ -7878,7 +7878,7 @@
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>14:45:15</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
@@ -7888,11 +7888,11 @@
       </c>
       <c r="C302" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D302" t="n">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="E302" t="inlineStr">
         <is>
@@ -8053,7 +8053,7 @@
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>16:19:35</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
@@ -8063,11 +8063,11 @@
       </c>
       <c r="C309" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D309" t="n">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
@@ -8078,7 +8078,7 @@
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:19:35</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
@@ -8088,11 +8088,11 @@
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D310" t="n">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="E310" t="inlineStr">
         <is>
@@ -8203,7 +8203,7 @@
     <row r="315">
       <c r="A315" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:19:35</t>
         </is>
       </c>
       <c r="B315" t="inlineStr">
@@ -8213,11 +8213,11 @@
       </c>
       <c r="C315" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D315" t="n">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="E315" t="inlineStr">
         <is>
@@ -8228,7 +8228,7 @@
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
-          <t>16:19:35</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
@@ -8238,11 +8238,11 @@
       </c>
       <c r="C316" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D316" t="n">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="E316" t="inlineStr">
         <is>
@@ -8528,7 +8528,7 @@
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>16:46:26</t>
+          <t>16:36:35</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
@@ -8538,11 +8538,11 @@
       </c>
       <c r="C328" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D328" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E328" t="inlineStr">
         <is>
@@ -8553,7 +8553,7 @@
     <row r="329">
       <c r="A329" t="inlineStr">
         <is>
-          <t>16:36:35</t>
+          <t>16:46:26</t>
         </is>
       </c>
       <c r="B329" t="inlineStr">
@@ -8563,11 +8563,11 @@
       </c>
       <c r="C329" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D329" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="E329" t="inlineStr">
         <is>
@@ -8738,7 +8738,7 @@
       </c>
       <c r="C336" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D336" t="n">
@@ -8763,7 +8763,7 @@
       </c>
       <c r="C337" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D337" t="n">
@@ -8888,7 +8888,7 @@
       </c>
       <c r="C342" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D342" t="n">
@@ -8913,7 +8913,7 @@
       </c>
       <c r="C343" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D343" t="n">
@@ -8938,7 +8938,7 @@
       </c>
       <c r="C344" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D344" t="n">
@@ -8963,7 +8963,7 @@
       </c>
       <c r="C345" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D345" t="n">
@@ -8988,7 +8988,7 @@
       </c>
       <c r="C346" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D346" t="n">
@@ -9338,7 +9338,7 @@
       </c>
       <c r="C360" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D360" t="n">
@@ -9363,7 +9363,7 @@
       </c>
       <c r="C361" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D361" t="n">
@@ -9663,7 +9663,7 @@
       </c>
       <c r="C373" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D373" t="n">
@@ -9688,7 +9688,7 @@
       </c>
       <c r="C374" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D374" t="n">
@@ -9838,7 +9838,7 @@
       </c>
       <c r="C380" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D380" t="n">
@@ -9863,7 +9863,7 @@
       </c>
       <c r="C381" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D381" t="n">
@@ -10203,21 +10203,21 @@
     <row r="395">
       <c r="A395" t="inlineStr">
         <is>
-          <t>16:53:56</t>
+          <t>18:36:52</t>
         </is>
       </c>
       <c r="B395" t="inlineStr">
         <is>
-          <t>18:39</t>
+          <t>18:37</t>
         </is>
       </c>
       <c r="C395" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D395" t="n">
-        <v>106</v>
+        <v>1</v>
       </c>
       <c r="E395" t="inlineStr">
         <is>
@@ -10228,21 +10228,21 @@
     <row r="396">
       <c r="A396" t="inlineStr">
         <is>
-          <t>17:57:31</t>
+          <t>18:36:52</t>
         </is>
       </c>
       <c r="B396" t="inlineStr">
         <is>
-          <t>18:40</t>
+          <t>18:37</t>
         </is>
       </c>
       <c r="C396" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D396" t="n">
-        <v>43</v>
+        <v>1</v>
       </c>
       <c r="E396" t="inlineStr">
         <is>
@@ -10253,21 +10253,21 @@
     <row r="397">
       <c r="A397" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>16:53:56</t>
         </is>
       </c>
       <c r="B397" t="inlineStr">
         <is>
-          <t>18:41</t>
+          <t>18:39</t>
         </is>
       </c>
       <c r="C397" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D397" t="n">
-        <v>23</v>
+        <v>106</v>
       </c>
       <c r="E397" t="inlineStr">
         <is>
@@ -10278,21 +10278,21 @@
     <row r="398">
       <c r="A398" t="inlineStr">
         <is>
-          <t>16:53:56</t>
+          <t>18:36:52</t>
         </is>
       </c>
       <c r="B398" t="inlineStr">
         <is>
-          <t>18:47</t>
+          <t>18:40</t>
         </is>
       </c>
       <c r="C398" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D398" t="n">
-        <v>114</v>
+        <v>4</v>
       </c>
       <c r="E398" t="inlineStr">
         <is>
@@ -10308,16 +10308,16 @@
       </c>
       <c r="B399" t="inlineStr">
         <is>
-          <t>18:48</t>
+          <t>18:40</t>
         </is>
       </c>
       <c r="C399" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D399" t="n">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="E399" t="inlineStr">
         <is>
@@ -10333,16 +10333,16 @@
       </c>
       <c r="B400" t="inlineStr">
         <is>
-          <t>18:49</t>
+          <t>18:41</t>
         </is>
       </c>
       <c r="C400" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D400" t="n">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="E400" t="inlineStr">
         <is>
@@ -10353,21 +10353,21 @@
     <row r="401">
       <c r="A401" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>18:36:52</t>
         </is>
       </c>
       <c r="B401" t="inlineStr">
         <is>
-          <t>18:57</t>
+          <t>18:47</t>
         </is>
       </c>
       <c r="C401" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D401" t="n">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="E401" t="inlineStr">
         <is>
@@ -10383,16 +10383,16 @@
       </c>
       <c r="B402" t="inlineStr">
         <is>
-          <t>18:58</t>
+          <t>18:48</t>
         </is>
       </c>
       <c r="C402" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D402" t="n">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="E402" t="inlineStr">
         <is>
@@ -10408,16 +10408,16 @@
       </c>
       <c r="B403" t="inlineStr">
         <is>
-          <t>18:59</t>
+          <t>18:49</t>
         </is>
       </c>
       <c r="C403" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D403" t="n">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="E403" t="inlineStr">
         <is>
@@ -10428,21 +10428,21 @@
     <row r="404">
       <c r="A404" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>18:36:52</t>
         </is>
       </c>
       <c r="B404" t="inlineStr">
         <is>
-          <t>19:01</t>
+          <t>18:56</t>
         </is>
       </c>
       <c r="C404" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D404" t="n">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="E404" t="inlineStr">
         <is>
@@ -10453,21 +10453,21 @@
     <row r="405">
       <c r="A405" t="inlineStr">
         <is>
-          <t>17:57:31</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B405" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>18:57</t>
         </is>
       </c>
       <c r="C405" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D405" t="n">
-        <v>67</v>
+        <v>39</v>
       </c>
       <c r="E405" t="inlineStr">
         <is>
@@ -10478,21 +10478,21 @@
     <row r="406">
       <c r="A406" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>18:36:52</t>
         </is>
       </c>
       <c r="B406" t="inlineStr">
         <is>
-          <t>19:05</t>
+          <t>18:58</t>
         </is>
       </c>
       <c r="C406" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D406" t="n">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="E406" t="inlineStr">
         <is>
@@ -10508,16 +10508,16 @@
       </c>
       <c r="B407" t="inlineStr">
         <is>
-          <t>19:05</t>
+          <t>18:59</t>
         </is>
       </c>
       <c r="C407" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D407" t="n">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="E407" t="inlineStr">
         <is>
@@ -10528,21 +10528,21 @@
     <row r="408">
       <c r="A408" t="inlineStr">
         <is>
-          <t>17:57:31</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B408" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>19:01</t>
         </is>
       </c>
       <c r="C408" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D408" t="n">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="E408" t="inlineStr">
         <is>
@@ -10553,21 +10553,21 @@
     <row r="409">
       <c r="A409" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>18:36:52</t>
         </is>
       </c>
       <c r="B409" t="inlineStr">
         <is>
-          <t>19:11</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="C409" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D409" t="n">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="E409" t="inlineStr">
         <is>
@@ -10578,21 +10578,21 @@
     <row r="410">
       <c r="A410" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>18:36:52</t>
         </is>
       </c>
       <c r="B410" t="inlineStr">
         <is>
-          <t>19:13</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="C410" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D410" t="n">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="E410" t="inlineStr">
         <is>
@@ -10603,21 +10603,21 @@
     <row r="411">
       <c r="A411" t="inlineStr">
         <is>
-          <t>17:57:31</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B411" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>19:05</t>
         </is>
       </c>
       <c r="C411" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D411" t="n">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="E411" t="inlineStr">
         <is>
@@ -10633,16 +10633,16 @@
       </c>
       <c r="B412" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>19:05</t>
         </is>
       </c>
       <c r="C412" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D412" t="n">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="E412" t="inlineStr">
         <is>
@@ -10653,21 +10653,21 @@
     <row r="413">
       <c r="A413" t="inlineStr">
         <is>
-          <t>17:57:31</t>
+          <t>18:36:52</t>
         </is>
       </c>
       <c r="B413" t="inlineStr">
         <is>
-          <t>19:20</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="C413" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D413" t="n">
-        <v>83</v>
+        <v>34</v>
       </c>
       <c r="E413" t="inlineStr">
         <is>
@@ -10683,16 +10683,16 @@
       </c>
       <c r="B414" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>19:11</t>
         </is>
       </c>
       <c r="C414" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D414" t="n">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E414" t="inlineStr">
         <is>
@@ -10703,21 +10703,21 @@
     <row r="415">
       <c r="A415" t="inlineStr">
         <is>
-          <t>17:57:31</t>
+          <t>18:36:52</t>
         </is>
       </c>
       <c r="B415" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="C415" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D415" t="n">
-        <v>84</v>
+        <v>36</v>
       </c>
       <c r="E415" t="inlineStr">
         <is>
@@ -10733,16 +10733,16 @@
       </c>
       <c r="B416" t="inlineStr">
         <is>
-          <t>19:22</t>
+          <t>19:13</t>
         </is>
       </c>
       <c r="C416" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D416" t="n">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="E416" t="inlineStr">
         <is>
@@ -10753,12 +10753,12 @@
     <row r="417">
       <c r="A417" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>18:36:52</t>
         </is>
       </c>
       <c r="B417" t="inlineStr">
         <is>
-          <t>19:29</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="C417" t="inlineStr">
@@ -10767,7 +10767,7 @@
         </is>
       </c>
       <c r="D417" t="n">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="E417" t="inlineStr">
         <is>
@@ -10778,21 +10778,21 @@
     <row r="418">
       <c r="A418" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>18:36:52</t>
         </is>
       </c>
       <c r="B418" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="C418" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D418" t="n">
-        <v>72</v>
+        <v>40</v>
       </c>
       <c r="E418" t="inlineStr">
         <is>
@@ -10808,16 +10808,16 @@
       </c>
       <c r="B419" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="C419" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D419" t="n">
-        <v>82</v>
+        <v>59</v>
       </c>
       <c r="E419" t="inlineStr">
         <is>
@@ -10828,21 +10828,21 @@
     <row r="420">
       <c r="A420" t="inlineStr">
         <is>
-          <t>17:57:31</t>
+          <t>18:36:52</t>
         </is>
       </c>
       <c r="B420" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>19:20</t>
         </is>
       </c>
       <c r="C420" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D420" t="n">
-        <v>113</v>
+        <v>44</v>
       </c>
       <c r="E420" t="inlineStr">
         <is>
@@ -10853,21 +10853,21 @@
     <row r="421">
       <c r="A421" t="inlineStr">
         <is>
-          <t>17:57:31</t>
+          <t>18:36:52</t>
         </is>
       </c>
       <c r="B421" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>19:20</t>
         </is>
       </c>
       <c r="C421" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D421" t="n">
-        <v>113</v>
+        <v>44</v>
       </c>
       <c r="E421" t="inlineStr">
         <is>
@@ -10883,16 +10883,16 @@
       </c>
       <c r="B422" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="C422" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D422" t="n">
-        <v>93</v>
+        <v>63</v>
       </c>
       <c r="E422" t="inlineStr">
         <is>
@@ -10903,21 +10903,21 @@
     <row r="423">
       <c r="A423" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>18:36:52</t>
         </is>
       </c>
       <c r="B423" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="C423" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D423" t="n">
-        <v>93</v>
+        <v>45</v>
       </c>
       <c r="E423" t="inlineStr">
         <is>
@@ -10928,21 +10928,21 @@
     <row r="424">
       <c r="A424" t="inlineStr">
         <is>
-          <t>17:57:31</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B424" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>19:22</t>
         </is>
       </c>
       <c r="C424" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D424" t="n">
-        <v>114</v>
+        <v>64</v>
       </c>
       <c r="E424" t="inlineStr">
         <is>
@@ -10953,21 +10953,21 @@
     <row r="425">
       <c r="A425" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>18:36:52</t>
         </is>
       </c>
       <c r="B425" t="inlineStr">
         <is>
-          <t>19:52</t>
+          <t>19:28</t>
         </is>
       </c>
       <c r="C425" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D425" t="n">
-        <v>94</v>
+        <v>52</v>
       </c>
       <c r="E425" t="inlineStr">
         <is>
@@ -10978,21 +10978,21 @@
     <row r="426">
       <c r="A426" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>18:36:52</t>
         </is>
       </c>
       <c r="B426" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>19:29</t>
         </is>
       </c>
       <c r="C426" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D426" t="n">
-        <v>102</v>
+        <v>53</v>
       </c>
       <c r="E426" t="inlineStr">
         <is>
@@ -11008,7 +11008,7 @@
       </c>
       <c r="B427" t="inlineStr">
         <is>
-          <t>20:10</t>
+          <t>19:29</t>
         </is>
       </c>
       <c r="C427" t="inlineStr">
@@ -11017,7 +11017,7 @@
         </is>
       </c>
       <c r="D427" t="n">
-        <v>112</v>
+        <v>71</v>
       </c>
       <c r="E427" t="inlineStr">
         <is>
@@ -11033,18 +11033,493 @@
       </c>
       <c r="B428" t="inlineStr">
         <is>
+          <t>19:30</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D428" t="n">
+        <v>72</v>
+      </c>
+      <c r="E428" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>18:36:52</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>19:39</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D429" t="n">
+        <v>63</v>
+      </c>
+      <c r="E429" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>18:18:12</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>19:40</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D430" t="n">
+        <v>82</v>
+      </c>
+      <c r="E430" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>18:36:52</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>19:49</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D431" t="n">
+        <v>73</v>
+      </c>
+      <c r="E431" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>18:36:52</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>19:50</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D432" t="n">
+        <v>74</v>
+      </c>
+      <c r="E432" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>17:57:31</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>19:50</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D433" t="n">
+        <v>113</v>
+      </c>
+      <c r="E433" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>18:18:12</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>19:51</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D434" t="n">
+        <v>93</v>
+      </c>
+      <c r="E434" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>18:36:52</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>19:51</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D435" t="n">
+        <v>75</v>
+      </c>
+      <c r="E435" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>18:18:12</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>19:51</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D436" t="n">
+        <v>93</v>
+      </c>
+      <c r="E436" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>18:18:12</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>19:52</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D437" t="n">
+        <v>94</v>
+      </c>
+      <c r="E437" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>18:36:52</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>19:59</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D438" t="n">
+        <v>83</v>
+      </c>
+      <c r="E438" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>18:36:52</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D439" t="n">
+        <v>84</v>
+      </c>
+      <c r="E439" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>18:18:12</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D440" t="n">
+        <v>102</v>
+      </c>
+      <c r="E440" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>18:18:12</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>20:10</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D441" t="n">
+        <v>112</v>
+      </c>
+      <c r="E441" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>18:36:52</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>20:10</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D442" t="n">
+        <v>94</v>
+      </c>
+      <c r="E442" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>18:18:12</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
           <t>20:11</t>
         </is>
       </c>
-      <c r="C428" t="inlineStr">
+      <c r="C443" t="inlineStr">
         <is>
           <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
-      <c r="D428" t="n">
+      <c r="D443" t="n">
         <v>113</v>
       </c>
-      <c r="E428" t="inlineStr">
+      <c r="E443" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>18:36:52</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>20:20</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D444" t="n">
+        <v>104</v>
+      </c>
+      <c r="E444" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>18:36:52</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>20:22</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D445" t="n">
+        <v>106</v>
+      </c>
+      <c r="E445" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>18:36:52</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>20:23</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D446" t="n">
+        <v>107</v>
+      </c>
+      <c r="E446" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>18:36:52</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>20:30</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D447" t="n">
+        <v>114</v>
+      </c>
+      <c r="E447" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -11061,7 +11536,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11079,14 +11554,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:18:12</t>
+          <t>Última actualización: 18:36:52</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 46</t>
+          <t>Total filas: 48</t>
         </is>
       </c>
     </row>
@@ -12195,7 +12670,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>17:57:31</t>
+          <t>18:36:52</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -12209,7 +12684,7 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>61</v>
+        <v>22</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -12245,23 +12720,73 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
+          <t>18:36:52</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>19:39</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>63</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
           <t>18:18:12</t>
         </is>
       </c>
-      <c r="B51" t="inlineStr">
+      <c r="B52" t="inlineStr">
         <is>
           <t>19:40</t>
         </is>
       </c>
-      <c r="C51" t="inlineStr">
+      <c r="C52" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D51" t="n">
+      <c r="D52" t="n">
         <v>82</v>
       </c>
-      <c r="E51" t="inlineStr">
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>18:36:52</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>20:23</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>107</v>
+      </c>
+      <c r="E53" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -12278,7 +12803,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E60"/>
+  <dimension ref="A1:E62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12296,14 +12821,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:18:12</t>
+          <t>Última actualización: 18:36:52</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 55</t>
+          <t>Total filas: 57</t>
         </is>
       </c>
     </row>
@@ -13612,7 +14137,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>16:53:56</t>
+          <t>18:36:52</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -13626,7 +14151,7 @@
         </is>
       </c>
       <c r="D57" t="n">
-        <v>118</v>
+        <v>15</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -13662,12 +14187,12 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>18:36:52</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>19:03</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -13676,7 +14201,7 @@
         </is>
       </c>
       <c r="D59" t="n">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -13692,18 +14217,68 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
+          <t>19:04</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>46</v>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>18:36:52</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>19:53</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>77</v>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>18:18:12</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
           <t>19:54</t>
         </is>
       </c>
-      <c r="C60" t="inlineStr">
+      <c r="C62" t="inlineStr">
         <is>
           <t>215C_LA PLATA</t>
         </is>
       </c>
-      <c r="D60" t="n">
+      <c r="D62" t="n">
         <v>96</v>
       </c>
-      <c r="E60" t="inlineStr">
+      <c r="E62" t="inlineStr">
         <is>
           <t>L6203</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 855
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-23.xlsx
+++ b/data/horarios-141-2026-01-23.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E447"/>
+  <dimension ref="A1:E452"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:36:52</t>
+          <t>Última actualización: 18:48:33</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 442</t>
+          <t>Total filas: 447</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1638,11 +1638,11 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>73</v>
+        <v>6</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -1653,7 +1653,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1663,11 +1663,11 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>6</v>
+        <v>73</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -1953,7 +1953,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1963,11 +1963,11 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -1978,7 +1978,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -1988,11 +1988,11 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2128,7 +2128,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -2138,11 +2138,11 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -2153,7 +2153,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -2163,11 +2163,11 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D73" t="n">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -2903,7 +2903,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>08:48:01</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -2913,11 +2913,11 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -2928,7 +2928,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>08:48:01</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -2938,11 +2938,11 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D104" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -3153,7 +3153,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3163,11 +3163,11 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>115</v>
+        <v>27</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3178,7 +3178,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
@@ -3188,11 +3188,11 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D114" t="n">
-        <v>27</v>
+        <v>115</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -3213,7 +3213,7 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D115" t="n">
@@ -3278,7 +3278,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>09:33:33</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -3288,11 +3288,11 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D118" t="n">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -3303,7 +3303,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>09:33:33</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -3313,11 +3313,11 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D119" t="n">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -3338,7 +3338,7 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D120" t="n">
@@ -3363,7 +3363,7 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D121" t="n">
@@ -3388,7 +3388,7 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D122" t="n">
@@ -3413,7 +3413,7 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D123" t="n">
@@ -4413,7 +4413,7 @@
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D163" t="n">
@@ -4438,7 +4438,7 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D164" t="n">
@@ -4928,7 +4928,7 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>10:57:35</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
@@ -4938,11 +4938,11 @@
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D184" t="n">
-        <v>12</v>
+        <v>77</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -4953,7 +4953,7 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>10:57:35</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
@@ -4963,11 +4963,11 @@
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D185" t="n">
-        <v>77</v>
+        <v>12</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -5528,7 +5528,7 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>12:54:24</t>
+          <t>12:37:00</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
@@ -5538,11 +5538,11 @@
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D208" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -5553,7 +5553,7 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>12:54:24</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
@@ -5563,11 +5563,11 @@
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D209" t="n">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -6138,7 +6138,7 @@
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D232" t="n">
@@ -6163,7 +6163,7 @@
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D233" t="n">
@@ -6238,7 +6238,7 @@
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D236" t="n">
@@ -6263,7 +6263,7 @@
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D237" t="n">
@@ -7478,7 +7478,7 @@
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>14:55:42</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
@@ -7488,11 +7488,11 @@
       </c>
       <c r="C286" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D286" t="n">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
@@ -7503,7 +7503,7 @@
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>14:55:42</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
@@ -7513,11 +7513,11 @@
       </c>
       <c r="C287" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D287" t="n">
-        <v>51</v>
+        <v>25</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
@@ -7728,7 +7728,7 @@
     <row r="296">
       <c r="A296" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
@@ -7738,11 +7738,11 @@
       </c>
       <c r="C296" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D296" t="n">
-        <v>36</v>
+        <v>2</v>
       </c>
       <c r="E296" t="inlineStr">
         <is>
@@ -7753,7 +7753,7 @@
     <row r="297">
       <c r="A297" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
@@ -7763,11 +7763,11 @@
       </c>
       <c r="C297" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D297" t="n">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="E297" t="inlineStr">
         <is>
@@ -8003,7 +8003,7 @@
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>16:19:35</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
@@ -8013,11 +8013,11 @@
       </c>
       <c r="C307" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D307" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="E307" t="inlineStr">
         <is>
@@ -8028,7 +8028,7 @@
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:19:35</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
@@ -8038,11 +8038,11 @@
       </c>
       <c r="C308" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D308" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="E308" t="inlineStr">
         <is>
@@ -8053,7 +8053,7 @@
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:19:35</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
@@ -8063,11 +8063,11 @@
       </c>
       <c r="C309" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D309" t="n">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
@@ -8103,7 +8103,7 @@
     <row r="311">
       <c r="A311" t="inlineStr">
         <is>
-          <t>16:19:35</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
@@ -8113,11 +8113,11 @@
       </c>
       <c r="C311" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D311" t="n">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="E311" t="inlineStr">
         <is>
@@ -8203,7 +8203,7 @@
     <row r="315">
       <c r="A315" t="inlineStr">
         <is>
-          <t>16:19:35</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B315" t="inlineStr">
@@ -8213,11 +8213,11 @@
       </c>
       <c r="C315" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D315" t="n">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="E315" t="inlineStr">
         <is>
@@ -8228,7 +8228,7 @@
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:19:35</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
@@ -8238,11 +8238,11 @@
       </c>
       <c r="C316" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D316" t="n">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="E316" t="inlineStr">
         <is>
@@ -8653,7 +8653,7 @@
     <row r="333">
       <c r="A333" t="inlineStr">
         <is>
-          <t>16:46:26</t>
+          <t>16:53:56</t>
         </is>
       </c>
       <c r="B333" t="inlineStr">
@@ -8663,11 +8663,11 @@
       </c>
       <c r="C333" t="inlineStr">
         <is>
-          <t>17_179 Y 38</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D333" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E333" t="inlineStr">
         <is>
@@ -8678,7 +8678,7 @@
     <row r="334">
       <c r="A334" t="inlineStr">
         <is>
-          <t>16:53:56</t>
+          <t>16:46:26</t>
         </is>
       </c>
       <c r="B334" t="inlineStr">
@@ -8688,11 +8688,11 @@
       </c>
       <c r="C334" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_179 Y 38</t>
         </is>
       </c>
       <c r="D334" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E334" t="inlineStr">
         <is>
@@ -8888,7 +8888,7 @@
       </c>
       <c r="C342" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D342" t="n">
@@ -8913,7 +8913,7 @@
       </c>
       <c r="C343" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D343" t="n">
@@ -8938,7 +8938,7 @@
       </c>
       <c r="C344" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D344" t="n">
@@ -9188,7 +9188,7 @@
       </c>
       <c r="C354" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D354" t="n">
@@ -9213,7 +9213,7 @@
       </c>
       <c r="C355" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D355" t="n">
@@ -9338,7 +9338,7 @@
       </c>
       <c r="C360" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D360" t="n">
@@ -9363,7 +9363,7 @@
       </c>
       <c r="C361" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D361" t="n">
@@ -9663,7 +9663,7 @@
       </c>
       <c r="C373" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D373" t="n">
@@ -9688,7 +9688,7 @@
       </c>
       <c r="C374" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D374" t="n">
@@ -10213,7 +10213,7 @@
       </c>
       <c r="C395" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D395" t="n">
@@ -10238,7 +10238,7 @@
       </c>
       <c r="C396" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D396" t="n">
@@ -10378,7 +10378,7 @@
     <row r="402">
       <c r="A402" t="inlineStr">
         <is>
-          <t>17:57:31</t>
+          <t>18:48:33</t>
         </is>
       </c>
       <c r="B402" t="inlineStr">
@@ -10392,7 +10392,7 @@
         </is>
       </c>
       <c r="D402" t="n">
-        <v>51</v>
+        <v>0</v>
       </c>
       <c r="E402" t="inlineStr">
         <is>
@@ -10403,7 +10403,7 @@
     <row r="403">
       <c r="A403" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>18:48:33</t>
         </is>
       </c>
       <c r="B403" t="inlineStr">
@@ -10413,11 +10413,11 @@
       </c>
       <c r="C403" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D403" t="n">
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="E403" t="inlineStr">
         <is>
@@ -10428,21 +10428,21 @@
     <row r="404">
       <c r="A404" t="inlineStr">
         <is>
-          <t>18:36:52</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B404" t="inlineStr">
         <is>
-          <t>18:56</t>
+          <t>18:49</t>
         </is>
       </c>
       <c r="C404" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D404" t="n">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="E404" t="inlineStr">
         <is>
@@ -10453,12 +10453,12 @@
     <row r="405">
       <c r="A405" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>18:48:33</t>
         </is>
       </c>
       <c r="B405" t="inlineStr">
         <is>
-          <t>18:57</t>
+          <t>18:56</t>
         </is>
       </c>
       <c r="C405" t="inlineStr">
@@ -10467,7 +10467,7 @@
         </is>
       </c>
       <c r="D405" t="n">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="E405" t="inlineStr">
         <is>
@@ -10478,21 +10478,21 @@
     <row r="406">
       <c r="A406" t="inlineStr">
         <is>
-          <t>18:36:52</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B406" t="inlineStr">
         <is>
-          <t>18:58</t>
+          <t>18:57</t>
         </is>
       </c>
       <c r="C406" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D406" t="n">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="E406" t="inlineStr">
         <is>
@@ -10503,12 +10503,12 @@
     <row r="407">
       <c r="A407" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>18:48:33</t>
         </is>
       </c>
       <c r="B407" t="inlineStr">
         <is>
-          <t>18:59</t>
+          <t>18:58</t>
         </is>
       </c>
       <c r="C407" t="inlineStr">
@@ -10517,7 +10517,7 @@
         </is>
       </c>
       <c r="D407" t="n">
-        <v>41</v>
+        <v>10</v>
       </c>
       <c r="E407" t="inlineStr">
         <is>
@@ -10533,16 +10533,16 @@
       </c>
       <c r="B408" t="inlineStr">
         <is>
-          <t>19:01</t>
+          <t>18:59</t>
         </is>
       </c>
       <c r="C408" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D408" t="n">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E408" t="inlineStr">
         <is>
@@ -10553,21 +10553,21 @@
     <row r="409">
       <c r="A409" t="inlineStr">
         <is>
-          <t>18:36:52</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B409" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>19:01</t>
         </is>
       </c>
       <c r="C409" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D409" t="n">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="E409" t="inlineStr">
         <is>
@@ -10578,7 +10578,7 @@
     <row r="410">
       <c r="A410" t="inlineStr">
         <is>
-          <t>18:36:52</t>
+          <t>18:48:33</t>
         </is>
       </c>
       <c r="B410" t="inlineStr">
@@ -10588,11 +10588,11 @@
       </c>
       <c r="C410" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D410" t="n">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="E410" t="inlineStr">
         <is>
@@ -10603,12 +10603,12 @@
     <row r="411">
       <c r="A411" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>18:48:33</t>
         </is>
       </c>
       <c r="B411" t="inlineStr">
         <is>
-          <t>19:05</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="C411" t="inlineStr">
@@ -10617,7 +10617,7 @@
         </is>
       </c>
       <c r="D411" t="n">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="E411" t="inlineStr">
         <is>
@@ -10638,7 +10638,7 @@
       </c>
       <c r="C412" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D412" t="n">
@@ -10653,21 +10653,21 @@
     <row r="413">
       <c r="A413" t="inlineStr">
         <is>
-          <t>18:36:52</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B413" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>19:05</t>
         </is>
       </c>
       <c r="C413" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D413" t="n">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="E413" t="inlineStr">
         <is>
@@ -10678,12 +10678,12 @@
     <row r="414">
       <c r="A414" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>18:48:33</t>
         </is>
       </c>
       <c r="B414" t="inlineStr">
         <is>
-          <t>19:11</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="C414" t="inlineStr">
@@ -10692,7 +10692,7 @@
         </is>
       </c>
       <c r="D414" t="n">
-        <v>53</v>
+        <v>22</v>
       </c>
       <c r="E414" t="inlineStr">
         <is>
@@ -10703,21 +10703,21 @@
     <row r="415">
       <c r="A415" t="inlineStr">
         <is>
-          <t>18:36:52</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B415" t="inlineStr">
         <is>
-          <t>19:12</t>
+          <t>19:11</t>
         </is>
       </c>
       <c r="C415" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D415" t="n">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="E415" t="inlineStr">
         <is>
@@ -10728,12 +10728,12 @@
     <row r="416">
       <c r="A416" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>18:48:33</t>
         </is>
       </c>
       <c r="B416" t="inlineStr">
         <is>
-          <t>19:13</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="C416" t="inlineStr">
@@ -10742,7 +10742,7 @@
         </is>
       </c>
       <c r="D416" t="n">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="E416" t="inlineStr">
         <is>
@@ -10753,21 +10753,21 @@
     <row r="417">
       <c r="A417" t="inlineStr">
         <is>
-          <t>18:36:52</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B417" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>19:13</t>
         </is>
       </c>
       <c r="C417" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D417" t="n">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="E417" t="inlineStr">
         <is>
@@ -10778,7 +10778,7 @@
     <row r="418">
       <c r="A418" t="inlineStr">
         <is>
-          <t>18:36:52</t>
+          <t>18:48:33</t>
         </is>
       </c>
       <c r="B418" t="inlineStr">
@@ -10788,11 +10788,11 @@
       </c>
       <c r="C418" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D418" t="n">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="E418" t="inlineStr">
         <is>
@@ -10803,12 +10803,12 @@
     <row r="419">
       <c r="A419" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>18:48:33</t>
         </is>
       </c>
       <c r="B419" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="C419" t="inlineStr">
@@ -10817,7 +10817,7 @@
         </is>
       </c>
       <c r="D419" t="n">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="E419" t="inlineStr">
         <is>
@@ -10828,21 +10828,21 @@
     <row r="420">
       <c r="A420" t="inlineStr">
         <is>
-          <t>18:36:52</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B420" t="inlineStr">
         <is>
-          <t>19:20</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="C420" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D420" t="n">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="E420" t="inlineStr">
         <is>
@@ -10853,7 +10853,7 @@
     <row r="421">
       <c r="A421" t="inlineStr">
         <is>
-          <t>18:36:52</t>
+          <t>18:48:33</t>
         </is>
       </c>
       <c r="B421" t="inlineStr">
@@ -10863,11 +10863,11 @@
       </c>
       <c r="C421" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D421" t="n">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="E421" t="inlineStr">
         <is>
@@ -10878,21 +10878,21 @@
     <row r="422">
       <c r="A422" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>18:48:33</t>
         </is>
       </c>
       <c r="B422" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>19:20</t>
         </is>
       </c>
       <c r="C422" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D422" t="n">
-        <v>63</v>
+        <v>32</v>
       </c>
       <c r="E422" t="inlineStr">
         <is>
@@ -10903,7 +10903,7 @@
     <row r="423">
       <c r="A423" t="inlineStr">
         <is>
-          <t>18:36:52</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B423" t="inlineStr">
@@ -10913,11 +10913,11 @@
       </c>
       <c r="C423" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D423" t="n">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="E423" t="inlineStr">
         <is>
@@ -10928,12 +10928,12 @@
     <row r="424">
       <c r="A424" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>18:48:33</t>
         </is>
       </c>
       <c r="B424" t="inlineStr">
         <is>
-          <t>19:22</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="C424" t="inlineStr">
@@ -10942,7 +10942,7 @@
         </is>
       </c>
       <c r="D424" t="n">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="E424" t="inlineStr">
         <is>
@@ -10953,21 +10953,21 @@
     <row r="425">
       <c r="A425" t="inlineStr">
         <is>
-          <t>18:36:52</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B425" t="inlineStr">
         <is>
-          <t>19:28</t>
+          <t>19:22</t>
         </is>
       </c>
       <c r="C425" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D425" t="n">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="E425" t="inlineStr">
         <is>
@@ -10983,16 +10983,16 @@
       </c>
       <c r="B426" t="inlineStr">
         <is>
-          <t>19:29</t>
+          <t>19:28</t>
         </is>
       </c>
       <c r="C426" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D426" t="n">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E426" t="inlineStr">
         <is>
@@ -11028,12 +11028,12 @@
     <row r="428">
       <c r="A428" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>18:36:52</t>
         </is>
       </c>
       <c r="B428" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>19:29</t>
         </is>
       </c>
       <c r="C428" t="inlineStr">
@@ -11042,7 +11042,7 @@
         </is>
       </c>
       <c r="D428" t="n">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="E428" t="inlineStr">
         <is>
@@ -11053,21 +11053,21 @@
     <row r="429">
       <c r="A429" t="inlineStr">
         <is>
-          <t>18:36:52</t>
+          <t>18:48:33</t>
         </is>
       </c>
       <c r="B429" t="inlineStr">
         <is>
-          <t>19:39</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="C429" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D429" t="n">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="E429" t="inlineStr">
         <is>
@@ -11078,21 +11078,21 @@
     <row r="430">
       <c r="A430" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>18:48:33</t>
         </is>
       </c>
       <c r="B430" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="C430" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D430" t="n">
-        <v>82</v>
+        <v>42</v>
       </c>
       <c r="E430" t="inlineStr">
         <is>
@@ -11103,21 +11103,21 @@
     <row r="431">
       <c r="A431" t="inlineStr">
         <is>
-          <t>18:36:52</t>
+          <t>18:48:33</t>
         </is>
       </c>
       <c r="B431" t="inlineStr">
         <is>
-          <t>19:49</t>
+          <t>19:34</t>
         </is>
       </c>
       <c r="C431" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D431" t="n">
-        <v>73</v>
+        <v>46</v>
       </c>
       <c r="E431" t="inlineStr">
         <is>
@@ -11133,16 +11133,16 @@
       </c>
       <c r="B432" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>19:39</t>
         </is>
       </c>
       <c r="C432" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D432" t="n">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="E432" t="inlineStr">
         <is>
@@ -11153,21 +11153,21 @@
     <row r="433">
       <c r="A433" t="inlineStr">
         <is>
-          <t>17:57:31</t>
+          <t>18:48:33</t>
         </is>
       </c>
       <c r="B433" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="C433" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D433" t="n">
-        <v>113</v>
+        <v>52</v>
       </c>
       <c r="E433" t="inlineStr">
         <is>
@@ -11178,12 +11178,12 @@
     <row r="434">
       <c r="A434" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>18:36:52</t>
         </is>
       </c>
       <c r="B434" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>19:49</t>
         </is>
       </c>
       <c r="C434" t="inlineStr">
@@ -11192,7 +11192,7 @@
         </is>
       </c>
       <c r="D434" t="n">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="E434" t="inlineStr">
         <is>
@@ -11203,21 +11203,21 @@
     <row r="435">
       <c r="A435" t="inlineStr">
         <is>
-          <t>18:36:52</t>
+          <t>18:48:33</t>
         </is>
       </c>
       <c r="B435" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>19:50</t>
         </is>
       </c>
       <c r="C435" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D435" t="n">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="E435" t="inlineStr">
         <is>
@@ -11228,12 +11228,12 @@
     <row r="436">
       <c r="A436" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>18:48:33</t>
         </is>
       </c>
       <c r="B436" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>19:50</t>
         </is>
       </c>
       <c r="C436" t="inlineStr">
@@ -11242,7 +11242,7 @@
         </is>
       </c>
       <c r="D436" t="n">
-        <v>93</v>
+        <v>62</v>
       </c>
       <c r="E436" t="inlineStr">
         <is>
@@ -11258,16 +11258,16 @@
       </c>
       <c r="B437" t="inlineStr">
         <is>
-          <t>19:52</t>
+          <t>19:51</t>
         </is>
       </c>
       <c r="C437" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D437" t="n">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E437" t="inlineStr">
         <is>
@@ -11278,21 +11278,21 @@
     <row r="438">
       <c r="A438" t="inlineStr">
         <is>
-          <t>18:36:52</t>
+          <t>18:48:33</t>
         </is>
       </c>
       <c r="B438" t="inlineStr">
         <is>
-          <t>19:59</t>
+          <t>19:51</t>
         </is>
       </c>
       <c r="C438" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D438" t="n">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="E438" t="inlineStr">
         <is>
@@ -11303,21 +11303,21 @@
     <row r="439">
       <c r="A439" t="inlineStr">
         <is>
-          <t>18:36:52</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B439" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>19:51</t>
         </is>
       </c>
       <c r="C439" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D439" t="n">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="E439" t="inlineStr">
         <is>
@@ -11333,16 +11333,16 @@
       </c>
       <c r="B440" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>19:52</t>
         </is>
       </c>
       <c r="C440" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D440" t="n">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="E440" t="inlineStr">
         <is>
@@ -11353,21 +11353,21 @@
     <row r="441">
       <c r="A441" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>18:48:33</t>
         </is>
       </c>
       <c r="B441" t="inlineStr">
         <is>
-          <t>20:10</t>
+          <t>19:59</t>
         </is>
       </c>
       <c r="C441" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D441" t="n">
-        <v>112</v>
+        <v>71</v>
       </c>
       <c r="E441" t="inlineStr">
         <is>
@@ -11378,21 +11378,21 @@
     <row r="442">
       <c r="A442" t="inlineStr">
         <is>
-          <t>18:36:52</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B442" t="inlineStr">
         <is>
-          <t>20:10</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="C442" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D442" t="n">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="E442" t="inlineStr">
         <is>
@@ -11403,21 +11403,21 @@
     <row r="443">
       <c r="A443" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>18:48:33</t>
         </is>
       </c>
       <c r="B443" t="inlineStr">
         <is>
-          <t>20:11</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="C443" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D443" t="n">
-        <v>113</v>
+        <v>72</v>
       </c>
       <c r="E443" t="inlineStr">
         <is>
@@ -11428,21 +11428,21 @@
     <row r="444">
       <c r="A444" t="inlineStr">
         <is>
-          <t>18:36:52</t>
+          <t>18:48:33</t>
         </is>
       </c>
       <c r="B444" t="inlineStr">
         <is>
-          <t>20:20</t>
+          <t>20:09</t>
         </is>
       </c>
       <c r="C444" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D444" t="n">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="E444" t="inlineStr">
         <is>
@@ -11453,21 +11453,21 @@
     <row r="445">
       <c r="A445" t="inlineStr">
         <is>
-          <t>18:36:52</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B445" t="inlineStr">
         <is>
-          <t>20:22</t>
+          <t>20:10</t>
         </is>
       </c>
       <c r="C445" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D445" t="n">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="E445" t="inlineStr">
         <is>
@@ -11478,21 +11478,21 @@
     <row r="446">
       <c r="A446" t="inlineStr">
         <is>
-          <t>18:36:52</t>
+          <t>18:48:33</t>
         </is>
       </c>
       <c r="B446" t="inlineStr">
         <is>
-          <t>20:23</t>
+          <t>20:10</t>
         </is>
       </c>
       <c r="C446" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D446" t="n">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="E446" t="inlineStr">
         <is>
@@ -11503,23 +11503,148 @@
     <row r="447">
       <c r="A447" t="inlineStr">
         <is>
+          <t>18:18:12</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>20:11</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D447" t="n">
+        <v>113</v>
+      </c>
+      <c r="E447" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>18:48:33</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>20:20</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D448" t="n">
+        <v>92</v>
+      </c>
+      <c r="E448" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>18:48:33</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>20:22</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D449" t="n">
+        <v>94</v>
+      </c>
+      <c r="E449" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>18:48:33</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>20:23</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D450" t="n">
+        <v>95</v>
+      </c>
+      <c r="E450" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
           <t>18:36:52</t>
         </is>
       </c>
-      <c r="B447" t="inlineStr">
+      <c r="B451" t="inlineStr">
         <is>
           <t>20:30</t>
         </is>
       </c>
-      <c r="C447" t="inlineStr">
+      <c r="C451" t="inlineStr">
         <is>
           <t>225_GOMEZ</t>
         </is>
       </c>
-      <c r="D447" t="n">
+      <c r="D451" t="n">
         <v>114</v>
       </c>
-      <c r="E447" t="inlineStr">
+      <c r="E451" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>18:48:33</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>20:31</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D452" t="n">
+        <v>103</v>
+      </c>
+      <c r="E452" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -11554,7 +11679,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:36:52</t>
+          <t>Última actualización: 18:48:33</t>
         </is>
       </c>
     </row>
@@ -12670,7 +12795,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>18:36:52</t>
+          <t>18:48:33</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -12684,7 +12809,7 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -12745,7 +12870,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>18:48:33</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -12759,7 +12884,7 @@
         </is>
       </c>
       <c r="D52" t="n">
-        <v>82</v>
+        <v>52</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -12770,7 +12895,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>18:36:52</t>
+          <t>18:48:33</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -12784,7 +12909,7 @@
         </is>
       </c>
       <c r="D53" t="n">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -12803,7 +12928,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E62"/>
+  <dimension ref="A1:E64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12821,14 +12946,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:36:52</t>
+          <t>Última actualización: 18:48:33</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 57</t>
+          <t>Total filas: 59</t>
         </is>
       </c>
     </row>
@@ -14162,7 +14287,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>18:48:33</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -14176,7 +14301,7 @@
         </is>
       </c>
       <c r="D58" t="n">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -14212,7 +14337,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>18:48:33</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -14226,7 +14351,7 @@
         </is>
       </c>
       <c r="D60" t="n">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -14281,6 +14406,56 @@
       <c r="E62" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>18:48:33</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>19:55</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>67</v>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>18:48:33</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>20:39</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>111</v>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 856
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-23.xlsx
+++ b/data/horarios-141-2026-01-23.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E452"/>
+  <dimension ref="A1:E456"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:48:33</t>
+          <t>Última actualización: 18:55:46</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 447</t>
+          <t>Total filas: 451</t>
         </is>
       </c>
     </row>
@@ -1513,7 +1513,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -1538,7 +1538,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -1628,7 +1628,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1638,11 +1638,11 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>6</v>
+        <v>73</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -1653,7 +1653,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1663,11 +1663,11 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>73</v>
+        <v>6</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -1778,7 +1778,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1788,11 +1788,11 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -1803,7 +1803,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1813,11 +1813,11 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>17</v>
+        <v>84</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D63" t="n">
@@ -1938,7 +1938,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -1963,7 +1963,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D65" t="n">
@@ -1978,7 +1978,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -1988,11 +1988,11 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2003,7 +2003,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -2013,11 +2013,11 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2528,7 +2528,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -2538,11 +2538,11 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -2553,7 +2553,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2563,11 +2563,11 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -2903,7 +2903,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>08:48:01</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -2913,11 +2913,11 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -2928,7 +2928,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>08:48:01</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -2938,11 +2938,11 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D104" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -3153,7 +3153,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3163,11 +3163,11 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>27</v>
+        <v>115</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3178,7 +3178,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
@@ -3188,11 +3188,11 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D114" t="n">
-        <v>115</v>
+        <v>27</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -3213,7 +3213,7 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D115" t="n">
@@ -3278,7 +3278,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>09:33:33</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -3288,11 +3288,11 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D118" t="n">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -3303,7 +3303,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>09:33:33</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -3313,11 +3313,11 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D119" t="n">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -4163,7 +4163,7 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D153" t="n">
@@ -4188,7 +4188,7 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D154" t="n">
@@ -4413,7 +4413,7 @@
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D163" t="n">
@@ -4438,7 +4438,7 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D164" t="n">
@@ -5003,7 +5003,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>10:27:29</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
@@ -5013,11 +5013,11 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D187" t="n">
-        <v>110</v>
+        <v>15</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -5028,7 +5028,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>10:27:29</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -5038,11 +5038,11 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D188" t="n">
-        <v>15</v>
+        <v>110</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5153,7 +5153,7 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>11:49:23</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
@@ -5163,11 +5163,11 @@
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D193" t="n">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
@@ -5178,7 +5178,7 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>11:49:23</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
@@ -5188,11 +5188,11 @@
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D194" t="n">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -5288,7 +5288,7 @@
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>17_179 Y 38</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D198" t="n">
@@ -5338,7 +5338,7 @@
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_179 Y 38</t>
         </is>
       </c>
       <c r="D200" t="n">
@@ -5528,7 +5528,7 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>12:54:24</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
@@ -5538,11 +5538,11 @@
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D208" t="n">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -5553,7 +5553,7 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>12:54:24</t>
+          <t>12:37:00</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
@@ -5563,11 +5563,11 @@
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D209" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -5813,7 +5813,7 @@
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D219" t="n">
@@ -5838,7 +5838,7 @@
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D220" t="n">
@@ -6313,7 +6313,7 @@
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D239" t="n">
@@ -6338,7 +6338,7 @@
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D240" t="n">
@@ -6353,7 +6353,7 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>13:51:20</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
@@ -6363,11 +6363,11 @@
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D241" t="n">
-        <v>80</v>
+        <v>6</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -6378,7 +6378,7 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>13:51:20</t>
+          <t>12:37:00</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
@@ -6388,11 +6388,11 @@
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D242" t="n">
-        <v>6</v>
+        <v>80</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -6838,7 +6838,7 @@
       </c>
       <c r="C260" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D260" t="n">
@@ -6863,7 +6863,7 @@
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D261" t="n">
@@ -7478,7 +7478,7 @@
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>14:55:42</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
@@ -7488,11 +7488,11 @@
       </c>
       <c r="C286" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D286" t="n">
-        <v>51</v>
+        <v>25</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
@@ -7503,7 +7503,7 @@
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>14:55:42</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
@@ -7513,11 +7513,11 @@
       </c>
       <c r="C287" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D287" t="n">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
@@ -7628,7 +7628,7 @@
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
@@ -7638,11 +7638,11 @@
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D292" t="n">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
@@ -7653,7 +7653,7 @@
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
@@ -7663,11 +7663,11 @@
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D293" t="n">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
@@ -7678,7 +7678,7 @@
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
@@ -7688,11 +7688,11 @@
       </c>
       <c r="C294" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D294" t="n">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
@@ -7703,7 +7703,7 @@
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
@@ -7713,11 +7713,11 @@
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D295" t="n">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
@@ -7853,7 +7853,7 @@
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>14:45:15</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
@@ -7863,11 +7863,11 @@
       </c>
       <c r="C301" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D301" t="n">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="E301" t="inlineStr">
         <is>
@@ -7878,7 +7878,7 @@
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>14:45:15</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
@@ -7888,11 +7888,11 @@
       </c>
       <c r="C302" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D302" t="n">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="E302" t="inlineStr">
         <is>
@@ -8003,7 +8003,7 @@
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:19:35</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
@@ -8013,11 +8013,11 @@
       </c>
       <c r="C307" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D307" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="E307" t="inlineStr">
         <is>
@@ -8028,7 +8028,7 @@
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>16:19:35</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
@@ -8038,11 +8038,11 @@
       </c>
       <c r="C308" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D308" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="E308" t="inlineStr">
         <is>
@@ -8078,7 +8078,7 @@
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>16:19:35</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
@@ -8088,11 +8088,11 @@
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D310" t="n">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="E310" t="inlineStr">
         <is>
@@ -8103,7 +8103,7 @@
     <row r="311">
       <c r="A311" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:19:35</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
@@ -8113,11 +8113,11 @@
       </c>
       <c r="C311" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D311" t="n">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="E311" t="inlineStr">
         <is>
@@ -8403,7 +8403,7 @@
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:36:35</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
@@ -8413,11 +8413,11 @@
       </c>
       <c r="C323" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D323" t="n">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="E323" t="inlineStr">
         <is>
@@ -8428,7 +8428,7 @@
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>16:36:35</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
@@ -8438,11 +8438,11 @@
       </c>
       <c r="C324" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D324" t="n">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="E324" t="inlineStr">
         <is>
@@ -8653,7 +8653,7 @@
     <row r="333">
       <c r="A333" t="inlineStr">
         <is>
-          <t>16:53:56</t>
+          <t>16:46:26</t>
         </is>
       </c>
       <c r="B333" t="inlineStr">
@@ -8663,11 +8663,11 @@
       </c>
       <c r="C333" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_179 Y 38</t>
         </is>
       </c>
       <c r="D333" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E333" t="inlineStr">
         <is>
@@ -8678,7 +8678,7 @@
     <row r="334">
       <c r="A334" t="inlineStr">
         <is>
-          <t>16:46:26</t>
+          <t>16:53:56</t>
         </is>
       </c>
       <c r="B334" t="inlineStr">
@@ -8688,11 +8688,11 @@
       </c>
       <c r="C334" t="inlineStr">
         <is>
-          <t>17_179 Y 38</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D334" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E334" t="inlineStr">
         <is>
@@ -8738,7 +8738,7 @@
       </c>
       <c r="C336" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D336" t="n">
@@ -8763,7 +8763,7 @@
       </c>
       <c r="C337" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D337" t="n">
@@ -8913,7 +8913,7 @@
       </c>
       <c r="C343" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D343" t="n">
@@ -8938,7 +8938,7 @@
       </c>
       <c r="C344" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D344" t="n">
@@ -9188,7 +9188,7 @@
       </c>
       <c r="C354" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D354" t="n">
@@ -9213,7 +9213,7 @@
       </c>
       <c r="C355" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D355" t="n">
@@ -9478,7 +9478,7 @@
     <row r="366">
       <c r="A366" t="inlineStr">
         <is>
-          <t>17:42:07</t>
+          <t>16:53:56</t>
         </is>
       </c>
       <c r="B366" t="inlineStr">
@@ -9488,11 +9488,11 @@
       </c>
       <c r="C366" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D366" t="n">
-        <v>9</v>
+        <v>58</v>
       </c>
       <c r="E366" t="inlineStr">
         <is>
@@ -9503,7 +9503,7 @@
     <row r="367">
       <c r="A367" t="inlineStr">
         <is>
-          <t>16:53:56</t>
+          <t>17:42:07</t>
         </is>
       </c>
       <c r="B367" t="inlineStr">
@@ -9513,11 +9513,11 @@
       </c>
       <c r="C367" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D367" t="n">
-        <v>58</v>
+        <v>9</v>
       </c>
       <c r="E367" t="inlineStr">
         <is>
@@ -9663,7 +9663,7 @@
       </c>
       <c r="C373" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D373" t="n">
@@ -9688,7 +9688,7 @@
       </c>
       <c r="C374" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D374" t="n">
@@ -10213,7 +10213,7 @@
       </c>
       <c r="C395" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D395" t="n">
@@ -10238,7 +10238,7 @@
       </c>
       <c r="C396" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D396" t="n">
@@ -10403,7 +10403,7 @@
     <row r="403">
       <c r="A403" t="inlineStr">
         <is>
-          <t>18:48:33</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B403" t="inlineStr">
@@ -10413,11 +10413,11 @@
       </c>
       <c r="C403" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D403" t="n">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="E403" t="inlineStr">
         <is>
@@ -10428,7 +10428,7 @@
     <row r="404">
       <c r="A404" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>18:48:33</t>
         </is>
       </c>
       <c r="B404" t="inlineStr">
@@ -10438,11 +10438,11 @@
       </c>
       <c r="C404" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D404" t="n">
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="E404" t="inlineStr">
         <is>
@@ -10478,21 +10478,21 @@
     <row r="406">
       <c r="A406" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>18:55:46</t>
         </is>
       </c>
       <c r="B406" t="inlineStr">
         <is>
-          <t>18:57</t>
+          <t>18:56</t>
         </is>
       </c>
       <c r="C406" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D406" t="n">
-        <v>39</v>
+        <v>1</v>
       </c>
       <c r="E406" t="inlineStr">
         <is>
@@ -10503,21 +10503,21 @@
     <row r="407">
       <c r="A407" t="inlineStr">
         <is>
-          <t>18:48:33</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B407" t="inlineStr">
         <is>
-          <t>18:58</t>
+          <t>18:57</t>
         </is>
       </c>
       <c r="C407" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D407" t="n">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="E407" t="inlineStr">
         <is>
@@ -10528,12 +10528,12 @@
     <row r="408">
       <c r="A408" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>18:55:46</t>
         </is>
       </c>
       <c r="B408" t="inlineStr">
         <is>
-          <t>18:59</t>
+          <t>18:58</t>
         </is>
       </c>
       <c r="C408" t="inlineStr">
@@ -10542,7 +10542,7 @@
         </is>
       </c>
       <c r="D408" t="n">
-        <v>41</v>
+        <v>3</v>
       </c>
       <c r="E408" t="inlineStr">
         <is>
@@ -10553,21 +10553,21 @@
     <row r="409">
       <c r="A409" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>18:55:46</t>
         </is>
       </c>
       <c r="B409" t="inlineStr">
         <is>
-          <t>19:01</t>
+          <t>18:58</t>
         </is>
       </c>
       <c r="C409" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D409" t="n">
-        <v>43</v>
+        <v>3</v>
       </c>
       <c r="E409" t="inlineStr">
         <is>
@@ -10578,21 +10578,21 @@
     <row r="410">
       <c r="A410" t="inlineStr">
         <is>
-          <t>18:48:33</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B410" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>18:59</t>
         </is>
       </c>
       <c r="C410" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D410" t="n">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="E410" t="inlineStr">
         <is>
@@ -10603,21 +10603,21 @@
     <row r="411">
       <c r="A411" t="inlineStr">
         <is>
-          <t>18:48:33</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B411" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>19:01</t>
         </is>
       </c>
       <c r="C411" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D411" t="n">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="E411" t="inlineStr">
         <is>
@@ -10628,12 +10628,12 @@
     <row r="412">
       <c r="A412" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>18:48:33</t>
         </is>
       </c>
       <c r="B412" t="inlineStr">
         <is>
-          <t>19:05</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="C412" t="inlineStr">
@@ -10642,7 +10642,7 @@
         </is>
       </c>
       <c r="D412" t="n">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="E412" t="inlineStr">
         <is>
@@ -10653,12 +10653,12 @@
     <row r="413">
       <c r="A413" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>18:55:46</t>
         </is>
       </c>
       <c r="B413" t="inlineStr">
         <is>
-          <t>19:05</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="C413" t="inlineStr">
@@ -10667,7 +10667,7 @@
         </is>
       </c>
       <c r="D413" t="n">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="E413" t="inlineStr">
         <is>
@@ -10678,21 +10678,21 @@
     <row r="414">
       <c r="A414" t="inlineStr">
         <is>
-          <t>18:48:33</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B414" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>19:05</t>
         </is>
       </c>
       <c r="C414" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D414" t="n">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="E414" t="inlineStr">
         <is>
@@ -10708,16 +10708,16 @@
       </c>
       <c r="B415" t="inlineStr">
         <is>
-          <t>19:11</t>
+          <t>19:05</t>
         </is>
       </c>
       <c r="C415" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D415" t="n">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E415" t="inlineStr">
         <is>
@@ -10728,21 +10728,21 @@
     <row r="416">
       <c r="A416" t="inlineStr">
         <is>
-          <t>18:48:33</t>
+          <t>18:55:46</t>
         </is>
       </c>
       <c r="B416" t="inlineStr">
         <is>
-          <t>19:12</t>
+          <t>19:06</t>
         </is>
       </c>
       <c r="C416" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D416" t="n">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="E416" t="inlineStr">
         <is>
@@ -10753,21 +10753,21 @@
     <row r="417">
       <c r="A417" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>18:55:46</t>
         </is>
       </c>
       <c r="B417" t="inlineStr">
         <is>
-          <t>19:13</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="C417" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D417" t="n">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="E417" t="inlineStr">
         <is>
@@ -10778,21 +10778,21 @@
     <row r="418">
       <c r="A418" t="inlineStr">
         <is>
-          <t>18:48:33</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B418" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>19:11</t>
         </is>
       </c>
       <c r="C418" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D418" t="n">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="E418" t="inlineStr">
         <is>
@@ -10803,21 +10803,21 @@
     <row r="419">
       <c r="A419" t="inlineStr">
         <is>
-          <t>18:48:33</t>
+          <t>18:55:46</t>
         </is>
       </c>
       <c r="B419" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="C419" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D419" t="n">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E419" t="inlineStr">
         <is>
@@ -10833,16 +10833,16 @@
       </c>
       <c r="B420" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>19:13</t>
         </is>
       </c>
       <c r="C420" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D420" t="n">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E420" t="inlineStr">
         <is>
@@ -10853,21 +10853,21 @@
     <row r="421">
       <c r="A421" t="inlineStr">
         <is>
-          <t>18:48:33</t>
+          <t>18:55:46</t>
         </is>
       </c>
       <c r="B421" t="inlineStr">
         <is>
-          <t>19:20</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="C421" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D421" t="n">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="E421" t="inlineStr">
         <is>
@@ -10878,21 +10878,21 @@
     <row r="422">
       <c r="A422" t="inlineStr">
         <is>
-          <t>18:48:33</t>
+          <t>18:55:46</t>
         </is>
       </c>
       <c r="B422" t="inlineStr">
         <is>
-          <t>19:20</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="C422" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D422" t="n">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="E422" t="inlineStr">
         <is>
@@ -10908,16 +10908,16 @@
       </c>
       <c r="B423" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="C423" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D423" t="n">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E423" t="inlineStr">
         <is>
@@ -10928,21 +10928,21 @@
     <row r="424">
       <c r="A424" t="inlineStr">
         <is>
-          <t>18:48:33</t>
+          <t>18:55:46</t>
         </is>
       </c>
       <c r="B424" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>19:20</t>
         </is>
       </c>
       <c r="C424" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D424" t="n">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="E424" t="inlineStr">
         <is>
@@ -10953,21 +10953,21 @@
     <row r="425">
       <c r="A425" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>18:55:46</t>
         </is>
       </c>
       <c r="B425" t="inlineStr">
         <is>
-          <t>19:22</t>
+          <t>19:20</t>
         </is>
       </c>
       <c r="C425" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D425" t="n">
-        <v>64</v>
+        <v>25</v>
       </c>
       <c r="E425" t="inlineStr">
         <is>
@@ -10978,21 +10978,21 @@
     <row r="426">
       <c r="A426" t="inlineStr">
         <is>
-          <t>18:36:52</t>
+          <t>18:55:46</t>
         </is>
       </c>
       <c r="B426" t="inlineStr">
         <is>
-          <t>19:28</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="C426" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D426" t="n">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="E426" t="inlineStr">
         <is>
@@ -11008,16 +11008,16 @@
       </c>
       <c r="B427" t="inlineStr">
         <is>
-          <t>19:29</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="C427" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D427" t="n">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E427" t="inlineStr">
         <is>
@@ -11028,21 +11028,21 @@
     <row r="428">
       <c r="A428" t="inlineStr">
         <is>
-          <t>18:36:52</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B428" t="inlineStr">
         <is>
-          <t>19:29</t>
+          <t>19:22</t>
         </is>
       </c>
       <c r="C428" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D428" t="n">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="E428" t="inlineStr">
         <is>
@@ -11053,21 +11053,21 @@
     <row r="429">
       <c r="A429" t="inlineStr">
         <is>
-          <t>18:48:33</t>
+          <t>18:36:52</t>
         </is>
       </c>
       <c r="B429" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>19:28</t>
         </is>
       </c>
       <c r="C429" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D429" t="n">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="E429" t="inlineStr">
         <is>
@@ -11078,21 +11078,21 @@
     <row r="430">
       <c r="A430" t="inlineStr">
         <is>
-          <t>18:48:33</t>
+          <t>18:36:52</t>
         </is>
       </c>
       <c r="B430" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>19:29</t>
         </is>
       </c>
       <c r="C430" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D430" t="n">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="E430" t="inlineStr">
         <is>
@@ -11103,21 +11103,21 @@
     <row r="431">
       <c r="A431" t="inlineStr">
         <is>
-          <t>18:48:33</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B431" t="inlineStr">
         <is>
-          <t>19:34</t>
+          <t>19:29</t>
         </is>
       </c>
       <c r="C431" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D431" t="n">
-        <v>46</v>
+        <v>71</v>
       </c>
       <c r="E431" t="inlineStr">
         <is>
@@ -11128,21 +11128,21 @@
     <row r="432">
       <c r="A432" t="inlineStr">
         <is>
-          <t>18:36:52</t>
+          <t>18:55:46</t>
         </is>
       </c>
       <c r="B432" t="inlineStr">
         <is>
-          <t>19:39</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="C432" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D432" t="n">
-        <v>63</v>
+        <v>35</v>
       </c>
       <c r="E432" t="inlineStr">
         <is>
@@ -11153,21 +11153,21 @@
     <row r="433">
       <c r="A433" t="inlineStr">
         <is>
-          <t>18:48:33</t>
+          <t>18:55:46</t>
         </is>
       </c>
       <c r="B433" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="C433" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D433" t="n">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="E433" t="inlineStr">
         <is>
@@ -11178,21 +11178,21 @@
     <row r="434">
       <c r="A434" t="inlineStr">
         <is>
-          <t>18:36:52</t>
+          <t>18:55:46</t>
         </is>
       </c>
       <c r="B434" t="inlineStr">
         <is>
-          <t>19:49</t>
+          <t>19:34</t>
         </is>
       </c>
       <c r="C434" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D434" t="n">
-        <v>73</v>
+        <v>39</v>
       </c>
       <c r="E434" t="inlineStr">
         <is>
@@ -11203,21 +11203,21 @@
     <row r="435">
       <c r="A435" t="inlineStr">
         <is>
-          <t>18:48:33</t>
+          <t>18:55:46</t>
         </is>
       </c>
       <c r="B435" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>19:39</t>
         </is>
       </c>
       <c r="C435" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D435" t="n">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="E435" t="inlineStr">
         <is>
@@ -11228,21 +11228,21 @@
     <row r="436">
       <c r="A436" t="inlineStr">
         <is>
-          <t>18:48:33</t>
+          <t>18:55:46</t>
         </is>
       </c>
       <c r="B436" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="C436" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D436" t="n">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="E436" t="inlineStr">
         <is>
@@ -11253,21 +11253,21 @@
     <row r="437">
       <c r="A437" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>18:48:33</t>
         </is>
       </c>
       <c r="B437" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="C437" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D437" t="n">
-        <v>93</v>
+        <v>52</v>
       </c>
       <c r="E437" t="inlineStr">
         <is>
@@ -11278,21 +11278,21 @@
     <row r="438">
       <c r="A438" t="inlineStr">
         <is>
-          <t>18:48:33</t>
+          <t>18:36:52</t>
         </is>
       </c>
       <c r="B438" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>19:49</t>
         </is>
       </c>
       <c r="C438" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D438" t="n">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="E438" t="inlineStr">
         <is>
@@ -11303,21 +11303,21 @@
     <row r="439">
       <c r="A439" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>18:55:46</t>
         </is>
       </c>
       <c r="B439" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>19:50</t>
         </is>
       </c>
       <c r="C439" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D439" t="n">
-        <v>93</v>
+        <v>55</v>
       </c>
       <c r="E439" t="inlineStr">
         <is>
@@ -11328,21 +11328,21 @@
     <row r="440">
       <c r="A440" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>18:55:46</t>
         </is>
       </c>
       <c r="B440" t="inlineStr">
         <is>
-          <t>19:52</t>
+          <t>19:50</t>
         </is>
       </c>
       <c r="C440" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D440" t="n">
-        <v>94</v>
+        <v>55</v>
       </c>
       <c r="E440" t="inlineStr">
         <is>
@@ -11353,21 +11353,21 @@
     <row r="441">
       <c r="A441" t="inlineStr">
         <is>
-          <t>18:48:33</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B441" t="inlineStr">
         <is>
-          <t>19:59</t>
+          <t>19:51</t>
         </is>
       </c>
       <c r="C441" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D441" t="n">
-        <v>71</v>
+        <v>93</v>
       </c>
       <c r="E441" t="inlineStr">
         <is>
@@ -11383,16 +11383,16 @@
       </c>
       <c r="B442" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>19:51</t>
         </is>
       </c>
       <c r="C442" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D442" t="n">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="E442" t="inlineStr">
         <is>
@@ -11403,21 +11403,21 @@
     <row r="443">
       <c r="A443" t="inlineStr">
         <is>
-          <t>18:48:33</t>
+          <t>18:55:46</t>
         </is>
       </c>
       <c r="B443" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>19:51</t>
         </is>
       </c>
       <c r="C443" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D443" t="n">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="E443" t="inlineStr">
         <is>
@@ -11428,21 +11428,21 @@
     <row r="444">
       <c r="A444" t="inlineStr">
         <is>
-          <t>18:48:33</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B444" t="inlineStr">
         <is>
-          <t>20:09</t>
+          <t>19:52</t>
         </is>
       </c>
       <c r="C444" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D444" t="n">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="E444" t="inlineStr">
         <is>
@@ -11453,21 +11453,21 @@
     <row r="445">
       <c r="A445" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>18:55:46</t>
         </is>
       </c>
       <c r="B445" t="inlineStr">
         <is>
-          <t>20:10</t>
+          <t>19:59</t>
         </is>
       </c>
       <c r="C445" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D445" t="n">
-        <v>112</v>
+        <v>64</v>
       </c>
       <c r="E445" t="inlineStr">
         <is>
@@ -11483,16 +11483,16 @@
       </c>
       <c r="B446" t="inlineStr">
         <is>
-          <t>20:10</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="C446" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D446" t="n">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="E446" t="inlineStr">
         <is>
@@ -11508,16 +11508,16 @@
       </c>
       <c r="B447" t="inlineStr">
         <is>
-          <t>20:11</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="C447" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D447" t="n">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="E447" t="inlineStr">
         <is>
@@ -11528,21 +11528,21 @@
     <row r="448">
       <c r="A448" t="inlineStr">
         <is>
-          <t>18:48:33</t>
+          <t>18:55:46</t>
         </is>
       </c>
       <c r="B448" t="inlineStr">
         <is>
-          <t>20:20</t>
+          <t>20:09</t>
         </is>
       </c>
       <c r="C448" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D448" t="n">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="E448" t="inlineStr">
         <is>
@@ -11553,21 +11553,21 @@
     <row r="449">
       <c r="A449" t="inlineStr">
         <is>
-          <t>18:48:33</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B449" t="inlineStr">
         <is>
-          <t>20:22</t>
+          <t>20:10</t>
         </is>
       </c>
       <c r="C449" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D449" t="n">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="E449" t="inlineStr">
         <is>
@@ -11578,21 +11578,21 @@
     <row r="450">
       <c r="A450" t="inlineStr">
         <is>
-          <t>18:48:33</t>
+          <t>18:55:46</t>
         </is>
       </c>
       <c r="B450" t="inlineStr">
         <is>
-          <t>20:23</t>
+          <t>20:10</t>
         </is>
       </c>
       <c r="C450" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D450" t="n">
-        <v>95</v>
+        <v>75</v>
       </c>
       <c r="E450" t="inlineStr">
         <is>
@@ -11603,21 +11603,21 @@
     <row r="451">
       <c r="A451" t="inlineStr">
         <is>
-          <t>18:36:52</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B451" t="inlineStr">
         <is>
-          <t>20:30</t>
+          <t>20:11</t>
         </is>
       </c>
       <c r="C451" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D451" t="n">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E451" t="inlineStr">
         <is>
@@ -11628,23 +11628,123 @@
     <row r="452">
       <c r="A452" t="inlineStr">
         <is>
-          <t>18:48:33</t>
+          <t>18:55:46</t>
         </is>
       </c>
       <c r="B452" t="inlineStr">
         <is>
+          <t>20:20</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D452" t="n">
+        <v>85</v>
+      </c>
+      <c r="E452" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>18:55:46</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>20:22</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D453" t="n">
+        <v>87</v>
+      </c>
+      <c r="E453" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>18:55:46</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>20:23</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D454" t="n">
+        <v>88</v>
+      </c>
+      <c r="E454" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>18:36:52</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>20:30</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D455" t="n">
+        <v>114</v>
+      </c>
+      <c r="E455" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>18:55:46</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
           <t>20:31</t>
         </is>
       </c>
-      <c r="C452" t="inlineStr">
+      <c r="C456" t="inlineStr">
         <is>
           <t>225_GOMEZ</t>
         </is>
       </c>
-      <c r="D452" t="n">
-        <v>103</v>
-      </c>
-      <c r="E452" t="inlineStr">
+      <c r="D456" t="n">
+        <v>96</v>
+      </c>
+      <c r="E456" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -11679,7 +11779,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:48:33</t>
+          <t>Última actualización: 18:55:46</t>
         </is>
       </c>
     </row>
@@ -12795,7 +12895,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>18:48:33</t>
+          <t>18:55:46</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -12809,7 +12909,7 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -12845,7 +12945,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>18:36:52</t>
+          <t>18:55:46</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -12859,7 +12959,7 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -12895,7 +12995,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>18:48:33</t>
+          <t>18:55:46</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -12909,7 +13009,7 @@
         </is>
       </c>
       <c r="D53" t="n">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -12946,7 +13046,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:48:33</t>
+          <t>Última actualización: 18:55:46</t>
         </is>
       </c>
     </row>
@@ -14312,7 +14412,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>18:36:52</t>
+          <t>18:55:46</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -14326,7 +14426,7 @@
         </is>
       </c>
       <c r="D59" t="n">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -14412,7 +14512,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>18:48:33</t>
+          <t>18:55:46</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -14426,7 +14526,7 @@
         </is>
       </c>
       <c r="D63" t="n">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -14437,7 +14537,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>18:48:33</t>
+          <t>18:55:46</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -14451,7 +14551,7 @@
         </is>
       </c>
       <c r="D64" t="n">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 857
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-23.xlsx
+++ b/data/horarios-141-2026-01-23.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E456"/>
+  <dimension ref="A1:E470"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:55:46</t>
+          <t>Última actualización: 19:15:13</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 451</t>
+          <t>Total filas: 465</t>
         </is>
       </c>
     </row>
@@ -1513,7 +1513,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -1538,7 +1538,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -1628,7 +1628,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1638,11 +1638,11 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>73</v>
+        <v>6</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -1653,7 +1653,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1663,11 +1663,11 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>6</v>
+        <v>73</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -1778,7 +1778,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1788,11 +1788,11 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>17</v>
+        <v>84</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -1803,7 +1803,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1813,11 +1813,11 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D63" t="n">
@@ -1938,7 +1938,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -1953,7 +1953,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1963,11 +1963,11 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -2003,7 +2003,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -2013,11 +2013,11 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2213,7 +2213,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D75" t="n">
@@ -2238,7 +2238,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D76" t="n">
@@ -2803,7 +2803,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -2813,11 +2813,11 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D99" t="n">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -2828,7 +2828,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -2838,11 +2838,11 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -2903,7 +2903,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>08:48:01</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -2913,11 +2913,11 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -2928,7 +2928,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>08:48:01</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -2938,11 +2938,11 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D104" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -3188,7 +3188,7 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D114" t="n">
@@ -3213,7 +3213,7 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D115" t="n">
@@ -3388,7 +3388,7 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D122" t="n">
@@ -3413,7 +3413,7 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D123" t="n">
@@ -4928,7 +4928,7 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>10:57:35</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
@@ -4938,11 +4938,11 @@
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D184" t="n">
-        <v>77</v>
+        <v>12</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -4953,7 +4953,7 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>10:57:35</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
@@ -4963,11 +4963,11 @@
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D185" t="n">
-        <v>12</v>
+        <v>77</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -5003,7 +5003,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>10:27:29</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
@@ -5013,11 +5013,11 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D187" t="n">
-        <v>15</v>
+        <v>110</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -5028,7 +5028,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>10:27:29</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -5038,11 +5038,11 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D188" t="n">
-        <v>110</v>
+        <v>15</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5063,7 +5063,7 @@
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D189" t="n">
@@ -5088,7 +5088,7 @@
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D190" t="n">
@@ -5153,7 +5153,7 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>11:49:23</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
@@ -5163,11 +5163,11 @@
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D193" t="n">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
@@ -5178,7 +5178,7 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>11:49:23</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
@@ -5188,11 +5188,11 @@
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D194" t="n">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -5288,7 +5288,7 @@
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_179 Y 38</t>
         </is>
       </c>
       <c r="D198" t="n">
@@ -5338,7 +5338,7 @@
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>17_179 Y 38</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D200" t="n">
@@ -5528,7 +5528,7 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>12:54:24</t>
+          <t>12:37:00</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
@@ -5538,11 +5538,11 @@
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D208" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -5553,7 +5553,7 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>12:54:24</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
@@ -5563,11 +5563,11 @@
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D209" t="n">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -5813,7 +5813,7 @@
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D219" t="n">
@@ -5838,7 +5838,7 @@
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D220" t="n">
@@ -5988,7 +5988,7 @@
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D226" t="n">
@@ -6013,7 +6013,7 @@
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D227" t="n">
@@ -6138,7 +6138,7 @@
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D232" t="n">
@@ -6163,7 +6163,7 @@
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D233" t="n">
@@ -6238,7 +6238,7 @@
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D236" t="n">
@@ -6263,7 +6263,7 @@
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D237" t="n">
@@ -6353,7 +6353,7 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>13:51:20</t>
+          <t>12:37:00</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
@@ -6363,11 +6363,11 @@
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D241" t="n">
-        <v>6</v>
+        <v>80</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -6378,7 +6378,7 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>13:51:20</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
@@ -6388,11 +6388,11 @@
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D242" t="n">
-        <v>80</v>
+        <v>6</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -7013,7 +7013,7 @@
       </c>
       <c r="C267" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D267" t="n">
@@ -7038,7 +7038,7 @@
       </c>
       <c r="C268" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D268" t="n">
@@ -7238,7 +7238,7 @@
       </c>
       <c r="C276" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D276" t="n">
@@ -7263,7 +7263,7 @@
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D277" t="n">
@@ -7478,7 +7478,7 @@
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>14:55:42</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
@@ -7488,11 +7488,11 @@
       </c>
       <c r="C286" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D286" t="n">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
@@ -7503,7 +7503,7 @@
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>14:55:42</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
@@ -7513,11 +7513,11 @@
       </c>
       <c r="C287" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D287" t="n">
-        <v>51</v>
+        <v>25</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
@@ -7553,7 +7553,7 @@
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>14:55:42</t>
+          <t>14:19:39</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
@@ -7563,11 +7563,11 @@
       </c>
       <c r="C289" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D289" t="n">
-        <v>58</v>
+        <v>94</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
@@ -7578,7 +7578,7 @@
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>14:19:39</t>
+          <t>14:55:42</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
@@ -7588,11 +7588,11 @@
       </c>
       <c r="C290" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D290" t="n">
-        <v>94</v>
+        <v>58</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
@@ -7628,7 +7628,7 @@
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
@@ -7638,11 +7638,11 @@
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D292" t="n">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
@@ -7653,7 +7653,7 @@
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
@@ -7663,11 +7663,11 @@
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D293" t="n">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
@@ -7728,7 +7728,7 @@
     <row r="296">
       <c r="A296" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
@@ -7738,11 +7738,11 @@
       </c>
       <c r="C296" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D296" t="n">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="E296" t="inlineStr">
         <is>
@@ -7753,7 +7753,7 @@
     <row r="297">
       <c r="A297" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
@@ -7763,11 +7763,11 @@
       </c>
       <c r="C297" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D297" t="n">
-        <v>36</v>
+        <v>2</v>
       </c>
       <c r="E297" t="inlineStr">
         <is>
@@ -7963,7 +7963,7 @@
       </c>
       <c r="C305" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>225_C ROCA-H SUR</t>
         </is>
       </c>
       <c r="D305" t="n">
@@ -7988,7 +7988,7 @@
       </c>
       <c r="C306" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D306" t="n">
@@ -8003,7 +8003,7 @@
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>16:19:35</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
@@ -8013,11 +8013,11 @@
       </c>
       <c r="C307" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D307" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="E307" t="inlineStr">
         <is>
@@ -8028,7 +8028,7 @@
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:19:35</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
@@ -8038,11 +8038,11 @@
       </c>
       <c r="C308" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D308" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="E308" t="inlineStr">
         <is>
@@ -8053,7 +8053,7 @@
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>16:19:35</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
@@ -8063,11 +8063,11 @@
       </c>
       <c r="C309" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D309" t="n">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
@@ -8078,7 +8078,7 @@
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:19:35</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
@@ -8088,11 +8088,11 @@
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D310" t="n">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="E310" t="inlineStr">
         <is>
@@ -8453,7 +8453,7 @@
     <row r="325">
       <c r="A325" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>16:36:35</t>
         </is>
       </c>
       <c r="B325" t="inlineStr">
@@ -8463,11 +8463,11 @@
       </c>
       <c r="C325" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D325" t="n">
-        <v>82</v>
+        <v>7</v>
       </c>
       <c r="E325" t="inlineStr">
         <is>
@@ -8478,7 +8478,7 @@
     <row r="326">
       <c r="A326" t="inlineStr">
         <is>
-          <t>16:36:35</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B326" t="inlineStr">
@@ -8488,11 +8488,11 @@
       </c>
       <c r="C326" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D326" t="n">
-        <v>7</v>
+        <v>82</v>
       </c>
       <c r="E326" t="inlineStr">
         <is>
@@ -8528,7 +8528,7 @@
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>16:36:35</t>
+          <t>16:46:26</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
@@ -8538,11 +8538,11 @@
       </c>
       <c r="C328" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D328" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="E328" t="inlineStr">
         <is>
@@ -8553,7 +8553,7 @@
     <row r="329">
       <c r="A329" t="inlineStr">
         <is>
-          <t>16:46:26</t>
+          <t>16:36:35</t>
         </is>
       </c>
       <c r="B329" t="inlineStr">
@@ -8563,11 +8563,11 @@
       </c>
       <c r="C329" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D329" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E329" t="inlineStr">
         <is>
@@ -8963,7 +8963,7 @@
       </c>
       <c r="C345" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D345" t="n">
@@ -8988,7 +8988,7 @@
       </c>
       <c r="C346" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D346" t="n">
@@ -9188,7 +9188,7 @@
       </c>
       <c r="C354" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D354" t="n">
@@ -9213,7 +9213,7 @@
       </c>
       <c r="C355" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D355" t="n">
@@ -9878,7 +9878,7 @@
     <row r="382">
       <c r="A382" t="inlineStr">
         <is>
-          <t>16:53:56</t>
+          <t>17:57:31</t>
         </is>
       </c>
       <c r="B382" t="inlineStr">
@@ -9888,11 +9888,11 @@
       </c>
       <c r="C382" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D382" t="n">
-        <v>87</v>
+        <v>23</v>
       </c>
       <c r="E382" t="inlineStr">
         <is>
@@ -9903,7 +9903,7 @@
     <row r="383">
       <c r="A383" t="inlineStr">
         <is>
-          <t>17:57:31</t>
+          <t>16:53:56</t>
         </is>
       </c>
       <c r="B383" t="inlineStr">
@@ -9913,11 +9913,11 @@
       </c>
       <c r="C383" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D383" t="n">
-        <v>23</v>
+        <v>87</v>
       </c>
       <c r="E383" t="inlineStr">
         <is>
@@ -10403,7 +10403,7 @@
     <row r="403">
       <c r="A403" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>18:48:33</t>
         </is>
       </c>
       <c r="B403" t="inlineStr">
@@ -10413,11 +10413,11 @@
       </c>
       <c r="C403" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D403" t="n">
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="E403" t="inlineStr">
         <is>
@@ -10428,7 +10428,7 @@
     <row r="404">
       <c r="A404" t="inlineStr">
         <is>
-          <t>18:48:33</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B404" t="inlineStr">
@@ -10438,11 +10438,11 @@
       </c>
       <c r="C404" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D404" t="n">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="E404" t="inlineStr">
         <is>
@@ -10538,7 +10538,7 @@
       </c>
       <c r="C408" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D408" t="n">
@@ -10563,7 +10563,7 @@
       </c>
       <c r="C409" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D409" t="n">
@@ -10628,7 +10628,7 @@
     <row r="412">
       <c r="A412" t="inlineStr">
         <is>
-          <t>18:48:33</t>
+          <t>18:55:46</t>
         </is>
       </c>
       <c r="B412" t="inlineStr">
@@ -10638,11 +10638,11 @@
       </c>
       <c r="C412" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D412" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E412" t="inlineStr">
         <is>
@@ -10653,7 +10653,7 @@
     <row r="413">
       <c r="A413" t="inlineStr">
         <is>
-          <t>18:55:46</t>
+          <t>18:48:33</t>
         </is>
       </c>
       <c r="B413" t="inlineStr">
@@ -10663,11 +10663,11 @@
       </c>
       <c r="C413" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D413" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E413" t="inlineStr">
         <is>
@@ -10688,7 +10688,7 @@
       </c>
       <c r="C414" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D414" t="n">
@@ -10713,7 +10713,7 @@
       </c>
       <c r="C415" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D415" t="n">
@@ -10903,7 +10903,7 @@
     <row r="423">
       <c r="A423" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>19:15:13</t>
         </is>
       </c>
       <c r="B423" t="inlineStr">
@@ -10917,7 +10917,7 @@
         </is>
       </c>
       <c r="D423" t="n">
-        <v>59</v>
+        <v>2</v>
       </c>
       <c r="E423" t="inlineStr">
         <is>
@@ -10938,7 +10938,7 @@
       </c>
       <c r="C424" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D424" t="n">
@@ -10963,7 +10963,7 @@
       </c>
       <c r="C425" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D425" t="n">
@@ -10978,7 +10978,7 @@
     <row r="426">
       <c r="A426" t="inlineStr">
         <is>
-          <t>18:55:46</t>
+          <t>19:15:13</t>
         </is>
       </c>
       <c r="B426" t="inlineStr">
@@ -10992,7 +10992,7 @@
         </is>
       </c>
       <c r="D426" t="n">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="E426" t="inlineStr">
         <is>
@@ -11003,7 +11003,7 @@
     <row r="427">
       <c r="A427" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>19:15:13</t>
         </is>
       </c>
       <c r="B427" t="inlineStr">
@@ -11017,7 +11017,7 @@
         </is>
       </c>
       <c r="D427" t="n">
-        <v>63</v>
+        <v>6</v>
       </c>
       <c r="E427" t="inlineStr">
         <is>
@@ -11138,7 +11138,7 @@
       </c>
       <c r="C432" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D432" t="n">
@@ -11153,7 +11153,7 @@
     <row r="433">
       <c r="A433" t="inlineStr">
         <is>
-          <t>18:55:46</t>
+          <t>19:15:13</t>
         </is>
       </c>
       <c r="B433" t="inlineStr">
@@ -11163,11 +11163,11 @@
       </c>
       <c r="C433" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D433" t="n">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="E433" t="inlineStr">
         <is>
@@ -11178,21 +11178,21 @@
     <row r="434">
       <c r="A434" t="inlineStr">
         <is>
-          <t>18:55:46</t>
+          <t>19:15:13</t>
         </is>
       </c>
       <c r="B434" t="inlineStr">
         <is>
-          <t>19:34</t>
+          <t>19:31</t>
         </is>
       </c>
       <c r="C434" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D434" t="n">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="E434" t="inlineStr">
         <is>
@@ -11208,16 +11208,16 @@
       </c>
       <c r="B435" t="inlineStr">
         <is>
-          <t>19:39</t>
+          <t>19:34</t>
         </is>
       </c>
       <c r="C435" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D435" t="n">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E435" t="inlineStr">
         <is>
@@ -11228,21 +11228,21 @@
     <row r="436">
       <c r="A436" t="inlineStr">
         <is>
-          <t>18:55:46</t>
+          <t>19:15:13</t>
         </is>
       </c>
       <c r="B436" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>19:35</t>
         </is>
       </c>
       <c r="C436" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D436" t="n">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="E436" t="inlineStr">
         <is>
@@ -11253,12 +11253,12 @@
     <row r="437">
       <c r="A437" t="inlineStr">
         <is>
-          <t>18:48:33</t>
+          <t>18:55:46</t>
         </is>
       </c>
       <c r="B437" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>19:39</t>
         </is>
       </c>
       <c r="C437" t="inlineStr">
@@ -11267,7 +11267,7 @@
         </is>
       </c>
       <c r="D437" t="n">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="E437" t="inlineStr">
         <is>
@@ -11278,21 +11278,21 @@
     <row r="438">
       <c r="A438" t="inlineStr">
         <is>
-          <t>18:36:52</t>
+          <t>19:15:13</t>
         </is>
       </c>
       <c r="B438" t="inlineStr">
         <is>
-          <t>19:49</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="C438" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D438" t="n">
-        <v>73</v>
+        <v>25</v>
       </c>
       <c r="E438" t="inlineStr">
         <is>
@@ -11308,16 +11308,16 @@
       </c>
       <c r="B439" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="C439" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D439" t="n">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="E439" t="inlineStr">
         <is>
@@ -11328,21 +11328,21 @@
     <row r="440">
       <c r="A440" t="inlineStr">
         <is>
-          <t>18:55:46</t>
+          <t>19:15:13</t>
         </is>
       </c>
       <c r="B440" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>19:41</t>
         </is>
       </c>
       <c r="C440" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D440" t="n">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="E440" t="inlineStr">
         <is>
@@ -11353,21 +11353,21 @@
     <row r="441">
       <c r="A441" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>19:15:13</t>
         </is>
       </c>
       <c r="B441" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>19:41</t>
         </is>
       </c>
       <c r="C441" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D441" t="n">
-        <v>93</v>
+        <v>26</v>
       </c>
       <c r="E441" t="inlineStr">
         <is>
@@ -11378,12 +11378,12 @@
     <row r="442">
       <c r="A442" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>18:36:52</t>
         </is>
       </c>
       <c r="B442" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>19:49</t>
         </is>
       </c>
       <c r="C442" t="inlineStr">
@@ -11392,7 +11392,7 @@
         </is>
       </c>
       <c r="D442" t="n">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="E442" t="inlineStr">
         <is>
@@ -11408,16 +11408,16 @@
       </c>
       <c r="B443" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>19:50</t>
         </is>
       </c>
       <c r="C443" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D443" t="n">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E443" t="inlineStr">
         <is>
@@ -11428,21 +11428,21 @@
     <row r="444">
       <c r="A444" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>19:15:13</t>
         </is>
       </c>
       <c r="B444" t="inlineStr">
         <is>
-          <t>19:52</t>
+          <t>19:50</t>
         </is>
       </c>
       <c r="C444" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D444" t="n">
-        <v>94</v>
+        <v>35</v>
       </c>
       <c r="E444" t="inlineStr">
         <is>
@@ -11453,21 +11453,21 @@
     <row r="445">
       <c r="A445" t="inlineStr">
         <is>
-          <t>18:55:46</t>
+          <t>19:15:13</t>
         </is>
       </c>
       <c r="B445" t="inlineStr">
         <is>
-          <t>19:59</t>
+          <t>19:51</t>
         </is>
       </c>
       <c r="C445" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D445" t="n">
-        <v>64</v>
+        <v>36</v>
       </c>
       <c r="E445" t="inlineStr">
         <is>
@@ -11478,21 +11478,21 @@
     <row r="446">
       <c r="A446" t="inlineStr">
         <is>
-          <t>18:48:33</t>
+          <t>19:15:13</t>
         </is>
       </c>
       <c r="B446" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>19:51</t>
         </is>
       </c>
       <c r="C446" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D446" t="n">
-        <v>72</v>
+        <v>36</v>
       </c>
       <c r="E446" t="inlineStr">
         <is>
@@ -11508,16 +11508,16 @@
       </c>
       <c r="B447" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>19:51</t>
         </is>
       </c>
       <c r="C447" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D447" t="n">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="E447" t="inlineStr">
         <is>
@@ -11528,21 +11528,21 @@
     <row r="448">
       <c r="A448" t="inlineStr">
         <is>
-          <t>18:55:46</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B448" t="inlineStr">
         <is>
-          <t>20:09</t>
+          <t>19:52</t>
         </is>
       </c>
       <c r="C448" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D448" t="n">
-        <v>74</v>
+        <v>94</v>
       </c>
       <c r="E448" t="inlineStr">
         <is>
@@ -11553,21 +11553,21 @@
     <row r="449">
       <c r="A449" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>19:15:13</t>
         </is>
       </c>
       <c r="B449" t="inlineStr">
         <is>
-          <t>20:10</t>
+          <t>19:59</t>
         </is>
       </c>
       <c r="C449" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D449" t="n">
-        <v>112</v>
+        <v>44</v>
       </c>
       <c r="E449" t="inlineStr">
         <is>
@@ -11578,21 +11578,21 @@
     <row r="450">
       <c r="A450" t="inlineStr">
         <is>
-          <t>18:55:46</t>
+          <t>18:48:33</t>
         </is>
       </c>
       <c r="B450" t="inlineStr">
         <is>
-          <t>20:10</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="C450" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D450" t="n">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E450" t="inlineStr">
         <is>
@@ -11608,16 +11608,16 @@
       </c>
       <c r="B451" t="inlineStr">
         <is>
-          <t>20:11</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="C451" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D451" t="n">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="E451" t="inlineStr">
         <is>
@@ -11628,21 +11628,21 @@
     <row r="452">
       <c r="A452" t="inlineStr">
         <is>
-          <t>18:55:46</t>
+          <t>19:15:13</t>
         </is>
       </c>
       <c r="B452" t="inlineStr">
         <is>
-          <t>20:20</t>
+          <t>20:09</t>
         </is>
       </c>
       <c r="C452" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D452" t="n">
-        <v>85</v>
+        <v>54</v>
       </c>
       <c r="E452" t="inlineStr">
         <is>
@@ -11653,21 +11653,21 @@
     <row r="453">
       <c r="A453" t="inlineStr">
         <is>
-          <t>18:55:46</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B453" t="inlineStr">
         <is>
-          <t>20:22</t>
+          <t>20:10</t>
         </is>
       </c>
       <c r="C453" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D453" t="n">
-        <v>87</v>
+        <v>112</v>
       </c>
       <c r="E453" t="inlineStr">
         <is>
@@ -11683,16 +11683,16 @@
       </c>
       <c r="B454" t="inlineStr">
         <is>
-          <t>20:23</t>
+          <t>20:10</t>
         </is>
       </c>
       <c r="C454" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D454" t="n">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="E454" t="inlineStr">
         <is>
@@ -11703,21 +11703,21 @@
     <row r="455">
       <c r="A455" t="inlineStr">
         <is>
-          <t>18:36:52</t>
+          <t>19:15:13</t>
         </is>
       </c>
       <c r="B455" t="inlineStr">
         <is>
-          <t>20:30</t>
+          <t>20:11</t>
         </is>
       </c>
       <c r="C455" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D455" t="n">
-        <v>114</v>
+        <v>56</v>
       </c>
       <c r="E455" t="inlineStr">
         <is>
@@ -11728,23 +11728,373 @@
     <row r="456">
       <c r="A456" t="inlineStr">
         <is>
+          <t>19:15:13</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>20:11</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D456" t="n">
+        <v>56</v>
+      </c>
+      <c r="E456" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>19:15:13</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>20:12</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D457" t="n">
+        <v>57</v>
+      </c>
+      <c r="E457" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
           <t>18:55:46</t>
         </is>
       </c>
-      <c r="B456" t="inlineStr">
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>20:20</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D458" t="n">
+        <v>85</v>
+      </c>
+      <c r="E458" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>19:15:13</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>20:21</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D459" t="n">
+        <v>66</v>
+      </c>
+      <c r="E459" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>19:15:13</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>20:22</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D460" t="n">
+        <v>67</v>
+      </c>
+      <c r="E460" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>18:55:46</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>20:23</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D461" t="n">
+        <v>88</v>
+      </c>
+      <c r="E461" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>19:15:13</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>20:24</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D462" t="n">
+        <v>69</v>
+      </c>
+      <c r="E462" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>18:36:52</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>20:30</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D463" t="n">
+        <v>114</v>
+      </c>
+      <c r="E463" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>19:15:13</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
         <is>
           <t>20:31</t>
         </is>
       </c>
-      <c r="C456" t="inlineStr">
+      <c r="C464" t="inlineStr">
         <is>
           <t>225_GOMEZ</t>
         </is>
       </c>
-      <c r="D456" t="n">
-        <v>96</v>
-      </c>
-      <c r="E456" t="inlineStr">
+      <c r="D464" t="n">
+        <v>76</v>
+      </c>
+      <c r="E464" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>19:15:13</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>20:44</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D465" t="n">
+        <v>89</v>
+      </c>
+      <c r="E465" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>19:15:13</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>20:52</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D466" t="n">
+        <v>97</v>
+      </c>
+      <c r="E466" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>19:15:13</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>20:56</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D467" t="n">
+        <v>101</v>
+      </c>
+      <c r="E467" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>19:15:13</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>20:57</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D468" t="n">
+        <v>102</v>
+      </c>
+      <c r="E468" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>19:15:13</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>21:04</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D469" t="n">
+        <v>109</v>
+      </c>
+      <c r="E469" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>19:15:13</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>21:08</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D470" t="n">
+        <v>113</v>
+      </c>
+      <c r="E470" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -11761,7 +12111,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E53"/>
+  <dimension ref="A1:E55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11779,14 +12129,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:55:46</t>
+          <t>Última actualización: 19:15:13</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 48</t>
+          <t>Total filas: 50</t>
         </is>
       </c>
     </row>
@@ -12970,7 +13320,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>18:48:33</t>
+          <t>19:15:13</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -12984,7 +13334,7 @@
         </is>
       </c>
       <c r="D52" t="n">
-        <v>52</v>
+        <v>25</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -13012,6 +13362,56 @@
         <v>88</v>
       </c>
       <c r="E53" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>19:15:13</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>20:24</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>69</v>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>19:15:13</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>21:08</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>113</v>
+      </c>
+      <c r="E55" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -13028,7 +13428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E64"/>
+  <dimension ref="A1:E65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13046,14 +13446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:55:46</t>
+          <t>Última actualización: 19:15:13</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 59</t>
+          <t>Total filas: 60</t>
         </is>
       </c>
     </row>
@@ -14537,23 +14937,48 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>18:55:46</t>
+          <t>19:15:13</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
+          <t>19:59</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>44</v>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>19:15:13</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
           <t>20:39</t>
         </is>
       </c>
-      <c r="C64" t="inlineStr">
+      <c r="C65" t="inlineStr">
         <is>
           <t>215A_LA PLATA</t>
         </is>
       </c>
-      <c r="D64" t="n">
-        <v>104</v>
-      </c>
-      <c r="E64" t="inlineStr">
+      <c r="D65" t="n">
+        <v>84</v>
+      </c>
+      <c r="E65" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 858
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-23.xlsx
+++ b/data/horarios-141-2026-01-23.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E470"/>
+  <dimension ref="A1:E476"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:15:13</t>
+          <t>Última actualización: 19:36:21</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 465</t>
+          <t>Total filas: 471</t>
         </is>
       </c>
     </row>
@@ -1313,7 +1313,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>86_EST CHICA-ESC AGRARIA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1338,7 +1338,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>86_EST CHICA-ESC AGRARIA</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1513,7 +1513,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -1538,7 +1538,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -1628,7 +1628,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1638,11 +1638,11 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>6</v>
+        <v>73</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -1653,7 +1653,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1663,11 +1663,11 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>73</v>
+        <v>6</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -1778,7 +1778,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1788,11 +1788,11 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -1803,7 +1803,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1813,11 +1813,11 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>17</v>
+        <v>84</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -1953,7 +1953,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1963,11 +1963,11 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -1988,7 +1988,7 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D66" t="n">
@@ -2003,7 +2003,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -2013,11 +2013,11 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2213,7 +2213,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D75" t="n">
@@ -2238,7 +2238,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D76" t="n">
@@ -2528,7 +2528,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -2538,11 +2538,11 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -2553,7 +2553,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2563,11 +2563,11 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -2803,7 +2803,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -2813,11 +2813,11 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D99" t="n">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -2828,7 +2828,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -2838,11 +2838,11 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -3153,7 +3153,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3163,11 +3163,11 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>115</v>
+        <v>27</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3188,7 +3188,7 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D114" t="n">
@@ -3203,7 +3203,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
@@ -3213,11 +3213,11 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D115" t="n">
-        <v>27</v>
+        <v>115</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -3278,7 +3278,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>09:33:33</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -3288,11 +3288,11 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D118" t="n">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -3303,7 +3303,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>09:33:33</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -3313,11 +3313,11 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D119" t="n">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -3338,7 +3338,7 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D120" t="n">
@@ -3363,7 +3363,7 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D121" t="n">
@@ -4163,7 +4163,7 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D153" t="n">
@@ -4188,7 +4188,7 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D154" t="n">
@@ -4413,7 +4413,7 @@
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D163" t="n">
@@ -4438,7 +4438,7 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D164" t="n">
@@ -4853,7 +4853,7 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>11:22:44</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
@@ -4863,11 +4863,11 @@
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D181" t="n">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
@@ -4878,7 +4878,7 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>11:22:44</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
@@ -4888,11 +4888,11 @@
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D182" t="n">
-        <v>44</v>
+        <v>4</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
@@ -4928,7 +4928,7 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>10:57:35</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
@@ -4938,11 +4938,11 @@
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D184" t="n">
-        <v>12</v>
+        <v>77</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -4953,7 +4953,7 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>10:57:35</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
@@ -4963,11 +4963,11 @@
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D185" t="n">
-        <v>77</v>
+        <v>12</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -5063,7 +5063,7 @@
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D189" t="n">
@@ -5088,7 +5088,7 @@
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D190" t="n">
@@ -5153,7 +5153,7 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>11:49:23</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
@@ -5163,11 +5163,11 @@
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D193" t="n">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
@@ -5178,7 +5178,7 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>11:49:23</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
@@ -5188,11 +5188,11 @@
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D194" t="n">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -5288,7 +5288,7 @@
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>17_179 Y 38</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D198" t="n">
@@ -5313,7 +5313,7 @@
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D199" t="n">
@@ -5338,7 +5338,7 @@
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_179 Y 38</t>
         </is>
       </c>
       <c r="D200" t="n">
@@ -5528,7 +5528,7 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>12:54:24</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
@@ -5538,11 +5538,11 @@
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D208" t="n">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -5553,7 +5553,7 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>12:54:24</t>
+          <t>12:37:00</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
@@ -5563,11 +5563,11 @@
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D209" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -5653,7 +5653,7 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>12:54:24</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
@@ -5663,11 +5663,11 @@
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D213" t="n">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -5678,7 +5678,7 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>12:54:24</t>
+          <t>12:37:00</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
@@ -5688,11 +5688,11 @@
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D214" t="n">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
@@ -5813,7 +5813,7 @@
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D219" t="n">
@@ -5838,7 +5838,7 @@
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D220" t="n">
@@ -6138,7 +6138,7 @@
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D232" t="n">
@@ -6163,7 +6163,7 @@
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D233" t="n">
@@ -6353,7 +6353,7 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>13:51:20</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
@@ -6363,11 +6363,11 @@
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D241" t="n">
-        <v>80</v>
+        <v>6</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -6378,7 +6378,7 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>13:51:20</t>
+          <t>12:37:00</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
@@ -6388,11 +6388,11 @@
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D242" t="n">
-        <v>6</v>
+        <v>80</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -6403,7 +6403,7 @@
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>13:18:32</t>
+          <t>13:51:20</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
@@ -6413,11 +6413,11 @@
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D243" t="n">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -6428,7 +6428,7 @@
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>13:51:20</t>
+          <t>13:18:32</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
@@ -6438,11 +6438,11 @@
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D244" t="n">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -6838,7 +6838,7 @@
       </c>
       <c r="C260" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D260" t="n">
@@ -6863,7 +6863,7 @@
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D261" t="n">
@@ -7013,7 +7013,7 @@
       </c>
       <c r="C267" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D267" t="n">
@@ -7038,7 +7038,7 @@
       </c>
       <c r="C268" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D268" t="n">
@@ -7478,7 +7478,7 @@
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>14:55:42</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
@@ -7488,11 +7488,11 @@
       </c>
       <c r="C286" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D286" t="n">
-        <v>51</v>
+        <v>25</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
@@ -7503,7 +7503,7 @@
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>14:55:42</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
@@ -7513,11 +7513,11 @@
       </c>
       <c r="C287" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D287" t="n">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
@@ -7553,7 +7553,7 @@
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>14:19:39</t>
+          <t>14:55:42</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
@@ -7563,11 +7563,11 @@
       </c>
       <c r="C289" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D289" t="n">
-        <v>94</v>
+        <v>58</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
@@ -7578,7 +7578,7 @@
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>14:55:42</t>
+          <t>14:19:39</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
@@ -7588,11 +7588,11 @@
       </c>
       <c r="C290" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D290" t="n">
-        <v>58</v>
+        <v>94</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
@@ -7678,7 +7678,7 @@
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
@@ -7688,11 +7688,11 @@
       </c>
       <c r="C294" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D294" t="n">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
@@ -7703,7 +7703,7 @@
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
@@ -7713,11 +7713,11 @@
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D295" t="n">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
@@ -7728,7 +7728,7 @@
     <row r="296">
       <c r="A296" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
@@ -7738,11 +7738,11 @@
       </c>
       <c r="C296" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D296" t="n">
-        <v>36</v>
+        <v>2</v>
       </c>
       <c r="E296" t="inlineStr">
         <is>
@@ -7753,7 +7753,7 @@
     <row r="297">
       <c r="A297" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
@@ -7763,11 +7763,11 @@
       </c>
       <c r="C297" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D297" t="n">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="E297" t="inlineStr">
         <is>
@@ -7963,7 +7963,7 @@
       </c>
       <c r="C305" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D305" t="n">
@@ -7988,7 +7988,7 @@
       </c>
       <c r="C306" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>225_C ROCA-H SUR</t>
         </is>
       </c>
       <c r="D306" t="n">
@@ -8003,7 +8003,7 @@
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:19:35</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
@@ -8013,11 +8013,11 @@
       </c>
       <c r="C307" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D307" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="E307" t="inlineStr">
         <is>
@@ -8028,7 +8028,7 @@
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>16:19:35</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
@@ -8038,11 +8038,11 @@
       </c>
       <c r="C308" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D308" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="E308" t="inlineStr">
         <is>
@@ -8088,7 +8088,7 @@
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D310" t="n">
@@ -8113,7 +8113,7 @@
       </c>
       <c r="C311" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D311" t="n">
@@ -8203,7 +8203,7 @@
     <row r="315">
       <c r="A315" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:19:35</t>
         </is>
       </c>
       <c r="B315" t="inlineStr">
@@ -8213,11 +8213,11 @@
       </c>
       <c r="C315" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D315" t="n">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="E315" t="inlineStr">
         <is>
@@ -8228,7 +8228,7 @@
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
-          <t>16:19:35</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
@@ -8238,11 +8238,11 @@
       </c>
       <c r="C316" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D316" t="n">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="E316" t="inlineStr">
         <is>
@@ -8403,7 +8403,7 @@
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>16:36:35</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
@@ -8413,11 +8413,11 @@
       </c>
       <c r="C323" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D323" t="n">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="E323" t="inlineStr">
         <is>
@@ -8428,7 +8428,7 @@
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:36:35</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
@@ -8438,11 +8438,11 @@
       </c>
       <c r="C324" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D324" t="n">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="E324" t="inlineStr">
         <is>
@@ -8453,7 +8453,7 @@
     <row r="325">
       <c r="A325" t="inlineStr">
         <is>
-          <t>16:36:35</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B325" t="inlineStr">
@@ -8463,11 +8463,11 @@
       </c>
       <c r="C325" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D325" t="n">
-        <v>7</v>
+        <v>82</v>
       </c>
       <c r="E325" t="inlineStr">
         <is>
@@ -8478,7 +8478,7 @@
     <row r="326">
       <c r="A326" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>16:36:35</t>
         </is>
       </c>
       <c r="B326" t="inlineStr">
@@ -8488,11 +8488,11 @@
       </c>
       <c r="C326" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D326" t="n">
-        <v>82</v>
+        <v>7</v>
       </c>
       <c r="E326" t="inlineStr">
         <is>
@@ -8888,7 +8888,7 @@
       </c>
       <c r="C342" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D342" t="n">
@@ -8913,7 +8913,7 @@
       </c>
       <c r="C343" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D343" t="n">
@@ -8938,7 +8938,7 @@
       </c>
       <c r="C344" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D344" t="n">
@@ -9338,7 +9338,7 @@
       </c>
       <c r="C360" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D360" t="n">
@@ -9363,7 +9363,7 @@
       </c>
       <c r="C361" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D361" t="n">
@@ -9663,7 +9663,7 @@
       </c>
       <c r="C373" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D373" t="n">
@@ -9688,7 +9688,7 @@
       </c>
       <c r="C374" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D374" t="n">
@@ -9878,7 +9878,7 @@
     <row r="382">
       <c r="A382" t="inlineStr">
         <is>
-          <t>17:57:31</t>
+          <t>16:53:56</t>
         </is>
       </c>
       <c r="B382" t="inlineStr">
@@ -9888,11 +9888,11 @@
       </c>
       <c r="C382" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D382" t="n">
-        <v>23</v>
+        <v>87</v>
       </c>
       <c r="E382" t="inlineStr">
         <is>
@@ -9903,7 +9903,7 @@
     <row r="383">
       <c r="A383" t="inlineStr">
         <is>
-          <t>16:53:56</t>
+          <t>17:57:31</t>
         </is>
       </c>
       <c r="B383" t="inlineStr">
@@ -9913,11 +9913,11 @@
       </c>
       <c r="C383" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D383" t="n">
-        <v>87</v>
+        <v>23</v>
       </c>
       <c r="E383" t="inlineStr">
         <is>
@@ -10278,7 +10278,7 @@
     <row r="398">
       <c r="A398" t="inlineStr">
         <is>
-          <t>18:36:52</t>
+          <t>17:57:31</t>
         </is>
       </c>
       <c r="B398" t="inlineStr">
@@ -10288,11 +10288,11 @@
       </c>
       <c r="C398" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D398" t="n">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="E398" t="inlineStr">
         <is>
@@ -10303,7 +10303,7 @@
     <row r="399">
       <c r="A399" t="inlineStr">
         <is>
-          <t>17:57:31</t>
+          <t>18:36:52</t>
         </is>
       </c>
       <c r="B399" t="inlineStr">
@@ -10313,11 +10313,11 @@
       </c>
       <c r="C399" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D399" t="n">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="E399" t="inlineStr">
         <is>
@@ -10403,7 +10403,7 @@
     <row r="403">
       <c r="A403" t="inlineStr">
         <is>
-          <t>18:48:33</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B403" t="inlineStr">
@@ -10413,11 +10413,11 @@
       </c>
       <c r="C403" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D403" t="n">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="E403" t="inlineStr">
         <is>
@@ -10428,7 +10428,7 @@
     <row r="404">
       <c r="A404" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>18:48:33</t>
         </is>
       </c>
       <c r="B404" t="inlineStr">
@@ -10438,11 +10438,11 @@
       </c>
       <c r="C404" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D404" t="n">
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="E404" t="inlineStr">
         <is>
@@ -10453,7 +10453,7 @@
     <row r="405">
       <c r="A405" t="inlineStr">
         <is>
-          <t>18:48:33</t>
+          <t>18:55:46</t>
         </is>
       </c>
       <c r="B405" t="inlineStr">
@@ -10463,11 +10463,11 @@
       </c>
       <c r="C405" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D405" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E405" t="inlineStr">
         <is>
@@ -10478,7 +10478,7 @@
     <row r="406">
       <c r="A406" t="inlineStr">
         <is>
-          <t>18:55:46</t>
+          <t>18:48:33</t>
         </is>
       </c>
       <c r="B406" t="inlineStr">
@@ -10488,11 +10488,11 @@
       </c>
       <c r="C406" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D406" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E406" t="inlineStr">
         <is>
@@ -10538,7 +10538,7 @@
       </c>
       <c r="C408" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D408" t="n">
@@ -10563,7 +10563,7 @@
       </c>
       <c r="C409" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D409" t="n">
@@ -10688,7 +10688,7 @@
       </c>
       <c r="C414" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D414" t="n">
@@ -10713,7 +10713,7 @@
       </c>
       <c r="C415" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D415" t="n">
@@ -10863,7 +10863,7 @@
       </c>
       <c r="C421" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D421" t="n">
@@ -10888,7 +10888,7 @@
       </c>
       <c r="C422" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D422" t="n">
@@ -10938,7 +10938,7 @@
       </c>
       <c r="C424" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D424" t="n">
@@ -10963,7 +10963,7 @@
       </c>
       <c r="C425" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D425" t="n">
@@ -11278,7 +11278,7 @@
     <row r="438">
       <c r="A438" t="inlineStr">
         <is>
-          <t>19:15:13</t>
+          <t>19:36:20</t>
         </is>
       </c>
       <c r="B438" t="inlineStr">
@@ -11288,11 +11288,11 @@
       </c>
       <c r="C438" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D438" t="n">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="E438" t="inlineStr">
         <is>
@@ -11303,7 +11303,7 @@
     <row r="439">
       <c r="A439" t="inlineStr">
         <is>
-          <t>18:55:46</t>
+          <t>19:36:20</t>
         </is>
       </c>
       <c r="B439" t="inlineStr">
@@ -11313,11 +11313,11 @@
       </c>
       <c r="C439" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D439" t="n">
-        <v>45</v>
+        <v>4</v>
       </c>
       <c r="E439" t="inlineStr">
         <is>
@@ -11403,7 +11403,7 @@
     <row r="443">
       <c r="A443" t="inlineStr">
         <is>
-          <t>18:55:46</t>
+          <t>19:36:20</t>
         </is>
       </c>
       <c r="B443" t="inlineStr">
@@ -11417,7 +11417,7 @@
         </is>
       </c>
       <c r="D443" t="n">
-        <v>55</v>
+        <v>14</v>
       </c>
       <c r="E443" t="inlineStr">
         <is>
@@ -11428,7 +11428,7 @@
     <row r="444">
       <c r="A444" t="inlineStr">
         <is>
-          <t>19:15:13</t>
+          <t>19:36:20</t>
         </is>
       </c>
       <c r="B444" t="inlineStr">
@@ -11442,7 +11442,7 @@
         </is>
       </c>
       <c r="D444" t="n">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="E444" t="inlineStr">
         <is>
@@ -11453,7 +11453,7 @@
     <row r="445">
       <c r="A445" t="inlineStr">
         <is>
-          <t>19:15:13</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B445" t="inlineStr">
@@ -11463,11 +11463,11 @@
       </c>
       <c r="C445" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D445" t="n">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="E445" t="inlineStr">
         <is>
@@ -11503,7 +11503,7 @@
     <row r="447">
       <c r="A447" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>19:36:20</t>
         </is>
       </c>
       <c r="B447" t="inlineStr">
@@ -11513,11 +11513,11 @@
       </c>
       <c r="C447" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D447" t="n">
-        <v>93</v>
+        <v>15</v>
       </c>
       <c r="E447" t="inlineStr">
         <is>
@@ -11578,7 +11578,7 @@
     <row r="450">
       <c r="A450" t="inlineStr">
         <is>
-          <t>18:48:33</t>
+          <t>19:36:20</t>
         </is>
       </c>
       <c r="B450" t="inlineStr">
@@ -11592,7 +11592,7 @@
         </is>
       </c>
       <c r="D450" t="n">
-        <v>72</v>
+        <v>24</v>
       </c>
       <c r="E450" t="inlineStr">
         <is>
@@ -11628,21 +11628,21 @@
     <row r="452">
       <c r="A452" t="inlineStr">
         <is>
-          <t>19:15:13</t>
+          <t>19:36:20</t>
         </is>
       </c>
       <c r="B452" t="inlineStr">
         <is>
-          <t>20:09</t>
+          <t>20:01</t>
         </is>
       </c>
       <c r="C452" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D452" t="n">
-        <v>54</v>
+        <v>25</v>
       </c>
       <c r="E452" t="inlineStr">
         <is>
@@ -11653,21 +11653,21 @@
     <row r="453">
       <c r="A453" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>19:36:20</t>
         </is>
       </c>
       <c r="B453" t="inlineStr">
         <is>
-          <t>20:10</t>
+          <t>20:03</t>
         </is>
       </c>
       <c r="C453" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D453" t="n">
-        <v>112</v>
+        <v>27</v>
       </c>
       <c r="E453" t="inlineStr">
         <is>
@@ -11678,21 +11678,21 @@
     <row r="454">
       <c r="A454" t="inlineStr">
         <is>
-          <t>18:55:46</t>
+          <t>19:36:20</t>
         </is>
       </c>
       <c r="B454" t="inlineStr">
         <is>
-          <t>20:10</t>
+          <t>20:09</t>
         </is>
       </c>
       <c r="C454" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D454" t="n">
-        <v>75</v>
+        <v>33</v>
       </c>
       <c r="E454" t="inlineStr">
         <is>
@@ -11703,12 +11703,12 @@
     <row r="455">
       <c r="A455" t="inlineStr">
         <is>
-          <t>19:15:13</t>
+          <t>19:36:20</t>
         </is>
       </c>
       <c r="B455" t="inlineStr">
         <is>
-          <t>20:11</t>
+          <t>20:10</t>
         </is>
       </c>
       <c r="C455" t="inlineStr">
@@ -11717,7 +11717,7 @@
         </is>
       </c>
       <c r="D455" t="n">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="E455" t="inlineStr">
         <is>
@@ -11728,21 +11728,21 @@
     <row r="456">
       <c r="A456" t="inlineStr">
         <is>
-          <t>19:15:13</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B456" t="inlineStr">
         <is>
-          <t>20:11</t>
+          <t>20:10</t>
         </is>
       </c>
       <c r="C456" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D456" t="n">
-        <v>56</v>
+        <v>112</v>
       </c>
       <c r="E456" t="inlineStr">
         <is>
@@ -11758,16 +11758,16 @@
       </c>
       <c r="B457" t="inlineStr">
         <is>
-          <t>20:12</t>
+          <t>20:11</t>
         </is>
       </c>
       <c r="C457" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D457" t="n">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E457" t="inlineStr">
         <is>
@@ -11778,21 +11778,21 @@
     <row r="458">
       <c r="A458" t="inlineStr">
         <is>
-          <t>18:55:46</t>
+          <t>19:36:20</t>
         </is>
       </c>
       <c r="B458" t="inlineStr">
         <is>
-          <t>20:20</t>
+          <t>20:11</t>
         </is>
       </c>
       <c r="C458" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D458" t="n">
-        <v>85</v>
+        <v>35</v>
       </c>
       <c r="E458" t="inlineStr">
         <is>
@@ -11803,21 +11803,21 @@
     <row r="459">
       <c r="A459" t="inlineStr">
         <is>
-          <t>19:15:13</t>
+          <t>19:36:20</t>
         </is>
       </c>
       <c r="B459" t="inlineStr">
         <is>
-          <t>20:21</t>
+          <t>20:12</t>
         </is>
       </c>
       <c r="C459" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D459" t="n">
-        <v>66</v>
+        <v>36</v>
       </c>
       <c r="E459" t="inlineStr">
         <is>
@@ -11828,21 +11828,21 @@
     <row r="460">
       <c r="A460" t="inlineStr">
         <is>
-          <t>19:15:13</t>
+          <t>18:55:46</t>
         </is>
       </c>
       <c r="B460" t="inlineStr">
         <is>
-          <t>20:22</t>
+          <t>20:20</t>
         </is>
       </c>
       <c r="C460" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D460" t="n">
-        <v>67</v>
+        <v>85</v>
       </c>
       <c r="E460" t="inlineStr">
         <is>
@@ -11853,21 +11853,21 @@
     <row r="461">
       <c r="A461" t="inlineStr">
         <is>
-          <t>18:55:46</t>
+          <t>19:36:20</t>
         </is>
       </c>
       <c r="B461" t="inlineStr">
         <is>
-          <t>20:23</t>
+          <t>20:21</t>
         </is>
       </c>
       <c r="C461" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D461" t="n">
-        <v>88</v>
+        <v>45</v>
       </c>
       <c r="E461" t="inlineStr">
         <is>
@@ -11878,21 +11878,21 @@
     <row r="462">
       <c r="A462" t="inlineStr">
         <is>
-          <t>19:15:13</t>
+          <t>19:36:20</t>
         </is>
       </c>
       <c r="B462" t="inlineStr">
         <is>
-          <t>20:24</t>
+          <t>20:22</t>
         </is>
       </c>
       <c r="C462" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D462" t="n">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="E462" t="inlineStr">
         <is>
@@ -11903,21 +11903,21 @@
     <row r="463">
       <c r="A463" t="inlineStr">
         <is>
-          <t>18:36:52</t>
+          <t>19:36:20</t>
         </is>
       </c>
       <c r="B463" t="inlineStr">
         <is>
-          <t>20:30</t>
+          <t>20:22</t>
         </is>
       </c>
       <c r="C463" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D463" t="n">
-        <v>114</v>
+        <v>46</v>
       </c>
       <c r="E463" t="inlineStr">
         <is>
@@ -11928,21 +11928,21 @@
     <row r="464">
       <c r="A464" t="inlineStr">
         <is>
-          <t>19:15:13</t>
+          <t>19:36:20</t>
         </is>
       </c>
       <c r="B464" t="inlineStr">
         <is>
-          <t>20:31</t>
+          <t>20:23</t>
         </is>
       </c>
       <c r="C464" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D464" t="n">
-        <v>76</v>
+        <v>47</v>
       </c>
       <c r="E464" t="inlineStr">
         <is>
@@ -11958,16 +11958,16 @@
       </c>
       <c r="B465" t="inlineStr">
         <is>
-          <t>20:44</t>
+          <t>20:24</t>
         </is>
       </c>
       <c r="C465" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D465" t="n">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="E465" t="inlineStr">
         <is>
@@ -11978,21 +11978,21 @@
     <row r="466">
       <c r="A466" t="inlineStr">
         <is>
-          <t>19:15:13</t>
+          <t>18:36:52</t>
         </is>
       </c>
       <c r="B466" t="inlineStr">
         <is>
-          <t>20:52</t>
+          <t>20:30</t>
         </is>
       </c>
       <c r="C466" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D466" t="n">
-        <v>97</v>
+        <v>114</v>
       </c>
       <c r="E466" t="inlineStr">
         <is>
@@ -12003,21 +12003,21 @@
     <row r="467">
       <c r="A467" t="inlineStr">
         <is>
-          <t>19:15:13</t>
+          <t>19:36:20</t>
         </is>
       </c>
       <c r="B467" t="inlineStr">
         <is>
-          <t>20:56</t>
+          <t>20:31</t>
         </is>
       </c>
       <c r="C467" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D467" t="n">
-        <v>101</v>
+        <v>55</v>
       </c>
       <c r="E467" t="inlineStr">
         <is>
@@ -12028,21 +12028,21 @@
     <row r="468">
       <c r="A468" t="inlineStr">
         <is>
-          <t>19:15:13</t>
+          <t>19:36:20</t>
         </is>
       </c>
       <c r="B468" t="inlineStr">
         <is>
-          <t>20:57</t>
+          <t>20:44</t>
         </is>
       </c>
       <c r="C468" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D468" t="n">
-        <v>102</v>
+        <v>68</v>
       </c>
       <c r="E468" t="inlineStr">
         <is>
@@ -12053,21 +12053,21 @@
     <row r="469">
       <c r="A469" t="inlineStr">
         <is>
-          <t>19:15:13</t>
+          <t>19:36:20</t>
         </is>
       </c>
       <c r="B469" t="inlineStr">
         <is>
-          <t>21:04</t>
+          <t>20:52</t>
         </is>
       </c>
       <c r="C469" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D469" t="n">
-        <v>109</v>
+        <v>76</v>
       </c>
       <c r="E469" t="inlineStr">
         <is>
@@ -12078,23 +12078,173 @@
     <row r="470">
       <c r="A470" t="inlineStr">
         <is>
+          <t>19:36:20</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>20:52</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D470" t="n">
+        <v>76</v>
+      </c>
+      <c r="E470" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
           <t>19:15:13</t>
         </is>
       </c>
-      <c r="B470" t="inlineStr">
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>20:56</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D471" t="n">
+        <v>101</v>
+      </c>
+      <c r="E471" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>19:36:20</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>20:57</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D472" t="n">
+        <v>81</v>
+      </c>
+      <c r="E472" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>19:36:20</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>21:04</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D473" t="n">
+        <v>88</v>
+      </c>
+      <c r="E473" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>19:36:20</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
         <is>
           <t>21:08</t>
         </is>
       </c>
-      <c r="C470" t="inlineStr">
+      <c r="C474" t="inlineStr">
         <is>
           <t>215B_EL PATO</t>
         </is>
       </c>
-      <c r="D470" t="n">
-        <v>113</v>
-      </c>
-      <c r="E470" t="inlineStr">
+      <c r="D474" t="n">
+        <v>92</v>
+      </c>
+      <c r="E474" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>19:36:20</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>21:21</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D475" t="n">
+        <v>105</v>
+      </c>
+      <c r="E475" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>19:36:20</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>21:23</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D476" t="n">
+        <v>107</v>
+      </c>
+      <c r="E476" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -12129,7 +12279,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:15:13</t>
+          <t>Última actualización: 19:36:21</t>
         </is>
       </c>
     </row>
@@ -13320,7 +13470,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>19:15:13</t>
+          <t>19:36:20</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -13334,7 +13484,7 @@
         </is>
       </c>
       <c r="D52" t="n">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -13345,7 +13495,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>18:55:46</t>
+          <t>19:36:20</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -13359,7 +13509,7 @@
         </is>
       </c>
       <c r="D53" t="n">
-        <v>88</v>
+        <v>47</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -13395,7 +13545,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>19:15:13</t>
+          <t>19:36:20</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -13409,7 +13559,7 @@
         </is>
       </c>
       <c r="D55" t="n">
-        <v>113</v>
+        <v>92</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -13428,7 +13578,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E65"/>
+  <dimension ref="A1:E67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13446,14 +13596,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:15:13</t>
+          <t>Última actualización: 19:36:21</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 60</t>
+          <t>Total filas: 62</t>
         </is>
       </c>
     </row>
@@ -14937,12 +15087,12 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>19:15:13</t>
+          <t>19:36:20</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>19:59</t>
+          <t>19:58</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -14951,7 +15101,7 @@
         </is>
       </c>
       <c r="D64" t="n">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -14967,20 +15117,70 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
+          <t>19:59</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>44</v>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>19:36:20</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
           <t>20:39</t>
         </is>
       </c>
-      <c r="C65" t="inlineStr">
+      <c r="C66" t="inlineStr">
         <is>
           <t>215A_LA PLATA</t>
         </is>
       </c>
-      <c r="D65" t="n">
-        <v>84</v>
-      </c>
-      <c r="E65" t="inlineStr">
+      <c r="D66" t="n">
+        <v>63</v>
+      </c>
+      <c r="E66" t="inlineStr">
         <is>
           <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>19:36:20</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>21:29</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>113</v>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 859
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-23.xlsx
+++ b/data/horarios-141-2026-01-23.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E476"/>
+  <dimension ref="A1:E484"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:36:21</t>
+          <t>Última actualización: 19:49:07</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 471</t>
+          <t>Total filas: 479</t>
         </is>
       </c>
     </row>
@@ -1313,7 +1313,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>86_EST CHICA-ESC AGRARIA</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1338,7 +1338,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>86_EST CHICA-ESC AGRARIA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1513,7 +1513,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -1538,7 +1538,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -1963,7 +1963,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D65" t="n">
@@ -1978,7 +1978,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -1988,11 +1988,11 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2003,7 +2003,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -2013,11 +2013,11 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2213,7 +2213,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D75" t="n">
@@ -2238,7 +2238,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D76" t="n">
@@ -2528,7 +2528,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -2538,11 +2538,11 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -2553,7 +2553,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2563,11 +2563,11 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -3163,7 +3163,7 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D113" t="n">
@@ -3188,7 +3188,7 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D114" t="n">
@@ -3278,7 +3278,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>09:33:33</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -3288,11 +3288,11 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D118" t="n">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -3303,7 +3303,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>09:33:33</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -3313,11 +3313,11 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D119" t="n">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -4163,7 +4163,7 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D153" t="n">
@@ -4188,7 +4188,7 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D154" t="n">
@@ -4413,7 +4413,7 @@
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D163" t="n">
@@ -4438,7 +4438,7 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D164" t="n">
@@ -4928,7 +4928,7 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>10:57:35</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
@@ -4938,11 +4938,11 @@
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D184" t="n">
-        <v>77</v>
+        <v>12</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -4953,7 +4953,7 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>10:57:35</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
@@ -4963,11 +4963,11 @@
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D185" t="n">
-        <v>12</v>
+        <v>77</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -5003,7 +5003,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>10:27:29</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
@@ -5013,11 +5013,11 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D187" t="n">
-        <v>110</v>
+        <v>15</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -5028,7 +5028,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>10:27:29</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -5038,11 +5038,11 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D188" t="n">
-        <v>15</v>
+        <v>110</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5063,7 +5063,7 @@
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D189" t="n">
@@ -5088,7 +5088,7 @@
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D190" t="n">
@@ -5528,7 +5528,7 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>12:54:24</t>
+          <t>12:37:00</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
@@ -5538,11 +5538,11 @@
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D208" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -5553,7 +5553,7 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>12:54:24</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
@@ -5563,11 +5563,11 @@
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D209" t="n">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -5653,7 +5653,7 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>12:54:24</t>
+          <t>12:37:00</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
@@ -5663,11 +5663,11 @@
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D213" t="n">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -5678,7 +5678,7 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>12:54:24</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
@@ -5688,11 +5688,11 @@
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D214" t="n">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
@@ -5988,7 +5988,7 @@
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D226" t="n">
@@ -6013,7 +6013,7 @@
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D227" t="n">
@@ -6188,7 +6188,7 @@
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D234" t="n">
@@ -6213,7 +6213,7 @@
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D235" t="n">
@@ -6353,7 +6353,7 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>13:51:20</t>
+          <t>12:37:00</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
@@ -6363,11 +6363,11 @@
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D241" t="n">
-        <v>6</v>
+        <v>80</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -6378,7 +6378,7 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>13:51:20</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
@@ -6388,11 +6388,11 @@
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D242" t="n">
-        <v>80</v>
+        <v>6</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -6403,7 +6403,7 @@
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>13:51:20</t>
+          <t>13:18:32</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
@@ -6413,11 +6413,11 @@
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D243" t="n">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -6428,7 +6428,7 @@
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>13:18:32</t>
+          <t>13:51:20</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
@@ -6438,11 +6438,11 @@
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D244" t="n">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -6838,7 +6838,7 @@
       </c>
       <c r="C260" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D260" t="n">
@@ -6863,7 +6863,7 @@
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D261" t="n">
@@ -7013,7 +7013,7 @@
       </c>
       <c r="C267" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D267" t="n">
@@ -7038,7 +7038,7 @@
       </c>
       <c r="C268" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D268" t="n">
@@ -7238,7 +7238,7 @@
       </c>
       <c r="C276" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D276" t="n">
@@ -7263,7 +7263,7 @@
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D277" t="n">
@@ -7478,7 +7478,7 @@
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>14:55:42</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
@@ -7488,11 +7488,11 @@
       </c>
       <c r="C286" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D286" t="n">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
@@ -7503,7 +7503,7 @@
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>14:55:42</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
@@ -7513,11 +7513,11 @@
       </c>
       <c r="C287" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D287" t="n">
-        <v>51</v>
+        <v>25</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
@@ -7553,7 +7553,7 @@
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>14:55:42</t>
+          <t>14:19:39</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
@@ -7563,11 +7563,11 @@
       </c>
       <c r="C289" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D289" t="n">
-        <v>58</v>
+        <v>94</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
@@ -7578,7 +7578,7 @@
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>14:19:39</t>
+          <t>14:55:42</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
@@ -7588,11 +7588,11 @@
       </c>
       <c r="C290" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D290" t="n">
-        <v>94</v>
+        <v>58</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
@@ -7728,7 +7728,7 @@
     <row r="296">
       <c r="A296" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
@@ -7738,11 +7738,11 @@
       </c>
       <c r="C296" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D296" t="n">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="E296" t="inlineStr">
         <is>
@@ -7753,7 +7753,7 @@
     <row r="297">
       <c r="A297" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
@@ -7763,11 +7763,11 @@
       </c>
       <c r="C297" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D297" t="n">
-        <v>36</v>
+        <v>2</v>
       </c>
       <c r="E297" t="inlineStr">
         <is>
@@ -7853,7 +7853,7 @@
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>14:45:15</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
@@ -7863,11 +7863,11 @@
       </c>
       <c r="C301" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D301" t="n">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="E301" t="inlineStr">
         <is>
@@ -7878,7 +7878,7 @@
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>14:45:15</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
@@ -7888,11 +7888,11 @@
       </c>
       <c r="C302" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D302" t="n">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="E302" t="inlineStr">
         <is>
@@ -7963,7 +7963,7 @@
       </c>
       <c r="C305" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>225_C ROCA-H SUR</t>
         </is>
       </c>
       <c r="D305" t="n">
@@ -7988,7 +7988,7 @@
       </c>
       <c r="C306" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D306" t="n">
@@ -8003,7 +8003,7 @@
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>16:19:35</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
@@ -8013,11 +8013,11 @@
       </c>
       <c r="C307" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D307" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="E307" t="inlineStr">
         <is>
@@ -8028,7 +8028,7 @@
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:19:35</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
@@ -8038,11 +8038,11 @@
       </c>
       <c r="C308" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D308" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="E308" t="inlineStr">
         <is>
@@ -8088,7 +8088,7 @@
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D310" t="n">
@@ -8113,7 +8113,7 @@
       </c>
       <c r="C311" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D311" t="n">
@@ -8203,7 +8203,7 @@
     <row r="315">
       <c r="A315" t="inlineStr">
         <is>
-          <t>16:19:35</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B315" t="inlineStr">
@@ -8213,11 +8213,11 @@
       </c>
       <c r="C315" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D315" t="n">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="E315" t="inlineStr">
         <is>
@@ -8228,7 +8228,7 @@
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:19:35</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
@@ -8238,11 +8238,11 @@
       </c>
       <c r="C316" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D316" t="n">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="E316" t="inlineStr">
         <is>
@@ -8453,7 +8453,7 @@
     <row r="325">
       <c r="A325" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>16:36:35</t>
         </is>
       </c>
       <c r="B325" t="inlineStr">
@@ -8463,11 +8463,11 @@
       </c>
       <c r="C325" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D325" t="n">
-        <v>82</v>
+        <v>7</v>
       </c>
       <c r="E325" t="inlineStr">
         <is>
@@ -8478,7 +8478,7 @@
     <row r="326">
       <c r="A326" t="inlineStr">
         <is>
-          <t>16:36:35</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B326" t="inlineStr">
@@ -8488,11 +8488,11 @@
       </c>
       <c r="C326" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D326" t="n">
-        <v>7</v>
+        <v>82</v>
       </c>
       <c r="E326" t="inlineStr">
         <is>
@@ -8528,7 +8528,7 @@
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>16:46:26</t>
+          <t>16:36:35</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
@@ -8538,11 +8538,11 @@
       </c>
       <c r="C328" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D328" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E328" t="inlineStr">
         <is>
@@ -8553,7 +8553,7 @@
     <row r="329">
       <c r="A329" t="inlineStr">
         <is>
-          <t>16:36:35</t>
+          <t>16:46:26</t>
         </is>
       </c>
       <c r="B329" t="inlineStr">
@@ -8563,11 +8563,11 @@
       </c>
       <c r="C329" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D329" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="E329" t="inlineStr">
         <is>
@@ -8738,7 +8738,7 @@
       </c>
       <c r="C336" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D336" t="n">
@@ -8763,7 +8763,7 @@
       </c>
       <c r="C337" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D337" t="n">
@@ -8888,7 +8888,7 @@
       </c>
       <c r="C342" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D342" t="n">
@@ -8913,7 +8913,7 @@
       </c>
       <c r="C343" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D343" t="n">
@@ -9478,7 +9478,7 @@
     <row r="366">
       <c r="A366" t="inlineStr">
         <is>
-          <t>16:53:56</t>
+          <t>17:42:07</t>
         </is>
       </c>
       <c r="B366" t="inlineStr">
@@ -9488,11 +9488,11 @@
       </c>
       <c r="C366" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D366" t="n">
-        <v>58</v>
+        <v>9</v>
       </c>
       <c r="E366" t="inlineStr">
         <is>
@@ -9503,7 +9503,7 @@
     <row r="367">
       <c r="A367" t="inlineStr">
         <is>
-          <t>17:42:07</t>
+          <t>16:53:56</t>
         </is>
       </c>
       <c r="B367" t="inlineStr">
@@ -9513,11 +9513,11 @@
       </c>
       <c r="C367" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D367" t="n">
-        <v>9</v>
+        <v>58</v>
       </c>
       <c r="E367" t="inlineStr">
         <is>
@@ -9663,7 +9663,7 @@
       </c>
       <c r="C373" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D373" t="n">
@@ -9688,7 +9688,7 @@
       </c>
       <c r="C374" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D374" t="n">
@@ -9838,7 +9838,7 @@
       </c>
       <c r="C380" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D380" t="n">
@@ -9863,7 +9863,7 @@
       </c>
       <c r="C381" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D381" t="n">
@@ -9878,7 +9878,7 @@
     <row r="382">
       <c r="A382" t="inlineStr">
         <is>
-          <t>16:53:56</t>
+          <t>17:57:31</t>
         </is>
       </c>
       <c r="B382" t="inlineStr">
@@ -9888,11 +9888,11 @@
       </c>
       <c r="C382" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D382" t="n">
-        <v>87</v>
+        <v>23</v>
       </c>
       <c r="E382" t="inlineStr">
         <is>
@@ -9903,7 +9903,7 @@
     <row r="383">
       <c r="A383" t="inlineStr">
         <is>
-          <t>17:57:31</t>
+          <t>16:53:56</t>
         </is>
       </c>
       <c r="B383" t="inlineStr">
@@ -9913,11 +9913,11 @@
       </c>
       <c r="C383" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D383" t="n">
-        <v>23</v>
+        <v>87</v>
       </c>
       <c r="E383" t="inlineStr">
         <is>
@@ -10278,7 +10278,7 @@
     <row r="398">
       <c r="A398" t="inlineStr">
         <is>
-          <t>17:57:31</t>
+          <t>18:36:52</t>
         </is>
       </c>
       <c r="B398" t="inlineStr">
@@ -10288,11 +10288,11 @@
       </c>
       <c r="C398" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D398" t="n">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="E398" t="inlineStr">
         <is>
@@ -10303,7 +10303,7 @@
     <row r="399">
       <c r="A399" t="inlineStr">
         <is>
-          <t>18:36:52</t>
+          <t>17:57:31</t>
         </is>
       </c>
       <c r="B399" t="inlineStr">
@@ -10313,11 +10313,11 @@
       </c>
       <c r="C399" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D399" t="n">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="E399" t="inlineStr">
         <is>
@@ -10538,7 +10538,7 @@
       </c>
       <c r="C408" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D408" t="n">
@@ -10563,7 +10563,7 @@
       </c>
       <c r="C409" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D409" t="n">
@@ -10628,7 +10628,7 @@
     <row r="412">
       <c r="A412" t="inlineStr">
         <is>
-          <t>18:55:46</t>
+          <t>18:48:33</t>
         </is>
       </c>
       <c r="B412" t="inlineStr">
@@ -10638,11 +10638,11 @@
       </c>
       <c r="C412" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D412" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E412" t="inlineStr">
         <is>
@@ -10653,7 +10653,7 @@
     <row r="413">
       <c r="A413" t="inlineStr">
         <is>
-          <t>18:48:33</t>
+          <t>18:55:46</t>
         </is>
       </c>
       <c r="B413" t="inlineStr">
@@ -10663,11 +10663,11 @@
       </c>
       <c r="C413" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D413" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E413" t="inlineStr">
         <is>
@@ -10688,7 +10688,7 @@
       </c>
       <c r="C414" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D414" t="n">
@@ -10713,7 +10713,7 @@
       </c>
       <c r="C415" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D415" t="n">
@@ -10863,7 +10863,7 @@
       </c>
       <c r="C421" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D421" t="n">
@@ -10888,7 +10888,7 @@
       </c>
       <c r="C422" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D422" t="n">
@@ -11128,7 +11128,7 @@
     <row r="432">
       <c r="A432" t="inlineStr">
         <is>
-          <t>18:55:46</t>
+          <t>19:15:13</t>
         </is>
       </c>
       <c r="B432" t="inlineStr">
@@ -11138,11 +11138,11 @@
       </c>
       <c r="C432" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D432" t="n">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="E432" t="inlineStr">
         <is>
@@ -11153,7 +11153,7 @@
     <row r="433">
       <c r="A433" t="inlineStr">
         <is>
-          <t>19:15:13</t>
+          <t>18:55:46</t>
         </is>
       </c>
       <c r="B433" t="inlineStr">
@@ -11163,11 +11163,11 @@
       </c>
       <c r="C433" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D433" t="n">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="E433" t="inlineStr">
         <is>
@@ -11338,7 +11338,7 @@
       </c>
       <c r="C440" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D440" t="n">
@@ -11363,7 +11363,7 @@
       </c>
       <c r="C441" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D441" t="n">
@@ -11428,7 +11428,7 @@
     <row r="444">
       <c r="A444" t="inlineStr">
         <is>
-          <t>19:36:20</t>
+          <t>19:49:07</t>
         </is>
       </c>
       <c r="B444" t="inlineStr">
@@ -11442,7 +11442,7 @@
         </is>
       </c>
       <c r="D444" t="n">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="E444" t="inlineStr">
         <is>
@@ -11453,7 +11453,7 @@
     <row r="445">
       <c r="A445" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>19:49:07</t>
         </is>
       </c>
       <c r="B445" t="inlineStr">
@@ -11463,11 +11463,11 @@
       </c>
       <c r="C445" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D445" t="n">
-        <v>93</v>
+        <v>2</v>
       </c>
       <c r="E445" t="inlineStr">
         <is>
@@ -11478,7 +11478,7 @@
     <row r="446">
       <c r="A446" t="inlineStr">
         <is>
-          <t>19:15:13</t>
+          <t>19:49:07</t>
         </is>
       </c>
       <c r="B446" t="inlineStr">
@@ -11492,7 +11492,7 @@
         </is>
       </c>
       <c r="D446" t="n">
-        <v>36</v>
+        <v>2</v>
       </c>
       <c r="E446" t="inlineStr">
         <is>
@@ -11503,7 +11503,7 @@
     <row r="447">
       <c r="A447" t="inlineStr">
         <is>
-          <t>19:36:20</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B447" t="inlineStr">
@@ -11513,11 +11513,11 @@
       </c>
       <c r="C447" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D447" t="n">
-        <v>15</v>
+        <v>93</v>
       </c>
       <c r="E447" t="inlineStr">
         <is>
@@ -11628,7 +11628,7 @@
     <row r="452">
       <c r="A452" t="inlineStr">
         <is>
-          <t>19:36:20</t>
+          <t>19:49:07</t>
         </is>
       </c>
       <c r="B452" t="inlineStr">
@@ -11638,11 +11638,11 @@
       </c>
       <c r="C452" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D452" t="n">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="E452" t="inlineStr">
         <is>
@@ -11653,21 +11653,21 @@
     <row r="453">
       <c r="A453" t="inlineStr">
         <is>
-          <t>19:36:20</t>
+          <t>19:49:07</t>
         </is>
       </c>
       <c r="B453" t="inlineStr">
         <is>
-          <t>20:03</t>
+          <t>20:01</t>
         </is>
       </c>
       <c r="C453" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D453" t="n">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="E453" t="inlineStr">
         <is>
@@ -11678,21 +11678,21 @@
     <row r="454">
       <c r="A454" t="inlineStr">
         <is>
-          <t>19:36:20</t>
+          <t>19:49:07</t>
         </is>
       </c>
       <c r="B454" t="inlineStr">
         <is>
-          <t>20:09</t>
+          <t>20:01</t>
         </is>
       </c>
       <c r="C454" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D454" t="n">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="E454" t="inlineStr">
         <is>
@@ -11708,16 +11708,16 @@
       </c>
       <c r="B455" t="inlineStr">
         <is>
-          <t>20:10</t>
+          <t>20:03</t>
         </is>
       </c>
       <c r="C455" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D455" t="n">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="E455" t="inlineStr">
         <is>
@@ -11728,12 +11728,12 @@
     <row r="456">
       <c r="A456" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>19:49:07</t>
         </is>
       </c>
       <c r="B456" t="inlineStr">
         <is>
-          <t>20:10</t>
+          <t>20:09</t>
         </is>
       </c>
       <c r="C456" t="inlineStr">
@@ -11742,7 +11742,7 @@
         </is>
       </c>
       <c r="D456" t="n">
-        <v>112</v>
+        <v>20</v>
       </c>
       <c r="E456" t="inlineStr">
         <is>
@@ -11753,21 +11753,21 @@
     <row r="457">
       <c r="A457" t="inlineStr">
         <is>
-          <t>19:15:13</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B457" t="inlineStr">
         <is>
-          <t>20:11</t>
+          <t>20:10</t>
         </is>
       </c>
       <c r="C457" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D457" t="n">
-        <v>56</v>
+        <v>112</v>
       </c>
       <c r="E457" t="inlineStr">
         <is>
@@ -11783,16 +11783,16 @@
       </c>
       <c r="B458" t="inlineStr">
         <is>
-          <t>20:11</t>
+          <t>20:10</t>
         </is>
       </c>
       <c r="C458" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D458" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E458" t="inlineStr">
         <is>
@@ -11803,21 +11803,21 @@
     <row r="459">
       <c r="A459" t="inlineStr">
         <is>
-          <t>19:36:20</t>
+          <t>19:49:07</t>
         </is>
       </c>
       <c r="B459" t="inlineStr">
         <is>
-          <t>20:12</t>
+          <t>20:11</t>
         </is>
       </c>
       <c r="C459" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D459" t="n">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="E459" t="inlineStr">
         <is>
@@ -11828,21 +11828,21 @@
     <row r="460">
       <c r="A460" t="inlineStr">
         <is>
-          <t>18:55:46</t>
+          <t>19:49:07</t>
         </is>
       </c>
       <c r="B460" t="inlineStr">
         <is>
-          <t>20:20</t>
+          <t>20:11</t>
         </is>
       </c>
       <c r="C460" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D460" t="n">
-        <v>85</v>
+        <v>22</v>
       </c>
       <c r="E460" t="inlineStr">
         <is>
@@ -11858,16 +11858,16 @@
       </c>
       <c r="B461" t="inlineStr">
         <is>
-          <t>20:21</t>
+          <t>20:12</t>
         </is>
       </c>
       <c r="C461" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D461" t="n">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="E461" t="inlineStr">
         <is>
@@ -11878,21 +11878,21 @@
     <row r="462">
       <c r="A462" t="inlineStr">
         <is>
-          <t>19:36:20</t>
+          <t>19:49:07</t>
         </is>
       </c>
       <c r="B462" t="inlineStr">
         <is>
-          <t>20:22</t>
+          <t>20:13</t>
         </is>
       </c>
       <c r="C462" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D462" t="n">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="E462" t="inlineStr">
         <is>
@@ -11903,21 +11903,21 @@
     <row r="463">
       <c r="A463" t="inlineStr">
         <is>
-          <t>19:36:20</t>
+          <t>18:55:46</t>
         </is>
       </c>
       <c r="B463" t="inlineStr">
         <is>
-          <t>20:22</t>
+          <t>20:20</t>
         </is>
       </c>
       <c r="C463" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D463" t="n">
-        <v>46</v>
+        <v>85</v>
       </c>
       <c r="E463" t="inlineStr">
         <is>
@@ -11928,21 +11928,21 @@
     <row r="464">
       <c r="A464" t="inlineStr">
         <is>
-          <t>19:36:20</t>
+          <t>19:49:07</t>
         </is>
       </c>
       <c r="B464" t="inlineStr">
         <is>
-          <t>20:23</t>
+          <t>20:21</t>
         </is>
       </c>
       <c r="C464" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D464" t="n">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="E464" t="inlineStr">
         <is>
@@ -11953,21 +11953,21 @@
     <row r="465">
       <c r="A465" t="inlineStr">
         <is>
-          <t>19:15:13</t>
+          <t>19:49:07</t>
         </is>
       </c>
       <c r="B465" t="inlineStr">
         <is>
-          <t>20:24</t>
+          <t>20:22</t>
         </is>
       </c>
       <c r="C465" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D465" t="n">
-        <v>69</v>
+        <v>33</v>
       </c>
       <c r="E465" t="inlineStr">
         <is>
@@ -11978,21 +11978,21 @@
     <row r="466">
       <c r="A466" t="inlineStr">
         <is>
-          <t>18:36:52</t>
+          <t>19:36:20</t>
         </is>
       </c>
       <c r="B466" t="inlineStr">
         <is>
-          <t>20:30</t>
+          <t>20:22</t>
         </is>
       </c>
       <c r="C466" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D466" t="n">
-        <v>114</v>
+        <v>46</v>
       </c>
       <c r="E466" t="inlineStr">
         <is>
@@ -12003,21 +12003,21 @@
     <row r="467">
       <c r="A467" t="inlineStr">
         <is>
-          <t>19:36:20</t>
+          <t>19:49:07</t>
         </is>
       </c>
       <c r="B467" t="inlineStr">
         <is>
-          <t>20:31</t>
+          <t>20:23</t>
         </is>
       </c>
       <c r="C467" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D467" t="n">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="E467" t="inlineStr">
         <is>
@@ -12033,16 +12033,16 @@
       </c>
       <c r="B468" t="inlineStr">
         <is>
-          <t>20:44</t>
+          <t>20:23</t>
         </is>
       </c>
       <c r="C468" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D468" t="n">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="E468" t="inlineStr">
         <is>
@@ -12053,21 +12053,21 @@
     <row r="469">
       <c r="A469" t="inlineStr">
         <is>
-          <t>19:36:20</t>
+          <t>19:49:07</t>
         </is>
       </c>
       <c r="B469" t="inlineStr">
         <is>
-          <t>20:52</t>
+          <t>20:24</t>
         </is>
       </c>
       <c r="C469" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D469" t="n">
-        <v>76</v>
+        <v>35</v>
       </c>
       <c r="E469" t="inlineStr">
         <is>
@@ -12078,21 +12078,21 @@
     <row r="470">
       <c r="A470" t="inlineStr">
         <is>
-          <t>19:36:20</t>
+          <t>18:36:52</t>
         </is>
       </c>
       <c r="B470" t="inlineStr">
         <is>
-          <t>20:52</t>
+          <t>20:30</t>
         </is>
       </c>
       <c r="C470" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D470" t="n">
-        <v>76</v>
+        <v>114</v>
       </c>
       <c r="E470" t="inlineStr">
         <is>
@@ -12103,21 +12103,21 @@
     <row r="471">
       <c r="A471" t="inlineStr">
         <is>
-          <t>19:15:13</t>
+          <t>19:49:07</t>
         </is>
       </c>
       <c r="B471" t="inlineStr">
         <is>
-          <t>20:56</t>
+          <t>20:31</t>
         </is>
       </c>
       <c r="C471" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D471" t="n">
-        <v>101</v>
+        <v>42</v>
       </c>
       <c r="E471" t="inlineStr">
         <is>
@@ -12128,21 +12128,21 @@
     <row r="472">
       <c r="A472" t="inlineStr">
         <is>
-          <t>19:36:20</t>
+          <t>19:49:07</t>
         </is>
       </c>
       <c r="B472" t="inlineStr">
         <is>
-          <t>20:57</t>
+          <t>20:44</t>
         </is>
       </c>
       <c r="C472" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D472" t="n">
-        <v>81</v>
+        <v>55</v>
       </c>
       <c r="E472" t="inlineStr">
         <is>
@@ -12153,21 +12153,21 @@
     <row r="473">
       <c r="A473" t="inlineStr">
         <is>
-          <t>19:36:20</t>
+          <t>19:49:07</t>
         </is>
       </c>
       <c r="B473" t="inlineStr">
         <is>
-          <t>21:04</t>
+          <t>20:52</t>
         </is>
       </c>
       <c r="C473" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D473" t="n">
-        <v>88</v>
+        <v>63</v>
       </c>
       <c r="E473" t="inlineStr">
         <is>
@@ -12183,16 +12183,16 @@
       </c>
       <c r="B474" t="inlineStr">
         <is>
-          <t>21:08</t>
+          <t>20:52</t>
         </is>
       </c>
       <c r="C474" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D474" t="n">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="E474" t="inlineStr">
         <is>
@@ -12203,21 +12203,21 @@
     <row r="475">
       <c r="A475" t="inlineStr">
         <is>
-          <t>19:36:20</t>
+          <t>19:49:07</t>
         </is>
       </c>
       <c r="B475" t="inlineStr">
         <is>
-          <t>21:21</t>
+          <t>20:53</t>
         </is>
       </c>
       <c r="C475" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D475" t="n">
-        <v>105</v>
+        <v>64</v>
       </c>
       <c r="E475" t="inlineStr">
         <is>
@@ -12228,23 +12228,223 @@
     <row r="476">
       <c r="A476" t="inlineStr">
         <is>
-          <t>19:36:20</t>
+          <t>19:15:13</t>
         </is>
       </c>
       <c r="B476" t="inlineStr">
         <is>
+          <t>20:56</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D476" t="n">
+        <v>101</v>
+      </c>
+      <c r="E476" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>19:49:07</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>20:57</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D477" t="n">
+        <v>68</v>
+      </c>
+      <c r="E477" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>19:49:07</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>21:04</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D478" t="n">
+        <v>75</v>
+      </c>
+      <c r="E478" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>19:49:07</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>21:08</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D479" t="n">
+        <v>79</v>
+      </c>
+      <c r="E479" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>19:49:07</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>21:21</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D480" t="n">
+        <v>92</v>
+      </c>
+      <c r="E480" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>19:49:07</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
           <t>21:23</t>
         </is>
       </c>
-      <c r="C476" t="inlineStr">
+      <c r="C481" t="inlineStr">
         <is>
           <t>10_OLMOS</t>
         </is>
       </c>
-      <c r="D476" t="n">
-        <v>107</v>
-      </c>
-      <c r="E476" t="inlineStr">
+      <c r="D481" t="n">
+        <v>94</v>
+      </c>
+      <c r="E481" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>19:49:07</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>21:38</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D482" t="n">
+        <v>109</v>
+      </c>
+      <c r="E482" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>19:49:07</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>21:38</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D483" t="n">
+        <v>109</v>
+      </c>
+      <c r="E483" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>19:49:07</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D484" t="n">
+        <v>118</v>
+      </c>
+      <c r="E484" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -12261,7 +12461,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E55"/>
+  <dimension ref="A1:E56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12279,14 +12479,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:36:21</t>
+          <t>Última actualización: 19:49:07</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 50</t>
+          <t>Total filas: 51</t>
         </is>
       </c>
     </row>
@@ -13520,7 +13720,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>19:15:13</t>
+          <t>19:49:07</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -13534,7 +13734,7 @@
         </is>
       </c>
       <c r="D54" t="n">
-        <v>69</v>
+        <v>35</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -13545,7 +13745,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>19:36:20</t>
+          <t>19:49:07</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -13559,9 +13759,34 @@
         </is>
       </c>
       <c r="D55" t="n">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="E55" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>19:49:07</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>118</v>
+      </c>
+      <c r="E56" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -13578,7 +13803,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E67"/>
+  <dimension ref="A1:E68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13596,14 +13821,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:36:21</t>
+          <t>Última actualización: 19:49:07</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 62</t>
+          <t>Total filas: 63</t>
         </is>
       </c>
     </row>
@@ -15087,12 +15312,12 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>19:36:20</t>
+          <t>19:49:07</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>19:58</t>
+          <t>19:56</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -15101,7 +15326,7 @@
         </is>
       </c>
       <c r="D64" t="n">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -15112,12 +15337,12 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>19:15:13</t>
+          <t>19:36:20</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>19:59</t>
+          <t>19:58</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -15126,7 +15351,7 @@
         </is>
       </c>
       <c r="D65" t="n">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -15137,48 +15362,73 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>19:36:20</t>
+          <t>19:15:13</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>20:39</t>
+          <t>19:59</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>L6173</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>19:36:20</t>
+          <t>19:49:07</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
+          <t>20:39</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>50</v>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>19:49:07</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
           <t>21:29</t>
         </is>
       </c>
-      <c r="C67" t="inlineStr">
+      <c r="C68" t="inlineStr">
         <is>
           <t>215C_LA PLATA</t>
         </is>
       </c>
-      <c r="D67" t="n">
-        <v>113</v>
-      </c>
-      <c r="E67" t="inlineStr">
+      <c r="D68" t="n">
+        <v>100</v>
+      </c>
+      <c r="E68" t="inlineStr">
         <is>
           <t>L6203</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 860
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-23.xlsx
+++ b/data/horarios-141-2026-01-23.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E484"/>
+  <dimension ref="A1:E486"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:49:07</t>
+          <t>Última actualización: 19:56:21</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 479</t>
+          <t>Total filas: 481</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D63" t="n">
@@ -1938,7 +1938,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -2128,7 +2128,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -2138,11 +2138,11 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -2153,7 +2153,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -2163,11 +2163,11 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D73" t="n">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -2803,7 +2803,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -2813,11 +2813,11 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D99" t="n">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -2828,7 +2828,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -2838,11 +2838,11 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -2903,7 +2903,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>08:48:01</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -2913,11 +2913,11 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -2928,7 +2928,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>08:48:01</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -2938,11 +2938,11 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D104" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -3153,7 +3153,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3163,11 +3163,11 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>27</v>
+        <v>115</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3188,7 +3188,7 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D114" t="n">
@@ -3203,7 +3203,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
@@ -3213,11 +3213,11 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D115" t="n">
-        <v>115</v>
+        <v>27</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -3278,7 +3278,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>09:33:33</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -3288,11 +3288,11 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D118" t="n">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -3303,7 +3303,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>09:33:33</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -3313,11 +3313,11 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D119" t="n">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -4163,7 +4163,7 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D153" t="n">
@@ -4188,7 +4188,7 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D154" t="n">
@@ -4413,7 +4413,7 @@
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D163" t="n">
@@ -4438,7 +4438,7 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D164" t="n">
@@ -4928,7 +4928,7 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>10:57:35</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
@@ -4938,11 +4938,11 @@
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D184" t="n">
-        <v>12</v>
+        <v>77</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -4953,7 +4953,7 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>10:57:35</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
@@ -4963,11 +4963,11 @@
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D185" t="n">
-        <v>77</v>
+        <v>12</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -5003,7 +5003,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>10:27:29</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
@@ -5013,11 +5013,11 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D187" t="n">
-        <v>15</v>
+        <v>110</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -5028,7 +5028,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>10:27:29</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -5038,11 +5038,11 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D188" t="n">
-        <v>110</v>
+        <v>15</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5288,7 +5288,7 @@
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D198" t="n">
@@ -5313,7 +5313,7 @@
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D199" t="n">
@@ -5813,7 +5813,7 @@
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D219" t="n">
@@ -5838,7 +5838,7 @@
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D220" t="n">
@@ -6238,7 +6238,7 @@
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D236" t="n">
@@ -6263,7 +6263,7 @@
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D237" t="n">
@@ -6313,7 +6313,7 @@
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D239" t="n">
@@ -6338,7 +6338,7 @@
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D240" t="n">
@@ -6353,7 +6353,7 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>13:51:20</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
@@ -6363,11 +6363,11 @@
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D241" t="n">
-        <v>80</v>
+        <v>6</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -6378,7 +6378,7 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>13:51:20</t>
+          <t>12:37:00</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
@@ -6388,11 +6388,11 @@
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D242" t="n">
-        <v>6</v>
+        <v>80</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -6838,7 +6838,7 @@
       </c>
       <c r="C260" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D260" t="n">
@@ -6863,7 +6863,7 @@
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D261" t="n">
@@ -7013,7 +7013,7 @@
       </c>
       <c r="C267" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D267" t="n">
@@ -7038,7 +7038,7 @@
       </c>
       <c r="C268" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D268" t="n">
@@ -7553,7 +7553,7 @@
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>14:19:39</t>
+          <t>14:55:42</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
@@ -7563,11 +7563,11 @@
       </c>
       <c r="C289" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D289" t="n">
-        <v>94</v>
+        <v>58</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
@@ -7578,7 +7578,7 @@
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>14:55:42</t>
+          <t>14:19:39</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
@@ -7588,11 +7588,11 @@
       </c>
       <c r="C290" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D290" t="n">
-        <v>58</v>
+        <v>94</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
@@ -8003,7 +8003,7 @@
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:19:35</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
@@ -8013,11 +8013,11 @@
       </c>
       <c r="C307" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D307" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="E307" t="inlineStr">
         <is>
@@ -8028,7 +8028,7 @@
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>16:19:35</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
@@ -8038,11 +8038,11 @@
       </c>
       <c r="C308" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D308" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="E308" t="inlineStr">
         <is>
@@ -8913,7 +8913,7 @@
       </c>
       <c r="C343" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D343" t="n">
@@ -8938,7 +8938,7 @@
       </c>
       <c r="C344" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D344" t="n">
@@ -9188,7 +9188,7 @@
       </c>
       <c r="C354" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D354" t="n">
@@ -9213,7 +9213,7 @@
       </c>
       <c r="C355" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D355" t="n">
@@ -9338,7 +9338,7 @@
       </c>
       <c r="C360" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D360" t="n">
@@ -9363,7 +9363,7 @@
       </c>
       <c r="C361" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D361" t="n">
@@ -10213,7 +10213,7 @@
       </c>
       <c r="C395" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D395" t="n">
@@ -10238,7 +10238,7 @@
       </c>
       <c r="C396" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D396" t="n">
@@ -10403,7 +10403,7 @@
     <row r="403">
       <c r="A403" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>18:48:33</t>
         </is>
       </c>
       <c r="B403" t="inlineStr">
@@ -10413,11 +10413,11 @@
       </c>
       <c r="C403" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D403" t="n">
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="E403" t="inlineStr">
         <is>
@@ -10428,7 +10428,7 @@
     <row r="404">
       <c r="A404" t="inlineStr">
         <is>
-          <t>18:48:33</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B404" t="inlineStr">
@@ -10438,11 +10438,11 @@
       </c>
       <c r="C404" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D404" t="n">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="E404" t="inlineStr">
         <is>
@@ -10538,7 +10538,7 @@
       </c>
       <c r="C408" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D408" t="n">
@@ -10563,7 +10563,7 @@
       </c>
       <c r="C409" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D409" t="n">
@@ -10628,7 +10628,7 @@
     <row r="412">
       <c r="A412" t="inlineStr">
         <is>
-          <t>18:48:33</t>
+          <t>18:55:46</t>
         </is>
       </c>
       <c r="B412" t="inlineStr">
@@ -10638,11 +10638,11 @@
       </c>
       <c r="C412" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D412" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E412" t="inlineStr">
         <is>
@@ -10653,7 +10653,7 @@
     <row r="413">
       <c r="A413" t="inlineStr">
         <is>
-          <t>18:55:46</t>
+          <t>18:48:33</t>
         </is>
       </c>
       <c r="B413" t="inlineStr">
@@ -10663,11 +10663,11 @@
       </c>
       <c r="C413" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D413" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E413" t="inlineStr">
         <is>
@@ -10688,7 +10688,7 @@
       </c>
       <c r="C414" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D414" t="n">
@@ -10713,7 +10713,7 @@
       </c>
       <c r="C415" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D415" t="n">
@@ -10863,7 +10863,7 @@
       </c>
       <c r="C421" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D421" t="n">
@@ -10888,7 +10888,7 @@
       </c>
       <c r="C422" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D422" t="n">
@@ -10938,7 +10938,7 @@
       </c>
       <c r="C424" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D424" t="n">
@@ -10963,7 +10963,7 @@
       </c>
       <c r="C425" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D425" t="n">
@@ -11078,7 +11078,7 @@
     <row r="430">
       <c r="A430" t="inlineStr">
         <is>
-          <t>18:36:52</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B430" t="inlineStr">
@@ -11088,11 +11088,11 @@
       </c>
       <c r="C430" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D430" t="n">
-        <v>53</v>
+        <v>71</v>
       </c>
       <c r="E430" t="inlineStr">
         <is>
@@ -11103,7 +11103,7 @@
     <row r="431">
       <c r="A431" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>18:36:52</t>
         </is>
       </c>
       <c r="B431" t="inlineStr">
@@ -11113,11 +11113,11 @@
       </c>
       <c r="C431" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D431" t="n">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="E431" t="inlineStr">
         <is>
@@ -11338,7 +11338,7 @@
       </c>
       <c r="C440" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D440" t="n">
@@ -11363,7 +11363,7 @@
       </c>
       <c r="C441" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D441" t="n">
@@ -11453,7 +11453,7 @@
     <row r="445">
       <c r="A445" t="inlineStr">
         <is>
-          <t>19:49:07</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B445" t="inlineStr">
@@ -11463,11 +11463,11 @@
       </c>
       <c r="C445" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D445" t="n">
-        <v>2</v>
+        <v>93</v>
       </c>
       <c r="E445" t="inlineStr">
         <is>
@@ -11503,7 +11503,7 @@
     <row r="447">
       <c r="A447" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>19:49:07</t>
         </is>
       </c>
       <c r="B447" t="inlineStr">
@@ -11513,11 +11513,11 @@
       </c>
       <c r="C447" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D447" t="n">
-        <v>93</v>
+        <v>2</v>
       </c>
       <c r="E447" t="inlineStr">
         <is>
@@ -11578,7 +11578,7 @@
     <row r="450">
       <c r="A450" t="inlineStr">
         <is>
-          <t>19:36:20</t>
+          <t>19:56:21</t>
         </is>
       </c>
       <c r="B450" t="inlineStr">
@@ -11588,11 +11588,11 @@
       </c>
       <c r="C450" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D450" t="n">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="E450" t="inlineStr">
         <is>
@@ -11603,7 +11603,7 @@
     <row r="451">
       <c r="A451" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>19:56:21</t>
         </is>
       </c>
       <c r="B451" t="inlineStr">
@@ -11613,11 +11613,11 @@
       </c>
       <c r="C451" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D451" t="n">
-        <v>102</v>
+        <v>4</v>
       </c>
       <c r="E451" t="inlineStr">
         <is>
@@ -11638,7 +11638,7 @@
       </c>
       <c r="C452" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D452" t="n">
@@ -11663,7 +11663,7 @@
       </c>
       <c r="C453" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D453" t="n">
@@ -11728,7 +11728,7 @@
     <row r="456">
       <c r="A456" t="inlineStr">
         <is>
-          <t>19:49:07</t>
+          <t>19:56:21</t>
         </is>
       </c>
       <c r="B456" t="inlineStr">
@@ -11742,7 +11742,7 @@
         </is>
       </c>
       <c r="D456" t="n">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E456" t="inlineStr">
         <is>
@@ -11753,7 +11753,7 @@
     <row r="457">
       <c r="A457" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>19:56:21</t>
         </is>
       </c>
       <c r="B457" t="inlineStr">
@@ -11763,11 +11763,11 @@
       </c>
       <c r="C457" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D457" t="n">
-        <v>112</v>
+        <v>14</v>
       </c>
       <c r="E457" t="inlineStr">
         <is>
@@ -11778,7 +11778,7 @@
     <row r="458">
       <c r="A458" t="inlineStr">
         <is>
-          <t>19:36:20</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B458" t="inlineStr">
@@ -11788,11 +11788,11 @@
       </c>
       <c r="C458" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D458" t="n">
-        <v>34</v>
+        <v>112</v>
       </c>
       <c r="E458" t="inlineStr">
         <is>
@@ -11828,7 +11828,7 @@
     <row r="460">
       <c r="A460" t="inlineStr">
         <is>
-          <t>19:49:07</t>
+          <t>19:56:21</t>
         </is>
       </c>
       <c r="B460" t="inlineStr">
@@ -11842,7 +11842,7 @@
         </is>
       </c>
       <c r="D460" t="n">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E460" t="inlineStr">
         <is>
@@ -11853,7 +11853,7 @@
     <row r="461">
       <c r="A461" t="inlineStr">
         <is>
-          <t>19:36:20</t>
+          <t>19:56:21</t>
         </is>
       </c>
       <c r="B461" t="inlineStr">
@@ -11867,7 +11867,7 @@
         </is>
       </c>
       <c r="D461" t="n">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="E461" t="inlineStr">
         <is>
@@ -11928,7 +11928,7 @@
     <row r="464">
       <c r="A464" t="inlineStr">
         <is>
-          <t>19:49:07</t>
+          <t>19:56:21</t>
         </is>
       </c>
       <c r="B464" t="inlineStr">
@@ -11942,7 +11942,7 @@
         </is>
       </c>
       <c r="D464" t="n">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="E464" t="inlineStr">
         <is>
@@ -11953,7 +11953,7 @@
     <row r="465">
       <c r="A465" t="inlineStr">
         <is>
-          <t>19:49:07</t>
+          <t>19:56:21</t>
         </is>
       </c>
       <c r="B465" t="inlineStr">
@@ -11967,7 +11967,7 @@
         </is>
       </c>
       <c r="D465" t="n">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E465" t="inlineStr">
         <is>
@@ -11978,7 +11978,7 @@
     <row r="466">
       <c r="A466" t="inlineStr">
         <is>
-          <t>19:36:20</t>
+          <t>19:56:21</t>
         </is>
       </c>
       <c r="B466" t="inlineStr">
@@ -11992,7 +11992,7 @@
         </is>
       </c>
       <c r="D466" t="n">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="E466" t="inlineStr">
         <is>
@@ -12028,7 +12028,7 @@
     <row r="468">
       <c r="A468" t="inlineStr">
         <is>
-          <t>19:36:20</t>
+          <t>19:56:21</t>
         </is>
       </c>
       <c r="B468" t="inlineStr">
@@ -12042,7 +12042,7 @@
         </is>
       </c>
       <c r="D468" t="n">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="E468" t="inlineStr">
         <is>
@@ -12103,7 +12103,7 @@
     <row r="471">
       <c r="A471" t="inlineStr">
         <is>
-          <t>19:49:07</t>
+          <t>19:56:21</t>
         </is>
       </c>
       <c r="B471" t="inlineStr">
@@ -12117,7 +12117,7 @@
         </is>
       </c>
       <c r="D471" t="n">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="E471" t="inlineStr">
         <is>
@@ -12128,21 +12128,21 @@
     <row r="472">
       <c r="A472" t="inlineStr">
         <is>
-          <t>19:49:07</t>
+          <t>19:56:21</t>
         </is>
       </c>
       <c r="B472" t="inlineStr">
         <is>
-          <t>20:44</t>
+          <t>20:34</t>
         </is>
       </c>
       <c r="C472" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D472" t="n">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="E472" t="inlineStr">
         <is>
@@ -12153,21 +12153,21 @@
     <row r="473">
       <c r="A473" t="inlineStr">
         <is>
-          <t>19:49:07</t>
+          <t>19:56:21</t>
         </is>
       </c>
       <c r="B473" t="inlineStr">
         <is>
-          <t>20:52</t>
+          <t>20:44</t>
         </is>
       </c>
       <c r="C473" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D473" t="n">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="E473" t="inlineStr">
         <is>
@@ -12178,7 +12178,7 @@
     <row r="474">
       <c r="A474" t="inlineStr">
         <is>
-          <t>19:36:20</t>
+          <t>19:56:21</t>
         </is>
       </c>
       <c r="B474" t="inlineStr">
@@ -12188,11 +12188,11 @@
       </c>
       <c r="C474" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D474" t="n">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="E474" t="inlineStr">
         <is>
@@ -12203,12 +12203,12 @@
     <row r="475">
       <c r="A475" t="inlineStr">
         <is>
-          <t>19:49:07</t>
+          <t>19:56:21</t>
         </is>
       </c>
       <c r="B475" t="inlineStr">
         <is>
-          <t>20:53</t>
+          <t>20:52</t>
         </is>
       </c>
       <c r="C475" t="inlineStr">
@@ -12217,7 +12217,7 @@
         </is>
       </c>
       <c r="D475" t="n">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="E475" t="inlineStr">
         <is>
@@ -12228,21 +12228,21 @@
     <row r="476">
       <c r="A476" t="inlineStr">
         <is>
-          <t>19:15:13</t>
+          <t>19:49:07</t>
         </is>
       </c>
       <c r="B476" t="inlineStr">
         <is>
-          <t>20:56</t>
+          <t>20:53</t>
         </is>
       </c>
       <c r="C476" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D476" t="n">
-        <v>101</v>
+        <v>64</v>
       </c>
       <c r="E476" t="inlineStr">
         <is>
@@ -12253,21 +12253,21 @@
     <row r="477">
       <c r="A477" t="inlineStr">
         <is>
-          <t>19:49:07</t>
+          <t>19:15:13</t>
         </is>
       </c>
       <c r="B477" t="inlineStr">
         <is>
-          <t>20:57</t>
+          <t>20:56</t>
         </is>
       </c>
       <c r="C477" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D477" t="n">
-        <v>68</v>
+        <v>101</v>
       </c>
       <c r="E477" t="inlineStr">
         <is>
@@ -12278,21 +12278,21 @@
     <row r="478">
       <c r="A478" t="inlineStr">
         <is>
-          <t>19:49:07</t>
+          <t>19:56:21</t>
         </is>
       </c>
       <c r="B478" t="inlineStr">
         <is>
-          <t>21:04</t>
+          <t>20:57</t>
         </is>
       </c>
       <c r="C478" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D478" t="n">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="E478" t="inlineStr">
         <is>
@@ -12303,21 +12303,21 @@
     <row r="479">
       <c r="A479" t="inlineStr">
         <is>
-          <t>19:49:07</t>
+          <t>19:56:21</t>
         </is>
       </c>
       <c r="B479" t="inlineStr">
         <is>
-          <t>21:08</t>
+          <t>21:04</t>
         </is>
       </c>
       <c r="C479" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D479" t="n">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="E479" t="inlineStr">
         <is>
@@ -12328,21 +12328,21 @@
     <row r="480">
       <c r="A480" t="inlineStr">
         <is>
-          <t>19:49:07</t>
+          <t>19:56:21</t>
         </is>
       </c>
       <c r="B480" t="inlineStr">
         <is>
-          <t>21:21</t>
+          <t>21:08</t>
         </is>
       </c>
       <c r="C480" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D480" t="n">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="E480" t="inlineStr">
         <is>
@@ -12353,21 +12353,21 @@
     <row r="481">
       <c r="A481" t="inlineStr">
         <is>
-          <t>19:49:07</t>
+          <t>19:56:21</t>
         </is>
       </c>
       <c r="B481" t="inlineStr">
         <is>
-          <t>21:23</t>
+          <t>21:21</t>
         </is>
       </c>
       <c r="C481" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D481" t="n">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="E481" t="inlineStr">
         <is>
@@ -12383,16 +12383,16 @@
       </c>
       <c r="B482" t="inlineStr">
         <is>
-          <t>21:38</t>
+          <t>21:23</t>
         </is>
       </c>
       <c r="C482" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D482" t="n">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="E482" t="inlineStr">
         <is>
@@ -12403,7 +12403,7 @@
     <row r="483">
       <c r="A483" t="inlineStr">
         <is>
-          <t>19:49:07</t>
+          <t>19:56:21</t>
         </is>
       </c>
       <c r="B483" t="inlineStr">
@@ -12417,7 +12417,7 @@
         </is>
       </c>
       <c r="D483" t="n">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E483" t="inlineStr">
         <is>
@@ -12428,23 +12428,73 @@
     <row r="484">
       <c r="A484" t="inlineStr">
         <is>
-          <t>19:49:07</t>
+          <t>19:56:21</t>
         </is>
       </c>
       <c r="B484" t="inlineStr">
         <is>
+          <t>21:38</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D484" t="n">
+        <v>102</v>
+      </c>
+      <c r="E484" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>19:56:21</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
           <t>21:47</t>
         </is>
       </c>
-      <c r="C484" t="inlineStr">
+      <c r="C485" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D484" t="n">
-        <v>118</v>
-      </c>
-      <c r="E484" t="inlineStr">
+      <c r="D485" t="n">
+        <v>111</v>
+      </c>
+      <c r="E485" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>19:56:21</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>21:53</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D486" t="n">
+        <v>117</v>
+      </c>
+      <c r="E486" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -12479,7 +12529,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:49:07</t>
+          <t>Última actualización: 19:56:21</t>
         </is>
       </c>
     </row>
@@ -13695,7 +13745,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>19:36:20</t>
+          <t>19:56:21</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -13709,7 +13759,7 @@
         </is>
       </c>
       <c r="D53" t="n">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -13745,7 +13795,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>19:49:07</t>
+          <t>19:56:21</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -13759,7 +13809,7 @@
         </is>
       </c>
       <c r="D55" t="n">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -13770,7 +13820,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>19:49:07</t>
+          <t>19:56:21</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -13784,7 +13834,7 @@
         </is>
       </c>
       <c r="D56" t="n">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -13821,7 +13871,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:49:07</t>
+          <t>Última actualización: 19:56:21</t>
         </is>
       </c>
     </row>
@@ -15337,7 +15387,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>19:36:20</t>
+          <t>19:56:21</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -15351,7 +15401,7 @@
         </is>
       </c>
       <c r="D65" t="n">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -15387,7 +15437,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>19:49:07</t>
+          <t>19:56:21</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -15401,7 +15451,7 @@
         </is>
       </c>
       <c r="D67" t="n">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -15412,7 +15462,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>19:49:07</t>
+          <t>19:56:21</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -15426,7 +15476,7 @@
         </is>
       </c>
       <c r="D68" t="n">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 861
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-23.xlsx
+++ b/data/horarios-141-2026-01-23.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E486"/>
+  <dimension ref="A1:E491"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:56:21</t>
+          <t>Última actualización: 20:15:27</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 481</t>
+          <t>Total filas: 486</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1638,11 +1638,11 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>73</v>
+        <v>6</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -1653,7 +1653,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1663,11 +1663,11 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>6</v>
+        <v>73</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -1778,7 +1778,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1788,11 +1788,11 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>17</v>
+        <v>84</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -1803,7 +1803,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1813,11 +1813,11 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D63" t="n">
@@ -1938,7 +1938,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -1963,7 +1963,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D65" t="n">
@@ -1978,7 +1978,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -1988,11 +1988,11 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2003,7 +2003,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -2013,11 +2013,11 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2128,7 +2128,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -2138,11 +2138,11 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -2153,7 +2153,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -2163,11 +2163,11 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D73" t="n">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -2213,7 +2213,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D75" t="n">
@@ -2238,7 +2238,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D76" t="n">
@@ -2528,7 +2528,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -2538,11 +2538,11 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -2553,7 +2553,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2563,11 +2563,11 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -2803,7 +2803,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -2813,11 +2813,11 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D99" t="n">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -2828,7 +2828,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -2838,11 +2838,11 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -2903,7 +2903,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>08:48:01</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -2913,11 +2913,11 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -2928,7 +2928,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>08:48:01</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -2938,11 +2938,11 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D104" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -3278,7 +3278,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>09:33:33</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -3288,11 +3288,11 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D118" t="n">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -3303,7 +3303,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>09:33:33</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -3313,11 +3313,11 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D119" t="n">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -3388,7 +3388,7 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D122" t="n">
@@ -3413,7 +3413,7 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D123" t="n">
@@ -4163,7 +4163,7 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D153" t="n">
@@ -4188,7 +4188,7 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D154" t="n">
@@ -4928,7 +4928,7 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>10:57:35</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
@@ -4938,11 +4938,11 @@
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D184" t="n">
-        <v>77</v>
+        <v>12</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -4953,7 +4953,7 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>10:57:35</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
@@ -4963,11 +4963,11 @@
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D185" t="n">
-        <v>12</v>
+        <v>77</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -5288,7 +5288,7 @@
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D198" t="n">
@@ -5313,7 +5313,7 @@
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D199" t="n">
@@ -5528,7 +5528,7 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>12:54:24</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
@@ -5538,11 +5538,11 @@
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D208" t="n">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -5553,7 +5553,7 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>12:54:24</t>
+          <t>12:37:00</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
@@ -5563,11 +5563,11 @@
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D209" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -5653,7 +5653,7 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>12:54:24</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
@@ -5663,11 +5663,11 @@
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D213" t="n">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -5678,7 +5678,7 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>12:54:24</t>
+          <t>12:37:00</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
@@ -5688,11 +5688,11 @@
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D214" t="n">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
@@ -5813,7 +5813,7 @@
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D219" t="n">
@@ -5838,7 +5838,7 @@
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D220" t="n">
@@ -6138,7 +6138,7 @@
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D232" t="n">
@@ -6163,7 +6163,7 @@
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D233" t="n">
@@ -6188,7 +6188,7 @@
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D234" t="n">
@@ -6213,7 +6213,7 @@
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D235" t="n">
@@ -7013,7 +7013,7 @@
       </c>
       <c r="C267" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D267" t="n">
@@ -7038,7 +7038,7 @@
       </c>
       <c r="C268" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D268" t="n">
@@ -7238,7 +7238,7 @@
       </c>
       <c r="C276" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D276" t="n">
@@ -7263,7 +7263,7 @@
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D277" t="n">
@@ -7478,7 +7478,7 @@
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>14:55:42</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
@@ -7488,11 +7488,11 @@
       </c>
       <c r="C286" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D286" t="n">
-        <v>51</v>
+        <v>25</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
@@ -7503,7 +7503,7 @@
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>14:55:42</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
@@ -7513,11 +7513,11 @@
       </c>
       <c r="C287" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D287" t="n">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
@@ -7678,7 +7678,7 @@
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
@@ -7688,11 +7688,11 @@
       </c>
       <c r="C294" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D294" t="n">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
@@ -7703,7 +7703,7 @@
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
@@ -7713,11 +7713,11 @@
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D295" t="n">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
@@ -7853,7 +7853,7 @@
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>14:45:15</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
@@ -7863,11 +7863,11 @@
       </c>
       <c r="C301" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D301" t="n">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="E301" t="inlineStr">
         <is>
@@ -7878,7 +7878,7 @@
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>14:45:15</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
@@ -7888,11 +7888,11 @@
       </c>
       <c r="C302" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D302" t="n">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="E302" t="inlineStr">
         <is>
@@ -8003,7 +8003,7 @@
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>16:19:35</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
@@ -8013,11 +8013,11 @@
       </c>
       <c r="C307" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D307" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="E307" t="inlineStr">
         <is>
@@ -8028,7 +8028,7 @@
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:19:35</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
@@ -8038,11 +8038,11 @@
       </c>
       <c r="C308" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D308" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="E308" t="inlineStr">
         <is>
@@ -8053,7 +8053,7 @@
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:19:35</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
@@ -8063,11 +8063,11 @@
       </c>
       <c r="C309" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D309" t="n">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
@@ -8088,7 +8088,7 @@
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D310" t="n">
@@ -8103,7 +8103,7 @@
     <row r="311">
       <c r="A311" t="inlineStr">
         <is>
-          <t>16:19:35</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
@@ -8113,11 +8113,11 @@
       </c>
       <c r="C311" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D311" t="n">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="E311" t="inlineStr">
         <is>
@@ -8403,7 +8403,7 @@
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:36:35</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
@@ -8413,11 +8413,11 @@
       </c>
       <c r="C323" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D323" t="n">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="E323" t="inlineStr">
         <is>
@@ -8428,7 +8428,7 @@
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>16:36:35</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
@@ -8438,11 +8438,11 @@
       </c>
       <c r="C324" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D324" t="n">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="E324" t="inlineStr">
         <is>
@@ -8453,7 +8453,7 @@
     <row r="325">
       <c r="A325" t="inlineStr">
         <is>
-          <t>16:36:35</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B325" t="inlineStr">
@@ -8463,11 +8463,11 @@
       </c>
       <c r="C325" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D325" t="n">
-        <v>7</v>
+        <v>82</v>
       </c>
       <c r="E325" t="inlineStr">
         <is>
@@ -8478,7 +8478,7 @@
     <row r="326">
       <c r="A326" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>16:36:35</t>
         </is>
       </c>
       <c r="B326" t="inlineStr">
@@ -8488,11 +8488,11 @@
       </c>
       <c r="C326" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D326" t="n">
-        <v>82</v>
+        <v>7</v>
       </c>
       <c r="E326" t="inlineStr">
         <is>
@@ -8738,7 +8738,7 @@
       </c>
       <c r="C336" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D336" t="n">
@@ -8763,7 +8763,7 @@
       </c>
       <c r="C337" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D337" t="n">
@@ -8888,7 +8888,7 @@
       </c>
       <c r="C342" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D342" t="n">
@@ -8913,7 +8913,7 @@
       </c>
       <c r="C343" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D343" t="n">
@@ -8938,7 +8938,7 @@
       </c>
       <c r="C344" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D344" t="n">
@@ -9663,7 +9663,7 @@
       </c>
       <c r="C373" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D373" t="n">
@@ -9688,7 +9688,7 @@
       </c>
       <c r="C374" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D374" t="n">
@@ -9838,7 +9838,7 @@
       </c>
       <c r="C380" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D380" t="n">
@@ -9863,7 +9863,7 @@
       </c>
       <c r="C381" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D381" t="n">
@@ -9878,7 +9878,7 @@
     <row r="382">
       <c r="A382" t="inlineStr">
         <is>
-          <t>17:57:31</t>
+          <t>16:53:56</t>
         </is>
       </c>
       <c r="B382" t="inlineStr">
@@ -9888,11 +9888,11 @@
       </c>
       <c r="C382" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D382" t="n">
-        <v>23</v>
+        <v>87</v>
       </c>
       <c r="E382" t="inlineStr">
         <is>
@@ -9903,7 +9903,7 @@
     <row r="383">
       <c r="A383" t="inlineStr">
         <is>
-          <t>16:53:56</t>
+          <t>17:57:31</t>
         </is>
       </c>
       <c r="B383" t="inlineStr">
@@ -9913,11 +9913,11 @@
       </c>
       <c r="C383" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D383" t="n">
-        <v>87</v>
+        <v>23</v>
       </c>
       <c r="E383" t="inlineStr">
         <is>
@@ -10453,7 +10453,7 @@
     <row r="405">
       <c r="A405" t="inlineStr">
         <is>
-          <t>18:55:46</t>
+          <t>18:48:33</t>
         </is>
       </c>
       <c r="B405" t="inlineStr">
@@ -10463,11 +10463,11 @@
       </c>
       <c r="C405" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D405" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E405" t="inlineStr">
         <is>
@@ -10478,7 +10478,7 @@
     <row r="406">
       <c r="A406" t="inlineStr">
         <is>
-          <t>18:48:33</t>
+          <t>18:55:46</t>
         </is>
       </c>
       <c r="B406" t="inlineStr">
@@ -10488,11 +10488,11 @@
       </c>
       <c r="C406" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D406" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E406" t="inlineStr">
         <is>
@@ -10628,7 +10628,7 @@
     <row r="412">
       <c r="A412" t="inlineStr">
         <is>
-          <t>18:55:46</t>
+          <t>18:48:33</t>
         </is>
       </c>
       <c r="B412" t="inlineStr">
@@ -10638,11 +10638,11 @@
       </c>
       <c r="C412" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D412" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E412" t="inlineStr">
         <is>
@@ -10653,7 +10653,7 @@
     <row r="413">
       <c r="A413" t="inlineStr">
         <is>
-          <t>18:48:33</t>
+          <t>18:55:46</t>
         </is>
       </c>
       <c r="B413" t="inlineStr">
@@ -10663,11 +10663,11 @@
       </c>
       <c r="C413" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D413" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E413" t="inlineStr">
         <is>
@@ -10863,7 +10863,7 @@
       </c>
       <c r="C421" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D421" t="n">
@@ -10888,7 +10888,7 @@
       </c>
       <c r="C422" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D422" t="n">
@@ -10938,7 +10938,7 @@
       </c>
       <c r="C424" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D424" t="n">
@@ -10963,7 +10963,7 @@
       </c>
       <c r="C425" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D425" t="n">
@@ -11128,7 +11128,7 @@
     <row r="432">
       <c r="A432" t="inlineStr">
         <is>
-          <t>19:15:13</t>
+          <t>18:55:46</t>
         </is>
       </c>
       <c r="B432" t="inlineStr">
@@ -11138,11 +11138,11 @@
       </c>
       <c r="C432" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D432" t="n">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="E432" t="inlineStr">
         <is>
@@ -11153,7 +11153,7 @@
     <row r="433">
       <c r="A433" t="inlineStr">
         <is>
-          <t>18:55:46</t>
+          <t>19:15:13</t>
         </is>
       </c>
       <c r="B433" t="inlineStr">
@@ -11163,11 +11163,11 @@
       </c>
       <c r="C433" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D433" t="n">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="E433" t="inlineStr">
         <is>
@@ -11288,7 +11288,7 @@
       </c>
       <c r="C438" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D438" t="n">
@@ -11313,7 +11313,7 @@
       </c>
       <c r="C439" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D439" t="n">
@@ -11338,7 +11338,7 @@
       </c>
       <c r="C440" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D440" t="n">
@@ -11363,7 +11363,7 @@
       </c>
       <c r="C441" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D441" t="n">
@@ -11403,7 +11403,7 @@
     <row r="443">
       <c r="A443" t="inlineStr">
         <is>
-          <t>19:36:20</t>
+          <t>19:49:07</t>
         </is>
       </c>
       <c r="B443" t="inlineStr">
@@ -11413,11 +11413,11 @@
       </c>
       <c r="C443" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D443" t="n">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="E443" t="inlineStr">
         <is>
@@ -11428,7 +11428,7 @@
     <row r="444">
       <c r="A444" t="inlineStr">
         <is>
-          <t>19:49:07</t>
+          <t>19:36:20</t>
         </is>
       </c>
       <c r="B444" t="inlineStr">
@@ -11438,11 +11438,11 @@
       </c>
       <c r="C444" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D444" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="E444" t="inlineStr">
         <is>
@@ -11453,7 +11453,7 @@
     <row r="445">
       <c r="A445" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>19:49:07</t>
         </is>
       </c>
       <c r="B445" t="inlineStr">
@@ -11463,11 +11463,11 @@
       </c>
       <c r="C445" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D445" t="n">
-        <v>93</v>
+        <v>2</v>
       </c>
       <c r="E445" t="inlineStr">
         <is>
@@ -11503,7 +11503,7 @@
     <row r="447">
       <c r="A447" t="inlineStr">
         <is>
-          <t>19:49:07</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B447" t="inlineStr">
@@ -11513,11 +11513,11 @@
       </c>
       <c r="C447" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D447" t="n">
-        <v>2</v>
+        <v>93</v>
       </c>
       <c r="E447" t="inlineStr">
         <is>
@@ -11928,7 +11928,7 @@
     <row r="464">
       <c r="A464" t="inlineStr">
         <is>
-          <t>19:56:21</t>
+          <t>20:15:27</t>
         </is>
       </c>
       <c r="B464" t="inlineStr">
@@ -11942,7 +11942,7 @@
         </is>
       </c>
       <c r="D464" t="n">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="E464" t="inlineStr">
         <is>
@@ -11953,7 +11953,7 @@
     <row r="465">
       <c r="A465" t="inlineStr">
         <is>
-          <t>19:56:21</t>
+          <t>20:15:27</t>
         </is>
       </c>
       <c r="B465" t="inlineStr">
@@ -11967,7 +11967,7 @@
         </is>
       </c>
       <c r="D465" t="n">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="E465" t="inlineStr">
         <is>
@@ -12003,7 +12003,7 @@
     <row r="467">
       <c r="A467" t="inlineStr">
         <is>
-          <t>19:49:07</t>
+          <t>20:15:27</t>
         </is>
       </c>
       <c r="B467" t="inlineStr">
@@ -12013,11 +12013,11 @@
       </c>
       <c r="C467" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D467" t="n">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="E467" t="inlineStr">
         <is>
@@ -12028,7 +12028,7 @@
     <row r="468">
       <c r="A468" t="inlineStr">
         <is>
-          <t>19:56:21</t>
+          <t>19:49:07</t>
         </is>
       </c>
       <c r="B468" t="inlineStr">
@@ -12038,11 +12038,11 @@
       </c>
       <c r="C468" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D468" t="n">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="E468" t="inlineStr">
         <is>
@@ -12103,7 +12103,7 @@
     <row r="471">
       <c r="A471" t="inlineStr">
         <is>
-          <t>19:56:21</t>
+          <t>20:15:27</t>
         </is>
       </c>
       <c r="B471" t="inlineStr">
@@ -12117,7 +12117,7 @@
         </is>
       </c>
       <c r="D471" t="n">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="E471" t="inlineStr">
         <is>
@@ -12128,7 +12128,7 @@
     <row r="472">
       <c r="A472" t="inlineStr">
         <is>
-          <t>19:56:21</t>
+          <t>20:15:27</t>
         </is>
       </c>
       <c r="B472" t="inlineStr">
@@ -12142,7 +12142,7 @@
         </is>
       </c>
       <c r="D472" t="n">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="E472" t="inlineStr">
         <is>
@@ -12153,7 +12153,7 @@
     <row r="473">
       <c r="A473" t="inlineStr">
         <is>
-          <t>19:56:21</t>
+          <t>20:15:27</t>
         </is>
       </c>
       <c r="B473" t="inlineStr">
@@ -12167,7 +12167,7 @@
         </is>
       </c>
       <c r="D473" t="n">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="E473" t="inlineStr">
         <is>
@@ -12178,7 +12178,7 @@
     <row r="474">
       <c r="A474" t="inlineStr">
         <is>
-          <t>19:56:21</t>
+          <t>20:15:27</t>
         </is>
       </c>
       <c r="B474" t="inlineStr">
@@ -12188,11 +12188,11 @@
       </c>
       <c r="C474" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D474" t="n">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="E474" t="inlineStr">
         <is>
@@ -12203,7 +12203,7 @@
     <row r="475">
       <c r="A475" t="inlineStr">
         <is>
-          <t>19:56:21</t>
+          <t>20:15:27</t>
         </is>
       </c>
       <c r="B475" t="inlineStr">
@@ -12213,11 +12213,11 @@
       </c>
       <c r="C475" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D475" t="n">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="E475" t="inlineStr">
         <is>
@@ -12278,12 +12278,12 @@
     <row r="478">
       <c r="A478" t="inlineStr">
         <is>
-          <t>19:56:21</t>
+          <t>20:15:27</t>
         </is>
       </c>
       <c r="B478" t="inlineStr">
         <is>
-          <t>20:57</t>
+          <t>20:56</t>
         </is>
       </c>
       <c r="C478" t="inlineStr">
@@ -12292,7 +12292,7 @@
         </is>
       </c>
       <c r="D478" t="n">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="E478" t="inlineStr">
         <is>
@@ -12308,16 +12308,16 @@
       </c>
       <c r="B479" t="inlineStr">
         <is>
-          <t>21:04</t>
+          <t>20:57</t>
         </is>
       </c>
       <c r="C479" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D479" t="n">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="E479" t="inlineStr">
         <is>
@@ -12328,21 +12328,21 @@
     <row r="480">
       <c r="A480" t="inlineStr">
         <is>
-          <t>19:56:21</t>
+          <t>20:15:27</t>
         </is>
       </c>
       <c r="B480" t="inlineStr">
         <is>
-          <t>21:08</t>
+          <t>21:01</t>
         </is>
       </c>
       <c r="C480" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D480" t="n">
-        <v>72</v>
+        <v>46</v>
       </c>
       <c r="E480" t="inlineStr">
         <is>
@@ -12353,21 +12353,21 @@
     <row r="481">
       <c r="A481" t="inlineStr">
         <is>
-          <t>19:56:21</t>
+          <t>20:15:27</t>
         </is>
       </c>
       <c r="B481" t="inlineStr">
         <is>
-          <t>21:21</t>
+          <t>21:04</t>
         </is>
       </c>
       <c r="C481" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D481" t="n">
-        <v>85</v>
+        <v>49</v>
       </c>
       <c r="E481" t="inlineStr">
         <is>
@@ -12378,21 +12378,21 @@
     <row r="482">
       <c r="A482" t="inlineStr">
         <is>
-          <t>19:49:07</t>
+          <t>20:15:27</t>
         </is>
       </c>
       <c r="B482" t="inlineStr">
         <is>
-          <t>21:23</t>
+          <t>21:08</t>
         </is>
       </c>
       <c r="C482" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D482" t="n">
-        <v>94</v>
+        <v>53</v>
       </c>
       <c r="E482" t="inlineStr">
         <is>
@@ -12403,21 +12403,21 @@
     <row r="483">
       <c r="A483" t="inlineStr">
         <is>
-          <t>19:56:21</t>
+          <t>20:15:27</t>
         </is>
       </c>
       <c r="B483" t="inlineStr">
         <is>
-          <t>21:38</t>
+          <t>21:21</t>
         </is>
       </c>
       <c r="C483" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D483" t="n">
-        <v>102</v>
+        <v>66</v>
       </c>
       <c r="E483" t="inlineStr">
         <is>
@@ -12428,21 +12428,21 @@
     <row r="484">
       <c r="A484" t="inlineStr">
         <is>
-          <t>19:56:21</t>
+          <t>20:15:27</t>
         </is>
       </c>
       <c r="B484" t="inlineStr">
         <is>
-          <t>21:38</t>
+          <t>21:23</t>
         </is>
       </c>
       <c r="C484" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D484" t="n">
-        <v>102</v>
+        <v>68</v>
       </c>
       <c r="E484" t="inlineStr">
         <is>
@@ -12453,21 +12453,21 @@
     <row r="485">
       <c r="A485" t="inlineStr">
         <is>
-          <t>19:56:21</t>
+          <t>20:15:27</t>
         </is>
       </c>
       <c r="B485" t="inlineStr">
         <is>
-          <t>21:47</t>
+          <t>21:23</t>
         </is>
       </c>
       <c r="C485" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D485" t="n">
-        <v>111</v>
+        <v>68</v>
       </c>
       <c r="E485" t="inlineStr">
         <is>
@@ -12478,23 +12478,148 @@
     <row r="486">
       <c r="A486" t="inlineStr">
         <is>
-          <t>19:56:21</t>
+          <t>20:15:27</t>
         </is>
       </c>
       <c r="B486" t="inlineStr">
         <is>
+          <t>21:32</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D486" t="n">
+        <v>77</v>
+      </c>
+      <c r="E486" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>20:15:27</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>21:38</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D487" t="n">
+        <v>83</v>
+      </c>
+      <c r="E487" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>20:15:27</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>21:38</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D488" t="n">
+        <v>83</v>
+      </c>
+      <c r="E488" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>20:15:27</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D489" t="n">
+        <v>92</v>
+      </c>
+      <c r="E489" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>20:15:27</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
           <t>21:53</t>
         </is>
       </c>
-      <c r="C486" t="inlineStr">
+      <c r="C490" t="inlineStr">
         <is>
           <t>10_OLMOS</t>
         </is>
       </c>
-      <c r="D486" t="n">
-        <v>117</v>
-      </c>
-      <c r="E486" t="inlineStr">
+      <c r="D490" t="n">
+        <v>98</v>
+      </c>
+      <c r="E490" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>20:15:27</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>22:08</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D491" t="n">
+        <v>113</v>
+      </c>
+      <c r="E491" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -12529,7 +12654,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:56:21</t>
+          <t>Última actualización: 20:15:27</t>
         </is>
       </c>
     </row>
@@ -13745,7 +13870,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>19:56:21</t>
+          <t>20:15:27</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -13759,7 +13884,7 @@
         </is>
       </c>
       <c r="D53" t="n">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -13795,7 +13920,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>19:56:21</t>
+          <t>20:15:27</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -13809,7 +13934,7 @@
         </is>
       </c>
       <c r="D55" t="n">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -13820,7 +13945,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>19:56:21</t>
+          <t>20:15:27</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -13834,7 +13959,7 @@
         </is>
       </c>
       <c r="D56" t="n">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -13853,7 +13978,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E68"/>
+  <dimension ref="A1:E69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13871,14 +13996,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:56:21</t>
+          <t>Última actualización: 20:15:27</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 63</t>
+          <t>Total filas: 64</t>
         </is>
       </c>
     </row>
@@ -15437,7 +15562,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>19:56:21</t>
+          <t>20:15:27</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -15451,7 +15576,7 @@
         </is>
       </c>
       <c r="D67" t="n">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -15462,7 +15587,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>19:56:21</t>
+          <t>20:15:27</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -15476,11 +15601,36 @@
         </is>
       </c>
       <c r="D68" t="n">
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>20:15:27</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>22:05</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>110</v>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 862
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-23.xlsx
+++ b/data/horarios-141-2026-01-23.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E491"/>
+  <dimension ref="A1:E503"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:15:27</t>
+          <t>Última actualización: 20:34:42</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 486</t>
+          <t>Total filas: 498</t>
         </is>
       </c>
     </row>
@@ -1513,7 +1513,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -1538,7 +1538,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -1778,7 +1778,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1788,11 +1788,11 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -1803,7 +1803,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1813,11 +1813,11 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>17</v>
+        <v>84</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D63" t="n">
@@ -1938,7 +1938,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -1963,7 +1963,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D65" t="n">
@@ -1988,7 +1988,7 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D66" t="n">
@@ -2528,7 +2528,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -2538,11 +2538,11 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -2553,7 +2553,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2563,11 +2563,11 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -3188,7 +3188,7 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D114" t="n">
@@ -3213,7 +3213,7 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D115" t="n">
@@ -4413,7 +4413,7 @@
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D163" t="n">
@@ -4438,7 +4438,7 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D164" t="n">
@@ -4853,7 +4853,7 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>11:22:44</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
@@ -4863,11 +4863,11 @@
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D181" t="n">
-        <v>44</v>
+        <v>4</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
@@ -4878,7 +4878,7 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>11:22:44</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
@@ -4888,11 +4888,11 @@
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D182" t="n">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
@@ -4928,7 +4928,7 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>10:57:35</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
@@ -4938,11 +4938,11 @@
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D184" t="n">
-        <v>12</v>
+        <v>77</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -4953,7 +4953,7 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>10:57:35</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
@@ -4963,11 +4963,11 @@
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D185" t="n">
-        <v>77</v>
+        <v>12</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -5063,7 +5063,7 @@
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D189" t="n">
@@ -5088,7 +5088,7 @@
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D190" t="n">
@@ -5153,7 +5153,7 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>11:49:23</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
@@ -5163,11 +5163,11 @@
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D193" t="n">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
@@ -5178,7 +5178,7 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>11:49:23</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
@@ -5188,11 +5188,11 @@
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D194" t="n">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -5288,7 +5288,7 @@
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_179 Y 38</t>
         </is>
       </c>
       <c r="D198" t="n">
@@ -5338,7 +5338,7 @@
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>17_179 Y 38</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D200" t="n">
@@ -5653,7 +5653,7 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>12:54:24</t>
+          <t>12:37:00</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
@@ -5663,11 +5663,11 @@
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D213" t="n">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -5678,7 +5678,7 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>12:54:24</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
@@ -5688,11 +5688,11 @@
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D214" t="n">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
@@ -5813,7 +5813,7 @@
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D219" t="n">
@@ -5838,7 +5838,7 @@
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D220" t="n">
@@ -5988,7 +5988,7 @@
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D226" t="n">
@@ -6013,7 +6013,7 @@
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D227" t="n">
@@ -6138,7 +6138,7 @@
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D232" t="n">
@@ -6163,7 +6163,7 @@
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D233" t="n">
@@ -6188,7 +6188,7 @@
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D234" t="n">
@@ -6213,7 +6213,7 @@
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D235" t="n">
@@ -6313,7 +6313,7 @@
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D239" t="n">
@@ -6338,7 +6338,7 @@
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D240" t="n">
@@ -6403,7 +6403,7 @@
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>13:18:32</t>
+          <t>13:51:20</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
@@ -6413,11 +6413,11 @@
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D243" t="n">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -6428,7 +6428,7 @@
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>13:51:20</t>
+          <t>13:18:32</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
@@ -6438,11 +6438,11 @@
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D244" t="n">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -7238,7 +7238,7 @@
       </c>
       <c r="C276" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D276" t="n">
@@ -7263,7 +7263,7 @@
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D277" t="n">
@@ -7728,7 +7728,7 @@
     <row r="296">
       <c r="A296" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
@@ -7738,11 +7738,11 @@
       </c>
       <c r="C296" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D296" t="n">
-        <v>36</v>
+        <v>2</v>
       </c>
       <c r="E296" t="inlineStr">
         <is>
@@ -7753,7 +7753,7 @@
     <row r="297">
       <c r="A297" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
@@ -7763,11 +7763,11 @@
       </c>
       <c r="C297" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D297" t="n">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="E297" t="inlineStr">
         <is>
@@ -7853,7 +7853,7 @@
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>14:45:15</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
@@ -7863,11 +7863,11 @@
       </c>
       <c r="C301" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D301" t="n">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="E301" t="inlineStr">
         <is>
@@ -7878,7 +7878,7 @@
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>14:45:15</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
@@ -7888,11 +7888,11 @@
       </c>
       <c r="C302" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D302" t="n">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="E302" t="inlineStr">
         <is>
@@ -8203,7 +8203,7 @@
     <row r="315">
       <c r="A315" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:19:35</t>
         </is>
       </c>
       <c r="B315" t="inlineStr">
@@ -8213,11 +8213,11 @@
       </c>
       <c r="C315" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D315" t="n">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="E315" t="inlineStr">
         <is>
@@ -8228,7 +8228,7 @@
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
-          <t>16:19:35</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
@@ -8238,11 +8238,11 @@
       </c>
       <c r="C316" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D316" t="n">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="E316" t="inlineStr">
         <is>
@@ -8528,7 +8528,7 @@
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>16:36:35</t>
+          <t>16:46:26</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
@@ -8538,11 +8538,11 @@
       </c>
       <c r="C328" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D328" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="E328" t="inlineStr">
         <is>
@@ -8553,7 +8553,7 @@
     <row r="329">
       <c r="A329" t="inlineStr">
         <is>
-          <t>16:46:26</t>
+          <t>16:36:35</t>
         </is>
       </c>
       <c r="B329" t="inlineStr">
@@ -8563,11 +8563,11 @@
       </c>
       <c r="C329" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D329" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E329" t="inlineStr">
         <is>
@@ -8738,7 +8738,7 @@
       </c>
       <c r="C336" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D336" t="n">
@@ -8763,7 +8763,7 @@
       </c>
       <c r="C337" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D337" t="n">
@@ -8888,7 +8888,7 @@
       </c>
       <c r="C342" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D342" t="n">
@@ -8913,7 +8913,7 @@
       </c>
       <c r="C343" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D343" t="n">
@@ -8963,7 +8963,7 @@
       </c>
       <c r="C345" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D345" t="n">
@@ -8988,7 +8988,7 @@
       </c>
       <c r="C346" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D346" t="n">
@@ -9188,7 +9188,7 @@
       </c>
       <c r="C354" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D354" t="n">
@@ -9213,7 +9213,7 @@
       </c>
       <c r="C355" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D355" t="n">
@@ -9338,7 +9338,7 @@
       </c>
       <c r="C360" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D360" t="n">
@@ -9363,7 +9363,7 @@
       </c>
       <c r="C361" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D361" t="n">
@@ -9478,7 +9478,7 @@
     <row r="366">
       <c r="A366" t="inlineStr">
         <is>
-          <t>17:42:07</t>
+          <t>16:53:56</t>
         </is>
       </c>
       <c r="B366" t="inlineStr">
@@ -9488,11 +9488,11 @@
       </c>
       <c r="C366" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D366" t="n">
-        <v>9</v>
+        <v>58</v>
       </c>
       <c r="E366" t="inlineStr">
         <is>
@@ -9503,7 +9503,7 @@
     <row r="367">
       <c r="A367" t="inlineStr">
         <is>
-          <t>16:53:56</t>
+          <t>17:42:07</t>
         </is>
       </c>
       <c r="B367" t="inlineStr">
@@ -9513,11 +9513,11 @@
       </c>
       <c r="C367" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D367" t="n">
-        <v>58</v>
+        <v>9</v>
       </c>
       <c r="E367" t="inlineStr">
         <is>
@@ -9838,7 +9838,7 @@
       </c>
       <c r="C380" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D380" t="n">
@@ -9863,7 +9863,7 @@
       </c>
       <c r="C381" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D381" t="n">
@@ -9878,7 +9878,7 @@
     <row r="382">
       <c r="A382" t="inlineStr">
         <is>
-          <t>16:53:56</t>
+          <t>17:57:31</t>
         </is>
       </c>
       <c r="B382" t="inlineStr">
@@ -9888,11 +9888,11 @@
       </c>
       <c r="C382" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D382" t="n">
-        <v>87</v>
+        <v>23</v>
       </c>
       <c r="E382" t="inlineStr">
         <is>
@@ -9903,7 +9903,7 @@
     <row r="383">
       <c r="A383" t="inlineStr">
         <is>
-          <t>17:57:31</t>
+          <t>16:53:56</t>
         </is>
       </c>
       <c r="B383" t="inlineStr">
@@ -9913,11 +9913,11 @@
       </c>
       <c r="C383" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D383" t="n">
-        <v>23</v>
+        <v>87</v>
       </c>
       <c r="E383" t="inlineStr">
         <is>
@@ -10213,7 +10213,7 @@
       </c>
       <c r="C395" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D395" t="n">
@@ -10238,7 +10238,7 @@
       </c>
       <c r="C396" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D396" t="n">
@@ -10278,7 +10278,7 @@
     <row r="398">
       <c r="A398" t="inlineStr">
         <is>
-          <t>18:36:52</t>
+          <t>17:57:31</t>
         </is>
       </c>
       <c r="B398" t="inlineStr">
@@ -10288,11 +10288,11 @@
       </c>
       <c r="C398" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D398" t="n">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="E398" t="inlineStr">
         <is>
@@ -10303,7 +10303,7 @@
     <row r="399">
       <c r="A399" t="inlineStr">
         <is>
-          <t>17:57:31</t>
+          <t>18:36:52</t>
         </is>
       </c>
       <c r="B399" t="inlineStr">
@@ -10313,11 +10313,11 @@
       </c>
       <c r="C399" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D399" t="n">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="E399" t="inlineStr">
         <is>
@@ -10453,7 +10453,7 @@
     <row r="405">
       <c r="A405" t="inlineStr">
         <is>
-          <t>18:48:33</t>
+          <t>18:55:46</t>
         </is>
       </c>
       <c r="B405" t="inlineStr">
@@ -10463,11 +10463,11 @@
       </c>
       <c r="C405" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D405" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E405" t="inlineStr">
         <is>
@@ -10478,7 +10478,7 @@
     <row r="406">
       <c r="A406" t="inlineStr">
         <is>
-          <t>18:55:46</t>
+          <t>18:48:33</t>
         </is>
       </c>
       <c r="B406" t="inlineStr">
@@ -10488,11 +10488,11 @@
       </c>
       <c r="C406" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D406" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E406" t="inlineStr">
         <is>
@@ -10628,7 +10628,7 @@
     <row r="412">
       <c r="A412" t="inlineStr">
         <is>
-          <t>18:48:33</t>
+          <t>18:55:46</t>
         </is>
       </c>
       <c r="B412" t="inlineStr">
@@ -10638,11 +10638,11 @@
       </c>
       <c r="C412" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D412" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E412" t="inlineStr">
         <is>
@@ -10653,7 +10653,7 @@
     <row r="413">
       <c r="A413" t="inlineStr">
         <is>
-          <t>18:55:46</t>
+          <t>18:48:33</t>
         </is>
       </c>
       <c r="B413" t="inlineStr">
@@ -10663,11 +10663,11 @@
       </c>
       <c r="C413" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D413" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E413" t="inlineStr">
         <is>
@@ -10863,7 +10863,7 @@
       </c>
       <c r="C421" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D421" t="n">
@@ -10888,7 +10888,7 @@
       </c>
       <c r="C422" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D422" t="n">
@@ -10938,7 +10938,7 @@
       </c>
       <c r="C424" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D424" t="n">
@@ -10963,7 +10963,7 @@
       </c>
       <c r="C425" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D425" t="n">
@@ -10988,7 +10988,7 @@
       </c>
       <c r="C426" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D426" t="n">
@@ -11013,7 +11013,7 @@
       </c>
       <c r="C427" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D427" t="n">
@@ -11078,7 +11078,7 @@
     <row r="430">
       <c r="A430" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>18:36:52</t>
         </is>
       </c>
       <c r="B430" t="inlineStr">
@@ -11088,11 +11088,11 @@
       </c>
       <c r="C430" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D430" t="n">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="E430" t="inlineStr">
         <is>
@@ -11103,7 +11103,7 @@
     <row r="431">
       <c r="A431" t="inlineStr">
         <is>
-          <t>18:36:52</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B431" t="inlineStr">
@@ -11113,11 +11113,11 @@
       </c>
       <c r="C431" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D431" t="n">
-        <v>53</v>
+        <v>71</v>
       </c>
       <c r="E431" t="inlineStr">
         <is>
@@ -11288,7 +11288,7 @@
       </c>
       <c r="C438" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D438" t="n">
@@ -11313,7 +11313,7 @@
       </c>
       <c r="C439" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D439" t="n">
@@ -11478,7 +11478,7 @@
     <row r="446">
       <c r="A446" t="inlineStr">
         <is>
-          <t>19:49:07</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B446" t="inlineStr">
@@ -11488,11 +11488,11 @@
       </c>
       <c r="C446" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D446" t="n">
-        <v>2</v>
+        <v>93</v>
       </c>
       <c r="E446" t="inlineStr">
         <is>
@@ -11503,7 +11503,7 @@
     <row r="447">
       <c r="A447" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>19:49:07</t>
         </is>
       </c>
       <c r="B447" t="inlineStr">
@@ -11513,11 +11513,11 @@
       </c>
       <c r="C447" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D447" t="n">
-        <v>93</v>
+        <v>2</v>
       </c>
       <c r="E447" t="inlineStr">
         <is>
@@ -11588,7 +11588,7 @@
       </c>
       <c r="C450" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D450" t="n">
@@ -11613,7 +11613,7 @@
       </c>
       <c r="C451" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D451" t="n">
@@ -11663,7 +11663,7 @@
       </c>
       <c r="C453" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D453" t="n">
@@ -11688,7 +11688,7 @@
       </c>
       <c r="C454" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D454" t="n">
@@ -11753,7 +11753,7 @@
     <row r="457">
       <c r="A457" t="inlineStr">
         <is>
-          <t>19:56:21</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B457" t="inlineStr">
@@ -11763,11 +11763,11 @@
       </c>
       <c r="C457" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D457" t="n">
-        <v>14</v>
+        <v>112</v>
       </c>
       <c r="E457" t="inlineStr">
         <is>
@@ -11778,7 +11778,7 @@
     <row r="458">
       <c r="A458" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>19:56:21</t>
         </is>
       </c>
       <c r="B458" t="inlineStr">
@@ -11788,11 +11788,11 @@
       </c>
       <c r="C458" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D458" t="n">
-        <v>112</v>
+        <v>14</v>
       </c>
       <c r="E458" t="inlineStr">
         <is>
@@ -11803,7 +11803,7 @@
     <row r="459">
       <c r="A459" t="inlineStr">
         <is>
-          <t>19:49:07</t>
+          <t>19:56:21</t>
         </is>
       </c>
       <c r="B459" t="inlineStr">
@@ -11813,11 +11813,11 @@
       </c>
       <c r="C459" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D459" t="n">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E459" t="inlineStr">
         <is>
@@ -11828,7 +11828,7 @@
     <row r="460">
       <c r="A460" t="inlineStr">
         <is>
-          <t>19:56:21</t>
+          <t>19:49:07</t>
         </is>
       </c>
       <c r="B460" t="inlineStr">
@@ -11838,11 +11838,11 @@
       </c>
       <c r="C460" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D460" t="n">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="E460" t="inlineStr">
         <is>
@@ -12153,7 +12153,7 @@
     <row r="473">
       <c r="A473" t="inlineStr">
         <is>
-          <t>20:15:27</t>
+          <t>20:34:42</t>
         </is>
       </c>
       <c r="B473" t="inlineStr">
@@ -12167,7 +12167,7 @@
         </is>
       </c>
       <c r="D473" t="n">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="E473" t="inlineStr">
         <is>
@@ -12178,7 +12178,7 @@
     <row r="474">
       <c r="A474" t="inlineStr">
         <is>
-          <t>20:15:27</t>
+          <t>20:34:42</t>
         </is>
       </c>
       <c r="B474" t="inlineStr">
@@ -12192,7 +12192,7 @@
         </is>
       </c>
       <c r="D474" t="n">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="E474" t="inlineStr">
         <is>
@@ -12278,7 +12278,7 @@
     <row r="478">
       <c r="A478" t="inlineStr">
         <is>
-          <t>20:15:27</t>
+          <t>20:34:42</t>
         </is>
       </c>
       <c r="B478" t="inlineStr">
@@ -12292,7 +12292,7 @@
         </is>
       </c>
       <c r="D478" t="n">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="E478" t="inlineStr">
         <is>
@@ -12328,7 +12328,7 @@
     <row r="480">
       <c r="A480" t="inlineStr">
         <is>
-          <t>20:15:27</t>
+          <t>20:34:42</t>
         </is>
       </c>
       <c r="B480" t="inlineStr">
@@ -12342,7 +12342,7 @@
         </is>
       </c>
       <c r="D480" t="n">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="E480" t="inlineStr">
         <is>
@@ -12378,12 +12378,12 @@
     <row r="482">
       <c r="A482" t="inlineStr">
         <is>
-          <t>20:15:27</t>
+          <t>20:34:42</t>
         </is>
       </c>
       <c r="B482" t="inlineStr">
         <is>
-          <t>21:08</t>
+          <t>21:07</t>
         </is>
       </c>
       <c r="C482" t="inlineStr">
@@ -12392,7 +12392,7 @@
         </is>
       </c>
       <c r="D482" t="n">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="E482" t="inlineStr">
         <is>
@@ -12408,16 +12408,16 @@
       </c>
       <c r="B483" t="inlineStr">
         <is>
-          <t>21:21</t>
+          <t>21:08</t>
         </is>
       </c>
       <c r="C483" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D483" t="n">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="E483" t="inlineStr">
         <is>
@@ -12428,21 +12428,21 @@
     <row r="484">
       <c r="A484" t="inlineStr">
         <is>
-          <t>20:15:27</t>
+          <t>20:34:42</t>
         </is>
       </c>
       <c r="B484" t="inlineStr">
         <is>
-          <t>21:23</t>
+          <t>21:10</t>
         </is>
       </c>
       <c r="C484" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D484" t="n">
-        <v>68</v>
+        <v>36</v>
       </c>
       <c r="E484" t="inlineStr">
         <is>
@@ -12453,21 +12453,21 @@
     <row r="485">
       <c r="A485" t="inlineStr">
         <is>
-          <t>20:15:27</t>
+          <t>20:34:42</t>
         </is>
       </c>
       <c r="B485" t="inlineStr">
         <is>
-          <t>21:23</t>
+          <t>21:16</t>
         </is>
       </c>
       <c r="C485" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D485" t="n">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="E485" t="inlineStr">
         <is>
@@ -12478,21 +12478,21 @@
     <row r="486">
       <c r="A486" t="inlineStr">
         <is>
-          <t>20:15:27</t>
+          <t>20:34:42</t>
         </is>
       </c>
       <c r="B486" t="inlineStr">
         <is>
-          <t>21:32</t>
+          <t>21:20</t>
         </is>
       </c>
       <c r="C486" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D486" t="n">
-        <v>77</v>
+        <v>46</v>
       </c>
       <c r="E486" t="inlineStr">
         <is>
@@ -12508,16 +12508,16 @@
       </c>
       <c r="B487" t="inlineStr">
         <is>
-          <t>21:38</t>
+          <t>21:21</t>
         </is>
       </c>
       <c r="C487" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D487" t="n">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="E487" t="inlineStr">
         <is>
@@ -12528,21 +12528,21 @@
     <row r="488">
       <c r="A488" t="inlineStr">
         <is>
-          <t>20:15:27</t>
+          <t>20:34:42</t>
         </is>
       </c>
       <c r="B488" t="inlineStr">
         <is>
-          <t>21:38</t>
+          <t>21:22</t>
         </is>
       </c>
       <c r="C488" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D488" t="n">
-        <v>83</v>
+        <v>48</v>
       </c>
       <c r="E488" t="inlineStr">
         <is>
@@ -12553,21 +12553,21 @@
     <row r="489">
       <c r="A489" t="inlineStr">
         <is>
-          <t>20:15:27</t>
+          <t>20:34:42</t>
         </is>
       </c>
       <c r="B489" t="inlineStr">
         <is>
-          <t>21:47</t>
+          <t>21:22</t>
         </is>
       </c>
       <c r="C489" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D489" t="n">
-        <v>92</v>
+        <v>48</v>
       </c>
       <c r="E489" t="inlineStr">
         <is>
@@ -12583,16 +12583,16 @@
       </c>
       <c r="B490" t="inlineStr">
         <is>
-          <t>21:53</t>
+          <t>21:23</t>
         </is>
       </c>
       <c r="C490" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D490" t="n">
-        <v>98</v>
+        <v>68</v>
       </c>
       <c r="E490" t="inlineStr">
         <is>
@@ -12608,18 +12608,318 @@
       </c>
       <c r="B491" t="inlineStr">
         <is>
+          <t>21:23</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D491" t="n">
+        <v>68</v>
+      </c>
+      <c r="E491" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>20:15:27</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>21:32</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D492" t="n">
+        <v>77</v>
+      </c>
+      <c r="E492" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>20:34:42</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>21:37</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D493" t="n">
+        <v>63</v>
+      </c>
+      <c r="E493" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>20:34:42</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>21:37</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D494" t="n">
+        <v>63</v>
+      </c>
+      <c r="E494" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>20:15:27</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>21:38</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D495" t="n">
+        <v>83</v>
+      </c>
+      <c r="E495" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>20:34:42</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>21:38</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D496" t="n">
+        <v>64</v>
+      </c>
+      <c r="E496" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>20:34:42</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D497" t="n">
+        <v>73</v>
+      </c>
+      <c r="E497" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>20:34:42</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>21:52</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D498" t="n">
+        <v>78</v>
+      </c>
+      <c r="E498" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>20:15:27</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>21:53</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D499" t="n">
+        <v>98</v>
+      </c>
+      <c r="E499" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>20:34:42</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
           <t>22:08</t>
         </is>
       </c>
-      <c r="C491" t="inlineStr">
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D500" t="n">
+        <v>94</v>
+      </c>
+      <c r="E500" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>20:15:27</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>22:08</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
         <is>
           <t>17_ROMERO</t>
         </is>
       </c>
-      <c r="D491" t="n">
+      <c r="D501" t="n">
         <v>113</v>
       </c>
-      <c r="E491" t="inlineStr">
+      <c r="E501" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>20:34:42</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>22:19</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D502" t="n">
+        <v>105</v>
+      </c>
+      <c r="E502" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>20:34:42</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>22:27</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D503" t="n">
+        <v>113</v>
+      </c>
+      <c r="E503" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -12636,7 +12936,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E56"/>
+  <dimension ref="A1:E57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12654,14 +12954,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:15:27</t>
+          <t>Última actualización: 20:34:42</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 51</t>
+          <t>Total filas: 52</t>
         </is>
       </c>
     </row>
@@ -13920,12 +14220,12 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>20:15:27</t>
+          <t>20:34:42</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>21:08</t>
+          <t>21:07</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -13934,7 +14234,7 @@
         </is>
       </c>
       <c r="D55" t="n">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -13950,18 +14250,43 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
+          <t>21:08</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>53</v>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>20:34:42</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
           <t>21:47</t>
         </is>
       </c>
-      <c r="C56" t="inlineStr">
+      <c r="C57" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D56" t="n">
-        <v>92</v>
-      </c>
-      <c r="E56" t="inlineStr">
+      <c r="D57" t="n">
+        <v>73</v>
+      </c>
+      <c r="E57" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -13978,7 +14303,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E69"/>
+  <dimension ref="A1:E73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13996,14 +14321,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:15:27</t>
+          <t>Última actualización: 20:34:42</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 64</t>
+          <t>Total filas: 68</t>
         </is>
       </c>
     </row>
@@ -15562,12 +15887,12 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>20:15:27</t>
+          <t>20:34:42</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>20:39</t>
+          <t>20:36</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -15576,7 +15901,7 @@
         </is>
       </c>
       <c r="D67" t="n">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -15592,43 +15917,143 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>21:29</t>
+          <t>20:39</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D68" t="n">
-        <v>74</v>
+        <v>24</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>L6203</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
+          <t>20:34:42</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>21:28</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>54</v>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
           <t>20:15:27</t>
         </is>
       </c>
-      <c r="B69" t="inlineStr">
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>21:29</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>74</v>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>20:34:42</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>22:04</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>90</v>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>20:15:27</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
         <is>
           <t>22:05</t>
         </is>
       </c>
-      <c r="C69" t="inlineStr">
+      <c r="C72" t="inlineStr">
         <is>
           <t>215A_LA PLATA</t>
         </is>
       </c>
-      <c r="D69" t="n">
+      <c r="D72" t="n">
         <v>110</v>
       </c>
-      <c r="E69" t="inlineStr">
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>20:34:42</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>22:20</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-40 Y 115</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>106</v>
+      </c>
+      <c r="E73" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 863
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-23.xlsx
+++ b/data/horarios-141-2026-01-23.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E503"/>
+  <dimension ref="A1:E508"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:34:42</t>
+          <t>Última actualización: 20:47:38</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 498</t>
+          <t>Total filas: 503</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1638,11 +1638,11 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>6</v>
+        <v>73</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -1653,7 +1653,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1663,11 +1663,11 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>73</v>
+        <v>6</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -1778,7 +1778,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1788,11 +1788,11 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>17</v>
+        <v>84</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -1803,7 +1803,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1813,11 +1813,11 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D63" t="n">
@@ -1938,7 +1938,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -1953,7 +1953,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1963,11 +1963,11 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -1988,7 +1988,7 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D66" t="n">
@@ -2003,7 +2003,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -2013,11 +2013,11 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2128,7 +2128,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -2138,11 +2138,11 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -2153,7 +2153,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -2163,11 +2163,11 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D73" t="n">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -2213,7 +2213,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D75" t="n">
@@ -2238,7 +2238,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D76" t="n">
@@ -3153,7 +3153,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3163,11 +3163,11 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>115</v>
+        <v>27</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3178,7 +3178,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
@@ -3188,11 +3188,11 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D114" t="n">
-        <v>27</v>
+        <v>115</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -3213,7 +3213,7 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D115" t="n">
@@ -3278,7 +3278,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>09:33:33</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -3288,11 +3288,11 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D118" t="n">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -3303,7 +3303,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>09:33:33</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -3313,11 +3313,11 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D119" t="n">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -3388,7 +3388,7 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D122" t="n">
@@ -3413,7 +3413,7 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D123" t="n">
@@ -5003,7 +5003,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>10:27:29</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
@@ -5013,11 +5013,11 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D187" t="n">
-        <v>110</v>
+        <v>15</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -5028,7 +5028,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>10:27:29</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -5038,11 +5038,11 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D188" t="n">
-        <v>15</v>
+        <v>110</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5153,7 +5153,7 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>11:49:23</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
@@ -5163,11 +5163,11 @@
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D193" t="n">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
@@ -5178,7 +5178,7 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>11:49:23</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
@@ -5188,11 +5188,11 @@
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D194" t="n">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -5288,7 +5288,7 @@
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>17_179 Y 38</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D198" t="n">
@@ -5338,7 +5338,7 @@
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_179 Y 38</t>
         </is>
       </c>
       <c r="D200" t="n">
@@ -5528,7 +5528,7 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>12:54:24</t>
+          <t>12:37:00</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
@@ -5538,11 +5538,11 @@
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D208" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -5553,7 +5553,7 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>12:54:24</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
@@ -5563,11 +5563,11 @@
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D209" t="n">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -6353,7 +6353,7 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>13:51:20</t>
+          <t>12:37:00</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
@@ -6363,11 +6363,11 @@
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D241" t="n">
-        <v>6</v>
+        <v>80</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -6378,7 +6378,7 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>13:51:20</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
@@ -6388,11 +6388,11 @@
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D242" t="n">
-        <v>80</v>
+        <v>6</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -6403,7 +6403,7 @@
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>13:51:20</t>
+          <t>13:18:32</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
@@ -6413,11 +6413,11 @@
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D243" t="n">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -6428,7 +6428,7 @@
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>13:18:32</t>
+          <t>13:51:20</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
@@ -6438,11 +6438,11 @@
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D244" t="n">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -7478,7 +7478,7 @@
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>14:55:42</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
@@ -7488,11 +7488,11 @@
       </c>
       <c r="C286" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D286" t="n">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
@@ -7503,7 +7503,7 @@
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>14:55:42</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
@@ -7513,11 +7513,11 @@
       </c>
       <c r="C287" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D287" t="n">
-        <v>51</v>
+        <v>25</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
@@ -7553,7 +7553,7 @@
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>14:55:42</t>
+          <t>14:19:39</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
@@ -7563,11 +7563,11 @@
       </c>
       <c r="C289" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D289" t="n">
-        <v>58</v>
+        <v>94</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
@@ -7578,7 +7578,7 @@
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>14:19:39</t>
+          <t>14:55:42</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
@@ -7588,11 +7588,11 @@
       </c>
       <c r="C290" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D290" t="n">
-        <v>94</v>
+        <v>58</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
@@ -7628,7 +7628,7 @@
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
@@ -7638,11 +7638,11 @@
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D292" t="n">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
@@ -7653,7 +7653,7 @@
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
@@ -7663,11 +7663,11 @@
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D293" t="n">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
@@ -7678,7 +7678,7 @@
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
@@ -7688,11 +7688,11 @@
       </c>
       <c r="C294" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D294" t="n">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
@@ -7703,7 +7703,7 @@
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
@@ -7713,11 +7713,11 @@
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D295" t="n">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
@@ -7853,7 +7853,7 @@
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>14:45:15</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
@@ -7863,11 +7863,11 @@
       </c>
       <c r="C301" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D301" t="n">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="E301" t="inlineStr">
         <is>
@@ -7878,7 +7878,7 @@
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>14:45:15</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
@@ -7888,11 +7888,11 @@
       </c>
       <c r="C302" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D302" t="n">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="E302" t="inlineStr">
         <is>
@@ -7963,7 +7963,7 @@
       </c>
       <c r="C305" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D305" t="n">
@@ -7988,7 +7988,7 @@
       </c>
       <c r="C306" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>225_C ROCA-H SUR</t>
         </is>
       </c>
       <c r="D306" t="n">
@@ -8203,7 +8203,7 @@
     <row r="315">
       <c r="A315" t="inlineStr">
         <is>
-          <t>16:19:35</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B315" t="inlineStr">
@@ -8213,11 +8213,11 @@
       </c>
       <c r="C315" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D315" t="n">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="E315" t="inlineStr">
         <is>
@@ -8228,7 +8228,7 @@
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:19:35</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
@@ -8238,11 +8238,11 @@
       </c>
       <c r="C316" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D316" t="n">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="E316" t="inlineStr">
         <is>
@@ -8528,7 +8528,7 @@
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>16:46:26</t>
+          <t>16:36:35</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
@@ -8538,11 +8538,11 @@
       </c>
       <c r="C328" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D328" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E328" t="inlineStr">
         <is>
@@ -8553,7 +8553,7 @@
     <row r="329">
       <c r="A329" t="inlineStr">
         <is>
-          <t>16:36:35</t>
+          <t>16:46:26</t>
         </is>
       </c>
       <c r="B329" t="inlineStr">
@@ -8563,11 +8563,11 @@
       </c>
       <c r="C329" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D329" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="E329" t="inlineStr">
         <is>
@@ -8738,7 +8738,7 @@
       </c>
       <c r="C336" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D336" t="n">
@@ -8763,7 +8763,7 @@
       </c>
       <c r="C337" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D337" t="n">
@@ -8888,7 +8888,7 @@
       </c>
       <c r="C342" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D342" t="n">
@@ -8913,7 +8913,7 @@
       </c>
       <c r="C343" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D343" t="n">
@@ -8963,7 +8963,7 @@
       </c>
       <c r="C345" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D345" t="n">
@@ -8988,7 +8988,7 @@
       </c>
       <c r="C346" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D346" t="n">
@@ -9188,7 +9188,7 @@
       </c>
       <c r="C354" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D354" t="n">
@@ -9213,7 +9213,7 @@
       </c>
       <c r="C355" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D355" t="n">
@@ -10538,7 +10538,7 @@
       </c>
       <c r="C408" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D408" t="n">
@@ -10563,7 +10563,7 @@
       </c>
       <c r="C409" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D409" t="n">
@@ -10938,7 +10938,7 @@
       </c>
       <c r="C424" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D424" t="n">
@@ -10963,7 +10963,7 @@
       </c>
       <c r="C425" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D425" t="n">
@@ -11478,7 +11478,7 @@
     <row r="446">
       <c r="A446" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>19:49:07</t>
         </is>
       </c>
       <c r="B446" t="inlineStr">
@@ -11488,11 +11488,11 @@
       </c>
       <c r="C446" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D446" t="n">
-        <v>93</v>
+        <v>2</v>
       </c>
       <c r="E446" t="inlineStr">
         <is>
@@ -11503,7 +11503,7 @@
     <row r="447">
       <c r="A447" t="inlineStr">
         <is>
-          <t>19:49:07</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B447" t="inlineStr">
@@ -11513,11 +11513,11 @@
       </c>
       <c r="C447" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D447" t="n">
-        <v>2</v>
+        <v>93</v>
       </c>
       <c r="E447" t="inlineStr">
         <is>
@@ -11638,7 +11638,7 @@
       </c>
       <c r="C452" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D452" t="n">
@@ -11663,7 +11663,7 @@
       </c>
       <c r="C453" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D453" t="n">
@@ -11688,7 +11688,7 @@
       </c>
       <c r="C454" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D454" t="n">
@@ -12003,7 +12003,7 @@
     <row r="467">
       <c r="A467" t="inlineStr">
         <is>
-          <t>20:15:27</t>
+          <t>19:49:07</t>
         </is>
       </c>
       <c r="B467" t="inlineStr">
@@ -12013,11 +12013,11 @@
       </c>
       <c r="C467" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D467" t="n">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="E467" t="inlineStr">
         <is>
@@ -12028,7 +12028,7 @@
     <row r="468">
       <c r="A468" t="inlineStr">
         <is>
-          <t>19:49:07</t>
+          <t>20:15:27</t>
         </is>
       </c>
       <c r="B468" t="inlineStr">
@@ -12038,11 +12038,11 @@
       </c>
       <c r="C468" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D468" t="n">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="E468" t="inlineStr">
         <is>
@@ -12178,7 +12178,7 @@
     <row r="474">
       <c r="A474" t="inlineStr">
         <is>
-          <t>20:34:42</t>
+          <t>20:47:38</t>
         </is>
       </c>
       <c r="B474" t="inlineStr">
@@ -12192,7 +12192,7 @@
         </is>
       </c>
       <c r="D474" t="n">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="E474" t="inlineStr">
         <is>
@@ -12203,7 +12203,7 @@
     <row r="475">
       <c r="A475" t="inlineStr">
         <is>
-          <t>20:15:27</t>
+          <t>20:47:38</t>
         </is>
       </c>
       <c r="B475" t="inlineStr">
@@ -12217,7 +12217,7 @@
         </is>
       </c>
       <c r="D475" t="n">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="E475" t="inlineStr">
         <is>
@@ -12253,7 +12253,7 @@
     <row r="477">
       <c r="A477" t="inlineStr">
         <is>
-          <t>19:15:13</t>
+          <t>20:47:38</t>
         </is>
       </c>
       <c r="B477" t="inlineStr">
@@ -12263,11 +12263,11 @@
       </c>
       <c r="C477" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D477" t="n">
-        <v>101</v>
+        <v>9</v>
       </c>
       <c r="E477" t="inlineStr">
         <is>
@@ -12278,7 +12278,7 @@
     <row r="478">
       <c r="A478" t="inlineStr">
         <is>
-          <t>20:34:42</t>
+          <t>19:15:13</t>
         </is>
       </c>
       <c r="B478" t="inlineStr">
@@ -12288,11 +12288,11 @@
       </c>
       <c r="C478" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D478" t="n">
-        <v>22</v>
+        <v>101</v>
       </c>
       <c r="E478" t="inlineStr">
         <is>
@@ -12328,7 +12328,7 @@
     <row r="480">
       <c r="A480" t="inlineStr">
         <is>
-          <t>20:34:42</t>
+          <t>20:47:38</t>
         </is>
       </c>
       <c r="B480" t="inlineStr">
@@ -12342,7 +12342,7 @@
         </is>
       </c>
       <c r="D480" t="n">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="E480" t="inlineStr">
         <is>
@@ -12353,7 +12353,7 @@
     <row r="481">
       <c r="A481" t="inlineStr">
         <is>
-          <t>20:15:27</t>
+          <t>20:47:38</t>
         </is>
       </c>
       <c r="B481" t="inlineStr">
@@ -12367,7 +12367,7 @@
         </is>
       </c>
       <c r="D481" t="n">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="E481" t="inlineStr">
         <is>
@@ -12378,7 +12378,7 @@
     <row r="482">
       <c r="A482" t="inlineStr">
         <is>
-          <t>20:34:42</t>
+          <t>20:47:38</t>
         </is>
       </c>
       <c r="B482" t="inlineStr">
@@ -12392,7 +12392,7 @@
         </is>
       </c>
       <c r="D482" t="n">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="E482" t="inlineStr">
         <is>
@@ -12453,7 +12453,7 @@
     <row r="485">
       <c r="A485" t="inlineStr">
         <is>
-          <t>20:34:42</t>
+          <t>20:47:38</t>
         </is>
       </c>
       <c r="B485" t="inlineStr">
@@ -12467,7 +12467,7 @@
         </is>
       </c>
       <c r="D485" t="n">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="E485" t="inlineStr">
         <is>
@@ -12478,7 +12478,7 @@
     <row r="486">
       <c r="A486" t="inlineStr">
         <is>
-          <t>20:34:42</t>
+          <t>20:47:38</t>
         </is>
       </c>
       <c r="B486" t="inlineStr">
@@ -12492,7 +12492,7 @@
         </is>
       </c>
       <c r="D486" t="n">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="E486" t="inlineStr">
         <is>
@@ -12538,7 +12538,7 @@
       </c>
       <c r="C488" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D488" t="n">
@@ -12553,7 +12553,7 @@
     <row r="489">
       <c r="A489" t="inlineStr">
         <is>
-          <t>20:34:42</t>
+          <t>20:47:38</t>
         </is>
       </c>
       <c r="B489" t="inlineStr">
@@ -12563,11 +12563,11 @@
       </c>
       <c r="C489" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D489" t="n">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="E489" t="inlineStr">
         <is>
@@ -12653,12 +12653,12 @@
     <row r="493">
       <c r="A493" t="inlineStr">
         <is>
-          <t>20:34:42</t>
+          <t>20:47:38</t>
         </is>
       </c>
       <c r="B493" t="inlineStr">
         <is>
-          <t>21:37</t>
+          <t>21:34</t>
         </is>
       </c>
       <c r="C493" t="inlineStr">
@@ -12667,7 +12667,7 @@
         </is>
       </c>
       <c r="D493" t="n">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="E493" t="inlineStr">
         <is>
@@ -12688,7 +12688,7 @@
       </c>
       <c r="C494" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D494" t="n">
@@ -12703,12 +12703,12 @@
     <row r="495">
       <c r="A495" t="inlineStr">
         <is>
-          <t>20:15:27</t>
+          <t>20:47:38</t>
         </is>
       </c>
       <c r="B495" t="inlineStr">
         <is>
-          <t>21:38</t>
+          <t>21:37</t>
         </is>
       </c>
       <c r="C495" t="inlineStr">
@@ -12717,7 +12717,7 @@
         </is>
       </c>
       <c r="D495" t="n">
-        <v>83</v>
+        <v>50</v>
       </c>
       <c r="E495" t="inlineStr">
         <is>
@@ -12728,7 +12728,7 @@
     <row r="496">
       <c r="A496" t="inlineStr">
         <is>
-          <t>20:34:42</t>
+          <t>20:15:27</t>
         </is>
       </c>
       <c r="B496" t="inlineStr">
@@ -12738,11 +12738,11 @@
       </c>
       <c r="C496" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D496" t="n">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="E496" t="inlineStr">
         <is>
@@ -12753,21 +12753,21 @@
     <row r="497">
       <c r="A497" t="inlineStr">
         <is>
-          <t>20:34:42</t>
+          <t>20:47:38</t>
         </is>
       </c>
       <c r="B497" t="inlineStr">
         <is>
-          <t>21:47</t>
+          <t>21:38</t>
         </is>
       </c>
       <c r="C497" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D497" t="n">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="E497" t="inlineStr">
         <is>
@@ -12778,21 +12778,21 @@
     <row r="498">
       <c r="A498" t="inlineStr">
         <is>
-          <t>20:34:42</t>
+          <t>20:47:38</t>
         </is>
       </c>
       <c r="B498" t="inlineStr">
         <is>
-          <t>21:52</t>
+          <t>21:47</t>
         </is>
       </c>
       <c r="C498" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D498" t="n">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="E498" t="inlineStr">
         <is>
@@ -12803,12 +12803,12 @@
     <row r="499">
       <c r="A499" t="inlineStr">
         <is>
-          <t>20:15:27</t>
+          <t>20:47:38</t>
         </is>
       </c>
       <c r="B499" t="inlineStr">
         <is>
-          <t>21:53</t>
+          <t>21:52</t>
         </is>
       </c>
       <c r="C499" t="inlineStr">
@@ -12817,7 +12817,7 @@
         </is>
       </c>
       <c r="D499" t="n">
-        <v>98</v>
+        <v>65</v>
       </c>
       <c r="E499" t="inlineStr">
         <is>
@@ -12828,21 +12828,21 @@
     <row r="500">
       <c r="A500" t="inlineStr">
         <is>
-          <t>20:34:42</t>
+          <t>20:15:27</t>
         </is>
       </c>
       <c r="B500" t="inlineStr">
         <is>
-          <t>22:08</t>
+          <t>21:53</t>
         </is>
       </c>
       <c r="C500" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D500" t="n">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="E500" t="inlineStr">
         <is>
@@ -12853,12 +12853,12 @@
     <row r="501">
       <c r="A501" t="inlineStr">
         <is>
-          <t>20:15:27</t>
+          <t>20:47:38</t>
         </is>
       </c>
       <c r="B501" t="inlineStr">
         <is>
-          <t>22:08</t>
+          <t>22:07</t>
         </is>
       </c>
       <c r="C501" t="inlineStr">
@@ -12867,7 +12867,7 @@
         </is>
       </c>
       <c r="D501" t="n">
-        <v>113</v>
+        <v>80</v>
       </c>
       <c r="E501" t="inlineStr">
         <is>
@@ -12878,21 +12878,21 @@
     <row r="502">
       <c r="A502" t="inlineStr">
         <is>
-          <t>20:34:42</t>
+          <t>20:15:27</t>
         </is>
       </c>
       <c r="B502" t="inlineStr">
         <is>
-          <t>22:19</t>
+          <t>22:08</t>
         </is>
       </c>
       <c r="C502" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D502" t="n">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="E502" t="inlineStr">
         <is>
@@ -12903,23 +12903,148 @@
     <row r="503">
       <c r="A503" t="inlineStr">
         <is>
+          <t>20:47:38</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>22:08</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D503" t="n">
+        <v>81</v>
+      </c>
+      <c r="E503" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
           <t>20:34:42</t>
         </is>
       </c>
-      <c r="B503" t="inlineStr">
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>22:19</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D504" t="n">
+        <v>105</v>
+      </c>
+      <c r="E504" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>20:47:38</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>22:22</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D505" t="n">
+        <v>95</v>
+      </c>
+      <c r="E505" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>20:47:38</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
         <is>
           <t>22:27</t>
         </is>
       </c>
-      <c r="C503" t="inlineStr">
+      <c r="C506" t="inlineStr">
         <is>
           <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
-      <c r="D503" t="n">
-        <v>113</v>
-      </c>
-      <c r="E503" t="inlineStr">
+      <c r="D506" t="n">
+        <v>100</v>
+      </c>
+      <c r="E506" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>20:47:38</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>22:32</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D507" t="n">
+        <v>105</v>
+      </c>
+      <c r="E507" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>20:47:38</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>22:39</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D508" t="n">
+        <v>112</v>
+      </c>
+      <c r="E508" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -12936,7 +13061,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E57"/>
+  <dimension ref="A1:E58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12954,14 +13079,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:34:42</t>
+          <t>Última actualización: 20:47:38</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 52</t>
+          <t>Total filas: 53</t>
         </is>
       </c>
     </row>
@@ -14220,7 +14345,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>20:34:42</t>
+          <t>20:47:38</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -14234,7 +14359,7 @@
         </is>
       </c>
       <c r="D55" t="n">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -14270,7 +14395,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>20:34:42</t>
+          <t>20:47:38</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -14284,9 +14409,34 @@
         </is>
       </c>
       <c r="D57" t="n">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="E57" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>20:47:38</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>22:39</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>112</v>
+      </c>
+      <c r="E58" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -14321,7 +14471,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:34:42</t>
+          <t>Última actualización: 20:47:38</t>
         </is>
       </c>
     </row>
@@ -15937,7 +16087,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>20:34:42</t>
+          <t>20:47:38</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -15951,7 +16101,7 @@
         </is>
       </c>
       <c r="D69" t="n">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -15987,7 +16137,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>20:34:42</t>
+          <t>20:47:38</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -16001,7 +16151,7 @@
         </is>
       </c>
       <c r="D71" t="n">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -16037,7 +16187,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>20:34:42</t>
+          <t>20:47:38</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -16051,7 +16201,7 @@
         </is>
       </c>
       <c r="D73" t="n">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 864
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-23.xlsx
+++ b/data/horarios-141-2026-01-23.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E508"/>
+  <dimension ref="A1:E519"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:47:38</t>
+          <t>Última actualización: 20:54:52</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 503</t>
+          <t>Total filas: 514</t>
         </is>
       </c>
     </row>
@@ -1313,7 +1313,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>86_EST CHICA-ESC AGRARIA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1338,7 +1338,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>86_EST CHICA-ESC AGRARIA</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1628,7 +1628,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>06:59:37</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1638,11 +1638,11 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>73</v>
+        <v>6</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -1653,7 +1653,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>06:59:37</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1663,11 +1663,11 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>6</v>
+        <v>73</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -1953,7 +1953,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1963,11 +1963,11 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -2003,7 +2003,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -2013,11 +2013,11 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2803,7 +2803,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -2813,11 +2813,11 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D99" t="n">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -2828,7 +2828,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -2838,11 +2838,11 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -3153,7 +3153,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3163,11 +3163,11 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>27</v>
+        <v>115</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3178,7 +3178,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
@@ -3188,11 +3188,11 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D114" t="n">
-        <v>115</v>
+        <v>27</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -3213,7 +3213,7 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D115" t="n">
@@ -3338,7 +3338,7 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D120" t="n">
@@ -3363,7 +3363,7 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D121" t="n">
@@ -4163,7 +4163,7 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D153" t="n">
@@ -4188,7 +4188,7 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D154" t="n">
@@ -4413,7 +4413,7 @@
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D163" t="n">
@@ -4438,7 +4438,7 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D164" t="n">
@@ -4928,7 +4928,7 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>10:57:35</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
@@ -4938,11 +4938,11 @@
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D184" t="n">
-        <v>77</v>
+        <v>12</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -4953,7 +4953,7 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>10:57:35</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
@@ -4963,11 +4963,11 @@
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D185" t="n">
-        <v>12</v>
+        <v>77</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -5153,7 +5153,7 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>11:49:23</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
@@ -5163,11 +5163,11 @@
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D193" t="n">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
@@ -5178,7 +5178,7 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>11:49:23</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
@@ -5188,11 +5188,11 @@
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D194" t="n">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -5288,7 +5288,7 @@
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_179 Y 38</t>
         </is>
       </c>
       <c r="D198" t="n">
@@ -5338,7 +5338,7 @@
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>17_179 Y 38</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D200" t="n">
@@ -5528,7 +5528,7 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>12:54:24</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
@@ -5538,11 +5538,11 @@
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D208" t="n">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -5553,7 +5553,7 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>12:54:24</t>
+          <t>12:37:00</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
@@ -5563,11 +5563,11 @@
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D209" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -5653,7 +5653,7 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>12:54:24</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
@@ -5663,11 +5663,11 @@
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D213" t="n">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -5678,7 +5678,7 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>12:54:24</t>
+          <t>12:37:00</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
@@ -5688,11 +5688,11 @@
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D214" t="n">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
@@ -5813,7 +5813,7 @@
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D219" t="n">
@@ -5838,7 +5838,7 @@
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D220" t="n">
@@ -6238,7 +6238,7 @@
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D236" t="n">
@@ -6263,7 +6263,7 @@
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D237" t="n">
@@ -6353,7 +6353,7 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>13:51:20</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
@@ -6363,11 +6363,11 @@
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D241" t="n">
-        <v>80</v>
+        <v>6</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -6378,7 +6378,7 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>13:51:20</t>
+          <t>12:37:00</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
@@ -6388,11 +6388,11 @@
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D242" t="n">
-        <v>6</v>
+        <v>80</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -6403,7 +6403,7 @@
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>13:18:32</t>
+          <t>13:51:20</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
@@ -6413,11 +6413,11 @@
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D243" t="n">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -6428,7 +6428,7 @@
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>13:51:20</t>
+          <t>13:18:32</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
@@ -6438,11 +6438,11 @@
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D244" t="n">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -7238,7 +7238,7 @@
       </c>
       <c r="C276" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D276" t="n">
@@ -7263,7 +7263,7 @@
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D277" t="n">
@@ -7478,7 +7478,7 @@
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>14:55:42</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
@@ -7488,11 +7488,11 @@
       </c>
       <c r="C286" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D286" t="n">
-        <v>51</v>
+        <v>25</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
@@ -7503,7 +7503,7 @@
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>14:55:42</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
@@ -7513,11 +7513,11 @@
       </c>
       <c r="C287" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D287" t="n">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
@@ -7553,7 +7553,7 @@
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>14:19:39</t>
+          <t>14:55:42</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
@@ -7563,11 +7563,11 @@
       </c>
       <c r="C289" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D289" t="n">
-        <v>94</v>
+        <v>58</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
@@ -7578,7 +7578,7 @@
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>14:55:42</t>
+          <t>14:19:39</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
@@ -7588,11 +7588,11 @@
       </c>
       <c r="C290" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D290" t="n">
-        <v>58</v>
+        <v>94</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
@@ -7963,7 +7963,7 @@
       </c>
       <c r="C305" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>225_C ROCA-H SUR</t>
         </is>
       </c>
       <c r="D305" t="n">
@@ -7988,7 +7988,7 @@
       </c>
       <c r="C306" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D306" t="n">
@@ -8003,7 +8003,7 @@
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:19:35</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
@@ -8013,11 +8013,11 @@
       </c>
       <c r="C307" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D307" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="E307" t="inlineStr">
         <is>
@@ -8028,7 +8028,7 @@
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>16:19:35</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
@@ -8038,11 +8038,11 @@
       </c>
       <c r="C308" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D308" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="E308" t="inlineStr">
         <is>
@@ -8053,7 +8053,7 @@
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>16:19:35</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
@@ -8063,11 +8063,11 @@
       </c>
       <c r="C309" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D309" t="n">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
@@ -8088,7 +8088,7 @@
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D310" t="n">
@@ -8103,7 +8103,7 @@
     <row r="311">
       <c r="A311" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:19:35</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
@@ -8113,11 +8113,11 @@
       </c>
       <c r="C311" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D311" t="n">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="E311" t="inlineStr">
         <is>
@@ -8203,7 +8203,7 @@
     <row r="315">
       <c r="A315" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:19:35</t>
         </is>
       </c>
       <c r="B315" t="inlineStr">
@@ -8213,11 +8213,11 @@
       </c>
       <c r="C315" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D315" t="n">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="E315" t="inlineStr">
         <is>
@@ -8228,7 +8228,7 @@
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
-          <t>16:19:35</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
@@ -8238,11 +8238,11 @@
       </c>
       <c r="C316" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D316" t="n">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="E316" t="inlineStr">
         <is>
@@ -8653,7 +8653,7 @@
     <row r="333">
       <c r="A333" t="inlineStr">
         <is>
-          <t>16:46:26</t>
+          <t>16:53:56</t>
         </is>
       </c>
       <c r="B333" t="inlineStr">
@@ -8663,11 +8663,11 @@
       </c>
       <c r="C333" t="inlineStr">
         <is>
-          <t>17_179 Y 38</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D333" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E333" t="inlineStr">
         <is>
@@ -8678,7 +8678,7 @@
     <row r="334">
       <c r="A334" t="inlineStr">
         <is>
-          <t>16:53:56</t>
+          <t>16:46:26</t>
         </is>
       </c>
       <c r="B334" t="inlineStr">
@@ -8688,11 +8688,11 @@
       </c>
       <c r="C334" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_179 Y 38</t>
         </is>
       </c>
       <c r="D334" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E334" t="inlineStr">
         <is>
@@ -8963,7 +8963,7 @@
       </c>
       <c r="C345" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D345" t="n">
@@ -8988,7 +8988,7 @@
       </c>
       <c r="C346" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D346" t="n">
@@ -9338,7 +9338,7 @@
       </c>
       <c r="C360" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D360" t="n">
@@ -9363,7 +9363,7 @@
       </c>
       <c r="C361" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D361" t="n">
@@ -9478,7 +9478,7 @@
     <row r="366">
       <c r="A366" t="inlineStr">
         <is>
-          <t>16:53:56</t>
+          <t>17:42:07</t>
         </is>
       </c>
       <c r="B366" t="inlineStr">
@@ -9488,11 +9488,11 @@
       </c>
       <c r="C366" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D366" t="n">
-        <v>58</v>
+        <v>9</v>
       </c>
       <c r="E366" t="inlineStr">
         <is>
@@ -9503,7 +9503,7 @@
     <row r="367">
       <c r="A367" t="inlineStr">
         <is>
-          <t>17:42:07</t>
+          <t>16:53:56</t>
         </is>
       </c>
       <c r="B367" t="inlineStr">
@@ -9513,11 +9513,11 @@
       </c>
       <c r="C367" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D367" t="n">
-        <v>9</v>
+        <v>58</v>
       </c>
       <c r="E367" t="inlineStr">
         <is>
@@ -9878,7 +9878,7 @@
     <row r="382">
       <c r="A382" t="inlineStr">
         <is>
-          <t>17:57:31</t>
+          <t>16:53:56</t>
         </is>
       </c>
       <c r="B382" t="inlineStr">
@@ -9888,11 +9888,11 @@
       </c>
       <c r="C382" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D382" t="n">
-        <v>23</v>
+        <v>87</v>
       </c>
       <c r="E382" t="inlineStr">
         <is>
@@ -9903,7 +9903,7 @@
     <row r="383">
       <c r="A383" t="inlineStr">
         <is>
-          <t>16:53:56</t>
+          <t>17:57:31</t>
         </is>
       </c>
       <c r="B383" t="inlineStr">
@@ -9913,11 +9913,11 @@
       </c>
       <c r="C383" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D383" t="n">
-        <v>87</v>
+        <v>23</v>
       </c>
       <c r="E383" t="inlineStr">
         <is>
@@ -10278,7 +10278,7 @@
     <row r="398">
       <c r="A398" t="inlineStr">
         <is>
-          <t>17:57:31</t>
+          <t>18:36:52</t>
         </is>
       </c>
       <c r="B398" t="inlineStr">
@@ -10288,11 +10288,11 @@
       </c>
       <c r="C398" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D398" t="n">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="E398" t="inlineStr">
         <is>
@@ -10303,7 +10303,7 @@
     <row r="399">
       <c r="A399" t="inlineStr">
         <is>
-          <t>18:36:52</t>
+          <t>17:57:31</t>
         </is>
       </c>
       <c r="B399" t="inlineStr">
@@ -10313,11 +10313,11 @@
       </c>
       <c r="C399" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D399" t="n">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="E399" t="inlineStr">
         <is>
@@ -10403,7 +10403,7 @@
     <row r="403">
       <c r="A403" t="inlineStr">
         <is>
-          <t>18:48:33</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B403" t="inlineStr">
@@ -10413,11 +10413,11 @@
       </c>
       <c r="C403" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D403" t="n">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="E403" t="inlineStr">
         <is>
@@ -10428,7 +10428,7 @@
     <row r="404">
       <c r="A404" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>18:48:33</t>
         </is>
       </c>
       <c r="B404" t="inlineStr">
@@ -10438,11 +10438,11 @@
       </c>
       <c r="C404" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D404" t="n">
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="E404" t="inlineStr">
         <is>
@@ -10453,7 +10453,7 @@
     <row r="405">
       <c r="A405" t="inlineStr">
         <is>
-          <t>18:55:46</t>
+          <t>18:48:33</t>
         </is>
       </c>
       <c r="B405" t="inlineStr">
@@ -10463,11 +10463,11 @@
       </c>
       <c r="C405" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D405" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E405" t="inlineStr">
         <is>
@@ -10478,7 +10478,7 @@
     <row r="406">
       <c r="A406" t="inlineStr">
         <is>
-          <t>18:48:33</t>
+          <t>18:55:46</t>
         </is>
       </c>
       <c r="B406" t="inlineStr">
@@ -10488,11 +10488,11 @@
       </c>
       <c r="C406" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D406" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E406" t="inlineStr">
         <is>
@@ -10538,7 +10538,7 @@
       </c>
       <c r="C408" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D408" t="n">
@@ -10563,7 +10563,7 @@
       </c>
       <c r="C409" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D409" t="n">
@@ -10628,7 +10628,7 @@
     <row r="412">
       <c r="A412" t="inlineStr">
         <is>
-          <t>18:55:46</t>
+          <t>18:48:33</t>
         </is>
       </c>
       <c r="B412" t="inlineStr">
@@ -10638,11 +10638,11 @@
       </c>
       <c r="C412" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D412" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E412" t="inlineStr">
         <is>
@@ -10653,7 +10653,7 @@
     <row r="413">
       <c r="A413" t="inlineStr">
         <is>
-          <t>18:48:33</t>
+          <t>18:55:46</t>
         </is>
       </c>
       <c r="B413" t="inlineStr">
@@ -10663,11 +10663,11 @@
       </c>
       <c r="C413" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D413" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E413" t="inlineStr">
         <is>
@@ -10688,7 +10688,7 @@
       </c>
       <c r="C414" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D414" t="n">
@@ -10713,7 +10713,7 @@
       </c>
       <c r="C415" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D415" t="n">
@@ -10863,7 +10863,7 @@
       </c>
       <c r="C421" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D421" t="n">
@@ -10888,7 +10888,7 @@
       </c>
       <c r="C422" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D422" t="n">
@@ -10988,7 +10988,7 @@
       </c>
       <c r="C426" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D426" t="n">
@@ -11013,7 +11013,7 @@
       </c>
       <c r="C427" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D427" t="n">
@@ -11078,7 +11078,7 @@
     <row r="430">
       <c r="A430" t="inlineStr">
         <is>
-          <t>18:36:52</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B430" t="inlineStr">
@@ -11088,11 +11088,11 @@
       </c>
       <c r="C430" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D430" t="n">
-        <v>53</v>
+        <v>71</v>
       </c>
       <c r="E430" t="inlineStr">
         <is>
@@ -11103,7 +11103,7 @@
     <row r="431">
       <c r="A431" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>18:36:52</t>
         </is>
       </c>
       <c r="B431" t="inlineStr">
@@ -11113,11 +11113,11 @@
       </c>
       <c r="C431" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D431" t="n">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="E431" t="inlineStr">
         <is>
@@ -11288,7 +11288,7 @@
       </c>
       <c r="C438" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D438" t="n">
@@ -11313,7 +11313,7 @@
       </c>
       <c r="C439" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D439" t="n">
@@ -11453,7 +11453,7 @@
     <row r="445">
       <c r="A445" t="inlineStr">
         <is>
-          <t>19:49:07</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B445" t="inlineStr">
@@ -11463,11 +11463,11 @@
       </c>
       <c r="C445" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D445" t="n">
-        <v>2</v>
+        <v>93</v>
       </c>
       <c r="E445" t="inlineStr">
         <is>
@@ -11503,7 +11503,7 @@
     <row r="447">
       <c r="A447" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>19:49:07</t>
         </is>
       </c>
       <c r="B447" t="inlineStr">
@@ -11513,11 +11513,11 @@
       </c>
       <c r="C447" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D447" t="n">
-        <v>93</v>
+        <v>2</v>
       </c>
       <c r="E447" t="inlineStr">
         <is>
@@ -11588,7 +11588,7 @@
       </c>
       <c r="C450" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D450" t="n">
@@ -11613,7 +11613,7 @@
       </c>
       <c r="C451" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D451" t="n">
@@ -11638,7 +11638,7 @@
       </c>
       <c r="C452" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D452" t="n">
@@ -11663,7 +11663,7 @@
       </c>
       <c r="C453" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D453" t="n">
@@ -11688,7 +11688,7 @@
       </c>
       <c r="C454" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D454" t="n">
@@ -11753,7 +11753,7 @@
     <row r="457">
       <c r="A457" t="inlineStr">
         <is>
-          <t>18:18:12</t>
+          <t>19:56:21</t>
         </is>
       </c>
       <c r="B457" t="inlineStr">
@@ -11763,11 +11763,11 @@
       </c>
       <c r="C457" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D457" t="n">
-        <v>112</v>
+        <v>14</v>
       </c>
       <c r="E457" t="inlineStr">
         <is>
@@ -11778,7 +11778,7 @@
     <row r="458">
       <c r="A458" t="inlineStr">
         <is>
-          <t>19:56:21</t>
+          <t>18:18:12</t>
         </is>
       </c>
       <c r="B458" t="inlineStr">
@@ -11788,11 +11788,11 @@
       </c>
       <c r="C458" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D458" t="n">
-        <v>14</v>
+        <v>112</v>
       </c>
       <c r="E458" t="inlineStr">
         <is>
@@ -11803,7 +11803,7 @@
     <row r="459">
       <c r="A459" t="inlineStr">
         <is>
-          <t>19:56:21</t>
+          <t>19:49:07</t>
         </is>
       </c>
       <c r="B459" t="inlineStr">
@@ -11813,11 +11813,11 @@
       </c>
       <c r="C459" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D459" t="n">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="E459" t="inlineStr">
         <is>
@@ -11828,7 +11828,7 @@
     <row r="460">
       <c r="A460" t="inlineStr">
         <is>
-          <t>19:49:07</t>
+          <t>19:56:21</t>
         </is>
       </c>
       <c r="B460" t="inlineStr">
@@ -11838,11 +11838,11 @@
       </c>
       <c r="C460" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D460" t="n">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E460" t="inlineStr">
         <is>
@@ -12188,7 +12188,7 @@
       </c>
       <c r="C474" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D474" t="n">
@@ -12213,7 +12213,7 @@
       </c>
       <c r="C475" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D475" t="n">
@@ -12253,21 +12253,21 @@
     <row r="477">
       <c r="A477" t="inlineStr">
         <is>
-          <t>20:47:38</t>
+          <t>20:54:52</t>
         </is>
       </c>
       <c r="B477" t="inlineStr">
         <is>
-          <t>20:56</t>
+          <t>20:55</t>
         </is>
       </c>
       <c r="C477" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D477" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E477" t="inlineStr">
         <is>
@@ -12278,7 +12278,7 @@
     <row r="478">
       <c r="A478" t="inlineStr">
         <is>
-          <t>19:15:13</t>
+          <t>20:54:52</t>
         </is>
       </c>
       <c r="B478" t="inlineStr">
@@ -12288,11 +12288,11 @@
       </c>
       <c r="C478" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D478" t="n">
-        <v>101</v>
+        <v>2</v>
       </c>
       <c r="E478" t="inlineStr">
         <is>
@@ -12303,21 +12303,21 @@
     <row r="479">
       <c r="A479" t="inlineStr">
         <is>
-          <t>19:56:21</t>
+          <t>19:15:13</t>
         </is>
       </c>
       <c r="B479" t="inlineStr">
         <is>
-          <t>20:57</t>
+          <t>20:56</t>
         </is>
       </c>
       <c r="C479" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D479" t="n">
-        <v>61</v>
+        <v>101</v>
       </c>
       <c r="E479" t="inlineStr">
         <is>
@@ -12328,21 +12328,21 @@
     <row r="480">
       <c r="A480" t="inlineStr">
         <is>
-          <t>20:47:38</t>
+          <t>19:56:21</t>
         </is>
       </c>
       <c r="B480" t="inlineStr">
         <is>
-          <t>21:01</t>
+          <t>20:57</t>
         </is>
       </c>
       <c r="C480" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D480" t="n">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="E480" t="inlineStr">
         <is>
@@ -12353,21 +12353,21 @@
     <row r="481">
       <c r="A481" t="inlineStr">
         <is>
-          <t>20:47:38</t>
+          <t>20:54:52</t>
         </is>
       </c>
       <c r="B481" t="inlineStr">
         <is>
-          <t>21:04</t>
+          <t>21:01</t>
         </is>
       </c>
       <c r="C481" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D481" t="n">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E481" t="inlineStr">
         <is>
@@ -12378,21 +12378,21 @@
     <row r="482">
       <c r="A482" t="inlineStr">
         <is>
-          <t>20:47:38</t>
+          <t>20:54:52</t>
         </is>
       </c>
       <c r="B482" t="inlineStr">
         <is>
-          <t>21:07</t>
+          <t>21:04</t>
         </is>
       </c>
       <c r="C482" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D482" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E482" t="inlineStr">
         <is>
@@ -12403,12 +12403,12 @@
     <row r="483">
       <c r="A483" t="inlineStr">
         <is>
-          <t>20:15:27</t>
+          <t>20:54:52</t>
         </is>
       </c>
       <c r="B483" t="inlineStr">
         <is>
-          <t>21:08</t>
+          <t>21:07</t>
         </is>
       </c>
       <c r="C483" t="inlineStr">
@@ -12417,7 +12417,7 @@
         </is>
       </c>
       <c r="D483" t="n">
-        <v>53</v>
+        <v>13</v>
       </c>
       <c r="E483" t="inlineStr">
         <is>
@@ -12428,21 +12428,21 @@
     <row r="484">
       <c r="A484" t="inlineStr">
         <is>
-          <t>20:34:42</t>
+          <t>20:15:27</t>
         </is>
       </c>
       <c r="B484" t="inlineStr">
         <is>
-          <t>21:10</t>
+          <t>21:08</t>
         </is>
       </c>
       <c r="C484" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D484" t="n">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="E484" t="inlineStr">
         <is>
@@ -12453,21 +12453,21 @@
     <row r="485">
       <c r="A485" t="inlineStr">
         <is>
-          <t>20:47:38</t>
+          <t>20:34:42</t>
         </is>
       </c>
       <c r="B485" t="inlineStr">
         <is>
-          <t>21:16</t>
+          <t>21:10</t>
         </is>
       </c>
       <c r="C485" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D485" t="n">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="E485" t="inlineStr">
         <is>
@@ -12478,21 +12478,21 @@
     <row r="486">
       <c r="A486" t="inlineStr">
         <is>
-          <t>20:47:38</t>
+          <t>20:54:52</t>
         </is>
       </c>
       <c r="B486" t="inlineStr">
         <is>
-          <t>21:20</t>
+          <t>21:16</t>
         </is>
       </c>
       <c r="C486" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D486" t="n">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="E486" t="inlineStr">
         <is>
@@ -12503,12 +12503,12 @@
     <row r="487">
       <c r="A487" t="inlineStr">
         <is>
-          <t>20:15:27</t>
+          <t>20:54:52</t>
         </is>
       </c>
       <c r="B487" t="inlineStr">
         <is>
-          <t>21:21</t>
+          <t>21:20</t>
         </is>
       </c>
       <c r="C487" t="inlineStr">
@@ -12517,7 +12517,7 @@
         </is>
       </c>
       <c r="D487" t="n">
-        <v>66</v>
+        <v>26</v>
       </c>
       <c r="E487" t="inlineStr">
         <is>
@@ -12528,21 +12528,21 @@
     <row r="488">
       <c r="A488" t="inlineStr">
         <is>
-          <t>20:34:42</t>
+          <t>20:15:27</t>
         </is>
       </c>
       <c r="B488" t="inlineStr">
         <is>
-          <t>21:22</t>
+          <t>21:21</t>
         </is>
       </c>
       <c r="C488" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D488" t="n">
-        <v>48</v>
+        <v>66</v>
       </c>
       <c r="E488" t="inlineStr">
         <is>
@@ -12553,7 +12553,7 @@
     <row r="489">
       <c r="A489" t="inlineStr">
         <is>
-          <t>20:47:38</t>
+          <t>20:54:52</t>
         </is>
       </c>
       <c r="B489" t="inlineStr">
@@ -12567,7 +12567,7 @@
         </is>
       </c>
       <c r="D489" t="n">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="E489" t="inlineStr">
         <is>
@@ -12578,21 +12578,21 @@
     <row r="490">
       <c r="A490" t="inlineStr">
         <is>
-          <t>20:15:27</t>
+          <t>20:34:42</t>
         </is>
       </c>
       <c r="B490" t="inlineStr">
         <is>
-          <t>21:23</t>
+          <t>21:22</t>
         </is>
       </c>
       <c r="C490" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D490" t="n">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="E490" t="inlineStr">
         <is>
@@ -12633,16 +12633,16 @@
       </c>
       <c r="B492" t="inlineStr">
         <is>
-          <t>21:32</t>
+          <t>21:23</t>
         </is>
       </c>
       <c r="C492" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D492" t="n">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="E492" t="inlineStr">
         <is>
@@ -12653,12 +12653,12 @@
     <row r="493">
       <c r="A493" t="inlineStr">
         <is>
-          <t>20:47:38</t>
+          <t>20:15:27</t>
         </is>
       </c>
       <c r="B493" t="inlineStr">
         <is>
-          <t>21:34</t>
+          <t>21:32</t>
         </is>
       </c>
       <c r="C493" t="inlineStr">
@@ -12667,7 +12667,7 @@
         </is>
       </c>
       <c r="D493" t="n">
-        <v>47</v>
+        <v>77</v>
       </c>
       <c r="E493" t="inlineStr">
         <is>
@@ -12678,12 +12678,12 @@
     <row r="494">
       <c r="A494" t="inlineStr">
         <is>
-          <t>20:34:42</t>
+          <t>20:54:52</t>
         </is>
       </c>
       <c r="B494" t="inlineStr">
         <is>
-          <t>21:37</t>
+          <t>21:33</t>
         </is>
       </c>
       <c r="C494" t="inlineStr">
@@ -12692,7 +12692,7 @@
         </is>
       </c>
       <c r="D494" t="n">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="E494" t="inlineStr">
         <is>
@@ -12708,16 +12708,16 @@
       </c>
       <c r="B495" t="inlineStr">
         <is>
-          <t>21:37</t>
+          <t>21:34</t>
         </is>
       </c>
       <c r="C495" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D495" t="n">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E495" t="inlineStr">
         <is>
@@ -12728,21 +12728,21 @@
     <row r="496">
       <c r="A496" t="inlineStr">
         <is>
-          <t>20:15:27</t>
+          <t>20:54:52</t>
         </is>
       </c>
       <c r="B496" t="inlineStr">
         <is>
-          <t>21:38</t>
+          <t>21:37</t>
         </is>
       </c>
       <c r="C496" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D496" t="n">
-        <v>83</v>
+        <v>43</v>
       </c>
       <c r="E496" t="inlineStr">
         <is>
@@ -12753,21 +12753,21 @@
     <row r="497">
       <c r="A497" t="inlineStr">
         <is>
-          <t>20:47:38</t>
+          <t>20:34:42</t>
         </is>
       </c>
       <c r="B497" t="inlineStr">
         <is>
-          <t>21:38</t>
+          <t>21:37</t>
         </is>
       </c>
       <c r="C497" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D497" t="n">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="E497" t="inlineStr">
         <is>
@@ -12778,21 +12778,21 @@
     <row r="498">
       <c r="A498" t="inlineStr">
         <is>
-          <t>20:47:38</t>
+          <t>20:54:52</t>
         </is>
       </c>
       <c r="B498" t="inlineStr">
         <is>
-          <t>21:47</t>
+          <t>21:37</t>
         </is>
       </c>
       <c r="C498" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D498" t="n">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="E498" t="inlineStr">
         <is>
@@ -12803,21 +12803,21 @@
     <row r="499">
       <c r="A499" t="inlineStr">
         <is>
-          <t>20:47:38</t>
+          <t>20:15:27</t>
         </is>
       </c>
       <c r="B499" t="inlineStr">
         <is>
-          <t>21:52</t>
+          <t>21:38</t>
         </is>
       </c>
       <c r="C499" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D499" t="n">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="E499" t="inlineStr">
         <is>
@@ -12828,21 +12828,21 @@
     <row r="500">
       <c r="A500" t="inlineStr">
         <is>
-          <t>20:15:27</t>
+          <t>20:47:38</t>
         </is>
       </c>
       <c r="B500" t="inlineStr">
         <is>
-          <t>21:53</t>
+          <t>21:38</t>
         </is>
       </c>
       <c r="C500" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D500" t="n">
-        <v>98</v>
+        <v>51</v>
       </c>
       <c r="E500" t="inlineStr">
         <is>
@@ -12853,12 +12853,12 @@
     <row r="501">
       <c r="A501" t="inlineStr">
         <is>
-          <t>20:47:38</t>
+          <t>20:54:52</t>
         </is>
       </c>
       <c r="B501" t="inlineStr">
         <is>
-          <t>22:07</t>
+          <t>21:44</t>
         </is>
       </c>
       <c r="C501" t="inlineStr">
@@ -12867,7 +12867,7 @@
         </is>
       </c>
       <c r="D501" t="n">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="E501" t="inlineStr">
         <is>
@@ -12878,21 +12878,21 @@
     <row r="502">
       <c r="A502" t="inlineStr">
         <is>
-          <t>20:15:27</t>
+          <t>20:54:52</t>
         </is>
       </c>
       <c r="B502" t="inlineStr">
         <is>
-          <t>22:08</t>
+          <t>21:46</t>
         </is>
       </c>
       <c r="C502" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D502" t="n">
-        <v>113</v>
+        <v>52</v>
       </c>
       <c r="E502" t="inlineStr">
         <is>
@@ -12908,16 +12908,16 @@
       </c>
       <c r="B503" t="inlineStr">
         <is>
-          <t>22:08</t>
+          <t>21:47</t>
         </is>
       </c>
       <c r="C503" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D503" t="n">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="E503" t="inlineStr">
         <is>
@@ -12928,21 +12928,21 @@
     <row r="504">
       <c r="A504" t="inlineStr">
         <is>
-          <t>20:34:42</t>
+          <t>20:47:38</t>
         </is>
       </c>
       <c r="B504" t="inlineStr">
         <is>
-          <t>22:19</t>
+          <t>21:52</t>
         </is>
       </c>
       <c r="C504" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D504" t="n">
-        <v>105</v>
+        <v>65</v>
       </c>
       <c r="E504" t="inlineStr">
         <is>
@@ -12953,21 +12953,21 @@
     <row r="505">
       <c r="A505" t="inlineStr">
         <is>
-          <t>20:47:38</t>
+          <t>20:15:27</t>
         </is>
       </c>
       <c r="B505" t="inlineStr">
         <is>
-          <t>22:22</t>
+          <t>21:53</t>
         </is>
       </c>
       <c r="C505" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D505" t="n">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="E505" t="inlineStr">
         <is>
@@ -12978,21 +12978,21 @@
     <row r="506">
       <c r="A506" t="inlineStr">
         <is>
-          <t>20:47:38</t>
+          <t>20:54:52</t>
         </is>
       </c>
       <c r="B506" t="inlineStr">
         <is>
-          <t>22:27</t>
+          <t>22:07</t>
         </is>
       </c>
       <c r="C506" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D506" t="n">
-        <v>100</v>
+        <v>73</v>
       </c>
       <c r="E506" t="inlineStr">
         <is>
@@ -13008,16 +13008,16 @@
       </c>
       <c r="B507" t="inlineStr">
         <is>
-          <t>22:32</t>
+          <t>22:07</t>
         </is>
       </c>
       <c r="C507" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D507" t="n">
-        <v>105</v>
+        <v>80</v>
       </c>
       <c r="E507" t="inlineStr">
         <is>
@@ -13033,18 +13033,293 @@
       </c>
       <c r="B508" t="inlineStr">
         <is>
+          <t>22:08</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D508" t="n">
+        <v>81</v>
+      </c>
+      <c r="E508" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>20:15:27</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>22:08</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D509" t="n">
+        <v>113</v>
+      </c>
+      <c r="E509" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>20:34:42</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>22:19</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D510" t="n">
+        <v>105</v>
+      </c>
+      <c r="E510" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>20:54:52</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>22:21</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D511" t="n">
+        <v>87</v>
+      </c>
+      <c r="E511" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>20:47:38</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>22:22</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D512" t="n">
+        <v>95</v>
+      </c>
+      <c r="E512" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>20:54:52</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>22:26</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D513" t="n">
+        <v>92</v>
+      </c>
+      <c r="E513" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>20:54:52</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>22:27</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D514" t="n">
+        <v>93</v>
+      </c>
+      <c r="E514" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>20:54:52</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>22:31</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D515" t="n">
+        <v>97</v>
+      </c>
+      <c r="E515" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>20:47:38</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>22:32</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D516" t="n">
+        <v>105</v>
+      </c>
+      <c r="E516" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>20:54:52</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>22:38</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D517" t="n">
+        <v>104</v>
+      </c>
+      <c r="E517" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>20:47:38</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
           <t>22:39</t>
         </is>
       </c>
-      <c r="C508" t="inlineStr">
+      <c r="C518" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D508" t="n">
+      <c r="D518" t="n">
         <v>112</v>
       </c>
-      <c r="E508" t="inlineStr">
+      <c r="E518" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>20:54:52</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>22:47</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D519" t="n">
+        <v>113</v>
+      </c>
+      <c r="E519" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -13061,7 +13336,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E58"/>
+  <dimension ref="A1:E60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13079,14 +13354,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:47:38</t>
+          <t>Última actualización: 20:54:52</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 53</t>
+          <t>Total filas: 55</t>
         </is>
       </c>
     </row>
@@ -14345,7 +14620,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>20:47:38</t>
+          <t>20:54:52</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -14359,7 +14634,7 @@
         </is>
       </c>
       <c r="D55" t="n">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -14395,12 +14670,12 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>20:47:38</t>
+          <t>20:54:52</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>21:47</t>
+          <t>21:46</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -14409,7 +14684,7 @@
         </is>
       </c>
       <c r="D57" t="n">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -14425,18 +14700,68 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
+          <t>21:47</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>60</v>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>20:54:52</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>22:38</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>104</v>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>20:47:38</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
           <t>22:39</t>
         </is>
       </c>
-      <c r="C58" t="inlineStr">
+      <c r="C60" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D58" t="n">
+      <c r="D60" t="n">
         <v>112</v>
       </c>
-      <c r="E58" t="inlineStr">
+      <c r="E60" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -14471,7 +14796,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:47:38</t>
+          <t>Última actualización: 20:54:52</t>
         </is>
       </c>
     </row>
@@ -16087,7 +16412,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>20:47:38</t>
+          <t>20:54:52</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -16101,7 +16426,7 @@
         </is>
       </c>
       <c r="D69" t="n">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -16137,7 +16462,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>20:47:38</t>
+          <t>20:54:52</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -16151,7 +16476,7 @@
         </is>
       </c>
       <c r="D71" t="n">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -16187,7 +16512,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>20:47:38</t>
+          <t>20:54:52</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -16201,7 +16526,7 @@
         </is>
       </c>
       <c r="D73" t="n">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 865
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-23.xlsx
+++ b/data/horarios-141-2026-01-23.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E519"/>
+  <dimension ref="A1:E529"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:54:52</t>
+          <t>Última actualización: 21:58:42</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 514</t>
+          <t>Total filas: 524</t>
         </is>
       </c>
     </row>
@@ -1313,7 +1313,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>86_EST CHICA-ESC AGRARIA</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1338,7 +1338,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>86_EST CHICA-ESC AGRARIA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1913,7 +1913,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D63" t="n">
@@ -1938,7 +1938,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -1963,7 +1963,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D65" t="n">
@@ -1978,7 +1978,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>05:52:07</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -1988,11 +1988,11 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2003,7 +2003,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>05:52:07</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -2013,11 +2013,11 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2803,7 +2803,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>08:13:38</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -2813,11 +2813,11 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D99" t="n">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -2828,7 +2828,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>08:13:38</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -2838,11 +2838,11 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -3153,7 +3153,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>07:28:14</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3163,11 +3163,11 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>115</v>
+        <v>27</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3178,7 +3178,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>07:28:14</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
@@ -3188,11 +3188,11 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D114" t="n">
-        <v>27</v>
+        <v>115</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -3278,7 +3278,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>09:33:33</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -3288,11 +3288,11 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D118" t="n">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -3303,7 +3303,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>09:33:33</t>
+          <t>08:56:26</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -3313,11 +3313,11 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D119" t="n">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -4163,7 +4163,7 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D153" t="n">
@@ -4188,7 +4188,7 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D154" t="n">
@@ -4853,7 +4853,7 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>11:22:44</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
@@ -4863,11 +4863,11 @@
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D181" t="n">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
@@ -4878,7 +4878,7 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>11:22:44</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
@@ -4888,11 +4888,11 @@
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D182" t="n">
-        <v>44</v>
+        <v>4</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
@@ -5153,7 +5153,7 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>11:49:23</t>
+          <t>12:02:21</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
@@ -5163,11 +5163,11 @@
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D193" t="n">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
@@ -5178,7 +5178,7 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>12:02:21</t>
+          <t>11:49:23</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
@@ -5188,11 +5188,11 @@
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D194" t="n">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -5653,7 +5653,7 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>12:54:24</t>
+          <t>12:37:00</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
@@ -5663,11 +5663,11 @@
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D213" t="n">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -5678,7 +5678,7 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>12:37:00</t>
+          <t>12:54:24</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
@@ -5688,11 +5688,11 @@
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D214" t="n">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
@@ -5813,7 +5813,7 @@
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D219" t="n">
@@ -5838,7 +5838,7 @@
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D220" t="n">
@@ -5988,7 +5988,7 @@
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D226" t="n">
@@ -6013,7 +6013,7 @@
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D227" t="n">
@@ -6313,7 +6313,7 @@
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D239" t="n">
@@ -6338,7 +6338,7 @@
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D240" t="n">
@@ -6403,7 +6403,7 @@
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>13:51:20</t>
+          <t>13:18:32</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
@@ -6413,11 +6413,11 @@
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D243" t="n">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -6428,7 +6428,7 @@
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>13:18:32</t>
+          <t>13:51:20</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
@@ -6438,11 +6438,11 @@
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D244" t="n">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -6838,7 +6838,7 @@
       </c>
       <c r="C260" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D260" t="n">
@@ -6863,7 +6863,7 @@
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D261" t="n">
@@ -7013,7 +7013,7 @@
       </c>
       <c r="C267" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D267" t="n">
@@ -7038,7 +7038,7 @@
       </c>
       <c r="C268" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D268" t="n">
@@ -7238,7 +7238,7 @@
       </c>
       <c r="C276" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D276" t="n">
@@ -7263,7 +7263,7 @@
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D277" t="n">
@@ -7628,7 +7628,7 @@
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
@@ -7638,11 +7638,11 @@
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D292" t="n">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
@@ -7653,7 +7653,7 @@
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
@@ -7663,11 +7663,11 @@
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D293" t="n">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
@@ -8053,7 +8053,7 @@
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:19:35</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
@@ -8063,11 +8063,11 @@
       </c>
       <c r="C309" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D309" t="n">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
@@ -8078,7 +8078,7 @@
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>16:19:35</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
@@ -8088,11 +8088,11 @@
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D310" t="n">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="E310" t="inlineStr">
         <is>
@@ -8113,7 +8113,7 @@
       </c>
       <c r="C311" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D311" t="n">
@@ -8203,7 +8203,7 @@
     <row r="315">
       <c r="A315" t="inlineStr">
         <is>
-          <t>16:19:35</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B315" t="inlineStr">
@@ -8213,11 +8213,11 @@
       </c>
       <c r="C315" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D315" t="n">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="E315" t="inlineStr">
         <is>
@@ -8228,7 +8228,7 @@
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:19:35</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
@@ -8238,11 +8238,11 @@
       </c>
       <c r="C316" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D316" t="n">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="E316" t="inlineStr">
         <is>
@@ -8403,7 +8403,7 @@
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>16:36:35</t>
+          <t>15:55:57</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
@@ -8413,11 +8413,11 @@
       </c>
       <c r="C323" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D323" t="n">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="E323" t="inlineStr">
         <is>
@@ -8428,7 +8428,7 @@
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>15:55:57</t>
+          <t>16:36:35</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
@@ -8438,11 +8438,11 @@
       </c>
       <c r="C324" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D324" t="n">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="E324" t="inlineStr">
         <is>
@@ -8453,7 +8453,7 @@
     <row r="325">
       <c r="A325" t="inlineStr">
         <is>
-          <t>15:21:03</t>
+          <t>16:36:35</t>
         </is>
       </c>
       <c r="B325" t="inlineStr">
@@ -8463,11 +8463,11 @@
       </c>
       <c r="C325" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D325" t="n">
-        <v>82</v>
+        <v>7</v>
       </c>
       <c r="E325" t="inlineStr">
         <is>
@@ -8478,7 +8478,7 @@
     <row r="326">
       <c r="A326" t="inlineStr">
         <is>
-          <t>16:36:35</t>
+          <t>15:21:03</t>
         </is>
       </c>
       <c r="B326" t="inlineStr">
@@ -8488,11 +8488,11 @@
       </c>
       <c r="C326" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D326" t="n">
-        <v>7</v>
+        <v>82</v>
       </c>
       <c r="E326" t="inlineStr">
         <is>
@@ -8738,7 +8738,7 @@
       </c>
       <c r="C336" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D336" t="n">
@@ -8763,7 +8763,7 @@
       </c>
       <c r="C337" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D337" t="n">
@@ -8888,7 +8888,7 @@
       </c>
       <c r="C342" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D342" t="n">
@@ -8913,7 +8913,7 @@
       </c>
       <c r="C343" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D343" t="n">
@@ -9188,7 +9188,7 @@
       </c>
       <c r="C354" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D354" t="n">
@@ -9213,7 +9213,7 @@
       </c>
       <c r="C355" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D355" t="n">
@@ -9338,7 +9338,7 @@
       </c>
       <c r="C360" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D360" t="n">
@@ -9363,7 +9363,7 @@
       </c>
       <c r="C361" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D361" t="n">
@@ -9663,7 +9663,7 @@
       </c>
       <c r="C373" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D373" t="n">
@@ -9688,7 +9688,7 @@
       </c>
       <c r="C374" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D374" t="n">
@@ -10688,7 +10688,7 @@
       </c>
       <c r="C414" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D414" t="n">
@@ -10713,7 +10713,7 @@
       </c>
       <c r="C415" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D415" t="n">
@@ -10863,7 +10863,7 @@
       </c>
       <c r="C421" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D421" t="n">
@@ -10888,7 +10888,7 @@
       </c>
       <c r="C422" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D422" t="n">
@@ -10938,7 +10938,7 @@
       </c>
       <c r="C424" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D424" t="n">
@@ -10963,7 +10963,7 @@
       </c>
       <c r="C425" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D425" t="n">
@@ -11338,7 +11338,7 @@
       </c>
       <c r="C440" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D440" t="n">
@@ -11363,7 +11363,7 @@
       </c>
       <c r="C441" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D441" t="n">
@@ -11403,7 +11403,7 @@
     <row r="443">
       <c r="A443" t="inlineStr">
         <is>
-          <t>19:49:07</t>
+          <t>19:36:20</t>
         </is>
       </c>
       <c r="B443" t="inlineStr">
@@ -11413,11 +11413,11 @@
       </c>
       <c r="C443" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D443" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="E443" t="inlineStr">
         <is>
@@ -11428,7 +11428,7 @@
     <row r="444">
       <c r="A444" t="inlineStr">
         <is>
-          <t>19:36:20</t>
+          <t>19:49:07</t>
         </is>
       </c>
       <c r="B444" t="inlineStr">
@@ -11438,11 +11438,11 @@
       </c>
       <c r="C444" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D444" t="n">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="E444" t="inlineStr">
         <is>
@@ -11488,7 +11488,7 @@
       </c>
       <c r="C446" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D446" t="n">
@@ -11513,7 +11513,7 @@
       </c>
       <c r="C447" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D447" t="n">
@@ -11588,7 +11588,7 @@
       </c>
       <c r="C450" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D450" t="n">
@@ -11613,7 +11613,7 @@
       </c>
       <c r="C451" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D451" t="n">
@@ -11803,7 +11803,7 @@
     <row r="459">
       <c r="A459" t="inlineStr">
         <is>
-          <t>19:49:07</t>
+          <t>19:56:21</t>
         </is>
       </c>
       <c r="B459" t="inlineStr">
@@ -11813,11 +11813,11 @@
       </c>
       <c r="C459" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D459" t="n">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E459" t="inlineStr">
         <is>
@@ -11828,7 +11828,7 @@
     <row r="460">
       <c r="A460" t="inlineStr">
         <is>
-          <t>19:56:21</t>
+          <t>19:49:07</t>
         </is>
       </c>
       <c r="B460" t="inlineStr">
@@ -11838,11 +11838,11 @@
       </c>
       <c r="C460" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D460" t="n">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="E460" t="inlineStr">
         <is>
@@ -11953,7 +11953,7 @@
     <row r="465">
       <c r="A465" t="inlineStr">
         <is>
-          <t>20:15:27</t>
+          <t>19:56:21</t>
         </is>
       </c>
       <c r="B465" t="inlineStr">
@@ -11963,11 +11963,11 @@
       </c>
       <c r="C465" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D465" t="n">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="E465" t="inlineStr">
         <is>
@@ -11978,7 +11978,7 @@
     <row r="466">
       <c r="A466" t="inlineStr">
         <is>
-          <t>19:56:21</t>
+          <t>20:15:27</t>
         </is>
       </c>
       <c r="B466" t="inlineStr">
@@ -11988,11 +11988,11 @@
       </c>
       <c r="C466" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D466" t="n">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="E466" t="inlineStr">
         <is>
@@ -12188,7 +12188,7 @@
       </c>
       <c r="C474" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D474" t="n">
@@ -12213,7 +12213,7 @@
       </c>
       <c r="C475" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D475" t="n">
@@ -12278,7 +12278,7 @@
     <row r="478">
       <c r="A478" t="inlineStr">
         <is>
-          <t>20:54:52</t>
+          <t>19:15:13</t>
         </is>
       </c>
       <c r="B478" t="inlineStr">
@@ -12288,11 +12288,11 @@
       </c>
       <c r="C478" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D478" t="n">
-        <v>2</v>
+        <v>101</v>
       </c>
       <c r="E478" t="inlineStr">
         <is>
@@ -12303,7 +12303,7 @@
     <row r="479">
       <c r="A479" t="inlineStr">
         <is>
-          <t>19:15:13</t>
+          <t>20:54:52</t>
         </is>
       </c>
       <c r="B479" t="inlineStr">
@@ -12313,11 +12313,11 @@
       </c>
       <c r="C479" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D479" t="n">
-        <v>101</v>
+        <v>2</v>
       </c>
       <c r="E479" t="inlineStr">
         <is>
@@ -12613,7 +12613,7 @@
       </c>
       <c r="C491" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D491" t="n">
@@ -12638,7 +12638,7 @@
       </c>
       <c r="C492" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D492" t="n">
@@ -12738,7 +12738,7 @@
       </c>
       <c r="C496" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D496" t="n">
@@ -12753,7 +12753,7 @@
     <row r="497">
       <c r="A497" t="inlineStr">
         <is>
-          <t>20:34:42</t>
+          <t>20:54:52</t>
         </is>
       </c>
       <c r="B497" t="inlineStr">
@@ -12763,11 +12763,11 @@
       </c>
       <c r="C497" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D497" t="n">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="E497" t="inlineStr">
         <is>
@@ -12778,7 +12778,7 @@
     <row r="498">
       <c r="A498" t="inlineStr">
         <is>
-          <t>20:54:52</t>
+          <t>20:34:42</t>
         </is>
       </c>
       <c r="B498" t="inlineStr">
@@ -12788,11 +12788,11 @@
       </c>
       <c r="C498" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D498" t="n">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="E498" t="inlineStr">
         <is>
@@ -12803,7 +12803,7 @@
     <row r="499">
       <c r="A499" t="inlineStr">
         <is>
-          <t>20:15:27</t>
+          <t>20:47:38</t>
         </is>
       </c>
       <c r="B499" t="inlineStr">
@@ -12813,11 +12813,11 @@
       </c>
       <c r="C499" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D499" t="n">
-        <v>83</v>
+        <v>51</v>
       </c>
       <c r="E499" t="inlineStr">
         <is>
@@ -12828,7 +12828,7 @@
     <row r="500">
       <c r="A500" t="inlineStr">
         <is>
-          <t>20:47:38</t>
+          <t>20:15:27</t>
         </is>
       </c>
       <c r="B500" t="inlineStr">
@@ -12838,11 +12838,11 @@
       </c>
       <c r="C500" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D500" t="n">
-        <v>51</v>
+        <v>83</v>
       </c>
       <c r="E500" t="inlineStr">
         <is>
@@ -12978,7 +12978,7 @@
     <row r="506">
       <c r="A506" t="inlineStr">
         <is>
-          <t>20:54:52</t>
+          <t>21:58:42</t>
         </is>
       </c>
       <c r="B506" t="inlineStr">
@@ -12988,11 +12988,11 @@
       </c>
       <c r="C506" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D506" t="n">
-        <v>73</v>
+        <v>9</v>
       </c>
       <c r="E506" t="inlineStr">
         <is>
@@ -13003,7 +13003,7 @@
     <row r="507">
       <c r="A507" t="inlineStr">
         <is>
-          <t>20:47:38</t>
+          <t>20:54:52</t>
         </is>
       </c>
       <c r="B507" t="inlineStr">
@@ -13013,11 +13013,11 @@
       </c>
       <c r="C507" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D507" t="n">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E507" t="inlineStr">
         <is>
@@ -13028,7 +13028,7 @@
     <row r="508">
       <c r="A508" t="inlineStr">
         <is>
-          <t>20:47:38</t>
+          <t>20:15:27</t>
         </is>
       </c>
       <c r="B508" t="inlineStr">
@@ -13038,11 +13038,11 @@
       </c>
       <c r="C508" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D508" t="n">
-        <v>81</v>
+        <v>113</v>
       </c>
       <c r="E508" t="inlineStr">
         <is>
@@ -13053,7 +13053,7 @@
     <row r="509">
       <c r="A509" t="inlineStr">
         <is>
-          <t>20:15:27</t>
+          <t>21:58:42</t>
         </is>
       </c>
       <c r="B509" t="inlineStr">
@@ -13063,11 +13063,11 @@
       </c>
       <c r="C509" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D509" t="n">
-        <v>113</v>
+        <v>10</v>
       </c>
       <c r="E509" t="inlineStr">
         <is>
@@ -13103,12 +13103,12 @@
     <row r="511">
       <c r="A511" t="inlineStr">
         <is>
-          <t>20:54:52</t>
+          <t>21:58:42</t>
         </is>
       </c>
       <c r="B511" t="inlineStr">
         <is>
-          <t>22:21</t>
+          <t>22:20</t>
         </is>
       </c>
       <c r="C511" t="inlineStr">
@@ -13117,7 +13117,7 @@
         </is>
       </c>
       <c r="D511" t="n">
-        <v>87</v>
+        <v>22</v>
       </c>
       <c r="E511" t="inlineStr">
         <is>
@@ -13128,12 +13128,12 @@
     <row r="512">
       <c r="A512" t="inlineStr">
         <is>
-          <t>20:47:38</t>
+          <t>20:54:52</t>
         </is>
       </c>
       <c r="B512" t="inlineStr">
         <is>
-          <t>22:22</t>
+          <t>22:21</t>
         </is>
       </c>
       <c r="C512" t="inlineStr">
@@ -13142,7 +13142,7 @@
         </is>
       </c>
       <c r="D512" t="n">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="E512" t="inlineStr">
         <is>
@@ -13153,21 +13153,21 @@
     <row r="513">
       <c r="A513" t="inlineStr">
         <is>
-          <t>20:54:52</t>
+          <t>20:47:38</t>
         </is>
       </c>
       <c r="B513" t="inlineStr">
         <is>
-          <t>22:26</t>
+          <t>22:22</t>
         </is>
       </c>
       <c r="C513" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D513" t="n">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="E513" t="inlineStr">
         <is>
@@ -13178,21 +13178,21 @@
     <row r="514">
       <c r="A514" t="inlineStr">
         <is>
-          <t>20:54:52</t>
+          <t>21:58:42</t>
         </is>
       </c>
       <c r="B514" t="inlineStr">
         <is>
-          <t>22:27</t>
+          <t>22:24</t>
         </is>
       </c>
       <c r="C514" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D514" t="n">
-        <v>93</v>
+        <v>26</v>
       </c>
       <c r="E514" t="inlineStr">
         <is>
@@ -13208,16 +13208,16 @@
       </c>
       <c r="B515" t="inlineStr">
         <is>
-          <t>22:31</t>
+          <t>22:26</t>
         </is>
       </c>
       <c r="C515" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D515" t="n">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E515" t="inlineStr">
         <is>
@@ -13228,21 +13228,21 @@
     <row r="516">
       <c r="A516" t="inlineStr">
         <is>
-          <t>20:47:38</t>
+          <t>21:58:42</t>
         </is>
       </c>
       <c r="B516" t="inlineStr">
         <is>
-          <t>22:32</t>
+          <t>22:26</t>
         </is>
       </c>
       <c r="C516" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D516" t="n">
-        <v>105</v>
+        <v>28</v>
       </c>
       <c r="E516" t="inlineStr">
         <is>
@@ -13253,21 +13253,21 @@
     <row r="517">
       <c r="A517" t="inlineStr">
         <is>
-          <t>20:54:52</t>
+          <t>21:58:42</t>
         </is>
       </c>
       <c r="B517" t="inlineStr">
         <is>
-          <t>22:38</t>
+          <t>22:27</t>
         </is>
       </c>
       <c r="C517" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D517" t="n">
-        <v>104</v>
+        <v>29</v>
       </c>
       <c r="E517" t="inlineStr">
         <is>
@@ -13278,21 +13278,21 @@
     <row r="518">
       <c r="A518" t="inlineStr">
         <is>
-          <t>20:47:38</t>
+          <t>20:54:52</t>
         </is>
       </c>
       <c r="B518" t="inlineStr">
         <is>
-          <t>22:39</t>
+          <t>22:31</t>
         </is>
       </c>
       <c r="C518" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D518" t="n">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="E518" t="inlineStr">
         <is>
@@ -13303,23 +13303,273 @@
     <row r="519">
       <c r="A519" t="inlineStr">
         <is>
+          <t>20:47:38</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>22:32</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D519" t="n">
+        <v>105</v>
+      </c>
+      <c r="E519" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>21:58:42</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>22:35</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D520" t="n">
+        <v>37</v>
+      </c>
+      <c r="E520" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
           <t>20:54:52</t>
         </is>
       </c>
-      <c r="B519" t="inlineStr">
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>22:38</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D521" t="n">
+        <v>104</v>
+      </c>
+      <c r="E521" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>21:58:42</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>22:39</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D522" t="n">
+        <v>41</v>
+      </c>
+      <c r="E522" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>21:58:42</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>22:46</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D523" t="n">
+        <v>48</v>
+      </c>
+      <c r="E523" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>20:54:52</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
         <is>
           <t>22:47</t>
         </is>
       </c>
-      <c r="C519" t="inlineStr">
+      <c r="C524" t="inlineStr">
         <is>
           <t>14_ABASTO</t>
         </is>
       </c>
-      <c r="D519" t="n">
+      <c r="D524" t="n">
         <v>113</v>
       </c>
-      <c r="E519" t="inlineStr">
+      <c r="E524" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>21:58:42</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>22:48</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D525" t="n">
+        <v>50</v>
+      </c>
+      <c r="E525" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>21:58:42</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>22:53</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D526" t="n">
+        <v>55</v>
+      </c>
+      <c r="E526" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>21:58:42</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>23:07</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="D527" t="n">
+        <v>69</v>
+      </c>
+      <c r="E527" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>21:58:42</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>23:12</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D528" t="n">
+        <v>74</v>
+      </c>
+      <c r="E528" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>21:58:42</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>23:40</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="D529" t="n">
+        <v>102</v>
+      </c>
+      <c r="E529" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -13336,7 +13586,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E60"/>
+  <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13354,14 +13604,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:54:52</t>
+          <t>Última actualización: 21:58:42</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 55</t>
+          <t>Total filas: 56</t>
         </is>
       </c>
     </row>
@@ -14745,7 +14995,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>20:47:38</t>
+          <t>21:58:42</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -14759,9 +15009,34 @@
         </is>
       </c>
       <c r="D60" t="n">
-        <v>112</v>
+        <v>41</v>
       </c>
       <c r="E60" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>21:58:42</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>23:40</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>102</v>
+      </c>
+      <c r="E61" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -14778,7 +15053,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E73"/>
+  <dimension ref="A1:E76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14796,14 +15071,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:54:52</t>
+          <t>Última actualización: 21:58:42</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 68</t>
+          <t>Total filas: 71</t>
         </is>
       </c>
     </row>
@@ -16462,12 +16737,12 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>20:54:52</t>
+          <t>21:58:42</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>22:04</t>
+          <t>21:58</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -16476,7 +16751,7 @@
         </is>
       </c>
       <c r="D71" t="n">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -16487,12 +16762,12 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>20:15:27</t>
+          <t>20:54:52</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>22:05</t>
+          <t>22:04</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -16501,7 +16776,7 @@
         </is>
       </c>
       <c r="D72" t="n">
-        <v>110</v>
+        <v>70</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -16512,23 +16787,98 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
+          <t>20:15:27</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>22:05</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>110</v>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
           <t>20:54:52</t>
         </is>
       </c>
-      <c r="B73" t="inlineStr">
+      <c r="B74" t="inlineStr">
         <is>
           <t>22:20</t>
         </is>
       </c>
-      <c r="C73" t="inlineStr">
+      <c r="C74" t="inlineStr">
         <is>
           <t>215B_LP-P MOR-40 Y 115</t>
         </is>
       </c>
-      <c r="D73" t="n">
+      <c r="D74" t="n">
         <v>86</v>
       </c>
-      <c r="E73" t="inlineStr">
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>21:58:42</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>22:23</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-40 Y 115</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>25</v>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>21:58:42</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>23:07</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>69</v>
+      </c>
+      <c r="E76" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>